<commit_message>
Atualização de bases das ligas, do dia: 24-02-2024 às 23:13
</commit_message>
<xml_diff>
--- a/Algeria Division 1/Algeria Division 1.xlsx
+++ b/Algeria Division 1/Algeria Division 1.xlsx
@@ -17265,7 +17265,7 @@
         <v>187</v>
       </c>
       <c r="B189">
-        <v>7624664</v>
+        <v>7624657</v>
       </c>
       <c r="C189" t="s">
         <v>28</v>
@@ -17277,73 +17277,73 @@
         <v>45296.46875</v>
       </c>
       <c r="F189" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G189" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="H189">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I189">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J189" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="K189">
-        <v>2.2</v>
+        <v>3</v>
       </c>
       <c r="L189">
         <v>2.8</v>
       </c>
       <c r="M189">
-        <v>3.25</v>
+        <v>2.375</v>
       </c>
       <c r="N189">
-        <v>2.4</v>
+        <v>4.333</v>
       </c>
       <c r="O189">
-        <v>2.7</v>
+        <v>3</v>
       </c>
       <c r="P189">
-        <v>3</v>
+        <v>1.85</v>
       </c>
       <c r="Q189">
-        <v>-0.25</v>
+        <v>0.5</v>
       </c>
       <c r="R189">
-        <v>2.05</v>
+        <v>1.85</v>
       </c>
       <c r="S189">
-        <v>1.75</v>
+        <v>1.95</v>
       </c>
       <c r="T189">
-        <v>1.75</v>
+        <v>2</v>
       </c>
       <c r="U189">
-        <v>1.9</v>
+        <v>2.025</v>
       </c>
       <c r="V189">
-        <v>1.9</v>
+        <v>1.775</v>
       </c>
       <c r="W189">
-        <v>1.4</v>
+        <v>-1</v>
       </c>
       <c r="X189">
         <v>-1</v>
       </c>
       <c r="Y189">
-        <v>-1</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="Z189">
-        <v>1.05</v>
+        <v>-1</v>
       </c>
       <c r="AA189">
-        <v>-1</v>
+        <v>0.95</v>
       </c>
       <c r="AB189">
-        <v>0.8999999999999999</v>
+        <v>1.025</v>
       </c>
       <c r="AC189">
         <v>-1</v>
@@ -17443,7 +17443,7 @@
         <v>189</v>
       </c>
       <c r="B191">
-        <v>7624657</v>
+        <v>7624664</v>
       </c>
       <c r="C191" t="s">
         <v>28</v>
@@ -17455,73 +17455,73 @@
         <v>45296.46875</v>
       </c>
       <c r="F191" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G191" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="H191">
+        <v>2</v>
+      </c>
+      <c r="I191">
         <v>1</v>
       </c>
-      <c r="I191">
-        <v>4</v>
-      </c>
       <c r="J191" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="K191">
-        <v>3</v>
+        <v>2.2</v>
       </c>
       <c r="L191">
         <v>2.8</v>
       </c>
       <c r="M191">
-        <v>2.375</v>
+        <v>3.25</v>
       </c>
       <c r="N191">
-        <v>4.333</v>
+        <v>2.4</v>
       </c>
       <c r="O191">
+        <v>2.7</v>
+      </c>
+      <c r="P191">
         <v>3</v>
       </c>
-      <c r="P191">
-        <v>1.85</v>
-      </c>
       <c r="Q191">
-        <v>0.5</v>
+        <v>-0.25</v>
       </c>
       <c r="R191">
-        <v>1.85</v>
+        <v>2.05</v>
       </c>
       <c r="S191">
-        <v>1.95</v>
+        <v>1.75</v>
       </c>
       <c r="T191">
-        <v>2</v>
+        <v>1.75</v>
       </c>
       <c r="U191">
-        <v>2.025</v>
+        <v>1.9</v>
       </c>
       <c r="V191">
-        <v>1.775</v>
+        <v>1.9</v>
       </c>
       <c r="W191">
-        <v>-1</v>
+        <v>1.4</v>
       </c>
       <c r="X191">
         <v>-1</v>
       </c>
       <c r="Y191">
-        <v>0.8500000000000001</v>
+        <v>-1</v>
       </c>
       <c r="Z191">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="AA191">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
       <c r="AB191">
-        <v>1.025</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AC191">
         <v>-1</v>
@@ -18867,7 +18867,7 @@
         <v>205</v>
       </c>
       <c r="B207">
-        <v>7567342</v>
+        <v>7567343</v>
       </c>
       <c r="C207" t="s">
         <v>28</v>
@@ -18879,76 +18879,76 @@
         <v>45310.47916666666</v>
       </c>
       <c r="F207" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="G207" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="H207">
         <v>1</v>
       </c>
       <c r="I207">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J207" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K207">
-        <v>2.5</v>
+        <v>1.727</v>
       </c>
       <c r="L207">
-        <v>2.8</v>
+        <v>3.4</v>
       </c>
       <c r="M207">
-        <v>2.8</v>
+        <v>4.2</v>
       </c>
       <c r="N207">
-        <v>2.375</v>
+        <v>2.15</v>
       </c>
       <c r="O207">
-        <v>2.7</v>
+        <v>3</v>
       </c>
       <c r="P207">
-        <v>3.2</v>
+        <v>3.1</v>
       </c>
       <c r="Q207">
-        <v>0</v>
+        <v>-0.25</v>
       </c>
       <c r="R207">
-        <v>1.725</v>
+        <v>1.95</v>
       </c>
       <c r="S207">
-        <v>2.075</v>
+        <v>1.85</v>
       </c>
       <c r="T207">
         <v>1.75</v>
       </c>
       <c r="U207">
-        <v>1.775</v>
+        <v>1.75</v>
       </c>
       <c r="V207">
-        <v>2.025</v>
+        <v>2.05</v>
       </c>
       <c r="W207">
-        <v>-1</v>
+        <v>1.15</v>
       </c>
       <c r="X207">
-        <v>1.7</v>
+        <v>-1</v>
       </c>
       <c r="Y207">
         <v>-1</v>
       </c>
       <c r="Z207">
-        <v>0</v>
+        <v>0.95</v>
       </c>
       <c r="AA207">
-        <v>-0</v>
+        <v>-1</v>
       </c>
       <c r="AB207">
-        <v>0.3875</v>
+        <v>-1</v>
       </c>
       <c r="AC207">
-        <v>-0.5</v>
+        <v>1.05</v>
       </c>
     </row>
     <row r="208" spans="1:29">
@@ -18956,7 +18956,7 @@
         <v>206</v>
       </c>
       <c r="B208">
-        <v>7567343</v>
+        <v>7567342</v>
       </c>
       <c r="C208" t="s">
         <v>28</v>
@@ -18968,76 +18968,76 @@
         <v>45310.47916666666</v>
       </c>
       <c r="F208" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="G208" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="H208">
         <v>1</v>
       </c>
       <c r="I208">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J208" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="K208">
-        <v>1.727</v>
+        <v>2.5</v>
       </c>
       <c r="L208">
-        <v>3.4</v>
+        <v>2.8</v>
       </c>
       <c r="M208">
-        <v>4.2</v>
+        <v>2.8</v>
       </c>
       <c r="N208">
-        <v>2.15</v>
+        <v>2.375</v>
       </c>
       <c r="O208">
-        <v>3</v>
+        <v>2.7</v>
       </c>
       <c r="P208">
-        <v>3.1</v>
+        <v>3.2</v>
       </c>
       <c r="Q208">
-        <v>-0.25</v>
+        <v>0</v>
       </c>
       <c r="R208">
-        <v>1.95</v>
+        <v>1.725</v>
       </c>
       <c r="S208">
-        <v>1.85</v>
+        <v>2.075</v>
       </c>
       <c r="T208">
         <v>1.75</v>
       </c>
       <c r="U208">
-        <v>1.75</v>
+        <v>1.775</v>
       </c>
       <c r="V208">
-        <v>2.05</v>
+        <v>2.025</v>
       </c>
       <c r="W208">
-        <v>1.15</v>
+        <v>-1</v>
       </c>
       <c r="X208">
-        <v>-1</v>
+        <v>1.7</v>
       </c>
       <c r="Y208">
         <v>-1</v>
       </c>
       <c r="Z208">
-        <v>0.95</v>
+        <v>0</v>
       </c>
       <c r="AA208">
-        <v>-1</v>
+        <v>-0</v>
       </c>
       <c r="AB208">
-        <v>-1</v>
+        <v>0.3875</v>
       </c>
       <c r="AC208">
-        <v>1.05</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="209" spans="1:29">

</xml_diff>

<commit_message>
Atualização de bases das ligas, do dia: 03-04-2024 às 22:09
</commit_message>
<xml_diff>
--- a/Algeria Division 1/Algeria Division 1.xlsx
+++ b/Algeria Division 1/Algeria Division 1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1042" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1054" uniqueCount="49">
   <si>
     <t>id</t>
   </si>
@@ -522,7 +522,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AC204"/>
+  <dimension ref="A1:AC207"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -8451,7 +8451,7 @@
         <v>88</v>
       </c>
       <c r="B90">
-        <v>7480688</v>
+        <v>7480684</v>
       </c>
       <c r="C90" t="s">
         <v>28</v>
@@ -8463,76 +8463,76 @@
         <v>45254.46875</v>
       </c>
       <c r="F90" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="G90" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H90">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I90">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J90" t="s">
         <v>48</v>
       </c>
       <c r="K90">
-        <v>1.7</v>
+        <v>1.85</v>
       </c>
       <c r="L90">
-        <v>3.2</v>
+        <v>3</v>
       </c>
       <c r="M90">
-        <v>4.75</v>
+        <v>4.25</v>
       </c>
       <c r="N90">
-        <v>1.95</v>
+        <v>2</v>
       </c>
       <c r="O90">
-        <v>3</v>
+        <v>2.9</v>
       </c>
       <c r="P90">
         <v>3.8</v>
       </c>
       <c r="Q90">
+        <v>-0.25</v>
+      </c>
+      <c r="R90">
+        <v>1.75</v>
+      </c>
+      <c r="S90">
+        <v>2.05</v>
+      </c>
+      <c r="T90">
+        <v>1.75</v>
+      </c>
+      <c r="U90">
+        <v>1.75</v>
+      </c>
+      <c r="V90">
+        <v>2.05</v>
+      </c>
+      <c r="W90">
+        <v>-1</v>
+      </c>
+      <c r="X90">
+        <v>1.9</v>
+      </c>
+      <c r="Y90">
+        <v>-1</v>
+      </c>
+      <c r="Z90">
         <v>-0.5</v>
       </c>
-      <c r="R90">
-        <v>1.975</v>
-      </c>
-      <c r="S90">
-        <v>1.825</v>
-      </c>
-      <c r="T90">
-        <v>2</v>
-      </c>
-      <c r="U90">
-        <v>1.925</v>
-      </c>
-      <c r="V90">
-        <v>1.875</v>
-      </c>
-      <c r="W90">
-        <v>-1</v>
-      </c>
-      <c r="X90">
-        <v>2</v>
-      </c>
-      <c r="Y90">
-        <v>-1</v>
-      </c>
-      <c r="Z90">
-        <v>-1</v>
-      </c>
       <c r="AA90">
-        <v>0.825</v>
+        <v>0.5249999999999999</v>
       </c>
       <c r="AB90">
-        <v>-1</v>
+        <v>0.375</v>
       </c>
       <c r="AC90">
-        <v>0.875</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="91" spans="1:29">
@@ -8540,7 +8540,7 @@
         <v>89</v>
       </c>
       <c r="B91">
-        <v>7480684</v>
+        <v>7480688</v>
       </c>
       <c r="C91" t="s">
         <v>28</v>
@@ -8552,76 +8552,76 @@
         <v>45254.46875</v>
       </c>
       <c r="F91" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="G91" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="H91">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I91">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J91" t="s">
         <v>48</v>
       </c>
       <c r="K91">
-        <v>1.85</v>
+        <v>1.7</v>
       </c>
       <c r="L91">
+        <v>3.2</v>
+      </c>
+      <c r="M91">
+        <v>4.75</v>
+      </c>
+      <c r="N91">
+        <v>1.95</v>
+      </c>
+      <c r="O91">
         <v>3</v>
-      </c>
-      <c r="M91">
-        <v>4.25</v>
-      </c>
-      <c r="N91">
-        <v>2</v>
-      </c>
-      <c r="O91">
-        <v>2.9</v>
       </c>
       <c r="P91">
         <v>3.8</v>
       </c>
       <c r="Q91">
-        <v>-0.25</v>
+        <v>-0.5</v>
       </c>
       <c r="R91">
-        <v>1.75</v>
+        <v>1.975</v>
       </c>
       <c r="S91">
-        <v>2.05</v>
+        <v>1.825</v>
       </c>
       <c r="T91">
-        <v>1.75</v>
+        <v>2</v>
       </c>
       <c r="U91">
-        <v>1.75</v>
+        <v>1.925</v>
       </c>
       <c r="V91">
-        <v>2.05</v>
+        <v>1.875</v>
       </c>
       <c r="W91">
         <v>-1</v>
       </c>
       <c r="X91">
-        <v>1.9</v>
+        <v>2</v>
       </c>
       <c r="Y91">
         <v>-1</v>
       </c>
       <c r="Z91">
-        <v>-0.5</v>
+        <v>-1</v>
       </c>
       <c r="AA91">
-        <v>0.5249999999999999</v>
+        <v>0.825</v>
       </c>
       <c r="AB91">
-        <v>0.375</v>
+        <v>-1</v>
       </c>
       <c r="AC91">
-        <v>-0.5</v>
+        <v>0.875</v>
       </c>
     </row>
     <row r="92" spans="1:29">
@@ -11299,7 +11299,7 @@
         <v>120</v>
       </c>
       <c r="B122">
-        <v>7656900</v>
+        <v>7624657</v>
       </c>
       <c r="C122" t="s">
         <v>28</v>
@@ -11311,55 +11311,55 @@
         <v>45296.46875</v>
       </c>
       <c r="F122" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="G122" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="H122">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I122">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J122" t="s">
         <v>46</v>
       </c>
       <c r="K122">
-        <v>1.833</v>
+        <v>3</v>
       </c>
       <c r="L122">
-        <v>3.1</v>
+        <v>2.8</v>
       </c>
       <c r="M122">
-        <v>4</v>
+        <v>2.375</v>
       </c>
       <c r="N122">
-        <v>2.875</v>
+        <v>4.333</v>
       </c>
       <c r="O122">
         <v>3</v>
       </c>
       <c r="P122">
-        <v>2.625</v>
+        <v>1.85</v>
       </c>
       <c r="Q122">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="R122">
-        <v>1.975</v>
+        <v>1.85</v>
       </c>
       <c r="S122">
-        <v>1.825</v>
+        <v>1.95</v>
       </c>
       <c r="T122">
         <v>2</v>
       </c>
       <c r="U122">
-        <v>1.925</v>
+        <v>2.025</v>
       </c>
       <c r="V122">
-        <v>1.875</v>
+        <v>1.775</v>
       </c>
       <c r="W122">
         <v>-1</v>
@@ -11368,19 +11368,19 @@
         <v>-1</v>
       </c>
       <c r="Y122">
-        <v>1.625</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="Z122">
         <v>-1</v>
       </c>
       <c r="AA122">
-        <v>0.825</v>
+        <v>0.95</v>
       </c>
       <c r="AB122">
-        <v>-1</v>
+        <v>1.025</v>
       </c>
       <c r="AC122">
-        <v>0.875</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="123" spans="1:29">
@@ -11477,7 +11477,7 @@
         <v>122</v>
       </c>
       <c r="B124">
-        <v>7624657</v>
+        <v>7656900</v>
       </c>
       <c r="C124" t="s">
         <v>28</v>
@@ -11489,55 +11489,55 @@
         <v>45296.46875</v>
       </c>
       <c r="F124" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="G124" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="H124">
+        <v>0</v>
+      </c>
+      <c r="I124">
         <v>1</v>
-      </c>
-      <c r="I124">
-        <v>4</v>
       </c>
       <c r="J124" t="s">
         <v>46</v>
       </c>
       <c r="K124">
-        <v>3</v>
+        <v>1.833</v>
       </c>
       <c r="L124">
-        <v>2.8</v>
+        <v>3.1</v>
       </c>
       <c r="M124">
-        <v>2.375</v>
+        <v>4</v>
       </c>
       <c r="N124">
-        <v>4.333</v>
+        <v>2.875</v>
       </c>
       <c r="O124">
         <v>3</v>
       </c>
       <c r="P124">
-        <v>1.85</v>
+        <v>2.625</v>
       </c>
       <c r="Q124">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="R124">
-        <v>1.85</v>
+        <v>1.975</v>
       </c>
       <c r="S124">
-        <v>1.95</v>
+        <v>1.825</v>
       </c>
       <c r="T124">
         <v>2</v>
       </c>
       <c r="U124">
-        <v>2.025</v>
+        <v>1.925</v>
       </c>
       <c r="V124">
-        <v>1.775</v>
+        <v>1.875</v>
       </c>
       <c r="W124">
         <v>-1</v>
@@ -11546,19 +11546,19 @@
         <v>-1</v>
       </c>
       <c r="Y124">
-        <v>0.8500000000000001</v>
+        <v>1.625</v>
       </c>
       <c r="Z124">
         <v>-1</v>
       </c>
       <c r="AA124">
-        <v>0.95</v>
+        <v>0.825</v>
       </c>
       <c r="AB124">
-        <v>1.025</v>
+        <v>-1</v>
       </c>
       <c r="AC124">
-        <v>-1</v>
+        <v>0.875</v>
       </c>
     </row>
     <row r="125" spans="1:29">
@@ -16283,7 +16283,7 @@
         <v>176</v>
       </c>
       <c r="B178">
-        <v>7823445</v>
+        <v>7823446</v>
       </c>
       <c r="C178" t="s">
         <v>28</v>
@@ -16295,13 +16295,13 @@
         <v>45346.53125</v>
       </c>
       <c r="F178" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="G178" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="H178">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I178">
         <v>1</v>
@@ -16310,43 +16310,43 @@
         <v>47</v>
       </c>
       <c r="K178">
-        <v>1.666</v>
+        <v>1.444</v>
       </c>
       <c r="L178">
-        <v>3.25</v>
+        <v>3.5</v>
       </c>
       <c r="M178">
-        <v>5</v>
+        <v>7.5</v>
       </c>
       <c r="N178">
-        <v>1.25</v>
+        <v>1.45</v>
       </c>
       <c r="O178">
-        <v>4.333</v>
+        <v>3.6</v>
       </c>
       <c r="P178">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="Q178">
-        <v>-1.5</v>
+        <v>-1</v>
       </c>
       <c r="R178">
-        <v>1.95</v>
+        <v>1.8</v>
       </c>
       <c r="S178">
-        <v>1.85</v>
+        <v>2</v>
       </c>
       <c r="T178">
         <v>2.25</v>
       </c>
       <c r="U178">
+        <v>1.925</v>
+      </c>
+      <c r="V178">
         <v>1.875</v>
       </c>
-      <c r="V178">
-        <v>1.925</v>
-      </c>
       <c r="W178">
-        <v>0.25</v>
+        <v>0.45</v>
       </c>
       <c r="X178">
         <v>-1</v>
@@ -16355,13 +16355,13 @@
         <v>-1</v>
       </c>
       <c r="Z178">
-        <v>-1</v>
+        <v>0.8</v>
       </c>
       <c r="AA178">
-        <v>0.8500000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AB178">
-        <v>0.875</v>
+        <v>0.925</v>
       </c>
       <c r="AC178">
         <v>-1</v>
@@ -16372,7 +16372,7 @@
         <v>177</v>
       </c>
       <c r="B179">
-        <v>7823446</v>
+        <v>7823445</v>
       </c>
       <c r="C179" t="s">
         <v>28</v>
@@ -16384,13 +16384,13 @@
         <v>45346.53125</v>
       </c>
       <c r="F179" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="G179" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="H179">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I179">
         <v>1</v>
@@ -16399,43 +16399,43 @@
         <v>47</v>
       </c>
       <c r="K179">
-        <v>1.444</v>
+        <v>1.666</v>
       </c>
       <c r="L179">
-        <v>3.5</v>
+        <v>3.25</v>
       </c>
       <c r="M179">
-        <v>7.5</v>
+        <v>5</v>
       </c>
       <c r="N179">
-        <v>1.45</v>
+        <v>1.25</v>
       </c>
       <c r="O179">
-        <v>3.6</v>
+        <v>4.333</v>
       </c>
       <c r="P179">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="Q179">
-        <v>-1</v>
+        <v>-1.5</v>
       </c>
       <c r="R179">
-        <v>1.8</v>
+        <v>1.95</v>
       </c>
       <c r="S179">
-        <v>2</v>
+        <v>1.85</v>
       </c>
       <c r="T179">
         <v>2.25</v>
       </c>
       <c r="U179">
+        <v>1.875</v>
+      </c>
+      <c r="V179">
         <v>1.925</v>
       </c>
-      <c r="V179">
-        <v>1.875</v>
-      </c>
       <c r="W179">
-        <v>0.45</v>
+        <v>0.25</v>
       </c>
       <c r="X179">
         <v>-1</v>
@@ -16444,13 +16444,13 @@
         <v>-1</v>
       </c>
       <c r="Z179">
-        <v>0.8</v>
+        <v>-1</v>
       </c>
       <c r="AA179">
-        <v>-1</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AB179">
-        <v>0.925</v>
+        <v>0.875</v>
       </c>
       <c r="AC179">
         <v>-1</v>
@@ -18152,7 +18152,7 @@
         <v>197</v>
       </c>
       <c r="B199">
-        <v>7971568</v>
+        <v>7971570</v>
       </c>
       <c r="C199" t="s">
         <v>28</v>
@@ -18164,76 +18164,76 @@
         <v>45375.75</v>
       </c>
       <c r="F199" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="G199" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="H199">
         <v>0</v>
       </c>
       <c r="I199">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J199" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="K199">
-        <v>1.5</v>
+        <v>2.25</v>
       </c>
       <c r="L199">
-        <v>3.6</v>
+        <v>2.875</v>
       </c>
       <c r="M199">
-        <v>6</v>
+        <v>3.1</v>
       </c>
       <c r="N199">
-        <v>1.5</v>
+        <v>2.4</v>
       </c>
       <c r="O199">
-        <v>3.8</v>
+        <v>2.8</v>
       </c>
       <c r="P199">
-        <v>5.25</v>
+        <v>2.8</v>
       </c>
       <c r="Q199">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="R199">
-        <v>1.925</v>
+        <v>1.975</v>
       </c>
       <c r="S199">
-        <v>1.875</v>
+        <v>1.825</v>
       </c>
       <c r="T199">
-        <v>2.5</v>
+        <v>1.75</v>
       </c>
       <c r="U199">
-        <v>1.95</v>
+        <v>1.775</v>
       </c>
       <c r="V199">
-        <v>1.85</v>
+        <v>2.025</v>
       </c>
       <c r="W199">
         <v>-1</v>
       </c>
       <c r="X199">
-        <v>2.8</v>
+        <v>-1</v>
       </c>
       <c r="Y199">
-        <v>-1</v>
+        <v>1.8</v>
       </c>
       <c r="Z199">
         <v>-1</v>
       </c>
       <c r="AA199">
-        <v>0.875</v>
+        <v>0.825</v>
       </c>
       <c r="AB199">
         <v>-1</v>
       </c>
       <c r="AC199">
-        <v>0.8500000000000001</v>
+        <v>1.025</v>
       </c>
     </row>
     <row r="200" spans="1:29">
@@ -18241,7 +18241,7 @@
         <v>198</v>
       </c>
       <c r="B200">
-        <v>7971570</v>
+        <v>7971568</v>
       </c>
       <c r="C200" t="s">
         <v>28</v>
@@ -18253,76 +18253,76 @@
         <v>45375.75</v>
       </c>
       <c r="F200" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="G200" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="H200">
         <v>0</v>
       </c>
       <c r="I200">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J200" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="K200">
-        <v>2.25</v>
+        <v>1.5</v>
       </c>
       <c r="L200">
-        <v>2.875</v>
+        <v>3.6</v>
       </c>
       <c r="M200">
-        <v>3.1</v>
+        <v>6</v>
       </c>
       <c r="N200">
-        <v>2.4</v>
+        <v>1.5</v>
       </c>
       <c r="O200">
+        <v>3.8</v>
+      </c>
+      <c r="P200">
+        <v>5.25</v>
+      </c>
+      <c r="Q200">
+        <v>-1</v>
+      </c>
+      <c r="R200">
+        <v>1.925</v>
+      </c>
+      <c r="S200">
+        <v>1.875</v>
+      </c>
+      <c r="T200">
+        <v>2.5</v>
+      </c>
+      <c r="U200">
+        <v>1.95</v>
+      </c>
+      <c r="V200">
+        <v>1.85</v>
+      </c>
+      <c r="W200">
+        <v>-1</v>
+      </c>
+      <c r="X200">
         <v>2.8</v>
       </c>
-      <c r="P200">
-        <v>2.8</v>
-      </c>
-      <c r="Q200">
-        <v>0</v>
-      </c>
-      <c r="R200">
-        <v>1.975</v>
-      </c>
-      <c r="S200">
-        <v>1.825</v>
-      </c>
-      <c r="T200">
-        <v>1.75</v>
-      </c>
-      <c r="U200">
-        <v>1.775</v>
-      </c>
-      <c r="V200">
-        <v>2.025</v>
-      </c>
-      <c r="W200">
-        <v>-1</v>
-      </c>
-      <c r="X200">
-        <v>-1</v>
-      </c>
       <c r="Y200">
-        <v>1.8</v>
+        <v>-1</v>
       </c>
       <c r="Z200">
         <v>-1</v>
       </c>
       <c r="AA200">
-        <v>0.825</v>
+        <v>0.875</v>
       </c>
       <c r="AB200">
         <v>-1</v>
       </c>
       <c r="AC200">
-        <v>1.025</v>
+        <v>0.8500000000000001</v>
       </c>
     </row>
     <row r="201" spans="1:29">
@@ -18624,45 +18624,267 @@
         <v>5</v>
       </c>
       <c r="N204">
-        <v>1.615</v>
+        <v>1.5</v>
       </c>
       <c r="O204">
-        <v>3.4</v>
+        <v>3.5</v>
       </c>
       <c r="P204">
+        <v>7</v>
+      </c>
+      <c r="Q204">
+        <v>-1</v>
+      </c>
+      <c r="R204">
+        <v>1.925</v>
+      </c>
+      <c r="S204">
+        <v>1.875</v>
+      </c>
+      <c r="T204">
+        <v>2</v>
+      </c>
+      <c r="U204">
+        <v>1.875</v>
+      </c>
+      <c r="V204">
+        <v>1.925</v>
+      </c>
+      <c r="W204">
+        <v>0</v>
+      </c>
+      <c r="X204">
+        <v>0</v>
+      </c>
+      <c r="Y204">
+        <v>0</v>
+      </c>
+      <c r="Z204">
+        <v>0</v>
+      </c>
+      <c r="AA204">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="205" spans="1:29">
+      <c r="A205" s="1">
+        <v>203</v>
+      </c>
+      <c r="B205">
+        <v>8007202</v>
+      </c>
+      <c r="C205" t="s">
+        <v>28</v>
+      </c>
+      <c r="D205" t="s">
+        <v>28</v>
+      </c>
+      <c r="E205" s="2">
+        <v>45387.48958333334</v>
+      </c>
+      <c r="F205" t="s">
+        <v>29</v>
+      </c>
+      <c r="G205" t="s">
+        <v>38</v>
+      </c>
+      <c r="K205">
+        <v>1.533</v>
+      </c>
+      <c r="L205">
+        <v>3.6</v>
+      </c>
+      <c r="M205">
         <v>5.5</v>
       </c>
-      <c r="Q204">
+      <c r="N205">
+        <v>1.571</v>
+      </c>
+      <c r="O205">
+        <v>3.5</v>
+      </c>
+      <c r="P205">
+        <v>5.25</v>
+      </c>
+      <c r="Q205">
         <v>-0.75</v>
       </c>
-      <c r="R204">
+      <c r="R205">
+        <v>1.775</v>
+      </c>
+      <c r="S205">
+        <v>2.025</v>
+      </c>
+      <c r="T205">
+        <v>2</v>
+      </c>
+      <c r="U205">
         <v>1.825</v>
       </c>
-      <c r="S204">
+      <c r="V205">
         <v>1.975</v>
       </c>
-      <c r="T204">
-        <v>2</v>
-      </c>
-      <c r="U204">
+      <c r="W205">
+        <v>0</v>
+      </c>
+      <c r="X205">
+        <v>0</v>
+      </c>
+      <c r="Y205">
+        <v>0</v>
+      </c>
+      <c r="Z205">
+        <v>0</v>
+      </c>
+      <c r="AA205">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="206" spans="1:29">
+      <c r="A206" s="1">
+        <v>204</v>
+      </c>
+      <c r="B206">
+        <v>8007204</v>
+      </c>
+      <c r="C206" t="s">
+        <v>28</v>
+      </c>
+      <c r="D206" t="s">
+        <v>28</v>
+      </c>
+      <c r="E206" s="2">
+        <v>45387.75</v>
+      </c>
+      <c r="F206" t="s">
+        <v>42</v>
+      </c>
+      <c r="G206" t="s">
+        <v>33</v>
+      </c>
+      <c r="K206">
+        <v>2</v>
+      </c>
+      <c r="L206">
+        <v>3</v>
+      </c>
+      <c r="M206">
+        <v>3.6</v>
+      </c>
+      <c r="N206">
+        <v>2.1</v>
+      </c>
+      <c r="O206">
+        <v>2.9</v>
+      </c>
+      <c r="P206">
+        <v>3.3</v>
+      </c>
+      <c r="Q206">
+        <v>-0.25</v>
+      </c>
+      <c r="R206">
+        <v>1.875</v>
+      </c>
+      <c r="S206">
+        <v>1.925</v>
+      </c>
+      <c r="T206">
+        <v>2</v>
+      </c>
+      <c r="U206">
         <v>1.825</v>
       </c>
-      <c r="V204">
+      <c r="V206">
         <v>1.975</v>
       </c>
-      <c r="W204">
-        <v>0</v>
-      </c>
-      <c r="X204">
-        <v>0</v>
-      </c>
-      <c r="Y204">
-        <v>0</v>
-      </c>
-      <c r="Z204">
-        <v>0</v>
-      </c>
-      <c r="AA204">
+      <c r="W206">
+        <v>0</v>
+      </c>
+      <c r="X206">
+        <v>0</v>
+      </c>
+      <c r="Y206">
+        <v>0</v>
+      </c>
+      <c r="Z206">
+        <v>0</v>
+      </c>
+      <c r="AA206">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="207" spans="1:29">
+      <c r="A207" s="1">
+        <v>205</v>
+      </c>
+      <c r="B207">
+        <v>8007205</v>
+      </c>
+      <c r="C207" t="s">
+        <v>28</v>
+      </c>
+      <c r="D207" t="s">
+        <v>28</v>
+      </c>
+      <c r="E207" s="2">
+        <v>45387.75</v>
+      </c>
+      <c r="F207" t="s">
+        <v>32</v>
+      </c>
+      <c r="G207" t="s">
+        <v>36</v>
+      </c>
+      <c r="K207">
+        <v>1.571</v>
+      </c>
+      <c r="L207">
+        <v>3.6</v>
+      </c>
+      <c r="M207">
+        <v>5</v>
+      </c>
+      <c r="N207">
+        <v>1.85</v>
+      </c>
+      <c r="O207">
+        <v>3.3</v>
+      </c>
+      <c r="P207">
+        <v>3.6</v>
+      </c>
+      <c r="Q207">
+        <v>-0.5</v>
+      </c>
+      <c r="R207">
+        <v>1.975</v>
+      </c>
+      <c r="S207">
+        <v>1.825</v>
+      </c>
+      <c r="T207">
+        <v>2</v>
+      </c>
+      <c r="U207">
+        <v>1.825</v>
+      </c>
+      <c r="V207">
+        <v>1.975</v>
+      </c>
+      <c r="W207">
+        <v>0</v>
+      </c>
+      <c r="X207">
+        <v>0</v>
+      </c>
+      <c r="Y207">
+        <v>0</v>
+      </c>
+      <c r="Z207">
+        <v>0</v>
+      </c>
+      <c r="AA207">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização de bases das ligas, do dia: 04-04-2024 às 23:22
</commit_message>
<xml_diff>
--- a/Algeria Division 1/Algeria Division 1.xlsx
+++ b/Algeria Division 1/Algeria Division 1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1054" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1050" uniqueCount="49">
   <si>
     <t>id</t>
   </si>
@@ -522,7 +522,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AC207"/>
+  <dimension ref="A1:AC206"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -8451,7 +8451,7 @@
         <v>88</v>
       </c>
       <c r="B90">
-        <v>7480684</v>
+        <v>7480688</v>
       </c>
       <c r="C90" t="s">
         <v>28</v>
@@ -8463,76 +8463,76 @@
         <v>45254.46875</v>
       </c>
       <c r="F90" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="G90" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="H90">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I90">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J90" t="s">
         <v>48</v>
       </c>
       <c r="K90">
-        <v>1.85</v>
+        <v>1.7</v>
       </c>
       <c r="L90">
+        <v>3.2</v>
+      </c>
+      <c r="M90">
+        <v>4.75</v>
+      </c>
+      <c r="N90">
+        <v>1.95</v>
+      </c>
+      <c r="O90">
         <v>3</v>
-      </c>
-      <c r="M90">
-        <v>4.25</v>
-      </c>
-      <c r="N90">
-        <v>2</v>
-      </c>
-      <c r="O90">
-        <v>2.9</v>
       </c>
       <c r="P90">
         <v>3.8</v>
       </c>
       <c r="Q90">
-        <v>-0.25</v>
+        <v>-0.5</v>
       </c>
       <c r="R90">
-        <v>1.75</v>
+        <v>1.975</v>
       </c>
       <c r="S90">
-        <v>2.05</v>
+        <v>1.825</v>
       </c>
       <c r="T90">
-        <v>1.75</v>
+        <v>2</v>
       </c>
       <c r="U90">
-        <v>1.75</v>
+        <v>1.925</v>
       </c>
       <c r="V90">
-        <v>2.05</v>
+        <v>1.875</v>
       </c>
       <c r="W90">
         <v>-1</v>
       </c>
       <c r="X90">
-        <v>1.9</v>
+        <v>2</v>
       </c>
       <c r="Y90">
         <v>-1</v>
       </c>
       <c r="Z90">
-        <v>-0.5</v>
+        <v>-1</v>
       </c>
       <c r="AA90">
-        <v>0.5249999999999999</v>
+        <v>0.825</v>
       </c>
       <c r="AB90">
-        <v>0.375</v>
+        <v>-1</v>
       </c>
       <c r="AC90">
-        <v>-0.5</v>
+        <v>0.875</v>
       </c>
     </row>
     <row r="91" spans="1:29">
@@ -8540,7 +8540,7 @@
         <v>89</v>
       </c>
       <c r="B91">
-        <v>7480688</v>
+        <v>7480684</v>
       </c>
       <c r="C91" t="s">
         <v>28</v>
@@ -8552,76 +8552,76 @@
         <v>45254.46875</v>
       </c>
       <c r="F91" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="G91" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H91">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I91">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J91" t="s">
         <v>48</v>
       </c>
       <c r="K91">
-        <v>1.7</v>
+        <v>1.85</v>
       </c>
       <c r="L91">
-        <v>3.2</v>
+        <v>3</v>
       </c>
       <c r="M91">
-        <v>4.75</v>
+        <v>4.25</v>
       </c>
       <c r="N91">
-        <v>1.95</v>
+        <v>2</v>
       </c>
       <c r="O91">
-        <v>3</v>
+        <v>2.9</v>
       </c>
       <c r="P91">
         <v>3.8</v>
       </c>
       <c r="Q91">
+        <v>-0.25</v>
+      </c>
+      <c r="R91">
+        <v>1.75</v>
+      </c>
+      <c r="S91">
+        <v>2.05</v>
+      </c>
+      <c r="T91">
+        <v>1.75</v>
+      </c>
+      <c r="U91">
+        <v>1.75</v>
+      </c>
+      <c r="V91">
+        <v>2.05</v>
+      </c>
+      <c r="W91">
+        <v>-1</v>
+      </c>
+      <c r="X91">
+        <v>1.9</v>
+      </c>
+      <c r="Y91">
+        <v>-1</v>
+      </c>
+      <c r="Z91">
         <v>-0.5</v>
       </c>
-      <c r="R91">
-        <v>1.975</v>
-      </c>
-      <c r="S91">
-        <v>1.825</v>
-      </c>
-      <c r="T91">
-        <v>2</v>
-      </c>
-      <c r="U91">
-        <v>1.925</v>
-      </c>
-      <c r="V91">
-        <v>1.875</v>
-      </c>
-      <c r="W91">
-        <v>-1</v>
-      </c>
-      <c r="X91">
-        <v>2</v>
-      </c>
-      <c r="Y91">
-        <v>-1</v>
-      </c>
-      <c r="Z91">
-        <v>-1</v>
-      </c>
       <c r="AA91">
-        <v>0.825</v>
+        <v>0.5249999999999999</v>
       </c>
       <c r="AB91">
-        <v>-1</v>
+        <v>0.375</v>
       </c>
       <c r="AC91">
-        <v>0.875</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="92" spans="1:29">
@@ -11299,7 +11299,7 @@
         <v>120</v>
       </c>
       <c r="B122">
-        <v>7624657</v>
+        <v>7656900</v>
       </c>
       <c r="C122" t="s">
         <v>28</v>
@@ -11311,55 +11311,55 @@
         <v>45296.46875</v>
       </c>
       <c r="F122" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="G122" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="H122">
+        <v>0</v>
+      </c>
+      <c r="I122">
         <v>1</v>
-      </c>
-      <c r="I122">
-        <v>4</v>
       </c>
       <c r="J122" t="s">
         <v>46</v>
       </c>
       <c r="K122">
-        <v>3</v>
+        <v>1.833</v>
       </c>
       <c r="L122">
-        <v>2.8</v>
+        <v>3.1</v>
       </c>
       <c r="M122">
-        <v>2.375</v>
+        <v>4</v>
       </c>
       <c r="N122">
-        <v>4.333</v>
+        <v>2.875</v>
       </c>
       <c r="O122">
         <v>3</v>
       </c>
       <c r="P122">
-        <v>1.85</v>
+        <v>2.625</v>
       </c>
       <c r="Q122">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="R122">
-        <v>1.85</v>
+        <v>1.975</v>
       </c>
       <c r="S122">
-        <v>1.95</v>
+        <v>1.825</v>
       </c>
       <c r="T122">
         <v>2</v>
       </c>
       <c r="U122">
-        <v>2.025</v>
+        <v>1.925</v>
       </c>
       <c r="V122">
-        <v>1.775</v>
+        <v>1.875</v>
       </c>
       <c r="W122">
         <v>-1</v>
@@ -11368,19 +11368,19 @@
         <v>-1</v>
       </c>
       <c r="Y122">
-        <v>0.8500000000000001</v>
+        <v>1.625</v>
       </c>
       <c r="Z122">
         <v>-1</v>
       </c>
       <c r="AA122">
-        <v>0.95</v>
+        <v>0.825</v>
       </c>
       <c r="AB122">
-        <v>1.025</v>
+        <v>-1</v>
       </c>
       <c r="AC122">
-        <v>-1</v>
+        <v>0.875</v>
       </c>
     </row>
     <row r="123" spans="1:29">
@@ -11477,7 +11477,7 @@
         <v>122</v>
       </c>
       <c r="B124">
-        <v>7656900</v>
+        <v>7624657</v>
       </c>
       <c r="C124" t="s">
         <v>28</v>
@@ -11489,55 +11489,55 @@
         <v>45296.46875</v>
       </c>
       <c r="F124" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="G124" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="H124">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I124">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J124" t="s">
         <v>46</v>
       </c>
       <c r="K124">
-        <v>1.833</v>
+        <v>3</v>
       </c>
       <c r="L124">
-        <v>3.1</v>
+        <v>2.8</v>
       </c>
       <c r="M124">
-        <v>4</v>
+        <v>2.375</v>
       </c>
       <c r="N124">
-        <v>2.875</v>
+        <v>4.333</v>
       </c>
       <c r="O124">
         <v>3</v>
       </c>
       <c r="P124">
-        <v>2.625</v>
+        <v>1.85</v>
       </c>
       <c r="Q124">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="R124">
-        <v>1.975</v>
+        <v>1.85</v>
       </c>
       <c r="S124">
-        <v>1.825</v>
+        <v>1.95</v>
       </c>
       <c r="T124">
         <v>2</v>
       </c>
       <c r="U124">
-        <v>1.925</v>
+        <v>2.025</v>
       </c>
       <c r="V124">
-        <v>1.875</v>
+        <v>1.775</v>
       </c>
       <c r="W124">
         <v>-1</v>
@@ -11546,19 +11546,19 @@
         <v>-1</v>
       </c>
       <c r="Y124">
-        <v>1.625</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="Z124">
         <v>-1</v>
       </c>
       <c r="AA124">
-        <v>0.825</v>
+        <v>0.95</v>
       </c>
       <c r="AB124">
-        <v>-1</v>
+        <v>1.025</v>
       </c>
       <c r="AC124">
-        <v>0.875</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="125" spans="1:29">
@@ -16283,7 +16283,7 @@
         <v>176</v>
       </c>
       <c r="B178">
-        <v>7823446</v>
+        <v>7823445</v>
       </c>
       <c r="C178" t="s">
         <v>28</v>
@@ -16295,13 +16295,13 @@
         <v>45346.53125</v>
       </c>
       <c r="F178" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="G178" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="H178">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I178">
         <v>1</v>
@@ -16310,43 +16310,43 @@
         <v>47</v>
       </c>
       <c r="K178">
-        <v>1.444</v>
+        <v>1.666</v>
       </c>
       <c r="L178">
-        <v>3.5</v>
+        <v>3.25</v>
       </c>
       <c r="M178">
-        <v>7.5</v>
+        <v>5</v>
       </c>
       <c r="N178">
-        <v>1.45</v>
+        <v>1.25</v>
       </c>
       <c r="O178">
-        <v>3.6</v>
+        <v>4.333</v>
       </c>
       <c r="P178">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="Q178">
-        <v>-1</v>
+        <v>-1.5</v>
       </c>
       <c r="R178">
-        <v>1.8</v>
+        <v>1.95</v>
       </c>
       <c r="S178">
-        <v>2</v>
+        <v>1.85</v>
       </c>
       <c r="T178">
         <v>2.25</v>
       </c>
       <c r="U178">
+        <v>1.875</v>
+      </c>
+      <c r="V178">
         <v>1.925</v>
       </c>
-      <c r="V178">
-        <v>1.875</v>
-      </c>
       <c r="W178">
-        <v>0.45</v>
+        <v>0.25</v>
       </c>
       <c r="X178">
         <v>-1</v>
@@ -16355,13 +16355,13 @@
         <v>-1</v>
       </c>
       <c r="Z178">
-        <v>0.8</v>
+        <v>-1</v>
       </c>
       <c r="AA178">
-        <v>-1</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AB178">
-        <v>0.925</v>
+        <v>0.875</v>
       </c>
       <c r="AC178">
         <v>-1</v>
@@ -16372,7 +16372,7 @@
         <v>177</v>
       </c>
       <c r="B179">
-        <v>7823445</v>
+        <v>7823446</v>
       </c>
       <c r="C179" t="s">
         <v>28</v>
@@ -16384,13 +16384,13 @@
         <v>45346.53125</v>
       </c>
       <c r="F179" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="G179" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="H179">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I179">
         <v>1</v>
@@ -16399,43 +16399,43 @@
         <v>47</v>
       </c>
       <c r="K179">
-        <v>1.666</v>
+        <v>1.444</v>
       </c>
       <c r="L179">
-        <v>3.25</v>
+        <v>3.5</v>
       </c>
       <c r="M179">
-        <v>5</v>
+        <v>7.5</v>
       </c>
       <c r="N179">
-        <v>1.25</v>
+        <v>1.45</v>
       </c>
       <c r="O179">
-        <v>4.333</v>
+        <v>3.6</v>
       </c>
       <c r="P179">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="Q179">
-        <v>-1.5</v>
+        <v>-1</v>
       </c>
       <c r="R179">
-        <v>1.95</v>
+        <v>1.8</v>
       </c>
       <c r="S179">
-        <v>1.85</v>
+        <v>2</v>
       </c>
       <c r="T179">
         <v>2.25</v>
       </c>
       <c r="U179">
+        <v>1.925</v>
+      </c>
+      <c r="V179">
         <v>1.875</v>
       </c>
-      <c r="V179">
-        <v>1.925</v>
-      </c>
       <c r="W179">
-        <v>0.25</v>
+        <v>0.45</v>
       </c>
       <c r="X179">
         <v>-1</v>
@@ -16444,13 +16444,13 @@
         <v>-1</v>
       </c>
       <c r="Z179">
-        <v>-1</v>
+        <v>0.8</v>
       </c>
       <c r="AA179">
-        <v>0.8500000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AB179">
-        <v>0.875</v>
+        <v>0.925</v>
       </c>
       <c r="AC179">
         <v>-1</v>
@@ -18152,7 +18152,7 @@
         <v>197</v>
       </c>
       <c r="B199">
-        <v>7971570</v>
+        <v>7971568</v>
       </c>
       <c r="C199" t="s">
         <v>28</v>
@@ -18164,76 +18164,76 @@
         <v>45375.75</v>
       </c>
       <c r="F199" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="G199" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="H199">
         <v>0</v>
       </c>
       <c r="I199">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J199" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="K199">
-        <v>2.25</v>
+        <v>1.5</v>
       </c>
       <c r="L199">
-        <v>2.875</v>
+        <v>3.6</v>
       </c>
       <c r="M199">
-        <v>3.1</v>
+        <v>6</v>
       </c>
       <c r="N199">
-        <v>2.4</v>
+        <v>1.5</v>
       </c>
       <c r="O199">
+        <v>3.8</v>
+      </c>
+      <c r="P199">
+        <v>5.25</v>
+      </c>
+      <c r="Q199">
+        <v>-1</v>
+      </c>
+      <c r="R199">
+        <v>1.925</v>
+      </c>
+      <c r="S199">
+        <v>1.875</v>
+      </c>
+      <c r="T199">
+        <v>2.5</v>
+      </c>
+      <c r="U199">
+        <v>1.95</v>
+      </c>
+      <c r="V199">
+        <v>1.85</v>
+      </c>
+      <c r="W199">
+        <v>-1</v>
+      </c>
+      <c r="X199">
         <v>2.8</v>
       </c>
-      <c r="P199">
-        <v>2.8</v>
-      </c>
-      <c r="Q199">
-        <v>0</v>
-      </c>
-      <c r="R199">
-        <v>1.975</v>
-      </c>
-      <c r="S199">
-        <v>1.825</v>
-      </c>
-      <c r="T199">
-        <v>1.75</v>
-      </c>
-      <c r="U199">
-        <v>1.775</v>
-      </c>
-      <c r="V199">
-        <v>2.025</v>
-      </c>
-      <c r="W199">
-        <v>-1</v>
-      </c>
-      <c r="X199">
-        <v>-1</v>
-      </c>
       <c r="Y199">
-        <v>1.8</v>
+        <v>-1</v>
       </c>
       <c r="Z199">
         <v>-1</v>
       </c>
       <c r="AA199">
-        <v>0.825</v>
+        <v>0.875</v>
       </c>
       <c r="AB199">
         <v>-1</v>
       </c>
       <c r="AC199">
-        <v>1.025</v>
+        <v>0.8500000000000001</v>
       </c>
     </row>
     <row r="200" spans="1:29">
@@ -18241,7 +18241,7 @@
         <v>198</v>
       </c>
       <c r="B200">
-        <v>7971568</v>
+        <v>7971570</v>
       </c>
       <c r="C200" t="s">
         <v>28</v>
@@ -18253,76 +18253,76 @@
         <v>45375.75</v>
       </c>
       <c r="F200" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="G200" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="H200">
         <v>0</v>
       </c>
       <c r="I200">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J200" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="K200">
-        <v>1.5</v>
+        <v>2.25</v>
       </c>
       <c r="L200">
-        <v>3.6</v>
+        <v>2.875</v>
       </c>
       <c r="M200">
-        <v>6</v>
+        <v>3.1</v>
       </c>
       <c r="N200">
-        <v>1.5</v>
+        <v>2.4</v>
       </c>
       <c r="O200">
-        <v>3.8</v>
+        <v>2.8</v>
       </c>
       <c r="P200">
-        <v>5.25</v>
+        <v>2.8</v>
       </c>
       <c r="Q200">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="R200">
-        <v>1.925</v>
+        <v>1.975</v>
       </c>
       <c r="S200">
-        <v>1.875</v>
+        <v>1.825</v>
       </c>
       <c r="T200">
-        <v>2.5</v>
+        <v>1.75</v>
       </c>
       <c r="U200">
-        <v>1.95</v>
+        <v>1.775</v>
       </c>
       <c r="V200">
-        <v>1.85</v>
+        <v>2.025</v>
       </c>
       <c r="W200">
         <v>-1</v>
       </c>
       <c r="X200">
-        <v>2.8</v>
+        <v>-1</v>
       </c>
       <c r="Y200">
-        <v>-1</v>
+        <v>1.8</v>
       </c>
       <c r="Z200">
         <v>-1</v>
       </c>
       <c r="AA200">
-        <v>0.875</v>
+        <v>0.825</v>
       </c>
       <c r="AB200">
         <v>-1</v>
       </c>
       <c r="AC200">
-        <v>0.8500000000000001</v>
+        <v>1.025</v>
       </c>
     </row>
     <row r="201" spans="1:29">
@@ -18597,7 +18597,7 @@
         <v>202</v>
       </c>
       <c r="B204">
-        <v>8007201</v>
+        <v>8007202</v>
       </c>
       <c r="C204" t="s">
         <v>28</v>
@@ -18606,49 +18606,49 @@
         <v>28</v>
       </c>
       <c r="E204" s="2">
-        <v>45386.75</v>
+        <v>45387.48958333334</v>
       </c>
       <c r="F204" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="G204" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="K204">
-        <v>1.615</v>
+        <v>1.533</v>
       </c>
       <c r="L204">
-        <v>3.4</v>
+        <v>3.6</v>
       </c>
       <c r="M204">
-        <v>5</v>
+        <v>5.5</v>
       </c>
       <c r="N204">
         <v>1.5</v>
       </c>
       <c r="O204">
-        <v>3.5</v>
+        <v>3.75</v>
       </c>
       <c r="P204">
-        <v>7</v>
+        <v>6.5</v>
       </c>
       <c r="Q204">
         <v>-1</v>
       </c>
       <c r="R204">
-        <v>1.925</v>
+        <v>1.975</v>
       </c>
       <c r="S204">
-        <v>1.875</v>
+        <v>1.825</v>
       </c>
       <c r="T204">
         <v>2</v>
       </c>
       <c r="U204">
-        <v>1.875</v>
+        <v>1.775</v>
       </c>
       <c r="V204">
-        <v>1.925</v>
+        <v>2.025</v>
       </c>
       <c r="W204">
         <v>0</v>
@@ -18671,7 +18671,7 @@
         <v>203</v>
       </c>
       <c r="B205">
-        <v>8007202</v>
+        <v>8007204</v>
       </c>
       <c r="C205" t="s">
         <v>28</v>
@@ -18680,43 +18680,43 @@
         <v>28</v>
       </c>
       <c r="E205" s="2">
-        <v>45387.48958333334</v>
+        <v>45387.75</v>
       </c>
       <c r="F205" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="G205" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="K205">
-        <v>1.533</v>
+        <v>2</v>
       </c>
       <c r="L205">
+        <v>3</v>
+      </c>
+      <c r="M205">
         <v>3.6</v>
       </c>
-      <c r="M205">
-        <v>5.5</v>
-      </c>
       <c r="N205">
-        <v>1.571</v>
+        <v>2.3</v>
       </c>
       <c r="O205">
-        <v>3.5</v>
+        <v>2.875</v>
       </c>
       <c r="P205">
-        <v>5.25</v>
+        <v>3</v>
       </c>
       <c r="Q205">
-        <v>-0.75</v>
+        <v>-0.25</v>
       </c>
       <c r="R205">
+        <v>2.025</v>
+      </c>
+      <c r="S205">
         <v>1.775</v>
       </c>
-      <c r="S205">
-        <v>2.025</v>
-      </c>
       <c r="T205">
-        <v>2</v>
+        <v>1.75</v>
       </c>
       <c r="U205">
         <v>1.825</v>
@@ -18745,7 +18745,7 @@
         <v>204</v>
       </c>
       <c r="B206">
-        <v>8007204</v>
+        <v>8007205</v>
       </c>
       <c r="C206" t="s">
         <v>28</v>
@@ -18757,47 +18757,47 @@
         <v>45387.75</v>
       </c>
       <c r="F206" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="G206" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="K206">
-        <v>2</v>
+        <v>1.571</v>
       </c>
       <c r="L206">
-        <v>3</v>
+        <v>3.6</v>
       </c>
       <c r="M206">
-        <v>3.6</v>
+        <v>5</v>
       </c>
       <c r="N206">
-        <v>2.1</v>
+        <v>2</v>
       </c>
       <c r="O206">
-        <v>2.9</v>
+        <v>3.1</v>
       </c>
       <c r="P206">
-        <v>3.3</v>
+        <v>3.4</v>
       </c>
       <c r="Q206">
-        <v>-0.25</v>
+        <v>-0.5</v>
       </c>
       <c r="R206">
-        <v>1.875</v>
+        <v>2.025</v>
       </c>
       <c r="S206">
-        <v>1.925</v>
+        <v>1.775</v>
       </c>
       <c r="T206">
         <v>2</v>
       </c>
       <c r="U206">
+        <v>1.975</v>
+      </c>
+      <c r="V206">
         <v>1.825</v>
       </c>
-      <c r="V206">
-        <v>1.975</v>
-      </c>
       <c r="W206">
         <v>0</v>
       </c>
@@ -18811,80 +18811,6 @@
         <v>0</v>
       </c>
       <c r="AA206">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="207" spans="1:29">
-      <c r="A207" s="1">
-        <v>205</v>
-      </c>
-      <c r="B207">
-        <v>8007205</v>
-      </c>
-      <c r="C207" t="s">
-        <v>28</v>
-      </c>
-      <c r="D207" t="s">
-        <v>28</v>
-      </c>
-      <c r="E207" s="2">
-        <v>45387.75</v>
-      </c>
-      <c r="F207" t="s">
-        <v>32</v>
-      </c>
-      <c r="G207" t="s">
-        <v>36</v>
-      </c>
-      <c r="K207">
-        <v>1.571</v>
-      </c>
-      <c r="L207">
-        <v>3.6</v>
-      </c>
-      <c r="M207">
-        <v>5</v>
-      </c>
-      <c r="N207">
-        <v>1.85</v>
-      </c>
-      <c r="O207">
-        <v>3.3</v>
-      </c>
-      <c r="P207">
-        <v>3.6</v>
-      </c>
-      <c r="Q207">
-        <v>-0.5</v>
-      </c>
-      <c r="R207">
-        <v>1.975</v>
-      </c>
-      <c r="S207">
-        <v>1.825</v>
-      </c>
-      <c r="T207">
-        <v>2</v>
-      </c>
-      <c r="U207">
-        <v>1.825</v>
-      </c>
-      <c r="V207">
-        <v>1.975</v>
-      </c>
-      <c r="W207">
-        <v>0</v>
-      </c>
-      <c r="X207">
-        <v>0</v>
-      </c>
-      <c r="Y207">
-        <v>0</v>
-      </c>
-      <c r="Z207">
-        <v>0</v>
-      </c>
-      <c r="AA207">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização de bases das ligas, do dia: 03-05-2024 às 22:15
</commit_message>
<xml_diff>
--- a/Algeria Division 1/Algeria Division 1.xlsx
+++ b/Algeria Division 1/Algeria Division 1.xlsx
@@ -124,13 +124,13 @@
     <t>JS Saoura</t>
   </si>
   <si>
+    <t>ES Setif</t>
+  </si>
+  <si>
     <t>MC Oran</t>
   </si>
   <si>
     <t>US Biskra</t>
-  </si>
-  <si>
-    <t>ES Setif</t>
   </si>
   <si>
     <t>NC Magra</t>
@@ -711,7 +711,7 @@
         <v>29</v>
       </c>
       <c r="F3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G3">
         <v>4</v>
@@ -1141,7 +1141,7 @@
         <v>34</v>
       </c>
       <c r="F8" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G8">
         <v>1</v>
@@ -1227,7 +1227,7 @@
         <v>34</v>
       </c>
       <c r="F9" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G9">
         <v>0</v>
@@ -1473,7 +1473,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>6765519</v>
+        <v>6765588</v>
       </c>
       <c r="C12" t="s">
         <v>27</v>
@@ -1482,16 +1482,16 @@
         <v>45108.54166666666</v>
       </c>
       <c r="E12" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F12" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I12" t="s">
         <v>46</v>
@@ -1506,37 +1506,37 @@
         <v>4.2</v>
       </c>
       <c r="M12">
-        <v>1.65</v>
+        <v>1.727</v>
       </c>
       <c r="N12">
-        <v>3.1</v>
+        <v>3.4</v>
       </c>
       <c r="O12">
-        <v>5.25</v>
+        <v>4.2</v>
       </c>
       <c r="P12">
         <v>-0.75</v>
       </c>
       <c r="Q12">
-        <v>1.9</v>
+        <v>2.025</v>
       </c>
       <c r="R12">
-        <v>1.9</v>
+        <v>1.775</v>
       </c>
       <c r="S12">
-        <v>1.75</v>
+        <v>2.25</v>
       </c>
       <c r="T12">
-        <v>1.9</v>
+        <v>1.95</v>
       </c>
       <c r="U12">
-        <v>1.9</v>
+        <v>1.85</v>
       </c>
       <c r="V12">
         <v>-1</v>
       </c>
       <c r="W12">
-        <v>2.1</v>
+        <v>2.4</v>
       </c>
       <c r="X12">
         <v>-1</v>
@@ -1545,13 +1545,13 @@
         <v>-1</v>
       </c>
       <c r="Z12">
-        <v>0.8999999999999999</v>
+        <v>0.7749999999999999</v>
       </c>
       <c r="AA12">
-        <v>0.8999999999999999</v>
+        <v>-1</v>
       </c>
       <c r="AB12">
-        <v>-1</v>
+        <v>0.8500000000000001</v>
       </c>
     </row>
     <row r="13" spans="1:28">
@@ -1559,7 +1559,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>6765585</v>
+        <v>6765519</v>
       </c>
       <c r="C13" t="s">
         <v>27</v>
@@ -1568,76 +1568,76 @@
         <v>45108.54166666666</v>
       </c>
       <c r="E13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I13" t="s">
         <v>46</v>
       </c>
       <c r="J13">
-        <v>2</v>
+        <v>1.8</v>
       </c>
       <c r="K13">
-        <v>2.8</v>
+        <v>3.2</v>
       </c>
       <c r="L13">
-        <v>4</v>
+        <v>4.2</v>
       </c>
       <c r="M13">
-        <v>2.05</v>
+        <v>1.65</v>
       </c>
       <c r="N13">
-        <v>2.7</v>
+        <v>3.1</v>
       </c>
       <c r="O13">
-        <v>4</v>
+        <v>5.25</v>
       </c>
       <c r="P13">
-        <v>-0.25</v>
+        <v>-0.75</v>
       </c>
       <c r="Q13">
-        <v>1.75</v>
+        <v>1.9</v>
       </c>
       <c r="R13">
-        <v>2.05</v>
+        <v>1.9</v>
       </c>
       <c r="S13">
         <v>1.75</v>
       </c>
       <c r="T13">
-        <v>1.875</v>
+        <v>1.9</v>
       </c>
       <c r="U13">
-        <v>1.925</v>
+        <v>1.9</v>
       </c>
       <c r="V13">
         <v>-1</v>
       </c>
       <c r="W13">
-        <v>1.7</v>
+        <v>2.1</v>
       </c>
       <c r="X13">
         <v>-1</v>
       </c>
       <c r="Y13">
-        <v>-0.5</v>
+        <v>-1</v>
       </c>
       <c r="Z13">
-        <v>0.5249999999999999</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AA13">
-        <v>0.4375</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AB13">
-        <v>-0.5</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="14" spans="1:28">
@@ -1645,7 +1645,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>6765586</v>
+        <v>6765585</v>
       </c>
       <c r="C14" t="s">
         <v>27</v>
@@ -1657,73 +1657,73 @@
         <v>37</v>
       </c>
       <c r="F14" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="G14">
         <v>1</v>
       </c>
       <c r="H14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I14" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="J14">
-        <v>1.7</v>
+        <v>2</v>
       </c>
       <c r="K14">
-        <v>3.2</v>
+        <v>2.8</v>
       </c>
       <c r="L14">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M14">
-        <v>1.65</v>
+        <v>2.05</v>
       </c>
       <c r="N14">
-        <v>3.1</v>
+        <v>2.7</v>
       </c>
       <c r="O14">
-        <v>5.5</v>
+        <v>4</v>
       </c>
       <c r="P14">
-        <v>-0.75</v>
+        <v>-0.25</v>
       </c>
       <c r="Q14">
-        <v>1.925</v>
+        <v>1.75</v>
       </c>
       <c r="R14">
-        <v>1.875</v>
+        <v>2.05</v>
       </c>
       <c r="S14">
         <v>1.75</v>
       </c>
       <c r="T14">
-        <v>1.775</v>
+        <v>1.875</v>
       </c>
       <c r="U14">
-        <v>2.025</v>
+        <v>1.925</v>
       </c>
       <c r="V14">
-        <v>0.6499999999999999</v>
+        <v>-1</v>
       </c>
       <c r="W14">
-        <v>-1</v>
+        <v>1.7</v>
       </c>
       <c r="X14">
         <v>-1</v>
       </c>
       <c r="Y14">
-        <v>0.4625</v>
+        <v>-0.5</v>
       </c>
       <c r="Z14">
+        <v>0.5249999999999999</v>
+      </c>
+      <c r="AA14">
+        <v>0.4375</v>
+      </c>
+      <c r="AB14">
         <v>-0.5</v>
-      </c>
-      <c r="AA14">
-        <v>-1</v>
-      </c>
-      <c r="AB14">
-        <v>1.025</v>
       </c>
     </row>
     <row r="15" spans="1:28">
@@ -1731,7 +1731,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>6765588</v>
+        <v>6765586</v>
       </c>
       <c r="C15" t="s">
         <v>27</v>
@@ -1743,73 +1743,73 @@
         <v>38</v>
       </c>
       <c r="F15" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15">
         <v>0</v>
       </c>
       <c r="I15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J15">
-        <v>1.8</v>
+        <v>1.7</v>
       </c>
       <c r="K15">
         <v>3.2</v>
       </c>
       <c r="L15">
-        <v>4.2</v>
+        <v>5</v>
       </c>
       <c r="M15">
-        <v>1.727</v>
+        <v>1.65</v>
       </c>
       <c r="N15">
-        <v>3.4</v>
+        <v>3.1</v>
       </c>
       <c r="O15">
-        <v>4.2</v>
+        <v>5.5</v>
       </c>
       <c r="P15">
         <v>-0.75</v>
       </c>
       <c r="Q15">
+        <v>1.925</v>
+      </c>
+      <c r="R15">
+        <v>1.875</v>
+      </c>
+      <c r="S15">
+        <v>1.75</v>
+      </c>
+      <c r="T15">
+        <v>1.775</v>
+      </c>
+      <c r="U15">
         <v>2.025</v>
       </c>
-      <c r="R15">
-        <v>1.775</v>
-      </c>
-      <c r="S15">
-        <v>2.25</v>
-      </c>
-      <c r="T15">
-        <v>1.95</v>
-      </c>
-      <c r="U15">
-        <v>1.85</v>
-      </c>
       <c r="V15">
-        <v>-1</v>
+        <v>0.6499999999999999</v>
       </c>
       <c r="W15">
-        <v>2.4</v>
+        <v>-1</v>
       </c>
       <c r="X15">
         <v>-1</v>
       </c>
       <c r="Y15">
-        <v>-1</v>
+        <v>0.4625</v>
       </c>
       <c r="Z15">
-        <v>0.7749999999999999</v>
+        <v>-0.5</v>
       </c>
       <c r="AA15">
         <v>-1</v>
       </c>
       <c r="AB15">
-        <v>0.8500000000000001</v>
+        <v>1.025</v>
       </c>
     </row>
     <row r="16" spans="1:28">
@@ -2161,7 +2161,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>6743989</v>
+        <v>6743297</v>
       </c>
       <c r="C20" t="s">
         <v>27</v>
@@ -2170,58 +2170,58 @@
         <v>45111.54166666666</v>
       </c>
       <c r="E20" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F20" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I20" t="s">
         <v>45</v>
       </c>
       <c r="J20">
-        <v>1.666</v>
+        <v>1.285</v>
       </c>
       <c r="K20">
-        <v>3.5</v>
+        <v>4.5</v>
       </c>
       <c r="L20">
-        <v>4.5</v>
+        <v>9</v>
       </c>
       <c r="M20">
-        <v>1.5</v>
+        <v>1.166</v>
       </c>
       <c r="N20">
-        <v>3.75</v>
+        <v>6</v>
       </c>
       <c r="O20">
-        <v>5.5</v>
+        <v>17</v>
       </c>
       <c r="P20">
-        <v>-1</v>
+        <v>-1.75</v>
       </c>
       <c r="Q20">
+        <v>1.825</v>
+      </c>
+      <c r="R20">
         <v>1.975</v>
       </c>
-      <c r="R20">
+      <c r="S20">
+        <v>2.5</v>
+      </c>
+      <c r="T20">
         <v>1.825</v>
       </c>
-      <c r="S20">
-        <v>2.25</v>
-      </c>
-      <c r="T20">
+      <c r="U20">
         <v>1.975</v>
       </c>
-      <c r="U20">
-        <v>1.825</v>
-      </c>
       <c r="V20">
-        <v>0.5</v>
+        <v>0.1659999999999999</v>
       </c>
       <c r="W20">
         <v>-1</v>
@@ -2230,16 +2230,16 @@
         <v>-1</v>
       </c>
       <c r="Y20">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Z20">
-        <v>0</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="AA20">
+        <v>-1</v>
+      </c>
+      <c r="AB20">
         <v>0.9750000000000001</v>
-      </c>
-      <c r="AB20">
-        <v>-1</v>
       </c>
     </row>
     <row r="21" spans="1:28">
@@ -2247,7 +2247,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>6744018</v>
+        <v>6743977</v>
       </c>
       <c r="C21" t="s">
         <v>27</v>
@@ -2256,76 +2256,76 @@
         <v>45111.54166666666</v>
       </c>
       <c r="E21" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F21" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G21">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I21" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="J21">
-        <v>2.2</v>
+        <v>1.444</v>
       </c>
       <c r="K21">
-        <v>2.875</v>
+        <v>3.6</v>
       </c>
       <c r="L21">
-        <v>3.2</v>
+        <v>7</v>
       </c>
       <c r="M21">
-        <v>1.85</v>
+        <v>1.363</v>
       </c>
       <c r="N21">
-        <v>2.9</v>
+        <v>3.8</v>
       </c>
       <c r="O21">
-        <v>4.5</v>
+        <v>8</v>
       </c>
       <c r="P21">
-        <v>-0.5</v>
+        <v>-1.25</v>
       </c>
       <c r="Q21">
-        <v>1.9</v>
+        <v>2</v>
       </c>
       <c r="R21">
-        <v>1.9</v>
+        <v>1.8</v>
       </c>
       <c r="S21">
-        <v>1.75</v>
+        <v>2.25</v>
       </c>
       <c r="T21">
-        <v>1.825</v>
+        <v>1.875</v>
       </c>
       <c r="U21">
-        <v>1.975</v>
+        <v>1.925</v>
       </c>
       <c r="V21">
-        <v>0.8500000000000001</v>
+        <v>-1</v>
       </c>
       <c r="W21">
-        <v>-1</v>
+        <v>2.8</v>
       </c>
       <c r="X21">
         <v>-1</v>
       </c>
       <c r="Y21">
-        <v>0.8999999999999999</v>
+        <v>-1</v>
       </c>
       <c r="Z21">
-        <v>-1</v>
+        <v>0.8</v>
       </c>
       <c r="AA21">
-        <v>0.825</v>
+        <v>-1</v>
       </c>
       <c r="AB21">
-        <v>-1</v>
+        <v>0.925</v>
       </c>
     </row>
     <row r="22" spans="1:28">
@@ -2333,7 +2333,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>6743978</v>
+        <v>6743989</v>
       </c>
       <c r="C22" t="s">
         <v>27</v>
@@ -2342,58 +2342,58 @@
         <v>45111.54166666666</v>
       </c>
       <c r="E22" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F22" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="G22">
         <v>2</v>
       </c>
       <c r="H22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I22" t="s">
         <v>45</v>
       </c>
       <c r="J22">
-        <v>2</v>
+        <v>1.666</v>
       </c>
       <c r="K22">
-        <v>2.9</v>
+        <v>3.5</v>
       </c>
       <c r="L22">
-        <v>3.6</v>
+        <v>4.5</v>
       </c>
       <c r="M22">
-        <v>2.1</v>
+        <v>1.5</v>
       </c>
       <c r="N22">
-        <v>2.9</v>
+        <v>3.75</v>
       </c>
       <c r="O22">
-        <v>3.6</v>
+        <v>5.5</v>
       </c>
       <c r="P22">
-        <v>-0.25</v>
+        <v>-1</v>
       </c>
       <c r="Q22">
+        <v>1.975</v>
+      </c>
+      <c r="R22">
         <v>1.825</v>
       </c>
-      <c r="R22">
+      <c r="S22">
+        <v>2.25</v>
+      </c>
+      <c r="T22">
         <v>1.975</v>
       </c>
-      <c r="S22">
-        <v>1.75</v>
-      </c>
-      <c r="T22">
-        <v>1.75</v>
-      </c>
       <c r="U22">
-        <v>2.05</v>
+        <v>1.825</v>
       </c>
       <c r="V22">
-        <v>1.1</v>
+        <v>0.5</v>
       </c>
       <c r="W22">
         <v>-1</v>
@@ -2402,16 +2402,16 @@
         <v>-1</v>
       </c>
       <c r="Y22">
-        <v>0.825</v>
+        <v>0</v>
       </c>
       <c r="Z22">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AA22">
-        <v>0.375</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="AB22">
-        <v>-0.5</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="23" spans="1:28">
@@ -2419,7 +2419,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>6744005</v>
+        <v>6743978</v>
       </c>
       <c r="C23" t="s">
         <v>27</v>
@@ -2428,13 +2428,13 @@
         <v>45111.54166666666</v>
       </c>
       <c r="E23" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="F23" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="G23">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H23">
         <v>0</v>
@@ -2443,43 +2443,43 @@
         <v>45</v>
       </c>
       <c r="J23">
-        <v>1.615</v>
+        <v>2</v>
       </c>
       <c r="K23">
-        <v>3.4</v>
+        <v>2.9</v>
       </c>
       <c r="L23">
-        <v>5</v>
+        <v>3.6</v>
       </c>
       <c r="M23">
-        <v>1.4</v>
+        <v>2.1</v>
       </c>
       <c r="N23">
-        <v>3.75</v>
+        <v>2.9</v>
       </c>
       <c r="O23">
-        <v>7.5</v>
+        <v>3.6</v>
       </c>
       <c r="P23">
-        <v>-1.25</v>
+        <v>-0.25</v>
       </c>
       <c r="Q23">
+        <v>1.825</v>
+      </c>
+      <c r="R23">
+        <v>1.975</v>
+      </c>
+      <c r="S23">
+        <v>1.75</v>
+      </c>
+      <c r="T23">
+        <v>1.75</v>
+      </c>
+      <c r="U23">
         <v>2.05</v>
       </c>
-      <c r="R23">
-        <v>1.75</v>
-      </c>
-      <c r="S23">
-        <v>2</v>
-      </c>
-      <c r="T23">
-        <v>1.85</v>
-      </c>
-      <c r="U23">
-        <v>1.95</v>
-      </c>
       <c r="V23">
-        <v>0.3999999999999999</v>
+        <v>1.1</v>
       </c>
       <c r="W23">
         <v>-1</v>
@@ -2488,16 +2488,16 @@
         <v>-1</v>
       </c>
       <c r="Y23">
+        <v>0.825</v>
+      </c>
+      <c r="Z23">
+        <v>-1</v>
+      </c>
+      <c r="AA23">
+        <v>0.375</v>
+      </c>
+      <c r="AB23">
         <v>-0.5</v>
-      </c>
-      <c r="Z23">
-        <v>0.375</v>
-      </c>
-      <c r="AA23">
-        <v>-1</v>
-      </c>
-      <c r="AB23">
-        <v>0.95</v>
       </c>
     </row>
     <row r="24" spans="1:28">
@@ -2505,7 +2505,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>6743977</v>
+        <v>6744018</v>
       </c>
       <c r="C24" t="s">
         <v>27</v>
@@ -2514,76 +2514,76 @@
         <v>45111.54166666666</v>
       </c>
       <c r="E24" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="F24" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G24">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I24" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J24">
-        <v>1.444</v>
+        <v>2.2</v>
       </c>
       <c r="K24">
-        <v>3.6</v>
+        <v>2.875</v>
       </c>
       <c r="L24">
-        <v>7</v>
+        <v>3.2</v>
       </c>
       <c r="M24">
-        <v>1.363</v>
+        <v>1.85</v>
       </c>
       <c r="N24">
-        <v>3.8</v>
+        <v>2.9</v>
       </c>
       <c r="O24">
-        <v>8</v>
+        <v>4.5</v>
       </c>
       <c r="P24">
-        <v>-1.25</v>
+        <v>-0.5</v>
       </c>
       <c r="Q24">
-        <v>2</v>
+        <v>1.9</v>
       </c>
       <c r="R24">
-        <v>1.8</v>
+        <v>1.9</v>
       </c>
       <c r="S24">
-        <v>2.25</v>
+        <v>1.75</v>
       </c>
       <c r="T24">
-        <v>1.875</v>
+        <v>1.825</v>
       </c>
       <c r="U24">
-        <v>1.925</v>
+        <v>1.975</v>
       </c>
       <c r="V24">
-        <v>-1</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="W24">
-        <v>2.8</v>
+        <v>-1</v>
       </c>
       <c r="X24">
         <v>-1</v>
       </c>
       <c r="Y24">
-        <v>-1</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="Z24">
-        <v>0.8</v>
+        <v>-1</v>
       </c>
       <c r="AA24">
-        <v>-1</v>
+        <v>0.825</v>
       </c>
       <c r="AB24">
-        <v>0.925</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="25" spans="1:28">
@@ -2591,7 +2591,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>6743297</v>
+        <v>6744005</v>
       </c>
       <c r="C25" t="s">
         <v>27</v>
@@ -2600,10 +2600,10 @@
         <v>45111.54166666666</v>
       </c>
       <c r="E25" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F25" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="G25">
         <v>1</v>
@@ -2615,43 +2615,43 @@
         <v>45</v>
       </c>
       <c r="J25">
-        <v>1.285</v>
+        <v>1.615</v>
       </c>
       <c r="K25">
-        <v>4.5</v>
+        <v>3.4</v>
       </c>
       <c r="L25">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="M25">
-        <v>1.166</v>
+        <v>1.4</v>
       </c>
       <c r="N25">
-        <v>6</v>
+        <v>3.75</v>
       </c>
       <c r="O25">
-        <v>17</v>
+        <v>7.5</v>
       </c>
       <c r="P25">
-        <v>-1.75</v>
+        <v>-1.25</v>
       </c>
       <c r="Q25">
-        <v>1.825</v>
+        <v>2.05</v>
       </c>
       <c r="R25">
-        <v>1.975</v>
+        <v>1.75</v>
       </c>
       <c r="S25">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="T25">
-        <v>1.825</v>
+        <v>1.85</v>
       </c>
       <c r="U25">
-        <v>1.975</v>
+        <v>1.95</v>
       </c>
       <c r="V25">
-        <v>0.1659999999999999</v>
+        <v>0.3999999999999999</v>
       </c>
       <c r="W25">
         <v>-1</v>
@@ -2660,16 +2660,16 @@
         <v>-1</v>
       </c>
       <c r="Y25">
-        <v>-1</v>
+        <v>-0.5</v>
       </c>
       <c r="Z25">
-        <v>0.9750000000000001</v>
+        <v>0.375</v>
       </c>
       <c r="AA25">
         <v>-1</v>
       </c>
       <c r="AB25">
-        <v>0.9750000000000001</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="26" spans="1:28">
@@ -2677,7 +2677,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>6872722</v>
+        <v>6872725</v>
       </c>
       <c r="C26" t="s">
         <v>27</v>
@@ -2686,13 +2686,13 @@
         <v>45114.55208333334</v>
       </c>
       <c r="E26" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F26" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="G26">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H26">
         <v>1</v>
@@ -2701,58 +2701,58 @@
         <v>45</v>
       </c>
       <c r="J26">
-        <v>1.45</v>
+        <v>1.285</v>
       </c>
       <c r="K26">
-        <v>3.6</v>
+        <v>4.5</v>
       </c>
       <c r="L26">
-        <v>6.5</v>
+        <v>10</v>
       </c>
       <c r="M26">
+        <v>1.25</v>
+      </c>
+      <c r="N26">
+        <v>5</v>
+      </c>
+      <c r="O26">
+        <v>11</v>
+      </c>
+      <c r="P26">
+        <v>-1.5</v>
+      </c>
+      <c r="Q26">
+        <v>1.9</v>
+      </c>
+      <c r="R26">
+        <v>1.9</v>
+      </c>
+      <c r="S26">
+        <v>2.25</v>
+      </c>
+      <c r="T26">
         <v>1.85</v>
       </c>
-      <c r="N26">
-        <v>3.1</v>
-      </c>
-      <c r="O26">
-        <v>4.2</v>
-      </c>
-      <c r="P26">
-        <v>-0.5</v>
-      </c>
-      <c r="Q26">
+      <c r="U26">
         <v>1.95</v>
       </c>
-      <c r="R26">
-        <v>1.85</v>
-      </c>
-      <c r="S26">
-        <v>2</v>
-      </c>
-      <c r="T26">
-        <v>2.025</v>
-      </c>
-      <c r="U26">
-        <v>1.775</v>
-      </c>
       <c r="V26">
+        <v>0.25</v>
+      </c>
+      <c r="W26">
+        <v>-1</v>
+      </c>
+      <c r="X26">
+        <v>-1</v>
+      </c>
+      <c r="Y26">
+        <v>-1</v>
+      </c>
+      <c r="Z26">
+        <v>0.8999999999999999</v>
+      </c>
+      <c r="AA26">
         <v>0.8500000000000001</v>
-      </c>
-      <c r="W26">
-        <v>-1</v>
-      </c>
-      <c r="X26">
-        <v>-1</v>
-      </c>
-      <c r="Y26">
-        <v>0.95</v>
-      </c>
-      <c r="Z26">
-        <v>-1</v>
-      </c>
-      <c r="AA26">
-        <v>1.025</v>
       </c>
       <c r="AB26">
         <v>-1</v>
@@ -2763,7 +2763,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>6872723</v>
+        <v>6872721</v>
       </c>
       <c r="C27" t="s">
         <v>27</v>
@@ -2772,76 +2772,76 @@
         <v>45114.55208333334</v>
       </c>
       <c r="E27" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G27">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H27">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I27" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J27">
-        <v>1.8</v>
+        <v>1.444</v>
       </c>
       <c r="K27">
-        <v>3.3</v>
+        <v>3.75</v>
       </c>
       <c r="L27">
-        <v>4.333</v>
+        <v>7</v>
       </c>
       <c r="M27">
-        <v>1.8</v>
+        <v>1.363</v>
       </c>
       <c r="N27">
-        <v>3.3</v>
+        <v>4.2</v>
       </c>
       <c r="O27">
-        <v>4.2</v>
+        <v>7</v>
       </c>
       <c r="P27">
+        <v>-1.25</v>
+      </c>
+      <c r="Q27">
+        <v>2.025</v>
+      </c>
+      <c r="R27">
+        <v>1.775</v>
+      </c>
+      <c r="S27">
+        <v>2</v>
+      </c>
+      <c r="T27">
+        <v>1.925</v>
+      </c>
+      <c r="U27">
+        <v>1.875</v>
+      </c>
+      <c r="V27">
+        <v>0.363</v>
+      </c>
+      <c r="W27">
+        <v>-1</v>
+      </c>
+      <c r="X27">
+        <v>-1</v>
+      </c>
+      <c r="Y27">
         <v>-0.5</v>
       </c>
-      <c r="Q27">
-        <v>1.8</v>
-      </c>
-      <c r="R27">
-        <v>2</v>
-      </c>
-      <c r="S27">
-        <v>2.25</v>
-      </c>
-      <c r="T27">
-        <v>2</v>
-      </c>
-      <c r="U27">
-        <v>1.8</v>
-      </c>
-      <c r="V27">
-        <v>-1</v>
-      </c>
-      <c r="W27">
-        <v>-1</v>
-      </c>
-      <c r="X27">
-        <v>3.2</v>
-      </c>
-      <c r="Y27">
-        <v>-1</v>
-      </c>
       <c r="Z27">
-        <v>1</v>
+        <v>0.3875</v>
       </c>
       <c r="AA27">
-        <v>-1</v>
+        <v>0.925</v>
       </c>
       <c r="AB27">
-        <v>0.8</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="28" spans="1:28">
@@ -2849,7 +2849,7 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>6872727</v>
+        <v>6872724</v>
       </c>
       <c r="C28" t="s">
         <v>27</v>
@@ -2858,49 +2858,49 @@
         <v>45114.55208333334</v>
       </c>
       <c r="E28" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="F28" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="G28">
         <v>1</v>
       </c>
       <c r="H28">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I28" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J28">
-        <v>1.571</v>
+        <v>1.55</v>
       </c>
       <c r="K28">
-        <v>3.4</v>
+        <v>3.25</v>
       </c>
       <c r="L28">
-        <v>6</v>
+        <v>6.5</v>
       </c>
       <c r="M28">
         <v>1.65</v>
       </c>
       <c r="N28">
-        <v>3.3</v>
+        <v>3.1</v>
       </c>
       <c r="O28">
-        <v>4.75</v>
+        <v>5.5</v>
       </c>
       <c r="P28">
         <v>-0.75</v>
       </c>
       <c r="Q28">
-        <v>1.95</v>
+        <v>1.9</v>
       </c>
       <c r="R28">
-        <v>1.85</v>
+        <v>1.9</v>
       </c>
       <c r="S28">
-        <v>2</v>
+        <v>1.75</v>
       </c>
       <c r="T28">
         <v>1.75</v>
@@ -2909,25 +2909,25 @@
         <v>2.05</v>
       </c>
       <c r="V28">
-        <v>-1</v>
+        <v>0.6499999999999999</v>
       </c>
       <c r="W28">
         <v>-1</v>
       </c>
       <c r="X28">
-        <v>3.75</v>
+        <v>-1</v>
       </c>
       <c r="Y28">
-        <v>-1</v>
+        <v>0.45</v>
       </c>
       <c r="Z28">
-        <v>0.8500000000000001</v>
+        <v>-0.5</v>
       </c>
       <c r="AA28">
-        <v>0.75</v>
+        <v>-1</v>
       </c>
       <c r="AB28">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
     </row>
     <row r="29" spans="1:28">
@@ -2935,7 +2935,7 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>6872726</v>
+        <v>6872727</v>
       </c>
       <c r="C29" t="s">
         <v>27</v>
@@ -2944,76 +2944,76 @@
         <v>45114.55208333334</v>
       </c>
       <c r="E29" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="F29" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G29">
         <v>1</v>
       </c>
       <c r="H29">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I29" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="J29">
+        <v>1.571</v>
+      </c>
+      <c r="K29">
+        <v>3.4</v>
+      </c>
+      <c r="L29">
+        <v>6</v>
+      </c>
+      <c r="M29">
+        <v>1.65</v>
+      </c>
+      <c r="N29">
+        <v>3.3</v>
+      </c>
+      <c r="O29">
+        <v>4.75</v>
+      </c>
+      <c r="P29">
+        <v>-0.75</v>
+      </c>
+      <c r="Q29">
+        <v>1.95</v>
+      </c>
+      <c r="R29">
         <v>1.85</v>
       </c>
-      <c r="K29">
-        <v>3.1</v>
-      </c>
-      <c r="L29">
-        <v>4.2</v>
-      </c>
-      <c r="M29">
-        <v>2.2</v>
-      </c>
-      <c r="N29">
-        <v>2.9</v>
-      </c>
-      <c r="O29">
-        <v>3.3</v>
-      </c>
-      <c r="P29">
-        <v>-0.25</v>
-      </c>
-      <c r="Q29">
-        <v>1.925</v>
-      </c>
-      <c r="R29">
-        <v>1.875</v>
-      </c>
       <c r="S29">
         <v>2</v>
       </c>
       <c r="T29">
-        <v>2</v>
+        <v>1.75</v>
       </c>
       <c r="U29">
-        <v>1.8</v>
+        <v>2.05</v>
       </c>
       <c r="V29">
         <v>-1</v>
       </c>
       <c r="W29">
-        <v>1.9</v>
+        <v>-1</v>
       </c>
       <c r="X29">
-        <v>-1</v>
+        <v>3.75</v>
       </c>
       <c r="Y29">
-        <v>-0.5</v>
+        <v>-1</v>
       </c>
       <c r="Z29">
-        <v>0.4375</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AA29">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="AB29">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="30" spans="1:28">
@@ -3021,7 +3021,7 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>6872721</v>
+        <v>6872722</v>
       </c>
       <c r="C30" t="s">
         <v>27</v>
@@ -3030,58 +3030,58 @@
         <v>45114.55208333334</v>
       </c>
       <c r="E30" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="F30" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="G30">
         <v>3</v>
       </c>
       <c r="H30">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I30" t="s">
         <v>45</v>
       </c>
       <c r="J30">
-        <v>1.444</v>
+        <v>1.45</v>
       </c>
       <c r="K30">
-        <v>3.75</v>
+        <v>3.6</v>
       </c>
       <c r="L30">
-        <v>7</v>
+        <v>6.5</v>
       </c>
       <c r="M30">
-        <v>1.363</v>
+        <v>1.85</v>
       </c>
       <c r="N30">
+        <v>3.1</v>
+      </c>
+      <c r="O30">
         <v>4.2</v>
       </c>
-      <c r="O30">
-        <v>7</v>
-      </c>
       <c r="P30">
-        <v>-1.25</v>
+        <v>-0.5</v>
       </c>
       <c r="Q30">
+        <v>1.95</v>
+      </c>
+      <c r="R30">
+        <v>1.85</v>
+      </c>
+      <c r="S30">
+        <v>2</v>
+      </c>
+      <c r="T30">
         <v>2.025</v>
       </c>
-      <c r="R30">
+      <c r="U30">
         <v>1.775</v>
       </c>
-      <c r="S30">
-        <v>2</v>
-      </c>
-      <c r="T30">
-        <v>1.925</v>
-      </c>
-      <c r="U30">
-        <v>1.875</v>
-      </c>
       <c r="V30">
-        <v>0.363</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="W30">
         <v>-1</v>
@@ -3090,13 +3090,13 @@
         <v>-1</v>
       </c>
       <c r="Y30">
-        <v>-0.5</v>
+        <v>0.95</v>
       </c>
       <c r="Z30">
-        <v>0.3875</v>
+        <v>-1</v>
       </c>
       <c r="AA30">
-        <v>0.925</v>
+        <v>1.025</v>
       </c>
       <c r="AB30">
         <v>-1</v>
@@ -3107,7 +3107,7 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>6872724</v>
+        <v>6872726</v>
       </c>
       <c r="C31" t="s">
         <v>27</v>
@@ -3116,76 +3116,76 @@
         <v>45114.55208333334</v>
       </c>
       <c r="E31" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F31" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="G31">
         <v>1</v>
       </c>
       <c r="H31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I31" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="J31">
-        <v>1.55</v>
+        <v>1.85</v>
       </c>
       <c r="K31">
-        <v>3.25</v>
+        <v>3.1</v>
       </c>
       <c r="L31">
-        <v>6.5</v>
+        <v>4.2</v>
       </c>
       <c r="M31">
-        <v>1.65</v>
+        <v>2.2</v>
       </c>
       <c r="N31">
-        <v>3.1</v>
+        <v>2.9</v>
       </c>
       <c r="O31">
-        <v>5.5</v>
+        <v>3.3</v>
       </c>
       <c r="P31">
-        <v>-0.75</v>
+        <v>-0.25</v>
       </c>
       <c r="Q31">
+        <v>1.925</v>
+      </c>
+      <c r="R31">
+        <v>1.875</v>
+      </c>
+      <c r="S31">
+        <v>2</v>
+      </c>
+      <c r="T31">
+        <v>2</v>
+      </c>
+      <c r="U31">
+        <v>1.8</v>
+      </c>
+      <c r="V31">
+        <v>-1</v>
+      </c>
+      <c r="W31">
         <v>1.9</v>
       </c>
-      <c r="R31">
-        <v>1.9</v>
-      </c>
-      <c r="S31">
-        <v>1.75</v>
-      </c>
-      <c r="T31">
-        <v>1.75</v>
-      </c>
-      <c r="U31">
-        <v>2.05</v>
-      </c>
-      <c r="V31">
-        <v>0.6499999999999999</v>
-      </c>
-      <c r="W31">
-        <v>-1</v>
-      </c>
       <c r="X31">
         <v>-1</v>
       </c>
       <c r="Y31">
-        <v>0.45</v>
+        <v>-0.5</v>
       </c>
       <c r="Z31">
-        <v>-0.5</v>
+        <v>0.4375</v>
       </c>
       <c r="AA31">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AB31">
-        <v>1.05</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:28">
@@ -3193,7 +3193,7 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>6872725</v>
+        <v>6872723</v>
       </c>
       <c r="C32" t="s">
         <v>27</v>
@@ -3202,76 +3202,76 @@
         <v>45114.55208333334</v>
       </c>
       <c r="E32" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="F32" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G32">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H32">
         <v>1</v>
       </c>
       <c r="I32" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="J32">
-        <v>1.285</v>
+        <v>1.8</v>
       </c>
       <c r="K32">
-        <v>4.5</v>
+        <v>3.3</v>
       </c>
       <c r="L32">
-        <v>10</v>
+        <v>4.333</v>
       </c>
       <c r="M32">
-        <v>1.25</v>
+        <v>1.8</v>
       </c>
       <c r="N32">
-        <v>5</v>
+        <v>3.3</v>
       </c>
       <c r="O32">
-        <v>11</v>
+        <v>4.2</v>
       </c>
       <c r="P32">
-        <v>-1.5</v>
+        <v>-0.5</v>
       </c>
       <c r="Q32">
-        <v>1.9</v>
+        <v>1.8</v>
       </c>
       <c r="R32">
-        <v>1.9</v>
+        <v>2</v>
       </c>
       <c r="S32">
         <v>2.25</v>
       </c>
       <c r="T32">
-        <v>1.85</v>
+        <v>2</v>
       </c>
       <c r="U32">
-        <v>1.95</v>
+        <v>1.8</v>
       </c>
       <c r="V32">
-        <v>0.25</v>
+        <v>-1</v>
       </c>
       <c r="W32">
         <v>-1</v>
       </c>
       <c r="X32">
-        <v>-1</v>
+        <v>3.2</v>
       </c>
       <c r="Y32">
         <v>-1</v>
       </c>
       <c r="Z32">
-        <v>0.8999999999999999</v>
+        <v>1</v>
       </c>
       <c r="AA32">
-        <v>0.8500000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AB32">
-        <v>-1</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="33" spans="1:28">
@@ -3279,7 +3279,7 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>6888615</v>
+        <v>6888613</v>
       </c>
       <c r="C33" t="s">
         <v>27</v>
@@ -3288,73 +3288,73 @@
         <v>45117.55208333334</v>
       </c>
       <c r="E33" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F33" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G33">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I33" t="s">
         <v>45</v>
       </c>
       <c r="J33">
-        <v>3.5</v>
+        <v>1.4</v>
       </c>
       <c r="K33">
-        <v>2.875</v>
+        <v>3.75</v>
       </c>
       <c r="L33">
-        <v>2.1</v>
+        <v>7.5</v>
       </c>
       <c r="M33">
-        <v>1.7</v>
+        <v>1.363</v>
       </c>
       <c r="N33">
-        <v>3</v>
+        <v>4.333</v>
       </c>
       <c r="O33">
-        <v>5.25</v>
+        <v>7</v>
       </c>
       <c r="P33">
+        <v>-1.25</v>
+      </c>
+      <c r="Q33">
+        <v>1.925</v>
+      </c>
+      <c r="R33">
+        <v>1.875</v>
+      </c>
+      <c r="S33">
+        <v>2.25</v>
+      </c>
+      <c r="T33">
+        <v>1.975</v>
+      </c>
+      <c r="U33">
+        <v>1.825</v>
+      </c>
+      <c r="V33">
+        <v>0.363</v>
+      </c>
+      <c r="W33">
+        <v>-1</v>
+      </c>
+      <c r="X33">
+        <v>-1</v>
+      </c>
+      <c r="Y33">
         <v>-0.5</v>
       </c>
-      <c r="Q33">
-        <v>1.775</v>
-      </c>
-      <c r="R33">
-        <v>2.025</v>
-      </c>
-      <c r="S33">
-        <v>2</v>
-      </c>
-      <c r="T33">
-        <v>1.875</v>
-      </c>
-      <c r="U33">
-        <v>1.925</v>
-      </c>
-      <c r="V33">
-        <v>0.7</v>
-      </c>
-      <c r="W33">
-        <v>-1</v>
-      </c>
-      <c r="X33">
-        <v>-1</v>
-      </c>
-      <c r="Y33">
-        <v>0.7749999999999999</v>
-      </c>
       <c r="Z33">
-        <v>-1</v>
+        <v>0.4375</v>
       </c>
       <c r="AA33">
-        <v>0.875</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="AB33">
         <v>-1</v>
@@ -3365,7 +3365,7 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>6888614</v>
+        <v>6888612</v>
       </c>
       <c r="C34" t="s">
         <v>27</v>
@@ -3374,76 +3374,76 @@
         <v>45117.55208333334</v>
       </c>
       <c r="E34" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="F34" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G34">
         <v>1</v>
       </c>
       <c r="H34">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I34" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J34">
-        <v>1.8</v>
+        <v>1.727</v>
       </c>
       <c r="K34">
         <v>3.2</v>
       </c>
       <c r="L34">
-        <v>4</v>
+        <v>4.5</v>
       </c>
       <c r="M34">
-        <v>2.5</v>
+        <v>1.65</v>
       </c>
       <c r="N34">
-        <v>3</v>
+        <v>3.3</v>
       </c>
       <c r="O34">
-        <v>2.625</v>
+        <v>5.75</v>
       </c>
       <c r="P34">
-        <v>0</v>
+        <v>-0.75</v>
       </c>
       <c r="Q34">
-        <v>1.85</v>
+        <v>1.875</v>
       </c>
       <c r="R34">
-        <v>1.95</v>
+        <v>1.925</v>
       </c>
       <c r="S34">
         <v>1.75</v>
       </c>
       <c r="T34">
-        <v>1.775</v>
+        <v>1.9</v>
       </c>
       <c r="U34">
-        <v>2.025</v>
+        <v>1.9</v>
       </c>
       <c r="V34">
-        <v>-1</v>
+        <v>0.6499999999999999</v>
       </c>
       <c r="W34">
         <v>-1</v>
       </c>
       <c r="X34">
-        <v>1.625</v>
+        <v>-1</v>
       </c>
       <c r="Y34">
-        <v>-1</v>
+        <v>0.4375</v>
       </c>
       <c r="Z34">
-        <v>0.95</v>
+        <v>-0.5</v>
       </c>
       <c r="AA34">
-        <v>0.7749999999999999</v>
+        <v>-1</v>
       </c>
       <c r="AB34">
-        <v>-1</v>
+        <v>0.8999999999999999</v>
       </c>
     </row>
     <row r="35" spans="1:28">
@@ -3451,7 +3451,7 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>6888609</v>
+        <v>6888611</v>
       </c>
       <c r="C35" t="s">
         <v>27</v>
@@ -3460,76 +3460,76 @@
         <v>45117.55208333334</v>
       </c>
       <c r="E35" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="F35" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="G35">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H35">
         <v>1</v>
       </c>
       <c r="I35" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J35">
-        <v>1.666</v>
+        <v>2.05</v>
       </c>
       <c r="K35">
-        <v>3</v>
+        <v>2.9</v>
       </c>
       <c r="L35">
-        <v>5.5</v>
+        <v>3.6</v>
       </c>
       <c r="M35">
-        <v>1.833</v>
+        <v>1.65</v>
       </c>
       <c r="N35">
-        <v>3</v>
+        <v>3.25</v>
       </c>
       <c r="O35">
-        <v>4.2</v>
+        <v>5</v>
       </c>
       <c r="P35">
-        <v>-0.5</v>
+        <v>-0.75</v>
       </c>
       <c r="Q35">
+        <v>1.9</v>
+      </c>
+      <c r="R35">
+        <v>1.9</v>
+      </c>
+      <c r="S35">
+        <v>2.25</v>
+      </c>
+      <c r="T35">
         <v>2.025</v>
       </c>
-      <c r="R35">
+      <c r="U35">
         <v>1.775</v>
       </c>
-      <c r="S35">
-        <v>2</v>
-      </c>
-      <c r="T35">
-        <v>1.95</v>
-      </c>
-      <c r="U35">
-        <v>1.85</v>
-      </c>
       <c r="V35">
-        <v>-1</v>
+        <v>0.6499999999999999</v>
       </c>
       <c r="W35">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="X35">
         <v>-1</v>
       </c>
       <c r="Y35">
-        <v>-1</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="Z35">
-        <v>0.7749999999999999</v>
+        <v>-1</v>
       </c>
       <c r="AA35">
-        <v>0</v>
+        <v>1.025</v>
       </c>
       <c r="AB35">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="36" spans="1:28">
@@ -3623,7 +3623,7 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>6888612</v>
+        <v>6888615</v>
       </c>
       <c r="C37" t="s">
         <v>27</v>
@@ -3632,13 +3632,13 @@
         <v>45117.55208333334</v>
       </c>
       <c r="E37" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="F37" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="G37">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H37">
         <v>0</v>
@@ -3647,43 +3647,43 @@
         <v>45</v>
       </c>
       <c r="J37">
-        <v>1.727</v>
+        <v>3.5</v>
       </c>
       <c r="K37">
-        <v>3.2</v>
+        <v>2.875</v>
       </c>
       <c r="L37">
-        <v>4.5</v>
+        <v>2.1</v>
       </c>
       <c r="M37">
-        <v>1.65</v>
+        <v>1.7</v>
       </c>
       <c r="N37">
-        <v>3.3</v>
+        <v>3</v>
       </c>
       <c r="O37">
-        <v>5.75</v>
+        <v>5.25</v>
       </c>
       <c r="P37">
-        <v>-0.75</v>
+        <v>-0.5</v>
       </c>
       <c r="Q37">
+        <v>1.775</v>
+      </c>
+      <c r="R37">
+        <v>2.025</v>
+      </c>
+      <c r="S37">
+        <v>2</v>
+      </c>
+      <c r="T37">
         <v>1.875</v>
       </c>
-      <c r="R37">
+      <c r="U37">
         <v>1.925</v>
       </c>
-      <c r="S37">
-        <v>1.75</v>
-      </c>
-      <c r="T37">
-        <v>1.9</v>
-      </c>
-      <c r="U37">
-        <v>1.9</v>
-      </c>
       <c r="V37">
-        <v>0.6499999999999999</v>
+        <v>0.7</v>
       </c>
       <c r="W37">
         <v>-1</v>
@@ -3692,16 +3692,16 @@
         <v>-1</v>
       </c>
       <c r="Y37">
-        <v>0.4375</v>
+        <v>0.7749999999999999</v>
       </c>
       <c r="Z37">
-        <v>-0.5</v>
+        <v>-1</v>
       </c>
       <c r="AA37">
-        <v>-1</v>
+        <v>0.875</v>
       </c>
       <c r="AB37">
-        <v>0.8999999999999999</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="38" spans="1:28">
@@ -3709,7 +3709,7 @@
         <v>36</v>
       </c>
       <c r="B38">
-        <v>6888611</v>
+        <v>6888609</v>
       </c>
       <c r="C38" t="s">
         <v>27</v>
@@ -3718,76 +3718,76 @@
         <v>45117.55208333334</v>
       </c>
       <c r="E38" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="F38" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="G38">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H38">
         <v>1</v>
       </c>
       <c r="I38" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="J38">
-        <v>2.05</v>
+        <v>1.666</v>
       </c>
       <c r="K38">
-        <v>2.9</v>
+        <v>3</v>
       </c>
       <c r="L38">
-        <v>3.6</v>
+        <v>5.5</v>
       </c>
       <c r="M38">
-        <v>1.65</v>
+        <v>1.833</v>
       </c>
       <c r="N38">
-        <v>3.25</v>
+        <v>3</v>
       </c>
       <c r="O38">
-        <v>5</v>
+        <v>4.2</v>
       </c>
       <c r="P38">
-        <v>-0.75</v>
+        <v>-0.5</v>
       </c>
       <c r="Q38">
-        <v>1.9</v>
+        <v>2.025</v>
       </c>
       <c r="R38">
-        <v>1.9</v>
+        <v>1.775</v>
       </c>
       <c r="S38">
-        <v>2.25</v>
+        <v>2</v>
       </c>
       <c r="T38">
-        <v>2.025</v>
+        <v>1.95</v>
       </c>
       <c r="U38">
-        <v>1.775</v>
+        <v>1.85</v>
       </c>
       <c r="V38">
-        <v>0.6499999999999999</v>
+        <v>-1</v>
       </c>
       <c r="W38">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="X38">
         <v>-1</v>
       </c>
       <c r="Y38">
-        <v>0.8999999999999999</v>
+        <v>-1</v>
       </c>
       <c r="Z38">
-        <v>-1</v>
+        <v>0.7749999999999999</v>
       </c>
       <c r="AA38">
-        <v>1.025</v>
+        <v>0</v>
       </c>
       <c r="AB38">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:28">
@@ -3795,7 +3795,7 @@
         <v>37</v>
       </c>
       <c r="B39">
-        <v>6888613</v>
+        <v>6888614</v>
       </c>
       <c r="C39" t="s">
         <v>27</v>
@@ -3804,73 +3804,73 @@
         <v>45117.55208333334</v>
       </c>
       <c r="E39" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="F39" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="G39">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H39">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I39" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="J39">
-        <v>1.4</v>
+        <v>1.8</v>
       </c>
       <c r="K39">
-        <v>3.75</v>
+        <v>3.2</v>
       </c>
       <c r="L39">
-        <v>7.5</v>
+        <v>4</v>
       </c>
       <c r="M39">
-        <v>1.363</v>
+        <v>2.5</v>
       </c>
       <c r="N39">
-        <v>4.333</v>
+        <v>3</v>
       </c>
       <c r="O39">
-        <v>7</v>
+        <v>2.625</v>
       </c>
       <c r="P39">
-        <v>-1.25</v>
+        <v>0</v>
       </c>
       <c r="Q39">
-        <v>1.925</v>
+        <v>1.85</v>
       </c>
       <c r="R39">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="S39">
-        <v>2.25</v>
+        <v>1.75</v>
       </c>
       <c r="T39">
-        <v>1.975</v>
+        <v>1.775</v>
       </c>
       <c r="U39">
-        <v>1.825</v>
+        <v>2.025</v>
       </c>
       <c r="V39">
-        <v>0.363</v>
+        <v>-1</v>
       </c>
       <c r="W39">
         <v>-1</v>
       </c>
       <c r="X39">
-        <v>-1</v>
+        <v>1.625</v>
       </c>
       <c r="Y39">
-        <v>-0.5</v>
+        <v>-1</v>
       </c>
       <c r="Z39">
-        <v>0.4375</v>
+        <v>0.95</v>
       </c>
       <c r="AA39">
-        <v>0.9750000000000001</v>
+        <v>0.7749999999999999</v>
       </c>
       <c r="AB39">
         <v>-1</v>
@@ -4065,7 +4065,7 @@
         <v>30</v>
       </c>
       <c r="F42" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G42">
         <v>1</v>
@@ -4237,7 +4237,7 @@
         <v>33</v>
       </c>
       <c r="F44" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G44">
         <v>2</v>
@@ -4495,7 +4495,7 @@
         <v>35</v>
       </c>
       <c r="F47" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G47">
         <v>1</v>
@@ -4569,7 +4569,7 @@
         <v>46</v>
       </c>
       <c r="B48">
-        <v>7239829</v>
+        <v>7230929</v>
       </c>
       <c r="C48" t="s">
         <v>27</v>
@@ -4578,73 +4578,73 @@
         <v>45191.5</v>
       </c>
       <c r="E48" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="F48" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="G48">
         <v>2</v>
       </c>
       <c r="H48">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I48" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="J48">
-        <v>1.95</v>
+        <v>3.3</v>
       </c>
       <c r="K48">
         <v>3</v>
       </c>
       <c r="L48">
-        <v>3.75</v>
+        <v>2.1</v>
       </c>
       <c r="M48">
-        <v>3.25</v>
+        <v>2.375</v>
       </c>
       <c r="N48">
-        <v>2.9</v>
+        <v>3</v>
       </c>
       <c r="O48">
-        <v>2.2</v>
+        <v>2.8</v>
       </c>
       <c r="P48">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="Q48">
-        <v>1.9</v>
+        <v>1.8</v>
       </c>
       <c r="R48">
-        <v>1.9</v>
+        <v>2</v>
       </c>
       <c r="S48">
-        <v>1.75</v>
+        <v>2</v>
       </c>
       <c r="T48">
-        <v>1.85</v>
+        <v>1.8</v>
       </c>
       <c r="U48">
-        <v>1.95</v>
+        <v>2</v>
       </c>
       <c r="V48">
-        <v>2.25</v>
+        <v>-1</v>
       </c>
       <c r="W48">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="X48">
         <v>-1</v>
       </c>
       <c r="Y48">
-        <v>0.8999999999999999</v>
+        <v>0</v>
       </c>
       <c r="Z48">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AA48">
-        <v>0.8500000000000001</v>
+        <v>0.8</v>
       </c>
       <c r="AB48">
         <v>-1</v>
@@ -4655,7 +4655,7 @@
         <v>47</v>
       </c>
       <c r="B49">
-        <v>7230929</v>
+        <v>7239829</v>
       </c>
       <c r="C49" t="s">
         <v>27</v>
@@ -4664,73 +4664,73 @@
         <v>45191.5</v>
       </c>
       <c r="E49" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="F49" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="G49">
         <v>2</v>
       </c>
       <c r="H49">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I49" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J49">
-        <v>3.3</v>
+        <v>1.95</v>
       </c>
       <c r="K49">
         <v>3</v>
       </c>
       <c r="L49">
-        <v>2.1</v>
+        <v>3.75</v>
       </c>
       <c r="M49">
-        <v>2.375</v>
+        <v>3.25</v>
       </c>
       <c r="N49">
-        <v>3</v>
+        <v>2.9</v>
       </c>
       <c r="O49">
-        <v>2.8</v>
+        <v>2.2</v>
       </c>
       <c r="P49">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="Q49">
-        <v>1.8</v>
+        <v>1.9</v>
       </c>
       <c r="R49">
-        <v>2</v>
+        <v>1.9</v>
       </c>
       <c r="S49">
-        <v>2</v>
+        <v>1.75</v>
       </c>
       <c r="T49">
-        <v>1.8</v>
+        <v>1.85</v>
       </c>
       <c r="U49">
-        <v>2</v>
+        <v>1.95</v>
       </c>
       <c r="V49">
-        <v>-1</v>
+        <v>2.25</v>
       </c>
       <c r="W49">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="X49">
         <v>-1</v>
       </c>
       <c r="Y49">
-        <v>0</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="Z49">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AA49">
-        <v>0.8</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AB49">
         <v>-1</v>
@@ -4922,7 +4922,7 @@
         <v>45192.625</v>
       </c>
       <c r="E52" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F52" t="s">
         <v>44</v>
@@ -5008,7 +5008,7 @@
         <v>45192.625</v>
       </c>
       <c r="E53" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F53" t="s">
         <v>35</v>
@@ -5094,7 +5094,7 @@
         <v>45192.625</v>
       </c>
       <c r="E54" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F54" t="s">
         <v>32</v>
@@ -5257,7 +5257,7 @@
         <v>54</v>
       </c>
       <c r="B56">
-        <v>7230948</v>
+        <v>7230934</v>
       </c>
       <c r="C56" t="s">
         <v>27</v>
@@ -5266,76 +5266,76 @@
         <v>45198.48958333334</v>
       </c>
       <c r="E56" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="F56" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="G56">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H56">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I56" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="J56">
         <v>3.2</v>
       </c>
       <c r="K56">
+        <v>2.8</v>
+      </c>
+      <c r="L56">
+        <v>2.25</v>
+      </c>
+      <c r="M56">
+        <v>1.95</v>
+      </c>
+      <c r="N56">
         <v>2.9</v>
       </c>
-      <c r="L56">
-        <v>2.2</v>
-      </c>
-      <c r="M56">
-        <v>2.05</v>
-      </c>
-      <c r="N56">
-        <v>3</v>
-      </c>
       <c r="O56">
-        <v>3.6</v>
+        <v>3.75</v>
       </c>
       <c r="P56">
         <v>-0.25</v>
       </c>
       <c r="Q56">
-        <v>1.75</v>
+        <v>1.775</v>
       </c>
       <c r="R56">
-        <v>2.05</v>
+        <v>2.025</v>
       </c>
       <c r="S56">
         <v>1.75</v>
       </c>
       <c r="T56">
+        <v>1.8</v>
+      </c>
+      <c r="U56">
+        <v>2</v>
+      </c>
+      <c r="V56">
+        <v>-1</v>
+      </c>
+      <c r="W56">
         <v>1.9</v>
       </c>
-      <c r="U56">
-        <v>1.9</v>
-      </c>
-      <c r="V56">
-        <v>1.05</v>
-      </c>
-      <c r="W56">
-        <v>-1</v>
-      </c>
       <c r="X56">
         <v>-1</v>
       </c>
       <c r="Y56">
-        <v>0.75</v>
+        <v>-0.5</v>
       </c>
       <c r="Z56">
-        <v>-1</v>
+        <v>0.5125</v>
       </c>
       <c r="AA56">
-        <v>0.8999999999999999</v>
+        <v>-1</v>
       </c>
       <c r="AB56">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:28">
@@ -5355,7 +5355,7 @@
         <v>39</v>
       </c>
       <c r="F57" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G57">
         <v>2</v>
@@ -5429,7 +5429,7 @@
         <v>56</v>
       </c>
       <c r="B58">
-        <v>7230934</v>
+        <v>7230948</v>
       </c>
       <c r="C58" t="s">
         <v>27</v>
@@ -5438,76 +5438,76 @@
         <v>45198.48958333334</v>
       </c>
       <c r="E58" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="F58" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="G58">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H58">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I58" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J58">
         <v>3.2</v>
       </c>
       <c r="K58">
-        <v>2.8</v>
+        <v>2.9</v>
       </c>
       <c r="L58">
-        <v>2.25</v>
+        <v>2.2</v>
       </c>
       <c r="M58">
-        <v>1.95</v>
+        <v>2.05</v>
       </c>
       <c r="N58">
-        <v>2.9</v>
+        <v>3</v>
       </c>
       <c r="O58">
-        <v>3.75</v>
+        <v>3.6</v>
       </c>
       <c r="P58">
         <v>-0.25</v>
       </c>
       <c r="Q58">
-        <v>1.775</v>
+        <v>1.75</v>
       </c>
       <c r="R58">
-        <v>2.025</v>
+        <v>2.05</v>
       </c>
       <c r="S58">
         <v>1.75</v>
       </c>
       <c r="T58">
-        <v>1.8</v>
+        <v>1.9</v>
       </c>
       <c r="U58">
-        <v>2</v>
+        <v>1.9</v>
       </c>
       <c r="V58">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="W58">
-        <v>1.9</v>
+        <v>-1</v>
       </c>
       <c r="X58">
         <v>-1</v>
       </c>
       <c r="Y58">
-        <v>-0.5</v>
+        <v>0.75</v>
       </c>
       <c r="Z58">
-        <v>0.5125</v>
+        <v>-1</v>
       </c>
       <c r="AA58">
-        <v>-1</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AB58">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="59" spans="1:28">
@@ -5773,7 +5773,7 @@
         <v>60</v>
       </c>
       <c r="B62">
-        <v>7230942</v>
+        <v>7230950</v>
       </c>
       <c r="C62" t="s">
         <v>27</v>
@@ -5782,58 +5782,58 @@
         <v>45205.48958333334</v>
       </c>
       <c r="E62" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="F62" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G62">
+        <v>5</v>
+      </c>
+      <c r="H62">
         <v>3</v>
-      </c>
-      <c r="H62">
-        <v>0</v>
       </c>
       <c r="I62" t="s">
         <v>45</v>
       </c>
       <c r="J62">
-        <v>1.571</v>
+        <v>1.727</v>
       </c>
       <c r="K62">
+        <v>3.25</v>
+      </c>
+      <c r="L62">
+        <v>4.333</v>
+      </c>
+      <c r="M62">
+        <v>1.5</v>
+      </c>
+      <c r="N62">
         <v>3.5</v>
       </c>
-      <c r="L62">
-        <v>5.25</v>
-      </c>
-      <c r="M62">
-        <v>1.666</v>
-      </c>
-      <c r="N62">
-        <v>3.3</v>
-      </c>
       <c r="O62">
-        <v>4.75</v>
+        <v>6</v>
       </c>
       <c r="P62">
-        <v>-0.75</v>
+        <v>-1</v>
       </c>
       <c r="Q62">
-        <v>1.95</v>
+        <v>1.925</v>
       </c>
       <c r="R62">
-        <v>1.85</v>
+        <v>1.875</v>
       </c>
       <c r="S62">
         <v>2</v>
       </c>
       <c r="T62">
-        <v>1.95</v>
+        <v>1.8</v>
       </c>
       <c r="U62">
-        <v>1.85</v>
+        <v>2</v>
       </c>
       <c r="V62">
-        <v>0.6659999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="W62">
         <v>-1</v>
@@ -5842,13 +5842,13 @@
         <v>-1</v>
       </c>
       <c r="Y62">
-        <v>0.95</v>
+        <v>0.925</v>
       </c>
       <c r="Z62">
         <v>-1</v>
       </c>
       <c r="AA62">
-        <v>0.95</v>
+        <v>0.8</v>
       </c>
       <c r="AB62">
         <v>-1</v>
@@ -5859,7 +5859,7 @@
         <v>61</v>
       </c>
       <c r="B63">
-        <v>7230950</v>
+        <v>7230942</v>
       </c>
       <c r="C63" t="s">
         <v>27</v>
@@ -5868,58 +5868,58 @@
         <v>45205.48958333334</v>
       </c>
       <c r="E63" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="F63" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G63">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H63">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I63" t="s">
         <v>45</v>
       </c>
       <c r="J63">
-        <v>1.727</v>
+        <v>1.571</v>
       </c>
       <c r="K63">
-        <v>3.25</v>
+        <v>3.5</v>
       </c>
       <c r="L63">
-        <v>4.333</v>
+        <v>5.25</v>
       </c>
       <c r="M63">
-        <v>1.5</v>
+        <v>1.666</v>
       </c>
       <c r="N63">
-        <v>3.5</v>
+        <v>3.3</v>
       </c>
       <c r="O63">
-        <v>6</v>
+        <v>4.75</v>
       </c>
       <c r="P63">
-        <v>-1</v>
+        <v>-0.75</v>
       </c>
       <c r="Q63">
-        <v>1.925</v>
+        <v>1.95</v>
       </c>
       <c r="R63">
-        <v>1.875</v>
+        <v>1.85</v>
       </c>
       <c r="S63">
         <v>2</v>
       </c>
       <c r="T63">
-        <v>1.8</v>
+        <v>1.95</v>
       </c>
       <c r="U63">
-        <v>2</v>
+        <v>1.85</v>
       </c>
       <c r="V63">
-        <v>0.5</v>
+        <v>0.6659999999999999</v>
       </c>
       <c r="W63">
         <v>-1</v>
@@ -5928,13 +5928,13 @@
         <v>-1</v>
       </c>
       <c r="Y63">
-        <v>0.925</v>
+        <v>0.95</v>
       </c>
       <c r="Z63">
         <v>-1</v>
       </c>
       <c r="AA63">
-        <v>0.8</v>
+        <v>0.95</v>
       </c>
       <c r="AB63">
         <v>-1</v>
@@ -5954,7 +5954,7 @@
         <v>45205.625</v>
       </c>
       <c r="E64" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F64" t="s">
         <v>29</v>
@@ -6040,7 +6040,7 @@
         <v>45205.625</v>
       </c>
       <c r="E65" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F65" t="s">
         <v>39</v>
@@ -6645,7 +6645,7 @@
         <v>29</v>
       </c>
       <c r="F72" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G72">
         <v>1</v>
@@ -6814,7 +6814,7 @@
         <v>45240.48958333334</v>
       </c>
       <c r="E74" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F74" t="s">
         <v>31</v>
@@ -6989,7 +6989,7 @@
         <v>30</v>
       </c>
       <c r="F76" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G76">
         <v>0</v>
@@ -7416,7 +7416,7 @@
         <v>45244.625</v>
       </c>
       <c r="E81" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F81" t="s">
         <v>34</v>
@@ -7674,7 +7674,7 @@
         <v>45247.53125</v>
       </c>
       <c r="E84" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F84" t="s">
         <v>30</v>
@@ -7935,7 +7935,7 @@
         <v>33</v>
       </c>
       <c r="F87" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G87">
         <v>2</v>
@@ -8018,7 +8018,7 @@
         <v>45248.58333333334</v>
       </c>
       <c r="E88" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F88" t="s">
         <v>34</v>
@@ -8451,7 +8451,7 @@
         <v>31</v>
       </c>
       <c r="F93" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G93">
         <v>1</v>
@@ -8881,7 +8881,7 @@
         <v>35</v>
       </c>
       <c r="F98" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G98">
         <v>0</v>
@@ -9050,7 +9050,7 @@
         <v>45262.58333333334</v>
       </c>
       <c r="E100" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F100" t="s">
         <v>31</v>
@@ -9566,10 +9566,10 @@
         <v>45269.58333333334</v>
       </c>
       <c r="E106" t="s">
+        <v>36</v>
+      </c>
+      <c r="F106" t="s">
         <v>38</v>
-      </c>
-      <c r="F106" t="s">
-        <v>37</v>
       </c>
       <c r="G106">
         <v>2</v>
@@ -9643,7 +9643,7 @@
         <v>105</v>
       </c>
       <c r="B107">
-        <v>7567197</v>
+        <v>7567876</v>
       </c>
       <c r="C107" t="s">
         <v>27</v>
@@ -9652,10 +9652,10 @@
         <v>45275.46875</v>
       </c>
       <c r="E107" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="F107" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="G107">
         <v>1</v>
@@ -9667,61 +9667,61 @@
         <v>46</v>
       </c>
       <c r="J107">
-        <v>2</v>
+        <v>4.75</v>
       </c>
       <c r="K107">
-        <v>3</v>
+        <v>3.1</v>
       </c>
       <c r="L107">
-        <v>3.6</v>
+        <v>1.727</v>
       </c>
       <c r="M107">
+        <v>6</v>
+      </c>
+      <c r="N107">
+        <v>3.1</v>
+      </c>
+      <c r="O107">
+        <v>1.65</v>
+      </c>
+      <c r="P107">
+        <v>0.75</v>
+      </c>
+      <c r="Q107">
+        <v>1.975</v>
+      </c>
+      <c r="R107">
+        <v>1.825</v>
+      </c>
+      <c r="S107">
+        <v>2</v>
+      </c>
+      <c r="T107">
+        <v>2</v>
+      </c>
+      <c r="U107">
+        <v>1.8</v>
+      </c>
+      <c r="V107">
+        <v>-1</v>
+      </c>
+      <c r="W107">
         <v>2.1</v>
       </c>
-      <c r="N107">
-        <v>2.9</v>
-      </c>
-      <c r="O107">
-        <v>3.5</v>
-      </c>
-      <c r="P107">
-        <v>-0.25</v>
-      </c>
-      <c r="Q107">
-        <v>1.825</v>
-      </c>
-      <c r="R107">
-        <v>1.975</v>
-      </c>
-      <c r="S107">
-        <v>1.75</v>
-      </c>
-      <c r="T107">
-        <v>1.85</v>
-      </c>
-      <c r="U107">
-        <v>1.95</v>
-      </c>
-      <c r="V107">
-        <v>-1</v>
-      </c>
-      <c r="W107">
-        <v>1.9</v>
-      </c>
       <c r="X107">
         <v>-1</v>
       </c>
       <c r="Y107">
-        <v>-0.5</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="Z107">
-        <v>0.4875</v>
+        <v>-1</v>
       </c>
       <c r="AA107">
-        <v>0.425</v>
+        <v>0</v>
       </c>
       <c r="AB107">
-        <v>-0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="108" spans="1:28">
@@ -9729,7 +9729,7 @@
         <v>106</v>
       </c>
       <c r="B108">
-        <v>7567876</v>
+        <v>7567197</v>
       </c>
       <c r="C108" t="s">
         <v>27</v>
@@ -9738,10 +9738,10 @@
         <v>45275.46875</v>
       </c>
       <c r="E108" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="F108" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="G108">
         <v>1</v>
@@ -9753,61 +9753,61 @@
         <v>46</v>
       </c>
       <c r="J108">
-        <v>4.75</v>
+        <v>2</v>
       </c>
       <c r="K108">
-        <v>3.1</v>
+        <v>3</v>
       </c>
       <c r="L108">
-        <v>1.727</v>
+        <v>3.6</v>
       </c>
       <c r="M108">
-        <v>6</v>
+        <v>2.1</v>
       </c>
       <c r="N108">
-        <v>3.1</v>
+        <v>2.9</v>
       </c>
       <c r="O108">
-        <v>1.65</v>
+        <v>3.5</v>
       </c>
       <c r="P108">
-        <v>0.75</v>
+        <v>-0.25</v>
       </c>
       <c r="Q108">
+        <v>1.825</v>
+      </c>
+      <c r="R108">
         <v>1.975</v>
       </c>
-      <c r="R108">
-        <v>1.825</v>
-      </c>
       <c r="S108">
-        <v>2</v>
+        <v>1.75</v>
       </c>
       <c r="T108">
-        <v>2</v>
+        <v>1.85</v>
       </c>
       <c r="U108">
-        <v>1.8</v>
+        <v>1.95</v>
       </c>
       <c r="V108">
         <v>-1</v>
       </c>
       <c r="W108">
-        <v>2.1</v>
+        <v>1.9</v>
       </c>
       <c r="X108">
         <v>-1</v>
       </c>
       <c r="Y108">
-        <v>0.9750000000000001</v>
+        <v>-0.5</v>
       </c>
       <c r="Z108">
-        <v>-1</v>
+        <v>0.4875</v>
       </c>
       <c r="AA108">
-        <v>0</v>
+        <v>0.425</v>
       </c>
       <c r="AB108">
-        <v>0</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="109" spans="1:28">
@@ -9999,7 +9999,7 @@
         <v>44</v>
       </c>
       <c r="F111" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G111">
         <v>1</v>
@@ -10254,10 +10254,10 @@
         <v>45276.625</v>
       </c>
       <c r="E114" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F114" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G114">
         <v>0</v>
@@ -10684,10 +10684,10 @@
         <v>45289.5</v>
       </c>
       <c r="E119" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F119" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G119">
         <v>1</v>
@@ -10770,7 +10770,7 @@
         <v>45289.58333333334</v>
       </c>
       <c r="E120" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F120" t="s">
         <v>43</v>
@@ -11031,7 +11031,7 @@
         <v>43</v>
       </c>
       <c r="F123" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G123">
         <v>2</v>
@@ -11117,7 +11117,7 @@
         <v>39</v>
       </c>
       <c r="F124" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G124">
         <v>0</v>
@@ -11289,7 +11289,7 @@
         <v>28</v>
       </c>
       <c r="F126" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G126">
         <v>1</v>
@@ -11544,7 +11544,7 @@
         <v>45300.625</v>
       </c>
       <c r="E129" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F129" t="s">
         <v>40</v>
@@ -11630,7 +11630,7 @@
         <v>45302.53125</v>
       </c>
       <c r="E130" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F130" t="s">
         <v>28</v>
@@ -11974,7 +11974,7 @@
         <v>45304.5</v>
       </c>
       <c r="E134" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F134" t="s">
         <v>32</v>
@@ -12146,7 +12146,7 @@
         <v>45304.58333333334</v>
       </c>
       <c r="E136" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F136" t="s">
         <v>43</v>
@@ -12321,7 +12321,7 @@
         <v>34</v>
       </c>
       <c r="F138" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G138">
         <v>2</v>
@@ -12395,7 +12395,7 @@
         <v>137</v>
       </c>
       <c r="B139">
-        <v>7567341</v>
+        <v>7567343</v>
       </c>
       <c r="C139" t="s">
         <v>27</v>
@@ -12404,76 +12404,76 @@
         <v>45310.47916666666</v>
       </c>
       <c r="E139" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F139" t="s">
         <v>36</v>
       </c>
       <c r="G139">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H139">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I139" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J139">
-        <v>1.5</v>
+        <v>1.727</v>
       </c>
       <c r="K139">
-        <v>3.6</v>
+        <v>3.4</v>
       </c>
       <c r="L139">
-        <v>6</v>
+        <v>4.2</v>
       </c>
       <c r="M139">
-        <v>1.615</v>
+        <v>2.15</v>
       </c>
       <c r="N139">
-        <v>3.3</v>
+        <v>3</v>
       </c>
       <c r="O139">
-        <v>5.5</v>
+        <v>3.1</v>
       </c>
       <c r="P139">
-        <v>-0.75</v>
+        <v>-0.25</v>
       </c>
       <c r="Q139">
+        <v>1.95</v>
+      </c>
+      <c r="R139">
         <v>1.85</v>
       </c>
-      <c r="R139">
-        <v>1.95</v>
-      </c>
       <c r="S139">
-        <v>2</v>
+        <v>1.75</v>
       </c>
       <c r="T139">
-        <v>1.975</v>
+        <v>1.75</v>
       </c>
       <c r="U139">
-        <v>1.825</v>
+        <v>2.05</v>
       </c>
       <c r="V139">
-        <v>-1</v>
+        <v>1.15</v>
       </c>
       <c r="W139">
         <v>-1</v>
       </c>
       <c r="X139">
-        <v>4.5</v>
+        <v>-1</v>
       </c>
       <c r="Y139">
-        <v>-1</v>
+        <v>0.95</v>
       </c>
       <c r="Z139">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
       <c r="AA139">
         <v>-1</v>
       </c>
       <c r="AB139">
-        <v>0.825</v>
+        <v>1.05</v>
       </c>
     </row>
     <row r="140" spans="1:28">
@@ -12481,7 +12481,7 @@
         <v>138</v>
       </c>
       <c r="B140">
-        <v>7567343</v>
+        <v>7567342</v>
       </c>
       <c r="C140" t="s">
         <v>27</v>
@@ -12490,76 +12490,76 @@
         <v>45310.47916666666</v>
       </c>
       <c r="E140" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="F140" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="G140">
         <v>1</v>
       </c>
       <c r="H140">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I140" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="J140">
-        <v>1.727</v>
+        <v>2.5</v>
       </c>
       <c r="K140">
-        <v>3.4</v>
+        <v>2.8</v>
       </c>
       <c r="L140">
-        <v>4.2</v>
+        <v>2.8</v>
       </c>
       <c r="M140">
-        <v>2.15</v>
+        <v>2.375</v>
       </c>
       <c r="N140">
-        <v>3</v>
+        <v>2.7</v>
       </c>
       <c r="O140">
-        <v>3.1</v>
+        <v>3.2</v>
       </c>
       <c r="P140">
-        <v>-0.25</v>
+        <v>0</v>
       </c>
       <c r="Q140">
-        <v>1.95</v>
+        <v>1.725</v>
       </c>
       <c r="R140">
-        <v>1.85</v>
+        <v>2.075</v>
       </c>
       <c r="S140">
         <v>1.75</v>
       </c>
       <c r="T140">
-        <v>1.75</v>
+        <v>1.775</v>
       </c>
       <c r="U140">
-        <v>2.05</v>
+        <v>2.025</v>
       </c>
       <c r="V140">
-        <v>1.15</v>
+        <v>-1</v>
       </c>
       <c r="W140">
-        <v>-1</v>
+        <v>1.7</v>
       </c>
       <c r="X140">
         <v>-1</v>
       </c>
       <c r="Y140">
-        <v>0.95</v>
+        <v>0</v>
       </c>
       <c r="Z140">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AA140">
-        <v>-1</v>
+        <v>0.3875</v>
       </c>
       <c r="AB140">
-        <v>1.05</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="141" spans="1:28">
@@ -12567,7 +12567,7 @@
         <v>139</v>
       </c>
       <c r="B141">
-        <v>7567342</v>
+        <v>7567341</v>
       </c>
       <c r="C141" t="s">
         <v>27</v>
@@ -12576,76 +12576,76 @@
         <v>45310.47916666666</v>
       </c>
       <c r="E141" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="F141" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="G141">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H141">
         <v>1</v>
       </c>
       <c r="I141" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="J141">
-        <v>2.5</v>
+        <v>1.5</v>
       </c>
       <c r="K141">
-        <v>2.8</v>
+        <v>3.6</v>
       </c>
       <c r="L141">
-        <v>2.8</v>
+        <v>6</v>
       </c>
       <c r="M141">
-        <v>2.375</v>
+        <v>1.615</v>
       </c>
       <c r="N141">
-        <v>2.7</v>
+        <v>3.3</v>
       </c>
       <c r="O141">
-        <v>3.2</v>
+        <v>5.5</v>
       </c>
       <c r="P141">
-        <v>0</v>
+        <v>-0.75</v>
       </c>
       <c r="Q141">
-        <v>1.725</v>
+        <v>1.85</v>
       </c>
       <c r="R141">
-        <v>2.075</v>
+        <v>1.95</v>
       </c>
       <c r="S141">
-        <v>1.75</v>
+        <v>2</v>
       </c>
       <c r="T141">
-        <v>1.775</v>
+        <v>1.975</v>
       </c>
       <c r="U141">
-        <v>2.025</v>
+        <v>1.825</v>
       </c>
       <c r="V141">
         <v>-1</v>
       </c>
       <c r="W141">
-        <v>1.7</v>
+        <v>-1</v>
       </c>
       <c r="X141">
-        <v>-1</v>
+        <v>4.5</v>
       </c>
       <c r="Y141">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Z141">
-        <v>0</v>
+        <v>0.95</v>
       </c>
       <c r="AA141">
-        <v>0.3875</v>
+        <v>-1</v>
       </c>
       <c r="AB141">
-        <v>-0.5</v>
+        <v>0.825</v>
       </c>
     </row>
     <row r="142" spans="1:28">
@@ -12923,7 +12923,7 @@
         <v>42</v>
       </c>
       <c r="F145" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G145">
         <v>1</v>
@@ -13092,7 +13092,7 @@
         <v>45314.54166666666</v>
       </c>
       <c r="E147" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F147" t="s">
         <v>40</v>
@@ -13350,7 +13350,7 @@
         <v>45317.53125</v>
       </c>
       <c r="E150" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F150" t="s">
         <v>28</v>
@@ -13436,7 +13436,7 @@
         <v>45317.54166666666</v>
       </c>
       <c r="E151" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F151" t="s">
         <v>42</v>
@@ -13694,7 +13694,7 @@
         <v>45318.5</v>
       </c>
       <c r="E154" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F154" t="s">
         <v>33</v>
@@ -13955,7 +13955,7 @@
         <v>40</v>
       </c>
       <c r="F157" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G157">
         <v>2</v>
@@ -14210,7 +14210,7 @@
         <v>45331.48958333334</v>
       </c>
       <c r="E160" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F160" t="s">
         <v>33</v>
@@ -14296,7 +14296,7 @@
         <v>45331.53125</v>
       </c>
       <c r="E161" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F161" t="s">
         <v>30</v>
@@ -14554,7 +14554,7 @@
         <v>45332.5</v>
       </c>
       <c r="E164" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F164" t="s">
         <v>35</v>
@@ -14815,7 +14815,7 @@
         <v>32</v>
       </c>
       <c r="F167" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G167">
         <v>3</v>
@@ -15159,7 +15159,7 @@
         <v>44</v>
       </c>
       <c r="F171" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G171">
         <v>2</v>
@@ -15245,7 +15245,7 @@
         <v>35</v>
       </c>
       <c r="F172" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G172">
         <v>1</v>
@@ -15414,7 +15414,7 @@
         <v>45345.5</v>
       </c>
       <c r="E174" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F174" t="s">
         <v>39</v>
@@ -15844,7 +15844,7 @@
         <v>45346.53125</v>
       </c>
       <c r="E179" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F179" t="s">
         <v>44</v>
@@ -15933,7 +15933,7 @@
         <v>39</v>
       </c>
       <c r="F180" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G180">
         <v>1</v>
@@ -16277,7 +16277,7 @@
         <v>29</v>
       </c>
       <c r="F184" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G184">
         <v>0</v>
@@ -16360,7 +16360,7 @@
         <v>45353.58333333334</v>
       </c>
       <c r="E185" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F185" t="s">
         <v>42</v>
@@ -16621,7 +16621,7 @@
         <v>31</v>
       </c>
       <c r="F188" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G188">
         <v>0</v>
@@ -16876,7 +16876,7 @@
         <v>45366.75</v>
       </c>
       <c r="E191" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F191" t="s">
         <v>29</v>
@@ -17048,7 +17048,7 @@
         <v>45367.75</v>
       </c>
       <c r="E193" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F193" t="s">
         <v>30</v>
@@ -17223,7 +17223,7 @@
         <v>34</v>
       </c>
       <c r="F195" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G195">
         <v>2</v>
@@ -17395,7 +17395,7 @@
         <v>30</v>
       </c>
       <c r="F197" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G197">
         <v>0</v>
@@ -17564,7 +17564,7 @@
         <v>45375.75</v>
       </c>
       <c r="E199" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F199" t="s">
         <v>33</v>
@@ -17653,7 +17653,7 @@
         <v>34</v>
       </c>
       <c r="F200" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G200">
         <v>1</v>
@@ -17997,7 +17997,7 @@
         <v>40</v>
       </c>
       <c r="F204" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G204">
         <v>2</v>
@@ -18157,7 +18157,7 @@
         <v>204</v>
       </c>
       <c r="B206">
-        <v>8007204</v>
+        <v>8007205</v>
       </c>
       <c r="C206" t="s">
         <v>27</v>
@@ -18166,49 +18166,49 @@
         <v>45387.75</v>
       </c>
       <c r="E206" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F206" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="G206">
         <v>1</v>
       </c>
       <c r="H206">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I206" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="J206">
-        <v>2</v>
+        <v>1.571</v>
       </c>
       <c r="K206">
-        <v>3</v>
+        <v>3.6</v>
       </c>
       <c r="L206">
+        <v>5</v>
+      </c>
+      <c r="M206">
+        <v>1.85</v>
+      </c>
+      <c r="N206">
+        <v>3.3</v>
+      </c>
+      <c r="O206">
         <v>3.6</v>
       </c>
-      <c r="M206">
-        <v>2.375</v>
-      </c>
-      <c r="N206">
-        <v>2.625</v>
-      </c>
-      <c r="O206">
-        <v>3.4</v>
-      </c>
       <c r="P206">
-        <v>-0.25</v>
+        <v>-0.5</v>
       </c>
       <c r="Q206">
-        <v>2.025</v>
+        <v>2</v>
       </c>
       <c r="R206">
-        <v>1.775</v>
+        <v>1.8</v>
       </c>
       <c r="S206">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="T206">
         <v>1.775</v>
@@ -18217,25 +18217,25 @@
         <v>2.025</v>
       </c>
       <c r="V206">
-        <v>1.375</v>
+        <v>-1</v>
       </c>
       <c r="W206">
         <v>-1</v>
       </c>
       <c r="X206">
-        <v>-1</v>
+        <v>2.6</v>
       </c>
       <c r="Y206">
-        <v>1.025</v>
+        <v>-1</v>
       </c>
       <c r="Z206">
-        <v>-1</v>
+        <v>0.8</v>
       </c>
       <c r="AA206">
-        <v>-1</v>
+        <v>0.7749999999999999</v>
       </c>
       <c r="AB206">
-        <v>1.025</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="207" spans="1:28">
@@ -18243,7 +18243,7 @@
         <v>205</v>
       </c>
       <c r="B207">
-        <v>8007203</v>
+        <v>8007204</v>
       </c>
       <c r="C207" t="s">
         <v>27</v>
@@ -18252,13 +18252,13 @@
         <v>45387.75</v>
       </c>
       <c r="E207" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="F207" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="G207">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H207">
         <v>0</v>
@@ -18267,43 +18267,43 @@
         <v>45</v>
       </c>
       <c r="J207">
-        <v>1.071</v>
+        <v>2</v>
       </c>
       <c r="K207">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="L207">
-        <v>34</v>
+        <v>3.6</v>
       </c>
       <c r="M207">
-        <v>1.035</v>
+        <v>2.375</v>
       </c>
       <c r="N207">
-        <v>15</v>
+        <v>2.625</v>
       </c>
       <c r="O207">
-        <v>41</v>
+        <v>3.4</v>
       </c>
       <c r="P207">
-        <v>-3.25</v>
+        <v>-0.25</v>
       </c>
       <c r="Q207">
-        <v>1.825</v>
+        <v>2.025</v>
       </c>
       <c r="R207">
-        <v>1.975</v>
+        <v>1.775</v>
       </c>
       <c r="S207">
-        <v>4</v>
+        <v>1.5</v>
       </c>
       <c r="T207">
-        <v>1.85</v>
+        <v>1.775</v>
       </c>
       <c r="U207">
-        <v>1.95</v>
+        <v>2.025</v>
       </c>
       <c r="V207">
-        <v>0.03499999999999992</v>
+        <v>1.375</v>
       </c>
       <c r="W207">
         <v>-1</v>
@@ -18312,16 +18312,16 @@
         <v>-1</v>
       </c>
       <c r="Y207">
-        <v>-0.5</v>
+        <v>1.025</v>
       </c>
       <c r="Z207">
-        <v>0.4875</v>
+        <v>-1</v>
       </c>
       <c r="AA207">
         <v>-1</v>
       </c>
       <c r="AB207">
-        <v>0.95</v>
+        <v>1.025</v>
       </c>
     </row>
     <row r="208" spans="1:28">
@@ -18329,7 +18329,7 @@
         <v>206</v>
       </c>
       <c r="B208">
-        <v>8007205</v>
+        <v>8007203</v>
       </c>
       <c r="C208" t="s">
         <v>27</v>
@@ -18338,76 +18338,76 @@
         <v>45387.75</v>
       </c>
       <c r="E208" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="F208" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="G208">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H208">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I208" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J208">
-        <v>1.571</v>
+        <v>1.071</v>
       </c>
       <c r="K208">
-        <v>3.6</v>
+        <v>8</v>
       </c>
       <c r="L208">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="M208">
+        <v>1.035</v>
+      </c>
+      <c r="N208">
+        <v>15</v>
+      </c>
+      <c r="O208">
+        <v>41</v>
+      </c>
+      <c r="P208">
+        <v>-3.25</v>
+      </c>
+      <c r="Q208">
+        <v>1.825</v>
+      </c>
+      <c r="R208">
+        <v>1.975</v>
+      </c>
+      <c r="S208">
+        <v>4</v>
+      </c>
+      <c r="T208">
         <v>1.85</v>
       </c>
-      <c r="N208">
-        <v>3.3</v>
-      </c>
-      <c r="O208">
-        <v>3.6</v>
-      </c>
-      <c r="P208">
+      <c r="U208">
+        <v>1.95</v>
+      </c>
+      <c r="V208">
+        <v>0.03499999999999992</v>
+      </c>
+      <c r="W208">
+        <v>-1</v>
+      </c>
+      <c r="X208">
+        <v>-1</v>
+      </c>
+      <c r="Y208">
         <v>-0.5</v>
       </c>
-      <c r="Q208">
-        <v>2</v>
-      </c>
-      <c r="R208">
-        <v>1.8</v>
-      </c>
-      <c r="S208">
-        <v>2</v>
-      </c>
-      <c r="T208">
-        <v>1.775</v>
-      </c>
-      <c r="U208">
-        <v>2.025</v>
-      </c>
-      <c r="V208">
-        <v>-1</v>
-      </c>
-      <c r="W208">
-        <v>-1</v>
-      </c>
-      <c r="X208">
-        <v>2.6</v>
-      </c>
-      <c r="Y208">
-        <v>-1</v>
-      </c>
       <c r="Z208">
-        <v>0.8</v>
+        <v>0.4875</v>
       </c>
       <c r="AA208">
-        <v>0.7749999999999999</v>
+        <v>-1</v>
       </c>
       <c r="AB208">
-        <v>-1</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="209" spans="1:28">
@@ -18599,7 +18599,7 @@
         <v>31</v>
       </c>
       <c r="F211" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G211">
         <v>3</v>
@@ -18768,7 +18768,7 @@
         <v>45401.5</v>
       </c>
       <c r="E213" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F213" t="s">
         <v>35</v>
@@ -19029,7 +19029,7 @@
         <v>40</v>
       </c>
       <c r="F216" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G216">
         <v>4</v>
@@ -19198,10 +19198,10 @@
         <v>45408.5</v>
       </c>
       <c r="E218" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F218" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G218">
         <v>2</v>
@@ -19447,7 +19447,7 @@
         <v>219</v>
       </c>
       <c r="B221">
-        <v>8129021</v>
+        <v>8129022</v>
       </c>
       <c r="C221" t="s">
         <v>27</v>
@@ -19456,73 +19456,73 @@
         <v>45409.5</v>
       </c>
       <c r="E221" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="F221" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="G221">
         <v>2</v>
       </c>
       <c r="H221">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I221" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="J221">
+        <v>1.909</v>
+      </c>
+      <c r="K221">
+        <v>3.1</v>
+      </c>
+      <c r="L221">
+        <v>3.75</v>
+      </c>
+      <c r="M221">
+        <v>2.45</v>
+      </c>
+      <c r="N221">
+        <v>3</v>
+      </c>
+      <c r="O221">
+        <v>2.75</v>
+      </c>
+      <c r="P221">
+        <v>0</v>
+      </c>
+      <c r="Q221">
+        <v>1.75</v>
+      </c>
+      <c r="R221">
+        <v>2.05</v>
+      </c>
+      <c r="S221">
+        <v>2</v>
+      </c>
+      <c r="T221">
         <v>1.8</v>
       </c>
-      <c r="K221">
-        <v>3.25</v>
-      </c>
-      <c r="L221">
-        <v>4</v>
-      </c>
-      <c r="M221">
-        <v>1.571</v>
-      </c>
-      <c r="N221">
-        <v>3.5</v>
-      </c>
-      <c r="O221">
-        <v>5.25</v>
-      </c>
-      <c r="P221">
-        <v>-0.75</v>
-      </c>
-      <c r="Q221">
-        <v>1.775</v>
-      </c>
-      <c r="R221">
-        <v>2.025</v>
-      </c>
-      <c r="S221">
-        <v>2.25</v>
-      </c>
-      <c r="T221">
-        <v>1.95</v>
-      </c>
       <c r="U221">
-        <v>1.85</v>
+        <v>2</v>
       </c>
       <c r="V221">
         <v>-1</v>
       </c>
       <c r="W221">
-        <v>2.5</v>
+        <v>-1</v>
       </c>
       <c r="X221">
-        <v>-1</v>
+        <v>1.75</v>
       </c>
       <c r="Y221">
         <v>-1</v>
       </c>
       <c r="Z221">
-        <v>1.025</v>
+        <v>1.05</v>
       </c>
       <c r="AA221">
-        <v>0.95</v>
+        <v>0.8</v>
       </c>
       <c r="AB221">
         <v>-1</v>
@@ -19533,7 +19533,7 @@
         <v>220</v>
       </c>
       <c r="B222">
-        <v>8129022</v>
+        <v>8129021</v>
       </c>
       <c r="C222" t="s">
         <v>27</v>
@@ -19542,73 +19542,73 @@
         <v>45409.5</v>
       </c>
       <c r="E222" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="F222" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="G222">
         <v>2</v>
       </c>
       <c r="H222">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I222" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J222">
-        <v>1.909</v>
+        <v>1.8</v>
       </c>
       <c r="K222">
-        <v>3.1</v>
+        <v>3.25</v>
       </c>
       <c r="L222">
-        <v>3.75</v>
+        <v>4</v>
       </c>
       <c r="M222">
-        <v>2.45</v>
+        <v>1.571</v>
       </c>
       <c r="N222">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="O222">
-        <v>2.75</v>
+        <v>5.25</v>
       </c>
       <c r="P222">
-        <v>0</v>
+        <v>-0.75</v>
       </c>
       <c r="Q222">
-        <v>1.75</v>
+        <v>1.775</v>
       </c>
       <c r="R222">
-        <v>2.05</v>
+        <v>2.025</v>
       </c>
       <c r="S222">
-        <v>2</v>
+        <v>2.25</v>
       </c>
       <c r="T222">
-        <v>1.8</v>
+        <v>1.95</v>
       </c>
       <c r="U222">
-        <v>2</v>
+        <v>1.85</v>
       </c>
       <c r="V222">
         <v>-1</v>
       </c>
       <c r="W222">
-        <v>-1</v>
+        <v>2.5</v>
       </c>
       <c r="X222">
-        <v>1.75</v>
+        <v>-1</v>
       </c>
       <c r="Y222">
         <v>-1</v>
       </c>
       <c r="Z222">
-        <v>1.05</v>
+        <v>1.025</v>
       </c>
       <c r="AA222">
-        <v>0.8</v>
+        <v>0.95</v>
       </c>
       <c r="AB222">
         <v>-1</v>
@@ -19714,7 +19714,7 @@
         <v>45410.625</v>
       </c>
       <c r="E224" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F224" t="s">
         <v>40</v>

</xml_diff>

<commit_message>
Atualização de bases das ligas, do dia: 28-05-2024 às 07:50
</commit_message>
<xml_diff>
--- a/Algeria Division 1/Algeria Division 1.xlsx
+++ b/Algeria Division 1/Algeria Division 1.xlsx
@@ -130,7 +130,7 @@
     <t>JS Saoura</t>
   </si>
   <si>
-    <t>NC Magra</t>
+    <t>RC Arba</t>
   </si>
   <si>
     <t>ES Setif</t>
@@ -142,7 +142,7 @@
     <t>MC Oran</t>
   </si>
   <si>
-    <t>RC Arba</t>
+    <t>NC Magra</t>
   </si>
   <si>
     <t>CR Belouizdad</t>
@@ -637,7 +637,7 @@
         <v>30</v>
       </c>
       <c r="F2" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -913,7 +913,7 @@
         <v>33</v>
       </c>
       <c r="F5" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="G5">
         <v>2</v>
@@ -1545,7 +1545,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>6765583</v>
+        <v>6765584</v>
       </c>
       <c r="C12" t="s">
         <v>29</v>
@@ -1557,7 +1557,7 @@
         <v>38</v>
       </c>
       <c r="F12" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="G12">
         <v>2</v>
@@ -1569,49 +1569,49 @@
         <v>1</v>
       </c>
       <c r="J12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K12" t="s">
         <v>49</v>
       </c>
       <c r="L12">
-        <v>2.8</v>
+        <v>2.4</v>
       </c>
       <c r="M12">
         <v>2.8</v>
       </c>
       <c r="N12">
-        <v>2.55</v>
+        <v>3</v>
       </c>
       <c r="O12">
-        <v>2</v>
+        <v>2.05</v>
       </c>
       <c r="P12">
         <v>3</v>
       </c>
       <c r="Q12">
-        <v>3.75</v>
+        <v>3.3</v>
       </c>
       <c r="R12">
         <v>-0.25</v>
       </c>
       <c r="S12">
-        <v>1.725</v>
+        <v>1.825</v>
       </c>
       <c r="T12">
-        <v>2.075</v>
+        <v>1.975</v>
       </c>
       <c r="U12">
-        <v>2</v>
+        <v>2.25</v>
       </c>
       <c r="V12">
-        <v>2.05</v>
+        <v>1.875</v>
       </c>
       <c r="W12">
-        <v>1.75</v>
+        <v>1.925</v>
       </c>
       <c r="X12">
-        <v>1</v>
+        <v>1.05</v>
       </c>
       <c r="Y12">
         <v>-1</v>
@@ -1620,13 +1620,13 @@
         <v>-1</v>
       </c>
       <c r="AA12">
-        <v>0.7250000000000001</v>
+        <v>0.825</v>
       </c>
       <c r="AB12">
         <v>-1</v>
       </c>
       <c r="AC12">
-        <v>1.05</v>
+        <v>0.875</v>
       </c>
       <c r="AD12">
         <v>-1</v>
@@ -1913,7 +1913,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>6765584</v>
+        <v>6765583</v>
       </c>
       <c r="C16" t="s">
         <v>29</v>
@@ -1925,7 +1925,7 @@
         <v>42</v>
       </c>
       <c r="F16" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G16">
         <v>2</v>
@@ -1937,64 +1937,64 @@
         <v>1</v>
       </c>
       <c r="J16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K16" t="s">
         <v>49</v>
       </c>
       <c r="L16">
-        <v>2.4</v>
+        <v>2.8</v>
       </c>
       <c r="M16">
         <v>2.8</v>
       </c>
       <c r="N16">
-        <v>3</v>
+        <v>2.55</v>
       </c>
       <c r="O16">
-        <v>2.05</v>
+        <v>2</v>
       </c>
       <c r="P16">
         <v>3</v>
       </c>
       <c r="Q16">
-        <v>3.3</v>
+        <v>3.75</v>
       </c>
       <c r="R16">
         <v>-0.25</v>
       </c>
       <c r="S16">
-        <v>1.825</v>
+        <v>1.725</v>
       </c>
       <c r="T16">
-        <v>1.975</v>
+        <v>2.075</v>
       </c>
       <c r="U16">
-        <v>2.25</v>
+        <v>2</v>
       </c>
       <c r="V16">
-        <v>1.875</v>
+        <v>2.05</v>
       </c>
       <c r="W16">
-        <v>1.925</v>
+        <v>1.75</v>
       </c>
       <c r="X16">
+        <v>1</v>
+      </c>
+      <c r="Y16">
+        <v>-1</v>
+      </c>
+      <c r="Z16">
+        <v>-1</v>
+      </c>
+      <c r="AA16">
+        <v>0.7250000000000001</v>
+      </c>
+      <c r="AB16">
+        <v>-1</v>
+      </c>
+      <c r="AC16">
         <v>1.05</v>
-      </c>
-      <c r="Y16">
-        <v>-1</v>
-      </c>
-      <c r="Z16">
-        <v>-1</v>
-      </c>
-      <c r="AA16">
-        <v>0.825</v>
-      </c>
-      <c r="AB16">
-        <v>-1</v>
-      </c>
-      <c r="AC16">
-        <v>0.875</v>
       </c>
       <c r="AD16">
         <v>-1</v>
@@ -2005,7 +2005,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>6765522</v>
+        <v>6765519</v>
       </c>
       <c r="C17" t="s">
         <v>29</v>
@@ -2014,16 +2014,16 @@
         <v>45108.54166666666</v>
       </c>
       <c r="E17" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="F17" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="G17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H17">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I17">
         <v>1</v>
@@ -2032,64 +2032,64 @@
         <v>0</v>
       </c>
       <c r="K17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="L17">
-        <v>1.363</v>
+        <v>1.8</v>
       </c>
       <c r="M17">
-        <v>4</v>
+        <v>3.2</v>
       </c>
       <c r="N17">
-        <v>8</v>
+        <v>4.2</v>
       </c>
       <c r="O17">
-        <v>1.4</v>
+        <v>1.65</v>
       </c>
       <c r="P17">
-        <v>3.75</v>
+        <v>3.1</v>
       </c>
       <c r="Q17">
-        <v>7.5</v>
+        <v>5.25</v>
       </c>
       <c r="R17">
-        <v>-1</v>
+        <v>-0.75</v>
       </c>
       <c r="S17">
+        <v>1.9</v>
+      </c>
+      <c r="T17">
+        <v>1.9</v>
+      </c>
+      <c r="U17">
         <v>1.75</v>
       </c>
-      <c r="T17">
-        <v>2.05</v>
-      </c>
-      <c r="U17">
-        <v>2.25</v>
-      </c>
       <c r="V17">
-        <v>2.025</v>
+        <v>1.9</v>
       </c>
       <c r="W17">
-        <v>1.775</v>
+        <v>1.9</v>
       </c>
       <c r="X17">
-        <v>0.3999999999999999</v>
+        <v>-1</v>
       </c>
       <c r="Y17">
-        <v>-1</v>
+        <v>2.1</v>
       </c>
       <c r="Z17">
         <v>-1</v>
       </c>
       <c r="AA17">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AB17">
-        <v>0</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AC17">
-        <v>-1</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AD17">
-        <v>0.7749999999999999</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="18" spans="1:30">
@@ -2097,7 +2097,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>6765519</v>
+        <v>6765522</v>
       </c>
       <c r="C18" t="s">
         <v>29</v>
@@ -2106,16 +2106,16 @@
         <v>45108.54166666666</v>
       </c>
       <c r="E18" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="F18" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="G18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H18">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I18">
         <v>1</v>
@@ -2124,64 +2124,64 @@
         <v>0</v>
       </c>
       <c r="K18" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="L18">
-        <v>1.8</v>
+        <v>1.363</v>
       </c>
       <c r="M18">
-        <v>3.2</v>
+        <v>4</v>
       </c>
       <c r="N18">
-        <v>4.2</v>
+        <v>8</v>
       </c>
       <c r="O18">
-        <v>1.65</v>
+        <v>1.4</v>
       </c>
       <c r="P18">
-        <v>3.1</v>
+        <v>3.75</v>
       </c>
       <c r="Q18">
-        <v>5.25</v>
+        <v>7.5</v>
       </c>
       <c r="R18">
-        <v>-0.75</v>
+        <v>-1</v>
       </c>
       <c r="S18">
-        <v>1.9</v>
+        <v>1.75</v>
       </c>
       <c r="T18">
-        <v>1.9</v>
+        <v>2.05</v>
       </c>
       <c r="U18">
-        <v>1.75</v>
+        <v>2.25</v>
       </c>
       <c r="V18">
-        <v>1.9</v>
+        <v>2.025</v>
       </c>
       <c r="W18">
-        <v>1.9</v>
+        <v>1.775</v>
       </c>
       <c r="X18">
-        <v>-1</v>
+        <v>0.3999999999999999</v>
       </c>
       <c r="Y18">
-        <v>2.1</v>
+        <v>-1</v>
       </c>
       <c r="Z18">
         <v>-1</v>
       </c>
       <c r="AA18">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AB18">
-        <v>0.8999999999999999</v>
+        <v>0</v>
       </c>
       <c r="AC18">
-        <v>0.8999999999999999</v>
+        <v>-1</v>
       </c>
       <c r="AD18">
-        <v>-1</v>
+        <v>0.7749999999999999</v>
       </c>
     </row>
     <row r="19" spans="1:30">
@@ -2201,7 +2201,7 @@
         <v>32</v>
       </c>
       <c r="F19" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="G19">
         <v>2</v>
@@ -2477,7 +2477,7 @@
         <v>36</v>
       </c>
       <c r="F22" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="G22">
         <v>0</v>
@@ -3118,7 +3118,7 @@
         <v>45114.55208333334</v>
       </c>
       <c r="E29" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="F29" t="s">
         <v>32</v>
@@ -3210,7 +3210,7 @@
         <v>45114.55208333334</v>
       </c>
       <c r="E30" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="F30" t="s">
         <v>34</v>
@@ -3477,7 +3477,7 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>6888615</v>
+        <v>6888609</v>
       </c>
       <c r="C33" t="s">
         <v>29</v>
@@ -3486,82 +3486,82 @@
         <v>45117.55208333334</v>
       </c>
       <c r="E33" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="F33" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G33">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I33">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K33" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="L33">
-        <v>3.5</v>
+        <v>1.666</v>
       </c>
       <c r="M33">
-        <v>2.875</v>
+        <v>3</v>
       </c>
       <c r="N33">
-        <v>2.1</v>
+        <v>5.5</v>
       </c>
       <c r="O33">
-        <v>1.7</v>
+        <v>1.833</v>
       </c>
       <c r="P33">
         <v>3</v>
       </c>
       <c r="Q33">
-        <v>5.25</v>
+        <v>4.2</v>
       </c>
       <c r="R33">
         <v>-0.5</v>
       </c>
       <c r="S33">
+        <v>2.025</v>
+      </c>
+      <c r="T33">
         <v>1.775</v>
       </c>
-      <c r="T33">
-        <v>2.025</v>
-      </c>
       <c r="U33">
         <v>2</v>
       </c>
       <c r="V33">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="W33">
-        <v>1.925</v>
+        <v>1.85</v>
       </c>
       <c r="X33">
-        <v>0.7</v>
+        <v>-1</v>
       </c>
       <c r="Y33">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="Z33">
         <v>-1</v>
       </c>
       <c r="AA33">
+        <v>-1</v>
+      </c>
+      <c r="AB33">
         <v>0.7749999999999999</v>
       </c>
-      <c r="AB33">
-        <v>-1</v>
-      </c>
       <c r="AC33">
-        <v>0.875</v>
+        <v>0</v>
       </c>
       <c r="AD33">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:30">
@@ -3569,7 +3569,7 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>6888614</v>
+        <v>6888610</v>
       </c>
       <c r="C34" t="s">
         <v>29</v>
@@ -3578,55 +3578,55 @@
         <v>45117.55208333334</v>
       </c>
       <c r="E34" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F34" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="G34">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H34">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I34">
         <v>1</v>
       </c>
       <c r="J34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K34" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="L34">
-        <v>1.8</v>
+        <v>1.25</v>
       </c>
       <c r="M34">
-        <v>3.2</v>
+        <v>4.5</v>
       </c>
       <c r="N34">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="O34">
-        <v>2.5</v>
+        <v>1.25</v>
       </c>
       <c r="P34">
-        <v>3</v>
+        <v>4.2</v>
       </c>
       <c r="Q34">
-        <v>2.625</v>
+        <v>12</v>
       </c>
       <c r="R34">
-        <v>0</v>
+        <v>-1.25</v>
       </c>
       <c r="S34">
-        <v>1.85</v>
+        <v>1.775</v>
       </c>
       <c r="T34">
-        <v>1.95</v>
+        <v>2.025</v>
       </c>
       <c r="U34">
-        <v>1.75</v>
+        <v>2</v>
       </c>
       <c r="V34">
         <v>1.775</v>
@@ -3635,25 +3635,25 @@
         <v>2.025</v>
       </c>
       <c r="X34">
-        <v>-1</v>
+        <v>0.25</v>
       </c>
       <c r="Y34">
         <v>-1</v>
       </c>
       <c r="Z34">
-        <v>1.625</v>
+        <v>-1</v>
       </c>
       <c r="AA34">
-        <v>-1</v>
+        <v>0.7749999999999999</v>
       </c>
       <c r="AB34">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
       <c r="AC34">
-        <v>0.7749999999999999</v>
+        <v>0</v>
       </c>
       <c r="AD34">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:30">
@@ -3661,7 +3661,7 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>6888613</v>
+        <v>6888611</v>
       </c>
       <c r="C35" t="s">
         <v>29</v>
@@ -3670,64 +3670,64 @@
         <v>45117.55208333334</v>
       </c>
       <c r="E35" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="F35" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="G35">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H35">
         <v>1</v>
       </c>
       <c r="I35">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K35" t="s">
         <v>49</v>
       </c>
       <c r="L35">
-        <v>1.4</v>
+        <v>2.05</v>
       </c>
       <c r="M35">
-        <v>3.75</v>
+        <v>2.9</v>
       </c>
       <c r="N35">
-        <v>7.5</v>
+        <v>3.6</v>
       </c>
       <c r="O35">
-        <v>1.363</v>
+        <v>1.65</v>
       </c>
       <c r="P35">
-        <v>4.333</v>
+        <v>3.25</v>
       </c>
       <c r="Q35">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="R35">
-        <v>-1.25</v>
+        <v>-0.75</v>
       </c>
       <c r="S35">
-        <v>1.925</v>
+        <v>1.9</v>
       </c>
       <c r="T35">
-        <v>1.875</v>
+        <v>1.9</v>
       </c>
       <c r="U35">
         <v>2.25</v>
       </c>
       <c r="V35">
-        <v>1.975</v>
+        <v>2.025</v>
       </c>
       <c r="W35">
-        <v>1.825</v>
+        <v>1.775</v>
       </c>
       <c r="X35">
-        <v>0.363</v>
+        <v>0.6499999999999999</v>
       </c>
       <c r="Y35">
         <v>-1</v>
@@ -3736,13 +3736,13 @@
         <v>-1</v>
       </c>
       <c r="AA35">
-        <v>-0.5</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AB35">
-        <v>0.4375</v>
+        <v>-1</v>
       </c>
       <c r="AC35">
-        <v>0.9750000000000001</v>
+        <v>1.025</v>
       </c>
       <c r="AD35">
         <v>-1</v>
@@ -3753,7 +3753,7 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>6888612</v>
+        <v>6888613</v>
       </c>
       <c r="C36" t="s">
         <v>29</v>
@@ -3762,19 +3762,19 @@
         <v>45117.55208333334</v>
       </c>
       <c r="E36" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="F36" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="G36">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J36">
         <v>0</v>
@@ -3783,43 +3783,43 @@
         <v>49</v>
       </c>
       <c r="L36">
-        <v>1.727</v>
+        <v>1.4</v>
       </c>
       <c r="M36">
-        <v>3.2</v>
+        <v>3.75</v>
       </c>
       <c r="N36">
-        <v>4.5</v>
+        <v>7.5</v>
       </c>
       <c r="O36">
-        <v>1.65</v>
+        <v>1.363</v>
       </c>
       <c r="P36">
-        <v>3.3</v>
+        <v>4.333</v>
       </c>
       <c r="Q36">
-        <v>5.75</v>
+        <v>7</v>
       </c>
       <c r="R36">
-        <v>-0.75</v>
+        <v>-1.25</v>
       </c>
       <c r="S36">
+        <v>1.925</v>
+      </c>
+      <c r="T36">
         <v>1.875</v>
       </c>
-      <c r="T36">
-        <v>1.925</v>
-      </c>
       <c r="U36">
-        <v>1.75</v>
+        <v>2.25</v>
       </c>
       <c r="V36">
-        <v>1.9</v>
+        <v>1.975</v>
       </c>
       <c r="W36">
-        <v>1.9</v>
+        <v>1.825</v>
       </c>
       <c r="X36">
-        <v>0.6499999999999999</v>
+        <v>0.363</v>
       </c>
       <c r="Y36">
         <v>-1</v>
@@ -3828,16 +3828,16 @@
         <v>-1</v>
       </c>
       <c r="AA36">
+        <v>-0.5</v>
+      </c>
+      <c r="AB36">
         <v>0.4375</v>
       </c>
-      <c r="AB36">
-        <v>-0.5</v>
-      </c>
       <c r="AC36">
-        <v>-1</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="AD36">
-        <v>0.8999999999999999</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="37" spans="1:30">
@@ -3845,7 +3845,7 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>6888609</v>
+        <v>6888614</v>
       </c>
       <c r="C37" t="s">
         <v>29</v>
@@ -3854,82 +3854,82 @@
         <v>45117.55208333334</v>
       </c>
       <c r="E37" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F37" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="G37">
         <v>1</v>
       </c>
       <c r="H37">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J37">
         <v>1</v>
       </c>
       <c r="K37" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L37">
-        <v>1.666</v>
+        <v>1.8</v>
       </c>
       <c r="M37">
-        <v>3</v>
+        <v>3.2</v>
       </c>
       <c r="N37">
-        <v>5.5</v>
+        <v>4</v>
       </c>
       <c r="O37">
-        <v>1.833</v>
+        <v>2.5</v>
       </c>
       <c r="P37">
         <v>3</v>
       </c>
       <c r="Q37">
-        <v>4.2</v>
+        <v>2.625</v>
       </c>
       <c r="R37">
-        <v>-0.5</v>
+        <v>0</v>
       </c>
       <c r="S37">
+        <v>1.85</v>
+      </c>
+      <c r="T37">
+        <v>1.95</v>
+      </c>
+      <c r="U37">
+        <v>1.75</v>
+      </c>
+      <c r="V37">
+        <v>1.775</v>
+      </c>
+      <c r="W37">
         <v>2.025</v>
       </c>
-      <c r="T37">
-        <v>1.775</v>
-      </c>
-      <c r="U37">
-        <v>2</v>
-      </c>
-      <c r="V37">
-        <v>1.95</v>
-      </c>
-      <c r="W37">
-        <v>1.85</v>
-      </c>
       <c r="X37">
         <v>-1</v>
       </c>
       <c r="Y37">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="Z37">
-        <v>-1</v>
+        <v>1.625</v>
       </c>
       <c r="AA37">
         <v>-1</v>
       </c>
       <c r="AB37">
+        <v>0.95</v>
+      </c>
+      <c r="AC37">
         <v>0.7749999999999999</v>
       </c>
-      <c r="AC37">
-        <v>0</v>
-      </c>
       <c r="AD37">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="38" spans="1:30">
@@ -3937,7 +3937,7 @@
         <v>36</v>
       </c>
       <c r="B38">
-        <v>6888611</v>
+        <v>6888615</v>
       </c>
       <c r="C38" t="s">
         <v>29</v>
@@ -3946,64 +3946,64 @@
         <v>45117.55208333334</v>
       </c>
       <c r="E38" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F38" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="G38">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I38">
         <v>2</v>
       </c>
       <c r="J38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K38" t="s">
         <v>49</v>
       </c>
       <c r="L38">
-        <v>2.05</v>
+        <v>3.5</v>
       </c>
       <c r="M38">
-        <v>2.9</v>
+        <v>2.875</v>
       </c>
       <c r="N38">
-        <v>3.6</v>
+        <v>2.1</v>
       </c>
       <c r="O38">
-        <v>1.65</v>
+        <v>1.7</v>
       </c>
       <c r="P38">
-        <v>3.25</v>
+        <v>3</v>
       </c>
       <c r="Q38">
-        <v>5</v>
+        <v>5.25</v>
       </c>
       <c r="R38">
-        <v>-0.75</v>
+        <v>-0.5</v>
       </c>
       <c r="S38">
-        <v>1.9</v>
+        <v>1.775</v>
       </c>
       <c r="T38">
-        <v>1.9</v>
+        <v>2.025</v>
       </c>
       <c r="U38">
-        <v>2.25</v>
+        <v>2</v>
       </c>
       <c r="V38">
-        <v>2.025</v>
+        <v>1.875</v>
       </c>
       <c r="W38">
-        <v>1.775</v>
+        <v>1.925</v>
       </c>
       <c r="X38">
-        <v>0.6499999999999999</v>
+        <v>0.7</v>
       </c>
       <c r="Y38">
         <v>-1</v>
@@ -4012,13 +4012,13 @@
         <v>-1</v>
       </c>
       <c r="AA38">
-        <v>0.8999999999999999</v>
+        <v>0.7749999999999999</v>
       </c>
       <c r="AB38">
         <v>-1</v>
       </c>
       <c r="AC38">
-        <v>1.025</v>
+        <v>0.875</v>
       </c>
       <c r="AD38">
         <v>-1</v>
@@ -4029,7 +4029,7 @@
         <v>37</v>
       </c>
       <c r="B39">
-        <v>6888610</v>
+        <v>6888612</v>
       </c>
       <c r="C39" t="s">
         <v>29</v>
@@ -4038,19 +4038,19 @@
         <v>45117.55208333334</v>
       </c>
       <c r="E39" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="F39" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G39">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H39">
         <v>0</v>
       </c>
       <c r="I39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J39">
         <v>0</v>
@@ -4059,43 +4059,43 @@
         <v>49</v>
       </c>
       <c r="L39">
-        <v>1.25</v>
+        <v>1.727</v>
       </c>
       <c r="M39">
+        <v>3.2</v>
+      </c>
+      <c r="N39">
         <v>4.5</v>
       </c>
-      <c r="N39">
-        <v>11</v>
-      </c>
       <c r="O39">
-        <v>1.25</v>
+        <v>1.65</v>
       </c>
       <c r="P39">
-        <v>4.2</v>
+        <v>3.3</v>
       </c>
       <c r="Q39">
-        <v>12</v>
+        <v>5.75</v>
       </c>
       <c r="R39">
-        <v>-1.25</v>
+        <v>-0.75</v>
       </c>
       <c r="S39">
-        <v>1.775</v>
+        <v>1.875</v>
       </c>
       <c r="T39">
-        <v>2.025</v>
+        <v>1.925</v>
       </c>
       <c r="U39">
-        <v>2</v>
+        <v>1.75</v>
       </c>
       <c r="V39">
-        <v>1.775</v>
+        <v>1.9</v>
       </c>
       <c r="W39">
-        <v>2.025</v>
+        <v>1.9</v>
       </c>
       <c r="X39">
-        <v>0.25</v>
+        <v>0.6499999999999999</v>
       </c>
       <c r="Y39">
         <v>-1</v>
@@ -4104,16 +4104,16 @@
         <v>-1</v>
       </c>
       <c r="AA39">
-        <v>0.7749999999999999</v>
+        <v>0.4375</v>
       </c>
       <c r="AB39">
-        <v>-1</v>
+        <v>-0.5</v>
       </c>
       <c r="AC39">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AD39">
-        <v>0</v>
+        <v>0.8999999999999999</v>
       </c>
     </row>
     <row r="40" spans="1:30">
@@ -4121,7 +4121,7 @@
         <v>38</v>
       </c>
       <c r="B40">
-        <v>6913588</v>
+        <v>6913587</v>
       </c>
       <c r="C40" t="s">
         <v>29</v>
@@ -4130,82 +4130,82 @@
         <v>45122.55208333334</v>
       </c>
       <c r="E40" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F40" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="G40">
         <v>1</v>
       </c>
       <c r="H40">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I40">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J40">
         <v>0</v>
       </c>
       <c r="K40" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="L40">
-        <v>2.3</v>
+        <v>1.727</v>
       </c>
       <c r="M40">
-        <v>3</v>
+        <v>3.2</v>
       </c>
       <c r="N40">
-        <v>2.875</v>
+        <v>4.5</v>
       </c>
       <c r="O40">
-        <v>1.85</v>
+        <v>1.65</v>
       </c>
       <c r="P40">
-        <v>3.25</v>
+        <v>3.4</v>
       </c>
       <c r="Q40">
-        <v>3.6</v>
+        <v>4.75</v>
       </c>
       <c r="R40">
+        <v>-0.75</v>
+      </c>
+      <c r="S40">
+        <v>1.925</v>
+      </c>
+      <c r="T40">
+        <v>1.875</v>
+      </c>
+      <c r="U40">
+        <v>2</v>
+      </c>
+      <c r="V40">
+        <v>1.9</v>
+      </c>
+      <c r="W40">
+        <v>1.9</v>
+      </c>
+      <c r="X40">
+        <v>0.6499999999999999</v>
+      </c>
+      <c r="Y40">
+        <v>-1</v>
+      </c>
+      <c r="Z40">
+        <v>-1</v>
+      </c>
+      <c r="AA40">
+        <v>0.4625</v>
+      </c>
+      <c r="AB40">
         <v>-0.5</v>
       </c>
-      <c r="S40">
-        <v>1.95</v>
-      </c>
-      <c r="T40">
-        <v>1.85</v>
-      </c>
-      <c r="U40">
-        <v>2.5</v>
-      </c>
-      <c r="V40">
-        <v>2</v>
-      </c>
-      <c r="W40">
-        <v>1.8</v>
-      </c>
-      <c r="X40">
-        <v>-1</v>
-      </c>
-      <c r="Y40">
-        <v>-1</v>
-      </c>
-      <c r="Z40">
-        <v>2.6</v>
-      </c>
-      <c r="AA40">
-        <v>-1</v>
-      </c>
-      <c r="AB40">
-        <v>0.8500000000000001</v>
-      </c>
       <c r="AC40">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AD40">
-        <v>-1</v>
+        <v>0.8999999999999999</v>
       </c>
     </row>
     <row r="41" spans="1:30">
@@ -4213,7 +4213,7 @@
         <v>39</v>
       </c>
       <c r="B41">
-        <v>6913587</v>
+        <v>6913588</v>
       </c>
       <c r="C41" t="s">
         <v>29</v>
@@ -4222,82 +4222,82 @@
         <v>45122.55208333334</v>
       </c>
       <c r="E41" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="F41" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="G41">
         <v>1</v>
       </c>
       <c r="H41">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I41">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J41">
         <v>0</v>
       </c>
       <c r="K41" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="L41">
-        <v>1.727</v>
+        <v>2.3</v>
       </c>
       <c r="M41">
-        <v>3.2</v>
+        <v>3</v>
       </c>
       <c r="N41">
-        <v>4.5</v>
+        <v>2.875</v>
       </c>
       <c r="O41">
-        <v>1.65</v>
+        <v>1.85</v>
       </c>
       <c r="P41">
-        <v>3.4</v>
+        <v>3.25</v>
       </c>
       <c r="Q41">
-        <v>4.75</v>
+        <v>3.6</v>
       </c>
       <c r="R41">
-        <v>-0.75</v>
+        <v>-0.5</v>
       </c>
       <c r="S41">
-        <v>1.925</v>
+        <v>1.95</v>
       </c>
       <c r="T41">
-        <v>1.875</v>
+        <v>1.85</v>
       </c>
       <c r="U41">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="V41">
-        <v>1.9</v>
+        <v>2</v>
       </c>
       <c r="W41">
-        <v>1.9</v>
+        <v>1.8</v>
       </c>
       <c r="X41">
-        <v>0.6499999999999999</v>
+        <v>-1</v>
       </c>
       <c r="Y41">
         <v>-1</v>
       </c>
       <c r="Z41">
-        <v>-1</v>
+        <v>2.6</v>
       </c>
       <c r="AA41">
-        <v>0.4625</v>
+        <v>-1</v>
       </c>
       <c r="AB41">
-        <v>-0.5</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AC41">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="AD41">
-        <v>0.8999999999999999</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="42" spans="1:30">
@@ -4590,7 +4590,7 @@
         <v>45185.5</v>
       </c>
       <c r="E45" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="F45" t="s">
         <v>34</v>
@@ -4857,7 +4857,7 @@
         <v>46</v>
       </c>
       <c r="B48">
-        <v>7230929</v>
+        <v>7239829</v>
       </c>
       <c r="C48" t="s">
         <v>29</v>
@@ -4866,16 +4866,16 @@
         <v>45191.5</v>
       </c>
       <c r="E48" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="F48" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="G48">
         <v>2</v>
       </c>
       <c r="H48">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I48">
         <v>1</v>
@@ -4884,61 +4884,61 @@
         <v>1</v>
       </c>
       <c r="K48" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="L48">
-        <v>3.3</v>
+        <v>1.95</v>
       </c>
       <c r="M48">
         <v>3</v>
       </c>
       <c r="N48">
-        <v>2.1</v>
+        <v>3.75</v>
       </c>
       <c r="O48">
-        <v>2.375</v>
+        <v>3.25</v>
       </c>
       <c r="P48">
-        <v>3</v>
+        <v>2.9</v>
       </c>
       <c r="Q48">
-        <v>2.8</v>
+        <v>2.2</v>
       </c>
       <c r="R48">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="S48">
-        <v>1.8</v>
+        <v>1.9</v>
       </c>
       <c r="T48">
-        <v>2</v>
+        <v>1.9</v>
       </c>
       <c r="U48">
-        <v>2</v>
+        <v>1.75</v>
       </c>
       <c r="V48">
-        <v>1.8</v>
+        <v>1.85</v>
       </c>
       <c r="W48">
-        <v>2</v>
+        <v>1.95</v>
       </c>
       <c r="X48">
-        <v>-1</v>
+        <v>2.25</v>
       </c>
       <c r="Y48">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="Z48">
         <v>-1</v>
       </c>
       <c r="AA48">
-        <v>0</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AB48">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AC48">
-        <v>0.8</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AD48">
         <v>-1</v>
@@ -4949,7 +4949,7 @@
         <v>47</v>
       </c>
       <c r="B49">
-        <v>7239829</v>
+        <v>7230929</v>
       </c>
       <c r="C49" t="s">
         <v>29</v>
@@ -4958,16 +4958,16 @@
         <v>45191.5</v>
       </c>
       <c r="E49" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="F49" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="G49">
         <v>2</v>
       </c>
       <c r="H49">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I49">
         <v>1</v>
@@ -4976,61 +4976,61 @@
         <v>1</v>
       </c>
       <c r="K49" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="L49">
-        <v>1.95</v>
+        <v>3.3</v>
       </c>
       <c r="M49">
         <v>3</v>
       </c>
       <c r="N49">
-        <v>3.75</v>
+        <v>2.1</v>
       </c>
       <c r="O49">
-        <v>3.25</v>
+        <v>2.375</v>
       </c>
       <c r="P49">
-        <v>2.9</v>
+        <v>3</v>
       </c>
       <c r="Q49">
-        <v>2.2</v>
+        <v>2.8</v>
       </c>
       <c r="R49">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="S49">
-        <v>1.9</v>
+        <v>1.8</v>
       </c>
       <c r="T49">
-        <v>1.9</v>
+        <v>2</v>
       </c>
       <c r="U49">
-        <v>1.75</v>
+        <v>2</v>
       </c>
       <c r="V49">
-        <v>1.85</v>
+        <v>1.8</v>
       </c>
       <c r="W49">
-        <v>1.95</v>
+        <v>2</v>
       </c>
       <c r="X49">
-        <v>2.25</v>
+        <v>-1</v>
       </c>
       <c r="Y49">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="Z49">
         <v>-1</v>
       </c>
       <c r="AA49">
-        <v>0.8999999999999999</v>
+        <v>0</v>
       </c>
       <c r="AB49">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AC49">
-        <v>0.8500000000000001</v>
+        <v>0.8</v>
       </c>
       <c r="AD49">
         <v>-1</v>
@@ -5145,7 +5145,7 @@
         <v>43</v>
       </c>
       <c r="F51" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="G51">
         <v>1</v>
@@ -5593,7 +5593,7 @@
         <v>54</v>
       </c>
       <c r="B56">
-        <v>7230936</v>
+        <v>7230948</v>
       </c>
       <c r="C56" t="s">
         <v>29</v>
@@ -5602,10 +5602,10 @@
         <v>45198.48958333334</v>
       </c>
       <c r="E56" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="F56" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="G56">
         <v>2</v>
@@ -5617,49 +5617,49 @@
         <v>0</v>
       </c>
       <c r="J56">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K56" t="s">
         <v>49</v>
       </c>
       <c r="L56">
-        <v>2</v>
+        <v>3.2</v>
       </c>
       <c r="M56">
-        <v>3</v>
+        <v>2.9</v>
       </c>
       <c r="N56">
-        <v>3.75</v>
+        <v>2.2</v>
       </c>
       <c r="O56">
-        <v>2</v>
+        <v>2.05</v>
       </c>
       <c r="P56">
         <v>3</v>
       </c>
       <c r="Q56">
-        <v>3.75</v>
+        <v>3.6</v>
       </c>
       <c r="R56">
         <v>-0.25</v>
       </c>
       <c r="S56">
-        <v>1.8</v>
+        <v>1.75</v>
       </c>
       <c r="T56">
-        <v>2</v>
+        <v>2.05</v>
       </c>
       <c r="U56">
         <v>1.75</v>
       </c>
       <c r="V56">
-        <v>1.825</v>
+        <v>1.9</v>
       </c>
       <c r="W56">
-        <v>1.975</v>
+        <v>1.9</v>
       </c>
       <c r="X56">
-        <v>1</v>
+        <v>1.05</v>
       </c>
       <c r="Y56">
         <v>-1</v>
@@ -5668,13 +5668,13 @@
         <v>-1</v>
       </c>
       <c r="AA56">
-        <v>0.8</v>
+        <v>0.75</v>
       </c>
       <c r="AB56">
         <v>-1</v>
       </c>
       <c r="AC56">
-        <v>0.825</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AD56">
         <v>-1</v>
@@ -5777,7 +5777,7 @@
         <v>56</v>
       </c>
       <c r="B58">
-        <v>7230948</v>
+        <v>7230936</v>
       </c>
       <c r="C58" t="s">
         <v>29</v>
@@ -5786,10 +5786,10 @@
         <v>45198.48958333334</v>
       </c>
       <c r="E58" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="F58" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="G58">
         <v>2</v>
@@ -5801,49 +5801,49 @@
         <v>0</v>
       </c>
       <c r="J58">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K58" t="s">
         <v>49</v>
       </c>
       <c r="L58">
-        <v>3.2</v>
+        <v>2</v>
       </c>
       <c r="M58">
-        <v>2.9</v>
+        <v>3</v>
       </c>
       <c r="N58">
-        <v>2.2</v>
+        <v>3.75</v>
       </c>
       <c r="O58">
-        <v>2.05</v>
+        <v>2</v>
       </c>
       <c r="P58">
         <v>3</v>
       </c>
       <c r="Q58">
-        <v>3.6</v>
+        <v>3.75</v>
       </c>
       <c r="R58">
         <v>-0.25</v>
       </c>
       <c r="S58">
-        <v>1.75</v>
+        <v>1.8</v>
       </c>
       <c r="T58">
-        <v>2.05</v>
+        <v>2</v>
       </c>
       <c r="U58">
         <v>1.75</v>
       </c>
       <c r="V58">
-        <v>1.9</v>
+        <v>1.825</v>
       </c>
       <c r="W58">
-        <v>1.9</v>
+        <v>1.975</v>
       </c>
       <c r="X58">
-        <v>1.05</v>
+        <v>1</v>
       </c>
       <c r="Y58">
         <v>-1</v>
@@ -5852,13 +5852,13 @@
         <v>-1</v>
       </c>
       <c r="AA58">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="AB58">
         <v>-1</v>
       </c>
       <c r="AC58">
-        <v>0.8999999999999999</v>
+        <v>0.825</v>
       </c>
       <c r="AD58">
         <v>-1</v>
@@ -6145,7 +6145,7 @@
         <v>60</v>
       </c>
       <c r="B62">
-        <v>7230942</v>
+        <v>7230950</v>
       </c>
       <c r="C62" t="s">
         <v>29</v>
@@ -6154,64 +6154,64 @@
         <v>45205.48958333334</v>
       </c>
       <c r="E62" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="F62" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="G62">
+        <v>5</v>
+      </c>
+      <c r="H62">
         <v>3</v>
       </c>
-      <c r="H62">
-        <v>0</v>
-      </c>
       <c r="I62">
         <v>2</v>
       </c>
       <c r="J62">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K62" t="s">
         <v>49</v>
       </c>
       <c r="L62">
-        <v>1.571</v>
+        <v>1.727</v>
       </c>
       <c r="M62">
+        <v>3.25</v>
+      </c>
+      <c r="N62">
+        <v>4.333</v>
+      </c>
+      <c r="O62">
+        <v>1.5</v>
+      </c>
+      <c r="P62">
         <v>3.5</v>
       </c>
-      <c r="N62">
-        <v>5.25</v>
-      </c>
-      <c r="O62">
-        <v>1.666</v>
-      </c>
-      <c r="P62">
-        <v>3.3</v>
-      </c>
       <c r="Q62">
-        <v>4.75</v>
+        <v>6</v>
       </c>
       <c r="R62">
-        <v>-0.75</v>
+        <v>-1</v>
       </c>
       <c r="S62">
-        <v>1.95</v>
+        <v>1.925</v>
       </c>
       <c r="T62">
-        <v>1.85</v>
+        <v>1.875</v>
       </c>
       <c r="U62">
         <v>2</v>
       </c>
       <c r="V62">
-        <v>1.95</v>
+        <v>1.8</v>
       </c>
       <c r="W62">
-        <v>1.85</v>
+        <v>2</v>
       </c>
       <c r="X62">
-        <v>0.6659999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="Y62">
         <v>-1</v>
@@ -6220,13 +6220,13 @@
         <v>-1</v>
       </c>
       <c r="AA62">
-        <v>0.95</v>
+        <v>0.925</v>
       </c>
       <c r="AB62">
         <v>-1</v>
       </c>
       <c r="AC62">
-        <v>0.95</v>
+        <v>0.8</v>
       </c>
       <c r="AD62">
         <v>-1</v>
@@ -6237,7 +6237,7 @@
         <v>61</v>
       </c>
       <c r="B63">
-        <v>7230950</v>
+        <v>7230942</v>
       </c>
       <c r="C63" t="s">
         <v>29</v>
@@ -6246,64 +6246,64 @@
         <v>45205.48958333334</v>
       </c>
       <c r="E63" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="F63" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G63">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H63">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I63">
         <v>2</v>
       </c>
       <c r="J63">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K63" t="s">
         <v>49</v>
       </c>
       <c r="L63">
-        <v>1.727</v>
+        <v>1.571</v>
       </c>
       <c r="M63">
-        <v>3.25</v>
+        <v>3.5</v>
       </c>
       <c r="N63">
-        <v>4.333</v>
+        <v>5.25</v>
       </c>
       <c r="O63">
-        <v>1.5</v>
+        <v>1.666</v>
       </c>
       <c r="P63">
-        <v>3.5</v>
+        <v>3.3</v>
       </c>
       <c r="Q63">
-        <v>6</v>
+        <v>4.75</v>
       </c>
       <c r="R63">
-        <v>-1</v>
+        <v>-0.75</v>
       </c>
       <c r="S63">
-        <v>1.925</v>
+        <v>1.95</v>
       </c>
       <c r="T63">
-        <v>1.875</v>
+        <v>1.85</v>
       </c>
       <c r="U63">
         <v>2</v>
       </c>
       <c r="V63">
-        <v>1.8</v>
+        <v>1.95</v>
       </c>
       <c r="W63">
-        <v>2</v>
+        <v>1.85</v>
       </c>
       <c r="X63">
-        <v>0.5</v>
+        <v>0.6659999999999999</v>
       </c>
       <c r="Y63">
         <v>-1</v>
@@ -6312,13 +6312,13 @@
         <v>-1</v>
       </c>
       <c r="AA63">
-        <v>0.925</v>
+        <v>0.95</v>
       </c>
       <c r="AB63">
         <v>-1</v>
       </c>
       <c r="AC63">
-        <v>0.8</v>
+        <v>0.95</v>
       </c>
       <c r="AD63">
         <v>-1</v>
@@ -6329,7 +6329,7 @@
         <v>62</v>
       </c>
       <c r="B64">
-        <v>7230940</v>
+        <v>7230941</v>
       </c>
       <c r="C64" t="s">
         <v>29</v>
@@ -6338,82 +6338,82 @@
         <v>45205.625</v>
       </c>
       <c r="E64" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F64" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="G64">
         <v>0</v>
       </c>
       <c r="H64">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="I64">
         <v>0</v>
       </c>
       <c r="J64">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K64" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="L64">
-        <v>1.833</v>
+        <v>1.727</v>
       </c>
       <c r="M64">
-        <v>3.1</v>
+        <v>3.2</v>
       </c>
       <c r="N64">
-        <v>4</v>
+        <v>4.5</v>
       </c>
       <c r="O64">
-        <v>1.909</v>
+        <v>1.571</v>
       </c>
       <c r="P64">
-        <v>3.1</v>
+        <v>3.4</v>
       </c>
       <c r="Q64">
-        <v>3.75</v>
+        <v>5.5</v>
       </c>
       <c r="R64">
-        <v>-0.5</v>
+        <v>-0.75</v>
       </c>
       <c r="S64">
+        <v>1.825</v>
+      </c>
+      <c r="T64">
         <v>1.975</v>
       </c>
-      <c r="T64">
-        <v>1.825</v>
-      </c>
       <c r="U64">
         <v>2</v>
       </c>
       <c r="V64">
-        <v>2</v>
+        <v>1.9</v>
       </c>
       <c r="W64">
-        <v>1.8</v>
+        <v>1.9</v>
       </c>
       <c r="X64">
         <v>-1</v>
       </c>
       <c r="Y64">
-        <v>-1</v>
+        <v>2.4</v>
       </c>
       <c r="Z64">
-        <v>2.75</v>
+        <v>-1</v>
       </c>
       <c r="AA64">
         <v>-1</v>
       </c>
       <c r="AB64">
-        <v>0.825</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="AC64">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AD64">
-        <v>-1</v>
+        <v>0.8999999999999999</v>
       </c>
     </row>
     <row r="65" spans="1:30">
@@ -6421,7 +6421,7 @@
         <v>63</v>
       </c>
       <c r="B65">
-        <v>7230941</v>
+        <v>7230940</v>
       </c>
       <c r="C65" t="s">
         <v>29</v>
@@ -6430,82 +6430,82 @@
         <v>45205.625</v>
       </c>
       <c r="E65" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F65" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G65">
         <v>0</v>
       </c>
       <c r="H65">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I65">
         <v>0</v>
       </c>
       <c r="J65">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K65" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L65">
-        <v>1.727</v>
+        <v>1.833</v>
       </c>
       <c r="M65">
-        <v>3.2</v>
+        <v>3.1</v>
       </c>
       <c r="N65">
-        <v>4.5</v>
+        <v>4</v>
       </c>
       <c r="O65">
-        <v>1.571</v>
+        <v>1.909</v>
       </c>
       <c r="P65">
-        <v>3.4</v>
+        <v>3.1</v>
       </c>
       <c r="Q65">
-        <v>5.5</v>
+        <v>3.75</v>
       </c>
       <c r="R65">
-        <v>-0.75</v>
+        <v>-0.5</v>
       </c>
       <c r="S65">
+        <v>1.975</v>
+      </c>
+      <c r="T65">
         <v>1.825</v>
       </c>
-      <c r="T65">
-        <v>1.975</v>
-      </c>
       <c r="U65">
         <v>2</v>
       </c>
       <c r="V65">
-        <v>1.9</v>
+        <v>2</v>
       </c>
       <c r="W65">
-        <v>1.9</v>
+        <v>1.8</v>
       </c>
       <c r="X65">
         <v>-1</v>
       </c>
       <c r="Y65">
-        <v>2.4</v>
+        <v>-1</v>
       </c>
       <c r="Z65">
-        <v>-1</v>
+        <v>2.75</v>
       </c>
       <c r="AA65">
         <v>-1</v>
       </c>
       <c r="AB65">
-        <v>0.9750000000000001</v>
+        <v>0.825</v>
       </c>
       <c r="AC65">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="AD65">
-        <v>0.8999999999999999</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="66" spans="1:30">
@@ -7433,7 +7433,7 @@
         <v>74</v>
       </c>
       <c r="B76">
-        <v>7427226</v>
+        <v>7427225</v>
       </c>
       <c r="C76" t="s">
         <v>29</v>
@@ -7442,82 +7442,82 @@
         <v>45241.45833333334</v>
       </c>
       <c r="E76" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="F76" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="G76">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H76">
         <v>1</v>
       </c>
       <c r="I76">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J76">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K76" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="L76">
-        <v>1.444</v>
+        <v>1.571</v>
       </c>
       <c r="M76">
-        <v>3.75</v>
+        <v>3.25</v>
       </c>
       <c r="N76">
-        <v>6.5</v>
+        <v>6</v>
       </c>
       <c r="O76">
-        <v>1.285</v>
+        <v>1.6</v>
       </c>
       <c r="P76">
-        <v>4.2</v>
+        <v>3.2</v>
       </c>
       <c r="Q76">
-        <v>11</v>
+        <v>5.75</v>
       </c>
       <c r="R76">
-        <v>-1.5</v>
+        <v>-0.75</v>
       </c>
       <c r="S76">
+        <v>1.85</v>
+      </c>
+      <c r="T76">
         <v>1.95</v>
       </c>
-      <c r="T76">
-        <v>1.85</v>
-      </c>
       <c r="U76">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="V76">
-        <v>2</v>
+        <v>1.8</v>
       </c>
       <c r="W76">
-        <v>1.8</v>
+        <v>2</v>
       </c>
       <c r="X76">
-        <v>-1</v>
+        <v>0.6000000000000001</v>
       </c>
       <c r="Y76">
         <v>-1</v>
       </c>
       <c r="Z76">
-        <v>10</v>
+        <v>-1</v>
       </c>
       <c r="AA76">
-        <v>-1</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AB76">
-        <v>0.8500000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AC76">
-        <v>-1</v>
+        <v>0.8</v>
       </c>
       <c r="AD76">
-        <v>0.8</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="77" spans="1:30">
@@ -7525,7 +7525,7 @@
         <v>75</v>
       </c>
       <c r="B77">
-        <v>7427225</v>
+        <v>7427226</v>
       </c>
       <c r="C77" t="s">
         <v>29</v>
@@ -7534,82 +7534,82 @@
         <v>45241.45833333334</v>
       </c>
       <c r="E77" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="F77" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="G77">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H77">
         <v>1</v>
       </c>
       <c r="I77">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J77">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K77" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="L77">
-        <v>1.571</v>
+        <v>1.444</v>
       </c>
       <c r="M77">
-        <v>3.25</v>
+        <v>3.75</v>
       </c>
       <c r="N77">
-        <v>6</v>
+        <v>6.5</v>
       </c>
       <c r="O77">
-        <v>1.6</v>
+        <v>1.285</v>
       </c>
       <c r="P77">
-        <v>3.2</v>
+        <v>4.2</v>
       </c>
       <c r="Q77">
-        <v>5.75</v>
+        <v>11</v>
       </c>
       <c r="R77">
-        <v>-0.75</v>
+        <v>-1.5</v>
       </c>
       <c r="S77">
+        <v>1.95</v>
+      </c>
+      <c r="T77">
         <v>1.85</v>
       </c>
-      <c r="T77">
-        <v>1.95</v>
-      </c>
       <c r="U77">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="V77">
+        <v>2</v>
+      </c>
+      <c r="W77">
         <v>1.8</v>
       </c>
-      <c r="W77">
-        <v>2</v>
-      </c>
       <c r="X77">
-        <v>0.6000000000000001</v>
+        <v>-1</v>
       </c>
       <c r="Y77">
         <v>-1</v>
       </c>
       <c r="Z77">
-        <v>-1</v>
+        <v>10</v>
       </c>
       <c r="AA77">
+        <v>-1</v>
+      </c>
+      <c r="AB77">
         <v>0.8500000000000001</v>
       </c>
-      <c r="AB77">
-        <v>-1</v>
-      </c>
       <c r="AC77">
+        <v>-1</v>
+      </c>
+      <c r="AD77">
         <v>0.8</v>
-      </c>
-      <c r="AD77">
-        <v>-1</v>
       </c>
     </row>
     <row r="78" spans="1:30">
@@ -7997,7 +7997,7 @@
         <v>33</v>
       </c>
       <c r="F82" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="G82">
         <v>0</v>
@@ -8822,7 +8822,7 @@
         <v>45254.46875</v>
       </c>
       <c r="E91" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="F91" t="s">
         <v>31</v>
@@ -9285,7 +9285,7 @@
         <v>44</v>
       </c>
       <c r="F96" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="G96">
         <v>4</v>
@@ -9457,7 +9457,7 @@
         <v>96</v>
       </c>
       <c r="B98">
-        <v>7513409</v>
+        <v>7513410</v>
       </c>
       <c r="C98" t="s">
         <v>29</v>
@@ -9466,82 +9466,82 @@
         <v>45262.53125</v>
       </c>
       <c r="E98" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="F98" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="G98">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H98">
         <v>0</v>
       </c>
       <c r="I98">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J98">
         <v>0</v>
       </c>
       <c r="K98" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="L98">
-        <v>1.25</v>
+        <v>1.666</v>
       </c>
       <c r="M98">
-        <v>4.333</v>
+        <v>3.25</v>
       </c>
       <c r="N98">
-        <v>12</v>
+        <v>4.75</v>
       </c>
       <c r="O98">
-        <v>1.285</v>
+        <v>1.65</v>
       </c>
       <c r="P98">
-        <v>4.2</v>
+        <v>3.3</v>
       </c>
       <c r="Q98">
-        <v>11</v>
+        <v>4.75</v>
       </c>
       <c r="R98">
-        <v>-1.5</v>
+        <v>-0.75</v>
       </c>
       <c r="S98">
-        <v>1.95</v>
+        <v>1.975</v>
       </c>
       <c r="T98">
-        <v>1.85</v>
+        <v>1.825</v>
       </c>
       <c r="U98">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="V98">
-        <v>1.9</v>
+        <v>1.825</v>
       </c>
       <c r="W98">
-        <v>1.9</v>
+        <v>1.975</v>
       </c>
       <c r="X98">
-        <v>0.2849999999999999</v>
+        <v>-1</v>
       </c>
       <c r="Y98">
-        <v>-1</v>
+        <v>2.3</v>
       </c>
       <c r="Z98">
         <v>-1</v>
       </c>
       <c r="AA98">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
       <c r="AB98">
-        <v>-1</v>
+        <v>0.825</v>
       </c>
       <c r="AC98">
         <v>-1</v>
       </c>
       <c r="AD98">
-        <v>0.8999999999999999</v>
+        <v>0.9750000000000001</v>
       </c>
     </row>
     <row r="99" spans="1:30">
@@ -9549,7 +9549,7 @@
         <v>97</v>
       </c>
       <c r="B99">
-        <v>7513410</v>
+        <v>7513409</v>
       </c>
       <c r="C99" t="s">
         <v>29</v>
@@ -9558,82 +9558,82 @@
         <v>45262.53125</v>
       </c>
       <c r="E99" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="F99" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="G99">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H99">
         <v>0</v>
       </c>
       <c r="I99">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J99">
         <v>0</v>
       </c>
       <c r="K99" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="L99">
-        <v>1.666</v>
+        <v>1.25</v>
       </c>
       <c r="M99">
-        <v>3.25</v>
+        <v>4.333</v>
       </c>
       <c r="N99">
-        <v>4.75</v>
+        <v>12</v>
       </c>
       <c r="O99">
-        <v>1.65</v>
+        <v>1.285</v>
       </c>
       <c r="P99">
-        <v>3.3</v>
+        <v>4.2</v>
       </c>
       <c r="Q99">
-        <v>4.75</v>
+        <v>11</v>
       </c>
       <c r="R99">
-        <v>-0.75</v>
+        <v>-1.5</v>
       </c>
       <c r="S99">
-        <v>1.975</v>
+        <v>1.95</v>
       </c>
       <c r="T99">
-        <v>1.825</v>
+        <v>1.85</v>
       </c>
       <c r="U99">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="V99">
-        <v>1.825</v>
+        <v>1.9</v>
       </c>
       <c r="W99">
-        <v>1.975</v>
+        <v>1.9</v>
       </c>
       <c r="X99">
-        <v>-1</v>
+        <v>0.2849999999999999</v>
       </c>
       <c r="Y99">
-        <v>2.3</v>
+        <v>-1</v>
       </c>
       <c r="Z99">
         <v>-1</v>
       </c>
       <c r="AA99">
-        <v>-1</v>
+        <v>0.95</v>
       </c>
       <c r="AB99">
-        <v>0.825</v>
+        <v>-1</v>
       </c>
       <c r="AC99">
         <v>-1</v>
       </c>
       <c r="AD99">
-        <v>0.9750000000000001</v>
+        <v>0.8999999999999999</v>
       </c>
     </row>
     <row r="100" spans="1:30">
@@ -10110,7 +10110,7 @@
         <v>45269.45833333334</v>
       </c>
       <c r="E105" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="F105" t="s">
         <v>30</v>
@@ -10757,7 +10757,7 @@
         <v>37</v>
       </c>
       <c r="F112" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="G112">
         <v>2</v>
@@ -11113,7 +11113,7 @@
         <v>114</v>
       </c>
       <c r="B116">
-        <v>7624465</v>
+        <v>7624517</v>
       </c>
       <c r="C116" t="s">
         <v>29</v>
@@ -11122,13 +11122,13 @@
         <v>45289.46875</v>
       </c>
       <c r="E116" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F116" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="G116">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H116">
         <v>0</v>
@@ -11140,64 +11140,64 @@
         <v>0</v>
       </c>
       <c r="K116" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="L116">
-        <v>1.4</v>
+        <v>2.2</v>
       </c>
       <c r="M116">
-        <v>3.9</v>
+        <v>2.75</v>
       </c>
       <c r="N116">
-        <v>7</v>
+        <v>3.4</v>
       </c>
       <c r="O116">
-        <v>1.65</v>
+        <v>2.15</v>
       </c>
       <c r="P116">
-        <v>3.4</v>
+        <v>2.8</v>
       </c>
       <c r="Q116">
-        <v>4.75</v>
+        <v>3.6</v>
       </c>
       <c r="R116">
-        <v>-0.75</v>
+        <v>-0.25</v>
       </c>
       <c r="S116">
-        <v>1.9</v>
+        <v>1.8</v>
       </c>
       <c r="T116">
-        <v>1.9</v>
+        <v>2</v>
       </c>
       <c r="U116">
-        <v>2.25</v>
+        <v>1.75</v>
       </c>
       <c r="V116">
-        <v>2</v>
+        <v>1.825</v>
       </c>
       <c r="W116">
+        <v>1.975</v>
+      </c>
+      <c r="X116">
+        <v>-1</v>
+      </c>
+      <c r="Y116">
         <v>1.8</v>
       </c>
-      <c r="X116">
-        <v>0.6499999999999999</v>
-      </c>
-      <c r="Y116">
-        <v>-1</v>
-      </c>
       <c r="Z116">
         <v>-1</v>
       </c>
       <c r="AA116">
-        <v>0.45</v>
+        <v>-0.5</v>
       </c>
       <c r="AB116">
-        <v>-0.5</v>
+        <v>0.5</v>
       </c>
       <c r="AC116">
         <v>-1</v>
       </c>
       <c r="AD116">
-        <v>0.8</v>
+        <v>0.9750000000000001</v>
       </c>
     </row>
     <row r="117" spans="1:30">
@@ -11205,7 +11205,7 @@
         <v>115</v>
       </c>
       <c r="B117">
-        <v>7624517</v>
+        <v>7624516</v>
       </c>
       <c r="C117" t="s">
         <v>29</v>
@@ -11214,16 +11214,16 @@
         <v>45289.46875</v>
       </c>
       <c r="E117" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F117" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="G117">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H117">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I117">
         <v>0</v>
@@ -11232,64 +11232,64 @@
         <v>0</v>
       </c>
       <c r="K117" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="L117">
-        <v>2.2</v>
+        <v>1.909</v>
       </c>
       <c r="M117">
-        <v>2.75</v>
+        <v>2.875</v>
       </c>
       <c r="N117">
-        <v>3.4</v>
+        <v>4.2</v>
       </c>
       <c r="O117">
-        <v>2.15</v>
+        <v>1.833</v>
       </c>
       <c r="P117">
-        <v>2.8</v>
+        <v>3</v>
       </c>
       <c r="Q117">
-        <v>3.6</v>
+        <v>4.75</v>
       </c>
       <c r="R117">
-        <v>-0.25</v>
+        <v>-0.5</v>
       </c>
       <c r="S117">
+        <v>1.85</v>
+      </c>
+      <c r="T117">
+        <v>1.95</v>
+      </c>
+      <c r="U117">
+        <v>2</v>
+      </c>
+      <c r="V117">
+        <v>2</v>
+      </c>
+      <c r="W117">
         <v>1.8</v>
       </c>
-      <c r="T117">
-        <v>2</v>
-      </c>
-      <c r="U117">
-        <v>1.75</v>
-      </c>
-      <c r="V117">
-        <v>1.825</v>
-      </c>
-      <c r="W117">
-        <v>1.975</v>
-      </c>
       <c r="X117">
-        <v>-1</v>
+        <v>0.833</v>
       </c>
       <c r="Y117">
-        <v>1.8</v>
+        <v>-1</v>
       </c>
       <c r="Z117">
         <v>-1</v>
       </c>
       <c r="AA117">
-        <v>-0.5</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AB117">
-        <v>0.5</v>
+        <v>-1</v>
       </c>
       <c r="AC117">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="AD117">
-        <v>0.9750000000000001</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="118" spans="1:30">
@@ -11297,7 +11297,7 @@
         <v>116</v>
       </c>
       <c r="B118">
-        <v>7624516</v>
+        <v>7624465</v>
       </c>
       <c r="C118" t="s">
         <v>29</v>
@@ -11306,16 +11306,16 @@
         <v>45289.46875</v>
       </c>
       <c r="E118" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="F118" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="G118">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H118">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I118">
         <v>0</v>
@@ -11327,34 +11327,34 @@
         <v>49</v>
       </c>
       <c r="L118">
-        <v>1.909</v>
+        <v>1.4</v>
       </c>
       <c r="M118">
-        <v>2.875</v>
+        <v>3.9</v>
       </c>
       <c r="N118">
-        <v>4.2</v>
+        <v>7</v>
       </c>
       <c r="O118">
-        <v>1.833</v>
+        <v>1.65</v>
       </c>
       <c r="P118">
-        <v>3</v>
+        <v>3.4</v>
       </c>
       <c r="Q118">
         <v>4.75</v>
       </c>
       <c r="R118">
-        <v>-0.5</v>
+        <v>-0.75</v>
       </c>
       <c r="S118">
-        <v>1.85</v>
+        <v>1.9</v>
       </c>
       <c r="T118">
-        <v>1.95</v>
+        <v>1.9</v>
       </c>
       <c r="U118">
-        <v>2</v>
+        <v>2.25</v>
       </c>
       <c r="V118">
         <v>2</v>
@@ -11363,7 +11363,7 @@
         <v>1.8</v>
       </c>
       <c r="X118">
-        <v>0.833</v>
+        <v>0.6499999999999999</v>
       </c>
       <c r="Y118">
         <v>-1</v>
@@ -11372,16 +11372,16 @@
         <v>-1</v>
       </c>
       <c r="AA118">
-        <v>0.8500000000000001</v>
+        <v>0.45</v>
       </c>
       <c r="AB118">
-        <v>-1</v>
+        <v>-0.5</v>
       </c>
       <c r="AC118">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AD118">
-        <v>-1</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="119" spans="1:30">
@@ -11481,7 +11481,7 @@
         <v>118</v>
       </c>
       <c r="B120">
-        <v>7624597</v>
+        <v>7624498</v>
       </c>
       <c r="C120" t="s">
         <v>29</v>
@@ -11490,82 +11490,82 @@
         <v>45289.58333333334</v>
       </c>
       <c r="E120" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="F120" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G120">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H120">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I120">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J120">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K120" t="s">
         <v>48</v>
       </c>
       <c r="L120">
-        <v>3.4</v>
+        <v>1.45</v>
       </c>
       <c r="M120">
-        <v>3.2</v>
+        <v>3.9</v>
       </c>
       <c r="N120">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="O120">
-        <v>3.4</v>
+        <v>1.45</v>
       </c>
       <c r="P120">
-        <v>2.9</v>
+        <v>3.8</v>
       </c>
       <c r="Q120">
-        <v>2.15</v>
+        <v>6.5</v>
       </c>
       <c r="R120">
-        <v>0.25</v>
+        <v>-1</v>
       </c>
       <c r="S120">
-        <v>1.925</v>
+        <v>1.775</v>
       </c>
       <c r="T120">
-        <v>1.875</v>
+        <v>2.025</v>
       </c>
       <c r="U120">
         <v>2</v>
       </c>
       <c r="V120">
-        <v>1.95</v>
+        <v>1.75</v>
       </c>
       <c r="W120">
-        <v>1.85</v>
+        <v>2.05</v>
       </c>
       <c r="X120">
         <v>-1</v>
       </c>
       <c r="Y120">
-        <v>1.9</v>
+        <v>2.8</v>
       </c>
       <c r="Z120">
         <v>-1</v>
       </c>
       <c r="AA120">
-        <v>0.4625</v>
+        <v>-1</v>
       </c>
       <c r="AB120">
-        <v>-0.5</v>
+        <v>1.025</v>
       </c>
       <c r="AC120">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AD120">
-        <v>0.8500000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="121" spans="1:30">
@@ -11573,7 +11573,7 @@
         <v>119</v>
       </c>
       <c r="B121">
-        <v>7624498</v>
+        <v>7624597</v>
       </c>
       <c r="C121" t="s">
         <v>29</v>
@@ -11582,82 +11582,82 @@
         <v>45289.58333333334</v>
       </c>
       <c r="E121" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="F121" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G121">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H121">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I121">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J121">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K121" t="s">
         <v>48</v>
       </c>
       <c r="L121">
-        <v>1.45</v>
+        <v>3.4</v>
       </c>
       <c r="M121">
-        <v>3.9</v>
+        <v>3.2</v>
       </c>
       <c r="N121">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="O121">
-        <v>1.45</v>
+        <v>3.4</v>
       </c>
       <c r="P121">
-        <v>3.8</v>
+        <v>2.9</v>
       </c>
       <c r="Q121">
-        <v>6.5</v>
+        <v>2.15</v>
       </c>
       <c r="R121">
-        <v>-1</v>
+        <v>0.25</v>
       </c>
       <c r="S121">
-        <v>1.775</v>
+        <v>1.925</v>
       </c>
       <c r="T121">
-        <v>2.025</v>
+        <v>1.875</v>
       </c>
       <c r="U121">
         <v>2</v>
       </c>
       <c r="V121">
-        <v>1.75</v>
+        <v>1.95</v>
       </c>
       <c r="W121">
-        <v>2.05</v>
+        <v>1.85</v>
       </c>
       <c r="X121">
         <v>-1</v>
       </c>
       <c r="Y121">
-        <v>2.8</v>
+        <v>1.9</v>
       </c>
       <c r="Z121">
         <v>-1</v>
       </c>
       <c r="AA121">
-        <v>-1</v>
+        <v>0.4625</v>
       </c>
       <c r="AB121">
-        <v>1.025</v>
+        <v>-0.5</v>
       </c>
       <c r="AC121">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AD121">
-        <v>0</v>
+        <v>0.8500000000000001</v>
       </c>
     </row>
     <row r="122" spans="1:30">
@@ -11766,7 +11766,7 @@
         <v>45296.46875</v>
       </c>
       <c r="E123" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="F123" t="s">
         <v>39</v>
@@ -12597,7 +12597,7 @@
         <v>35</v>
       </c>
       <c r="F132" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="G132">
         <v>0</v>
@@ -13422,7 +13422,7 @@
         <v>45310.47916666666</v>
       </c>
       <c r="E141" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="F141" t="s">
         <v>32</v>
@@ -13965,7 +13965,7 @@
         <v>145</v>
       </c>
       <c r="B147">
-        <v>7590958</v>
+        <v>7624533</v>
       </c>
       <c r="C147" t="s">
         <v>29</v>
@@ -13974,10 +13974,10 @@
         <v>45314.54166666666</v>
       </c>
       <c r="E147" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="F147" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="G147">
         <v>0</v>
@@ -13995,31 +13995,31 @@
         <v>48</v>
       </c>
       <c r="L147">
-        <v>2.6</v>
+        <v>1.4</v>
       </c>
       <c r="M147">
-        <v>2.9</v>
+        <v>3.75</v>
       </c>
       <c r="N147">
-        <v>2.6</v>
+        <v>7.5</v>
       </c>
       <c r="O147">
-        <v>3.3</v>
+        <v>1.5</v>
       </c>
       <c r="P147">
-        <v>3</v>
+        <v>3.4</v>
       </c>
       <c r="Q147">
-        <v>2.15</v>
+        <v>6.5</v>
       </c>
       <c r="R147">
-        <v>0.25</v>
+        <v>-1</v>
       </c>
       <c r="S147">
-        <v>1.9</v>
+        <v>1.975</v>
       </c>
       <c r="T147">
-        <v>1.9</v>
+        <v>1.825</v>
       </c>
       <c r="U147">
         <v>2</v>
@@ -14034,16 +14034,16 @@
         <v>-1</v>
       </c>
       <c r="Y147">
-        <v>2</v>
+        <v>2.4</v>
       </c>
       <c r="Z147">
         <v>-1</v>
       </c>
       <c r="AA147">
-        <v>0.45</v>
+        <v>-1</v>
       </c>
       <c r="AB147">
-        <v>-0.5</v>
+        <v>0.825</v>
       </c>
       <c r="AC147">
         <v>-1</v>
@@ -14057,7 +14057,7 @@
         <v>146</v>
       </c>
       <c r="B148">
-        <v>7624533</v>
+        <v>7590958</v>
       </c>
       <c r="C148" t="s">
         <v>29</v>
@@ -14066,10 +14066,10 @@
         <v>45314.54166666666</v>
       </c>
       <c r="E148" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="F148" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="G148">
         <v>0</v>
@@ -14087,31 +14087,31 @@
         <v>48</v>
       </c>
       <c r="L148">
-        <v>1.4</v>
+        <v>2.6</v>
       </c>
       <c r="M148">
-        <v>3.75</v>
+        <v>2.9</v>
       </c>
       <c r="N148">
-        <v>7.5</v>
+        <v>2.6</v>
       </c>
       <c r="O148">
-        <v>1.5</v>
+        <v>3.3</v>
       </c>
       <c r="P148">
-        <v>3.4</v>
+        <v>3</v>
       </c>
       <c r="Q148">
-        <v>6.5</v>
+        <v>2.15</v>
       </c>
       <c r="R148">
-        <v>-1</v>
+        <v>0.25</v>
       </c>
       <c r="S148">
-        <v>1.975</v>
+        <v>1.9</v>
       </c>
       <c r="T148">
-        <v>1.825</v>
+        <v>1.9</v>
       </c>
       <c r="U148">
         <v>2</v>
@@ -14126,16 +14126,16 @@
         <v>-1</v>
       </c>
       <c r="Y148">
-        <v>2.4</v>
+        <v>2</v>
       </c>
       <c r="Z148">
         <v>-1</v>
       </c>
       <c r="AA148">
-        <v>-1</v>
+        <v>0.45</v>
       </c>
       <c r="AB148">
-        <v>0.825</v>
+        <v>-0.5</v>
       </c>
       <c r="AC148">
         <v>-1</v>
@@ -14805,7 +14805,7 @@
         <v>36</v>
       </c>
       <c r="F156" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="G156">
         <v>3</v>
@@ -15541,7 +15541,7 @@
         <v>34</v>
       </c>
       <c r="F164" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="G164">
         <v>1</v>
@@ -15897,7 +15897,7 @@
         <v>166</v>
       </c>
       <c r="B168">
-        <v>7768182</v>
+        <v>7768219</v>
       </c>
       <c r="C168" t="s">
         <v>29</v>
@@ -15906,82 +15906,82 @@
         <v>45338.47916666666</v>
       </c>
       <c r="E168" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="F168" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G168">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H168">
         <v>0</v>
       </c>
       <c r="I168">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J168">
         <v>0</v>
       </c>
       <c r="K168" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="L168">
-        <v>2</v>
+        <v>1.833</v>
       </c>
       <c r="M168">
-        <v>2.9</v>
+        <v>3</v>
       </c>
       <c r="N168">
-        <v>3.75</v>
+        <v>4.2</v>
       </c>
       <c r="O168">
-        <v>2.375</v>
+        <v>1.833</v>
       </c>
       <c r="P168">
-        <v>2.9</v>
+        <v>2.8</v>
       </c>
       <c r="Q168">
-        <v>3</v>
+        <v>4.5</v>
       </c>
       <c r="R168">
-        <v>-0.25</v>
+        <v>-0.5</v>
       </c>
       <c r="S168">
-        <v>2.075</v>
+        <v>1.95</v>
       </c>
       <c r="T168">
-        <v>1.725</v>
+        <v>1.85</v>
       </c>
       <c r="U168">
         <v>1.75</v>
       </c>
       <c r="V168">
-        <v>1.75</v>
+        <v>1.975</v>
       </c>
       <c r="W168">
-        <v>2.05</v>
+        <v>1.825</v>
       </c>
       <c r="X168">
-        <v>1.375</v>
+        <v>-1</v>
       </c>
       <c r="Y168">
-        <v>-1</v>
+        <v>1.8</v>
       </c>
       <c r="Z168">
         <v>-1</v>
       </c>
       <c r="AA168">
-        <v>1.075</v>
+        <v>-1</v>
       </c>
       <c r="AB168">
-        <v>-1</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AC168">
         <v>-1</v>
       </c>
       <c r="AD168">
-        <v>1.05</v>
+        <v>0.825</v>
       </c>
     </row>
     <row r="169" spans="1:30">
@@ -15989,7 +15989,7 @@
         <v>167</v>
       </c>
       <c r="B169">
-        <v>7768219</v>
+        <v>7768182</v>
       </c>
       <c r="C169" t="s">
         <v>29</v>
@@ -15998,82 +15998,82 @@
         <v>45338.47916666666</v>
       </c>
       <c r="E169" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F169" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G169">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H169">
         <v>0</v>
       </c>
       <c r="I169">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J169">
         <v>0</v>
       </c>
       <c r="K169" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="L169">
-        <v>1.833</v>
+        <v>2</v>
       </c>
       <c r="M169">
+        <v>2.9</v>
+      </c>
+      <c r="N169">
+        <v>3.75</v>
+      </c>
+      <c r="O169">
+        <v>2.375</v>
+      </c>
+      <c r="P169">
+        <v>2.9</v>
+      </c>
+      <c r="Q169">
         <v>3</v>
       </c>
-      <c r="N169">
-        <v>4.2</v>
-      </c>
-      <c r="O169">
-        <v>1.833</v>
-      </c>
-      <c r="P169">
-        <v>2.8</v>
-      </c>
-      <c r="Q169">
-        <v>4.5</v>
-      </c>
       <c r="R169">
-        <v>-0.5</v>
+        <v>-0.25</v>
       </c>
       <c r="S169">
-        <v>1.95</v>
+        <v>2.075</v>
       </c>
       <c r="T169">
-        <v>1.85</v>
+        <v>1.725</v>
       </c>
       <c r="U169">
         <v>1.75</v>
       </c>
       <c r="V169">
-        <v>1.975</v>
+        <v>1.75</v>
       </c>
       <c r="W169">
-        <v>1.825</v>
+        <v>2.05</v>
       </c>
       <c r="X169">
-        <v>-1</v>
+        <v>1.375</v>
       </c>
       <c r="Y169">
-        <v>1.8</v>
+        <v>-1</v>
       </c>
       <c r="Z169">
         <v>-1</v>
       </c>
       <c r="AA169">
-        <v>-1</v>
+        <v>1.075</v>
       </c>
       <c r="AB169">
-        <v>0.8500000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AC169">
         <v>-1</v>
       </c>
       <c r="AD169">
-        <v>0.825</v>
+        <v>1.05</v>
       </c>
     </row>
     <row r="170" spans="1:30">
@@ -16553,7 +16553,7 @@
         <v>40</v>
       </c>
       <c r="F175" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="G175">
         <v>0</v>
@@ -17010,7 +17010,7 @@
         <v>45352.5</v>
       </c>
       <c r="E180" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="F180" t="s">
         <v>41</v>
@@ -17277,7 +17277,7 @@
         <v>181</v>
       </c>
       <c r="B183">
-        <v>7883991</v>
+        <v>7883988</v>
       </c>
       <c r="C183" t="s">
         <v>29</v>
@@ -17286,67 +17286,67 @@
         <v>45353.54166666666</v>
       </c>
       <c r="E183" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F183" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="G183">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H183">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I183">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J183">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K183" t="s">
         <v>48</v>
       </c>
       <c r="L183">
-        <v>1.727</v>
+        <v>2.25</v>
       </c>
       <c r="M183">
+        <v>3</v>
+      </c>
+      <c r="N183">
+        <v>3.1</v>
+      </c>
+      <c r="O183">
+        <v>1.909</v>
+      </c>
+      <c r="P183">
         <v>3.2</v>
       </c>
-      <c r="N183">
-        <v>4.5</v>
-      </c>
-      <c r="O183">
-        <v>1.5</v>
-      </c>
-      <c r="P183">
-        <v>3.6</v>
-      </c>
       <c r="Q183">
-        <v>6</v>
+        <v>3.75</v>
       </c>
       <c r="R183">
-        <v>-1</v>
+        <v>-0.5</v>
       </c>
       <c r="S183">
-        <v>1.95</v>
+        <v>1.975</v>
       </c>
       <c r="T183">
-        <v>1.85</v>
+        <v>1.825</v>
       </c>
       <c r="U183">
         <v>2</v>
       </c>
       <c r="V183">
-        <v>1.8</v>
+        <v>1.775</v>
       </c>
       <c r="W183">
-        <v>2</v>
+        <v>2.025</v>
       </c>
       <c r="X183">
         <v>-1</v>
       </c>
       <c r="Y183">
-        <v>2.6</v>
+        <v>2.2</v>
       </c>
       <c r="Z183">
         <v>-1</v>
@@ -17355,13 +17355,13 @@
         <v>-1</v>
       </c>
       <c r="AB183">
-        <v>0.8500000000000001</v>
+        <v>0.825</v>
       </c>
       <c r="AC183">
-        <v>-1</v>
+        <v>0.7749999999999999</v>
       </c>
       <c r="AD183">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="184" spans="1:30">
@@ -17369,7 +17369,7 @@
         <v>182</v>
       </c>
       <c r="B184">
-        <v>7883988</v>
+        <v>7883991</v>
       </c>
       <c r="C184" t="s">
         <v>29</v>
@@ -17378,67 +17378,67 @@
         <v>45353.54166666666</v>
       </c>
       <c r="E184" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F184" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="G184">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H184">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I184">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J184">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K184" t="s">
         <v>48</v>
       </c>
       <c r="L184">
-        <v>2.25</v>
+        <v>1.727</v>
       </c>
       <c r="M184">
-        <v>3</v>
+        <v>3.2</v>
       </c>
       <c r="N184">
-        <v>3.1</v>
+        <v>4.5</v>
       </c>
       <c r="O184">
-        <v>1.909</v>
+        <v>1.5</v>
       </c>
       <c r="P184">
-        <v>3.2</v>
+        <v>3.6</v>
       </c>
       <c r="Q184">
-        <v>3.75</v>
+        <v>6</v>
       </c>
       <c r="R184">
-        <v>-0.5</v>
+        <v>-1</v>
       </c>
       <c r="S184">
-        <v>1.975</v>
+        <v>1.95</v>
       </c>
       <c r="T184">
-        <v>1.825</v>
+        <v>1.85</v>
       </c>
       <c r="U184">
         <v>2</v>
       </c>
       <c r="V184">
-        <v>1.775</v>
+        <v>1.8</v>
       </c>
       <c r="W184">
-        <v>2.025</v>
+        <v>2</v>
       </c>
       <c r="X184">
         <v>-1</v>
       </c>
       <c r="Y184">
-        <v>2.2</v>
+        <v>2.6</v>
       </c>
       <c r="Z184">
         <v>-1</v>
@@ -17447,13 +17447,13 @@
         <v>-1</v>
       </c>
       <c r="AB184">
-        <v>0.825</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AC184">
-        <v>0.7749999999999999</v>
+        <v>-1</v>
       </c>
       <c r="AD184">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="185" spans="1:30">
@@ -17657,7 +17657,7 @@
         <v>45</v>
       </c>
       <c r="F187" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="G187">
         <v>3</v>
@@ -18298,7 +18298,7 @@
         <v>45370.47916666666</v>
       </c>
       <c r="E194" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="F194" t="s">
         <v>43</v>
@@ -18666,7 +18666,7 @@
         <v>45375.47916666666</v>
       </c>
       <c r="E198" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="F198" t="s">
         <v>33</v>
@@ -19313,7 +19313,7 @@
         <v>31</v>
       </c>
       <c r="F205" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="G205">
         <v>0</v>
@@ -20037,7 +20037,7 @@
         <v>211</v>
       </c>
       <c r="B213">
-        <v>8082744</v>
+        <v>8082746</v>
       </c>
       <c r="C213" t="s">
         <v>29</v>
@@ -20046,82 +20046,82 @@
         <v>45401.5</v>
       </c>
       <c r="E213" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F213" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="G213">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H213">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I213">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J213">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K213" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="L213">
-        <v>3.6</v>
+        <v>1.533</v>
       </c>
       <c r="M213">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="N213">
-        <v>2</v>
+        <v>5.5</v>
       </c>
       <c r="O213">
-        <v>4.5</v>
+        <v>1.727</v>
       </c>
       <c r="P213">
-        <v>3</v>
+        <v>3.25</v>
       </c>
       <c r="Q213">
-        <v>1.833</v>
+        <v>4.333</v>
       </c>
       <c r="R213">
-        <v>0.5</v>
+        <v>-0.5</v>
       </c>
       <c r="S213">
-        <v>1.925</v>
+        <v>1.775</v>
       </c>
       <c r="T213">
-        <v>1.875</v>
+        <v>2.025</v>
       </c>
       <c r="U213">
         <v>2</v>
       </c>
       <c r="V213">
-        <v>2.025</v>
+        <v>1.75</v>
       </c>
       <c r="W213">
-        <v>1.775</v>
+        <v>2.05</v>
       </c>
       <c r="X213">
-        <v>-1</v>
+        <v>0.7270000000000001</v>
       </c>
       <c r="Y213">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="Z213">
         <v>-1</v>
       </c>
       <c r="AA213">
-        <v>0.925</v>
+        <v>0.7749999999999999</v>
       </c>
       <c r="AB213">
         <v>-1</v>
       </c>
       <c r="AC213">
-        <v>-1</v>
+        <v>0.75</v>
       </c>
       <c r="AD213">
-        <v>0.7749999999999999</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="214" spans="1:30">
@@ -20129,7 +20129,7 @@
         <v>212</v>
       </c>
       <c r="B214">
-        <v>8082746</v>
+        <v>8082743</v>
       </c>
       <c r="C214" t="s">
         <v>29</v>
@@ -20138,16 +20138,16 @@
         <v>45401.5</v>
       </c>
       <c r="E214" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="F214" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="G214">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H214">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I214">
         <v>1</v>
@@ -20156,61 +20156,61 @@
         <v>1</v>
       </c>
       <c r="K214" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="L214">
-        <v>1.533</v>
+        <v>2</v>
       </c>
       <c r="M214">
-        <v>3.5</v>
+        <v>3.1</v>
       </c>
       <c r="N214">
-        <v>5.5</v>
+        <v>3.4</v>
       </c>
       <c r="O214">
-        <v>1.727</v>
+        <v>1.666</v>
       </c>
       <c r="P214">
-        <v>3.25</v>
+        <v>3.75</v>
       </c>
       <c r="Q214">
         <v>4.333</v>
       </c>
       <c r="R214">
-        <v>-0.5</v>
+        <v>-0.75</v>
       </c>
       <c r="S214">
+        <v>1.9</v>
+      </c>
+      <c r="T214">
+        <v>1.9</v>
+      </c>
+      <c r="U214">
+        <v>2.25</v>
+      </c>
+      <c r="V214">
+        <v>2.025</v>
+      </c>
+      <c r="W214">
         <v>1.775</v>
       </c>
-      <c r="T214">
-        <v>2.025</v>
-      </c>
-      <c r="U214">
-        <v>2</v>
-      </c>
-      <c r="V214">
-        <v>1.75</v>
-      </c>
-      <c r="W214">
-        <v>2.05</v>
-      </c>
       <c r="X214">
-        <v>0.7270000000000001</v>
+        <v>-1</v>
       </c>
       <c r="Y214">
         <v>-1</v>
       </c>
       <c r="Z214">
-        <v>-1</v>
+        <v>3.333</v>
       </c>
       <c r="AA214">
-        <v>0.7749999999999999</v>
+        <v>-1</v>
       </c>
       <c r="AB214">
-        <v>-1</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AC214">
-        <v>0.75</v>
+        <v>1.025</v>
       </c>
       <c r="AD214">
         <v>-1</v>
@@ -20221,7 +20221,7 @@
         <v>213</v>
       </c>
       <c r="B215">
-        <v>8082743</v>
+        <v>8082744</v>
       </c>
       <c r="C215" t="s">
         <v>29</v>
@@ -20230,55 +20230,55 @@
         <v>45401.5</v>
       </c>
       <c r="E215" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="F215" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="G215">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H215">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I215">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J215">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K215" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="L215">
-        <v>2</v>
+        <v>3.6</v>
       </c>
       <c r="M215">
-        <v>3.1</v>
+        <v>3</v>
       </c>
       <c r="N215">
-        <v>3.4</v>
+        <v>2</v>
       </c>
       <c r="O215">
-        <v>1.666</v>
+        <v>4.5</v>
       </c>
       <c r="P215">
-        <v>3.75</v>
+        <v>3</v>
       </c>
       <c r="Q215">
-        <v>4.333</v>
+        <v>1.833</v>
       </c>
       <c r="R215">
-        <v>-0.75</v>
+        <v>0.5</v>
       </c>
       <c r="S215">
-        <v>1.9</v>
+        <v>1.925</v>
       </c>
       <c r="T215">
-        <v>1.9</v>
+        <v>1.875</v>
       </c>
       <c r="U215">
-        <v>2.25</v>
+        <v>2</v>
       </c>
       <c r="V215">
         <v>2.025</v>
@@ -20290,22 +20290,22 @@
         <v>-1</v>
       </c>
       <c r="Y215">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="Z215">
-        <v>3.333</v>
+        <v>-1</v>
       </c>
       <c r="AA215">
-        <v>-1</v>
+        <v>0.925</v>
       </c>
       <c r="AB215">
-        <v>0.8999999999999999</v>
+        <v>-1</v>
       </c>
       <c r="AC215">
-        <v>1.025</v>
+        <v>-1</v>
       </c>
       <c r="AD215">
-        <v>-1</v>
+        <v>0.7749999999999999</v>
       </c>
     </row>
     <row r="216" spans="1:30">
@@ -20785,7 +20785,7 @@
         <v>30</v>
       </c>
       <c r="F221" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="G221">
         <v>2</v>
@@ -21794,7 +21794,7 @@
         <v>45423.54166666666</v>
       </c>
       <c r="E232" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="F232" t="s">
         <v>37</v>
@@ -22533,7 +22533,7 @@
         <v>46</v>
       </c>
       <c r="F240" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="G240">
         <v>0</v>
@@ -23509,7 +23509,7 @@
         <v>39</v>
       </c>
       <c r="F251" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="G251">
         <v>0</v>

</xml_diff>

<commit_message>
Atualização de bases das ligas, do dia: 12-06-2024 às 23:38
</commit_message>
<xml_diff>
--- a/Algeria Division 1/Algeria Division 1.xlsx
+++ b/Algeria Division 1/Algeria Division 1.xlsx
@@ -106,10 +106,10 @@
     <t>Algeria Division 1</t>
   </si>
   <si>
-    <t>CS Constantine</t>
+    <t>Paradou AC</t>
   </si>
   <si>
-    <t>Paradou AC</t>
+    <t>CS Constantine</t>
   </si>
   <si>
     <t>ASO Chlef</t>
@@ -625,7 +625,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>6687389</v>
+        <v>6687391</v>
       </c>
       <c r="C2" t="s">
         <v>29</v>
@@ -637,16 +637,16 @@
         <v>30</v>
       </c>
       <c r="F2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H2">
         <v>0</v>
       </c>
       <c r="I2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J2">
         <v>0</v>
@@ -655,43 +655,43 @@
         <v>47</v>
       </c>
       <c r="L2">
-        <v>1.363</v>
+        <v>1.444</v>
       </c>
       <c r="M2">
-        <v>4.333</v>
+        <v>3.6</v>
       </c>
       <c r="N2">
-        <v>7.5</v>
+        <v>7</v>
       </c>
       <c r="O2">
-        <v>1.363</v>
+        <v>1.65</v>
       </c>
       <c r="P2">
-        <v>4.333</v>
+        <v>3.4</v>
       </c>
       <c r="Q2">
-        <v>7.5</v>
+        <v>5</v>
       </c>
       <c r="R2">
-        <v>-1.25</v>
+        <v>-0.75</v>
       </c>
       <c r="S2">
-        <v>1.875</v>
+        <v>1.8</v>
       </c>
       <c r="T2">
-        <v>1.925</v>
+        <v>2</v>
       </c>
       <c r="U2">
-        <v>2.5</v>
+        <v>2.25</v>
       </c>
       <c r="V2">
-        <v>2</v>
+        <v>1.9</v>
       </c>
       <c r="W2">
-        <v>1.8</v>
+        <v>1.9</v>
       </c>
       <c r="X2">
-        <v>0.363</v>
+        <v>0.6499999999999999</v>
       </c>
       <c r="Y2">
         <v>-1</v>
@@ -700,16 +700,16 @@
         <v>-1</v>
       </c>
       <c r="AA2">
-        <v>0.875</v>
+        <v>0.8</v>
       </c>
       <c r="AB2">
         <v>-1</v>
       </c>
       <c r="AC2">
-        <v>-1</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AD2">
-        <v>0.8</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="3" spans="1:30">
@@ -717,7 +717,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>6687391</v>
+        <v>6687389</v>
       </c>
       <c r="C3" t="s">
         <v>29</v>
@@ -729,16 +729,16 @@
         <v>31</v>
       </c>
       <c r="F3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H3">
         <v>0</v>
       </c>
       <c r="I3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J3">
         <v>0</v>
@@ -747,43 +747,43 @@
         <v>47</v>
       </c>
       <c r="L3">
-        <v>1.444</v>
+        <v>1.363</v>
       </c>
       <c r="M3">
-        <v>3.6</v>
+        <v>4.333</v>
       </c>
       <c r="N3">
-        <v>7</v>
+        <v>7.5</v>
       </c>
       <c r="O3">
-        <v>1.65</v>
+        <v>1.363</v>
       </c>
       <c r="P3">
-        <v>3.4</v>
+        <v>4.333</v>
       </c>
       <c r="Q3">
-        <v>5</v>
+        <v>7.5</v>
       </c>
       <c r="R3">
-        <v>-0.75</v>
+        <v>-1.25</v>
       </c>
       <c r="S3">
+        <v>1.875</v>
+      </c>
+      <c r="T3">
+        <v>1.925</v>
+      </c>
+      <c r="U3">
+        <v>2.5</v>
+      </c>
+      <c r="V3">
+        <v>2</v>
+      </c>
+      <c r="W3">
         <v>1.8</v>
       </c>
-      <c r="T3">
-        <v>2</v>
-      </c>
-      <c r="U3">
-        <v>2.25</v>
-      </c>
-      <c r="V3">
-        <v>1.9</v>
-      </c>
-      <c r="W3">
-        <v>1.9</v>
-      </c>
       <c r="X3">
-        <v>0.6499999999999999</v>
+        <v>0.363</v>
       </c>
       <c r="Y3">
         <v>-1</v>
@@ -792,16 +792,16 @@
         <v>-1</v>
       </c>
       <c r="AA3">
+        <v>0.875</v>
+      </c>
+      <c r="AB3">
+        <v>-1</v>
+      </c>
+      <c r="AC3">
+        <v>-1</v>
+      </c>
+      <c r="AD3">
         <v>0.8</v>
-      </c>
-      <c r="AB3">
-        <v>-1</v>
-      </c>
-      <c r="AC3">
-        <v>0.8999999999999999</v>
-      </c>
-      <c r="AD3">
-        <v>-1</v>
       </c>
     </row>
     <row r="4" spans="1:30">
@@ -1557,7 +1557,7 @@
         <v>38</v>
       </c>
       <c r="F12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G12">
         <v>0</v>
@@ -1729,7 +1729,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>6765519</v>
+        <v>6765522</v>
       </c>
       <c r="C14" t="s">
         <v>29</v>
@@ -1738,16 +1738,16 @@
         <v>45108.54166666666</v>
       </c>
       <c r="E14" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="F14" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H14">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I14">
         <v>1</v>
@@ -1756,64 +1756,64 @@
         <v>0</v>
       </c>
       <c r="K14" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="L14">
-        <v>1.8</v>
+        <v>1.363</v>
       </c>
       <c r="M14">
-        <v>3.2</v>
+        <v>4</v>
       </c>
       <c r="N14">
-        <v>4.2</v>
+        <v>8</v>
       </c>
       <c r="O14">
-        <v>1.65</v>
+        <v>1.4</v>
       </c>
       <c r="P14">
-        <v>3.1</v>
+        <v>3.75</v>
       </c>
       <c r="Q14">
-        <v>5.25</v>
+        <v>7.5</v>
       </c>
       <c r="R14">
-        <v>-0.75</v>
+        <v>-1</v>
       </c>
       <c r="S14">
-        <v>1.9</v>
+        <v>1.75</v>
       </c>
       <c r="T14">
-        <v>1.9</v>
+        <v>2.05</v>
       </c>
       <c r="U14">
-        <v>1.75</v>
+        <v>2.25</v>
       </c>
       <c r="V14">
-        <v>1.9</v>
+        <v>2.025</v>
       </c>
       <c r="W14">
-        <v>1.9</v>
+        <v>1.775</v>
       </c>
       <c r="X14">
-        <v>-1</v>
+        <v>0.3999999999999999</v>
       </c>
       <c r="Y14">
-        <v>2.1</v>
+        <v>-1</v>
       </c>
       <c r="Z14">
         <v>-1</v>
       </c>
       <c r="AA14">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AB14">
-        <v>0.8999999999999999</v>
+        <v>0</v>
       </c>
       <c r="AC14">
-        <v>0.8999999999999999</v>
+        <v>-1</v>
       </c>
       <c r="AD14">
-        <v>-1</v>
+        <v>0.7749999999999999</v>
       </c>
     </row>
     <row r="15" spans="1:30">
@@ -1821,7 +1821,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>6765522</v>
+        <v>6765583</v>
       </c>
       <c r="C15" t="s">
         <v>29</v>
@@ -1830,64 +1830,64 @@
         <v>45108.54166666666</v>
       </c>
       <c r="E15" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I15">
         <v>1</v>
       </c>
       <c r="J15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K15" t="s">
         <v>47</v>
       </c>
       <c r="L15">
-        <v>1.363</v>
+        <v>2.8</v>
       </c>
       <c r="M15">
-        <v>4</v>
+        <v>2.8</v>
       </c>
       <c r="N15">
-        <v>8</v>
+        <v>2.55</v>
       </c>
       <c r="O15">
-        <v>1.4</v>
+        <v>2</v>
       </c>
       <c r="P15">
+        <v>3</v>
+      </c>
+      <c r="Q15">
         <v>3.75</v>
       </c>
-      <c r="Q15">
-        <v>7.5</v>
-      </c>
       <c r="R15">
-        <v>-1</v>
+        <v>-0.25</v>
       </c>
       <c r="S15">
+        <v>1.725</v>
+      </c>
+      <c r="T15">
+        <v>2.075</v>
+      </c>
+      <c r="U15">
+        <v>2</v>
+      </c>
+      <c r="V15">
+        <v>2.05</v>
+      </c>
+      <c r="W15">
         <v>1.75</v>
       </c>
-      <c r="T15">
-        <v>2.05</v>
-      </c>
-      <c r="U15">
-        <v>2.25</v>
-      </c>
-      <c r="V15">
-        <v>2.025</v>
-      </c>
-      <c r="W15">
-        <v>1.775</v>
-      </c>
       <c r="X15">
-        <v>0.3999999999999999</v>
+        <v>1</v>
       </c>
       <c r="Y15">
         <v>-1</v>
@@ -1896,16 +1896,16 @@
         <v>-1</v>
       </c>
       <c r="AA15">
-        <v>0</v>
+        <v>0.7250000000000001</v>
       </c>
       <c r="AB15">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AC15">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="AD15">
-        <v>0.7749999999999999</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="16" spans="1:30">
@@ -1913,7 +1913,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>6765583</v>
+        <v>6765584</v>
       </c>
       <c r="C16" t="s">
         <v>29</v>
@@ -1922,10 +1922,10 @@
         <v>45108.54166666666</v>
       </c>
       <c r="E16" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F16" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="G16">
         <v>2</v>
@@ -1937,49 +1937,49 @@
         <v>1</v>
       </c>
       <c r="J16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K16" t="s">
         <v>47</v>
       </c>
       <c r="L16">
-        <v>2.8</v>
+        <v>2.4</v>
       </c>
       <c r="M16">
         <v>2.8</v>
       </c>
       <c r="N16">
-        <v>2.55</v>
+        <v>3</v>
       </c>
       <c r="O16">
-        <v>2</v>
+        <v>2.05</v>
       </c>
       <c r="P16">
         <v>3</v>
       </c>
       <c r="Q16">
-        <v>3.75</v>
+        <v>3.3</v>
       </c>
       <c r="R16">
         <v>-0.25</v>
       </c>
       <c r="S16">
-        <v>1.725</v>
+        <v>1.825</v>
       </c>
       <c r="T16">
-        <v>2.075</v>
+        <v>1.975</v>
       </c>
       <c r="U16">
-        <v>2</v>
+        <v>2.25</v>
       </c>
       <c r="V16">
-        <v>2.05</v>
+        <v>1.875</v>
       </c>
       <c r="W16">
-        <v>1.75</v>
+        <v>1.925</v>
       </c>
       <c r="X16">
-        <v>1</v>
+        <v>1.05</v>
       </c>
       <c r="Y16">
         <v>-1</v>
@@ -1988,13 +1988,13 @@
         <v>-1</v>
       </c>
       <c r="AA16">
-        <v>0.7250000000000001</v>
+        <v>0.825</v>
       </c>
       <c r="AB16">
         <v>-1</v>
       </c>
       <c r="AC16">
-        <v>1.05</v>
+        <v>0.875</v>
       </c>
       <c r="AD16">
         <v>-1</v>
@@ -2005,7 +2005,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>6765584</v>
+        <v>6765585</v>
       </c>
       <c r="C17" t="s">
         <v>29</v>
@@ -2014,55 +2014,55 @@
         <v>45108.54166666666</v>
       </c>
       <c r="E17" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F17" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H17">
         <v>1</v>
       </c>
       <c r="I17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J17">
         <v>0</v>
       </c>
       <c r="K17" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="L17">
-        <v>2.4</v>
+        <v>2</v>
       </c>
       <c r="M17">
         <v>2.8</v>
       </c>
       <c r="N17">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O17">
         <v>2.05</v>
       </c>
       <c r="P17">
-        <v>3</v>
+        <v>2.7</v>
       </c>
       <c r="Q17">
-        <v>3.3</v>
+        <v>4</v>
       </c>
       <c r="R17">
         <v>-0.25</v>
       </c>
       <c r="S17">
-        <v>1.825</v>
+        <v>1.75</v>
       </c>
       <c r="T17">
-        <v>1.975</v>
+        <v>2.05</v>
       </c>
       <c r="U17">
-        <v>2.25</v>
+        <v>1.75</v>
       </c>
       <c r="V17">
         <v>1.875</v>
@@ -2071,25 +2071,25 @@
         <v>1.925</v>
       </c>
       <c r="X17">
-        <v>1.05</v>
+        <v>-1</v>
       </c>
       <c r="Y17">
-        <v>-1</v>
+        <v>1.7</v>
       </c>
       <c r="Z17">
         <v>-1</v>
       </c>
       <c r="AA17">
-        <v>0.825</v>
+        <v>-0.5</v>
       </c>
       <c r="AB17">
-        <v>-1</v>
+        <v>0.5249999999999999</v>
       </c>
       <c r="AC17">
-        <v>0.875</v>
+        <v>0.4375</v>
       </c>
       <c r="AD17">
-        <v>-1</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="18" spans="1:30">
@@ -2097,7 +2097,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>6765585</v>
+        <v>6765519</v>
       </c>
       <c r="C18" t="s">
         <v>29</v>
@@ -2106,19 +2106,19 @@
         <v>45108.54166666666</v>
       </c>
       <c r="E18" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="F18" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J18">
         <v>0</v>
@@ -2127,61 +2127,61 @@
         <v>49</v>
       </c>
       <c r="L18">
-        <v>2</v>
+        <v>1.8</v>
       </c>
       <c r="M18">
-        <v>2.8</v>
+        <v>3.2</v>
       </c>
       <c r="N18">
-        <v>4</v>
+        <v>4.2</v>
       </c>
       <c r="O18">
-        <v>2.05</v>
+        <v>1.65</v>
       </c>
       <c r="P18">
-        <v>2.7</v>
+        <v>3.1</v>
       </c>
       <c r="Q18">
-        <v>4</v>
+        <v>5.25</v>
       </c>
       <c r="R18">
-        <v>-0.25</v>
+        <v>-0.75</v>
       </c>
       <c r="S18">
-        <v>1.75</v>
+        <v>1.9</v>
       </c>
       <c r="T18">
-        <v>2.05</v>
+        <v>1.9</v>
       </c>
       <c r="U18">
         <v>1.75</v>
       </c>
       <c r="V18">
-        <v>1.875</v>
+        <v>1.9</v>
       </c>
       <c r="W18">
-        <v>1.925</v>
+        <v>1.9</v>
       </c>
       <c r="X18">
         <v>-1</v>
       </c>
       <c r="Y18">
-        <v>1.7</v>
+        <v>2.1</v>
       </c>
       <c r="Z18">
         <v>-1</v>
       </c>
       <c r="AA18">
-        <v>-0.5</v>
+        <v>-1</v>
       </c>
       <c r="AB18">
-        <v>0.5249999999999999</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AC18">
-        <v>0.4375</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AD18">
-        <v>-0.5</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="19" spans="1:30">
@@ -2189,7 +2189,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>6743977</v>
+        <v>6744018</v>
       </c>
       <c r="C19" t="s">
         <v>29</v>
@@ -2198,16 +2198,16 @@
         <v>45111.54166666666</v>
       </c>
       <c r="E19" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="F19" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G19">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I19">
         <v>0</v>
@@ -2216,64 +2216,64 @@
         <v>0</v>
       </c>
       <c r="K19" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="L19">
-        <v>1.444</v>
+        <v>2.2</v>
       </c>
       <c r="M19">
-        <v>3.6</v>
+        <v>2.875</v>
       </c>
       <c r="N19">
-        <v>7</v>
+        <v>3.2</v>
       </c>
       <c r="O19">
-        <v>1.363</v>
+        <v>1.85</v>
       </c>
       <c r="P19">
-        <v>3.8</v>
+        <v>2.9</v>
       </c>
       <c r="Q19">
-        <v>8</v>
+        <v>4.5</v>
       </c>
       <c r="R19">
-        <v>-1.25</v>
+        <v>-0.5</v>
       </c>
       <c r="S19">
-        <v>2</v>
+        <v>1.9</v>
       </c>
       <c r="T19">
-        <v>1.8</v>
+        <v>1.9</v>
       </c>
       <c r="U19">
-        <v>2.25</v>
+        <v>1.75</v>
       </c>
       <c r="V19">
-        <v>1.875</v>
+        <v>1.825</v>
       </c>
       <c r="W19">
-        <v>1.925</v>
+        <v>1.975</v>
       </c>
       <c r="X19">
-        <v>-1</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="Y19">
-        <v>2.8</v>
+        <v>-1</v>
       </c>
       <c r="Z19">
         <v>-1</v>
       </c>
       <c r="AA19">
-        <v>-1</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AB19">
-        <v>0.8</v>
+        <v>-1</v>
       </c>
       <c r="AC19">
-        <v>-1</v>
+        <v>0.825</v>
       </c>
       <c r="AD19">
-        <v>0.925</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="20" spans="1:30">
@@ -2290,7 +2290,7 @@
         <v>45111.54166666666</v>
       </c>
       <c r="E20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F20" t="s">
         <v>44</v>
@@ -2373,7 +2373,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>6744018</v>
+        <v>6743977</v>
       </c>
       <c r="C21" t="s">
         <v>29</v>
@@ -2382,16 +2382,16 @@
         <v>45111.54166666666</v>
       </c>
       <c r="E21" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="F21" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="G21">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I21">
         <v>0</v>
@@ -2400,64 +2400,64 @@
         <v>0</v>
       </c>
       <c r="K21" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="L21">
-        <v>2.2</v>
+        <v>1.444</v>
       </c>
       <c r="M21">
-        <v>2.875</v>
+        <v>3.6</v>
       </c>
       <c r="N21">
-        <v>3.2</v>
+        <v>7</v>
       </c>
       <c r="O21">
-        <v>1.85</v>
+        <v>1.363</v>
       </c>
       <c r="P21">
-        <v>2.9</v>
+        <v>3.8</v>
       </c>
       <c r="Q21">
-        <v>4.5</v>
+        <v>8</v>
       </c>
       <c r="R21">
-        <v>-0.5</v>
+        <v>-1.25</v>
       </c>
       <c r="S21">
-        <v>1.9</v>
+        <v>2</v>
       </c>
       <c r="T21">
-        <v>1.9</v>
+        <v>1.8</v>
       </c>
       <c r="U21">
-        <v>1.75</v>
+        <v>2.25</v>
       </c>
       <c r="V21">
-        <v>1.825</v>
+        <v>1.875</v>
       </c>
       <c r="W21">
-        <v>1.975</v>
+        <v>1.925</v>
       </c>
       <c r="X21">
-        <v>0.8500000000000001</v>
+        <v>-1</v>
       </c>
       <c r="Y21">
-        <v>-1</v>
+        <v>2.8</v>
       </c>
       <c r="Z21">
         <v>-1</v>
       </c>
       <c r="AA21">
-        <v>0.8999999999999999</v>
+        <v>-1</v>
       </c>
       <c r="AB21">
-        <v>-1</v>
+        <v>0.8</v>
       </c>
       <c r="AC21">
-        <v>0.825</v>
+        <v>-1</v>
       </c>
       <c r="AD21">
-        <v>-1</v>
+        <v>0.925</v>
       </c>
     </row>
     <row r="22" spans="1:30">
@@ -2465,7 +2465,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>6743989</v>
+        <v>6858630</v>
       </c>
       <c r="C22" t="s">
         <v>29</v>
@@ -2474,82 +2474,82 @@
         <v>45111.54166666666</v>
       </c>
       <c r="E22" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F22" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G22">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K22" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="L22">
-        <v>1.666</v>
+        <v>2.375</v>
       </c>
       <c r="M22">
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="N22">
-        <v>4.5</v>
+        <v>2.8</v>
       </c>
       <c r="O22">
-        <v>1.5</v>
+        <v>2.45</v>
       </c>
       <c r="P22">
-        <v>3.75</v>
+        <v>2.8</v>
       </c>
       <c r="Q22">
-        <v>5.5</v>
+        <v>3</v>
       </c>
       <c r="R22">
-        <v>-1</v>
+        <v>-0.25</v>
       </c>
       <c r="S22">
-        <v>1.975</v>
+        <v>2.075</v>
       </c>
       <c r="T22">
-        <v>1.825</v>
+        <v>1.725</v>
       </c>
       <c r="U22">
-        <v>2.25</v>
+        <v>1.75</v>
       </c>
       <c r="V22">
-        <v>1.975</v>
+        <v>1.775</v>
       </c>
       <c r="W22">
-        <v>1.825</v>
+        <v>2.025</v>
       </c>
       <c r="X22">
-        <v>0.5</v>
+        <v>-1</v>
       </c>
       <c r="Y22">
-        <v>-1</v>
+        <v>1.8</v>
       </c>
       <c r="Z22">
         <v>-1</v>
       </c>
       <c r="AA22">
-        <v>0</v>
+        <v>-0.5</v>
       </c>
       <c r="AB22">
-        <v>0</v>
+        <v>0.3625</v>
       </c>
       <c r="AC22">
-        <v>0.9750000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AD22">
-        <v>-1</v>
+        <v>1.025</v>
       </c>
     </row>
     <row r="23" spans="1:30">
@@ -2557,7 +2557,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>6743297</v>
+        <v>6743978</v>
       </c>
       <c r="C23" t="s">
         <v>29</v>
@@ -2566,13 +2566,13 @@
         <v>45111.54166666666</v>
       </c>
       <c r="E23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F23" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="G23">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H23">
         <v>0</v>
@@ -2587,25 +2587,25 @@
         <v>47</v>
       </c>
       <c r="L23">
-        <v>1.285</v>
+        <v>2</v>
       </c>
       <c r="M23">
-        <v>4.5</v>
+        <v>2.9</v>
       </c>
       <c r="N23">
-        <v>9</v>
+        <v>3.6</v>
       </c>
       <c r="O23">
-        <v>1.166</v>
+        <v>2.1</v>
       </c>
       <c r="P23">
-        <v>6</v>
+        <v>2.9</v>
       </c>
       <c r="Q23">
-        <v>17</v>
+        <v>3.6</v>
       </c>
       <c r="R23">
-        <v>-1.75</v>
+        <v>-0.25</v>
       </c>
       <c r="S23">
         <v>1.825</v>
@@ -2614,16 +2614,16 @@
         <v>1.975</v>
       </c>
       <c r="U23">
-        <v>2.5</v>
+        <v>1.75</v>
       </c>
       <c r="V23">
-        <v>1.825</v>
+        <v>1.75</v>
       </c>
       <c r="W23">
-        <v>1.975</v>
+        <v>2.05</v>
       </c>
       <c r="X23">
-        <v>0.1659999999999999</v>
+        <v>1.1</v>
       </c>
       <c r="Y23">
         <v>-1</v>
@@ -2632,16 +2632,16 @@
         <v>-1</v>
       </c>
       <c r="AA23">
-        <v>-1</v>
+        <v>0.825</v>
       </c>
       <c r="AB23">
-        <v>0.9750000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AC23">
-        <v>-1</v>
+        <v>0.375</v>
       </c>
       <c r="AD23">
-        <v>0.9750000000000001</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="24" spans="1:30">
@@ -2649,7 +2649,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>6743978</v>
+        <v>6743297</v>
       </c>
       <c r="C24" t="s">
         <v>29</v>
@@ -2658,13 +2658,13 @@
         <v>45111.54166666666</v>
       </c>
       <c r="E24" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F24" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="G24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H24">
         <v>0</v>
@@ -2679,25 +2679,25 @@
         <v>47</v>
       </c>
       <c r="L24">
-        <v>2</v>
+        <v>1.285</v>
       </c>
       <c r="M24">
-        <v>2.9</v>
+        <v>4.5</v>
       </c>
       <c r="N24">
-        <v>3.6</v>
+        <v>9</v>
       </c>
       <c r="O24">
-        <v>2.1</v>
+        <v>1.166</v>
       </c>
       <c r="P24">
-        <v>2.9</v>
+        <v>6</v>
       </c>
       <c r="Q24">
-        <v>3.6</v>
+        <v>17</v>
       </c>
       <c r="R24">
-        <v>-0.25</v>
+        <v>-1.75</v>
       </c>
       <c r="S24">
         <v>1.825</v>
@@ -2706,16 +2706,16 @@
         <v>1.975</v>
       </c>
       <c r="U24">
-        <v>1.75</v>
+        <v>2.5</v>
       </c>
       <c r="V24">
-        <v>1.75</v>
+        <v>1.825</v>
       </c>
       <c r="W24">
-        <v>2.05</v>
+        <v>1.975</v>
       </c>
       <c r="X24">
-        <v>1.1</v>
+        <v>0.1659999999999999</v>
       </c>
       <c r="Y24">
         <v>-1</v>
@@ -2724,16 +2724,16 @@
         <v>-1</v>
       </c>
       <c r="AA24">
-        <v>0.825</v>
+        <v>-1</v>
       </c>
       <c r="AB24">
-        <v>-1</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="AC24">
-        <v>0.375</v>
+        <v>-1</v>
       </c>
       <c r="AD24">
-        <v>-0.5</v>
+        <v>0.9750000000000001</v>
       </c>
     </row>
     <row r="25" spans="1:30">
@@ -2741,7 +2741,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>6858630</v>
+        <v>6743989</v>
       </c>
       <c r="C25" t="s">
         <v>29</v>
@@ -2750,82 +2750,82 @@
         <v>45111.54166666666</v>
       </c>
       <c r="E25" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="F25" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="G25">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K25" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="L25">
-        <v>2.375</v>
+        <v>1.666</v>
       </c>
       <c r="M25">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="N25">
-        <v>2.8</v>
+        <v>4.5</v>
       </c>
       <c r="O25">
-        <v>2.45</v>
+        <v>1.5</v>
       </c>
       <c r="P25">
-        <v>2.8</v>
+        <v>3.75</v>
       </c>
       <c r="Q25">
-        <v>3</v>
+        <v>5.5</v>
       </c>
       <c r="R25">
-        <v>-0.25</v>
+        <v>-1</v>
       </c>
       <c r="S25">
-        <v>2.075</v>
+        <v>1.975</v>
       </c>
       <c r="T25">
-        <v>1.725</v>
+        <v>1.825</v>
       </c>
       <c r="U25">
-        <v>1.75</v>
+        <v>2.25</v>
       </c>
       <c r="V25">
-        <v>1.775</v>
+        <v>1.975</v>
       </c>
       <c r="W25">
-        <v>2.025</v>
+        <v>1.825</v>
       </c>
       <c r="X25">
-        <v>-1</v>
+        <v>0.5</v>
       </c>
       <c r="Y25">
-        <v>1.8</v>
+        <v>-1</v>
       </c>
       <c r="Z25">
         <v>-1</v>
       </c>
       <c r="AA25">
-        <v>-0.5</v>
+        <v>0</v>
       </c>
       <c r="AB25">
-        <v>0.3625</v>
+        <v>0</v>
       </c>
       <c r="AC25">
-        <v>-1</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="AD25">
-        <v>1.025</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="26" spans="1:30">
@@ -2833,7 +2833,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>6872724</v>
+        <v>6872723</v>
       </c>
       <c r="C26" t="s">
         <v>29</v>
@@ -2842,16 +2842,16 @@
         <v>45114.55208333334</v>
       </c>
       <c r="E26" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="F26" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="G26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I26">
         <v>0</v>
@@ -2860,64 +2860,64 @@
         <v>0</v>
       </c>
       <c r="K26" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="L26">
-        <v>1.55</v>
+        <v>1.8</v>
       </c>
       <c r="M26">
-        <v>3.25</v>
+        <v>3.3</v>
       </c>
       <c r="N26">
-        <v>6.5</v>
+        <v>4.333</v>
       </c>
       <c r="O26">
-        <v>1.65</v>
+        <v>1.8</v>
       </c>
       <c r="P26">
-        <v>3.1</v>
+        <v>3.3</v>
       </c>
       <c r="Q26">
-        <v>5.5</v>
+        <v>4.2</v>
       </c>
       <c r="R26">
-        <v>-0.75</v>
+        <v>-0.5</v>
       </c>
       <c r="S26">
-        <v>1.9</v>
+        <v>1.8</v>
       </c>
       <c r="T26">
-        <v>1.9</v>
+        <v>2</v>
       </c>
       <c r="U26">
-        <v>1.75</v>
+        <v>2.25</v>
       </c>
       <c r="V26">
-        <v>1.75</v>
+        <v>2</v>
       </c>
       <c r="W26">
-        <v>2.05</v>
+        <v>1.8</v>
       </c>
       <c r="X26">
-        <v>0.6499999999999999</v>
+        <v>-1</v>
       </c>
       <c r="Y26">
         <v>-1</v>
       </c>
       <c r="Z26">
-        <v>-1</v>
+        <v>3.2</v>
       </c>
       <c r="AA26">
-        <v>0.45</v>
+        <v>-1</v>
       </c>
       <c r="AB26">
-        <v>-0.5</v>
+        <v>1</v>
       </c>
       <c r="AC26">
         <v>-1</v>
       </c>
       <c r="AD26">
-        <v>1.05</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="27" spans="1:30">
@@ -2925,7 +2925,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>6872723</v>
+        <v>6872722</v>
       </c>
       <c r="C27" t="s">
         <v>29</v>
@@ -2934,40 +2934,40 @@
         <v>45114.55208333334</v>
       </c>
       <c r="E27" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="F27" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="G27">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H27">
         <v>1</v>
       </c>
       <c r="I27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K27" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L27">
-        <v>1.8</v>
+        <v>1.45</v>
       </c>
       <c r="M27">
-        <v>3.3</v>
+        <v>3.6</v>
       </c>
       <c r="N27">
-        <v>4.333</v>
+        <v>6.5</v>
       </c>
       <c r="O27">
-        <v>1.8</v>
+        <v>1.85</v>
       </c>
       <c r="P27">
-        <v>3.3</v>
+        <v>3.1</v>
       </c>
       <c r="Q27">
         <v>4.2</v>
@@ -2976,40 +2976,40 @@
         <v>-0.5</v>
       </c>
       <c r="S27">
-        <v>1.8</v>
+        <v>1.95</v>
       </c>
       <c r="T27">
-        <v>2</v>
+        <v>1.85</v>
       </c>
       <c r="U27">
-        <v>2.25</v>
+        <v>2</v>
       </c>
       <c r="V27">
-        <v>2</v>
+        <v>2.025</v>
       </c>
       <c r="W27">
-        <v>1.8</v>
+        <v>1.775</v>
       </c>
       <c r="X27">
-        <v>-1</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="Y27">
         <v>-1</v>
       </c>
       <c r="Z27">
-        <v>3.2</v>
+        <v>-1</v>
       </c>
       <c r="AA27">
-        <v>-1</v>
+        <v>0.95</v>
       </c>
       <c r="AB27">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AC27">
-        <v>-1</v>
+        <v>1.025</v>
       </c>
       <c r="AD27">
-        <v>0.8</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="28" spans="1:30">
@@ -3017,7 +3017,7 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>6872722</v>
+        <v>6872724</v>
       </c>
       <c r="C28" t="s">
         <v>29</v>
@@ -3026,82 +3026,82 @@
         <v>45114.55208333334</v>
       </c>
       <c r="E28" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="F28" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="G28">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K28" t="s">
         <v>47</v>
       </c>
       <c r="L28">
-        <v>1.45</v>
+        <v>1.55</v>
       </c>
       <c r="M28">
-        <v>3.6</v>
+        <v>3.25</v>
       </c>
       <c r="N28">
         <v>6.5</v>
       </c>
       <c r="O28">
-        <v>1.85</v>
+        <v>1.65</v>
       </c>
       <c r="P28">
         <v>3.1</v>
       </c>
       <c r="Q28">
-        <v>4.2</v>
+        <v>5.5</v>
       </c>
       <c r="R28">
+        <v>-0.75</v>
+      </c>
+      <c r="S28">
+        <v>1.9</v>
+      </c>
+      <c r="T28">
+        <v>1.9</v>
+      </c>
+      <c r="U28">
+        <v>1.75</v>
+      </c>
+      <c r="V28">
+        <v>1.75</v>
+      </c>
+      <c r="W28">
+        <v>2.05</v>
+      </c>
+      <c r="X28">
+        <v>0.6499999999999999</v>
+      </c>
+      <c r="Y28">
+        <v>-1</v>
+      </c>
+      <c r="Z28">
+        <v>-1</v>
+      </c>
+      <c r="AA28">
+        <v>0.45</v>
+      </c>
+      <c r="AB28">
         <v>-0.5</v>
       </c>
-      <c r="S28">
-        <v>1.95</v>
-      </c>
-      <c r="T28">
-        <v>1.85</v>
-      </c>
-      <c r="U28">
-        <v>2</v>
-      </c>
-      <c r="V28">
-        <v>2.025</v>
-      </c>
-      <c r="W28">
-        <v>1.775</v>
-      </c>
-      <c r="X28">
-        <v>0.8500000000000001</v>
-      </c>
-      <c r="Y28">
-        <v>-1</v>
-      </c>
-      <c r="Z28">
-        <v>-1</v>
-      </c>
-      <c r="AA28">
-        <v>0.95</v>
-      </c>
-      <c r="AB28">
-        <v>-1</v>
-      </c>
       <c r="AC28">
-        <v>1.025</v>
+        <v>-1</v>
       </c>
       <c r="AD28">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
     </row>
     <row r="29" spans="1:30">
@@ -3213,7 +3213,7 @@
         <v>32</v>
       </c>
       <c r="F30" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G30">
         <v>3</v>
@@ -3477,7 +3477,7 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>6888611</v>
+        <v>6888610</v>
       </c>
       <c r="C33" t="s">
         <v>29</v>
@@ -3486,64 +3486,64 @@
         <v>45117.55208333334</v>
       </c>
       <c r="E33" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F33" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="G33">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I33">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K33" t="s">
         <v>47</v>
       </c>
       <c r="L33">
-        <v>2.05</v>
+        <v>1.25</v>
       </c>
       <c r="M33">
-        <v>2.9</v>
+        <v>4.5</v>
       </c>
       <c r="N33">
-        <v>3.6</v>
+        <v>11</v>
       </c>
       <c r="O33">
-        <v>1.65</v>
+        <v>1.25</v>
       </c>
       <c r="P33">
-        <v>3.25</v>
+        <v>4.2</v>
       </c>
       <c r="Q33">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="R33">
-        <v>-0.75</v>
+        <v>-1.25</v>
       </c>
       <c r="S33">
-        <v>1.9</v>
+        <v>1.775</v>
       </c>
       <c r="T33">
-        <v>1.9</v>
+        <v>2.025</v>
       </c>
       <c r="U33">
-        <v>2.25</v>
+        <v>2</v>
       </c>
       <c r="V33">
+        <v>1.775</v>
+      </c>
+      <c r="W33">
         <v>2.025</v>
       </c>
-      <c r="W33">
-        <v>1.775</v>
-      </c>
       <c r="X33">
-        <v>0.6499999999999999</v>
+        <v>0.25</v>
       </c>
       <c r="Y33">
         <v>-1</v>
@@ -3552,16 +3552,16 @@
         <v>-1</v>
       </c>
       <c r="AA33">
-        <v>0.8999999999999999</v>
+        <v>0.7749999999999999</v>
       </c>
       <c r="AB33">
         <v>-1</v>
       </c>
       <c r="AC33">
-        <v>1.025</v>
+        <v>0</v>
       </c>
       <c r="AD33">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:30">
@@ -3569,7 +3569,7 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>6888610</v>
+        <v>6888609</v>
       </c>
       <c r="C34" t="s">
         <v>29</v>
@@ -3578,76 +3578,76 @@
         <v>45117.55208333334</v>
       </c>
       <c r="E34" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="F34" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G34">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K34" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="L34">
-        <v>1.25</v>
+        <v>1.666</v>
       </c>
       <c r="M34">
-        <v>4.5</v>
+        <v>3</v>
       </c>
       <c r="N34">
-        <v>11</v>
+        <v>5.5</v>
       </c>
       <c r="O34">
-        <v>1.25</v>
+        <v>1.833</v>
       </c>
       <c r="P34">
+        <v>3</v>
+      </c>
+      <c r="Q34">
         <v>4.2</v>
       </c>
-      <c r="Q34">
-        <v>12</v>
-      </c>
       <c r="R34">
-        <v>-1.25</v>
+        <v>-0.5</v>
       </c>
       <c r="S34">
+        <v>2.025</v>
+      </c>
+      <c r="T34">
         <v>1.775</v>
       </c>
-      <c r="T34">
-        <v>2.025</v>
-      </c>
       <c r="U34">
         <v>2</v>
       </c>
       <c r="V34">
-        <v>1.775</v>
+        <v>1.95</v>
       </c>
       <c r="W34">
-        <v>2.025</v>
+        <v>1.85</v>
       </c>
       <c r="X34">
-        <v>0.25</v>
+        <v>-1</v>
       </c>
       <c r="Y34">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="Z34">
         <v>-1</v>
       </c>
       <c r="AA34">
+        <v>-1</v>
+      </c>
+      <c r="AB34">
         <v>0.7749999999999999</v>
-      </c>
-      <c r="AB34">
-        <v>-1</v>
       </c>
       <c r="AC34">
         <v>0</v>
@@ -3661,7 +3661,7 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>6888615</v>
+        <v>6888612</v>
       </c>
       <c r="C35" t="s">
         <v>29</v>
@@ -3670,19 +3670,19 @@
         <v>45117.55208333334</v>
       </c>
       <c r="E35" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="F35" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G35">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H35">
         <v>0</v>
       </c>
       <c r="I35">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J35">
         <v>0</v>
@@ -3691,61 +3691,61 @@
         <v>47</v>
       </c>
       <c r="L35">
-        <v>3.5</v>
+        <v>1.727</v>
       </c>
       <c r="M35">
-        <v>2.875</v>
+        <v>3.2</v>
       </c>
       <c r="N35">
-        <v>2.1</v>
+        <v>4.5</v>
       </c>
       <c r="O35">
-        <v>1.7</v>
+        <v>1.65</v>
       </c>
       <c r="P35">
-        <v>3</v>
+        <v>3.3</v>
       </c>
       <c r="Q35">
-        <v>5.25</v>
+        <v>5.75</v>
       </c>
       <c r="R35">
+        <v>-0.75</v>
+      </c>
+      <c r="S35">
+        <v>1.875</v>
+      </c>
+      <c r="T35">
+        <v>1.925</v>
+      </c>
+      <c r="U35">
+        <v>1.75</v>
+      </c>
+      <c r="V35">
+        <v>1.9</v>
+      </c>
+      <c r="W35">
+        <v>1.9</v>
+      </c>
+      <c r="X35">
+        <v>0.6499999999999999</v>
+      </c>
+      <c r="Y35">
+        <v>-1</v>
+      </c>
+      <c r="Z35">
+        <v>-1</v>
+      </c>
+      <c r="AA35">
+        <v>0.4375</v>
+      </c>
+      <c r="AB35">
         <v>-0.5</v>
       </c>
-      <c r="S35">
-        <v>1.775</v>
-      </c>
-      <c r="T35">
-        <v>2.025</v>
-      </c>
-      <c r="U35">
-        <v>2</v>
-      </c>
-      <c r="V35">
-        <v>1.875</v>
-      </c>
-      <c r="W35">
-        <v>1.925</v>
-      </c>
-      <c r="X35">
-        <v>0.7</v>
-      </c>
-      <c r="Y35">
-        <v>-1</v>
-      </c>
-      <c r="Z35">
-        <v>-1</v>
-      </c>
-      <c r="AA35">
-        <v>0.7749999999999999</v>
-      </c>
-      <c r="AB35">
-        <v>-1</v>
-      </c>
       <c r="AC35">
-        <v>0.875</v>
+        <v>-1</v>
       </c>
       <c r="AD35">
-        <v>-1</v>
+        <v>0.8999999999999999</v>
       </c>
     </row>
     <row r="36" spans="1:30">
@@ -3753,7 +3753,7 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>6888614</v>
+        <v>6888611</v>
       </c>
       <c r="C36" t="s">
         <v>29</v>
@@ -3762,79 +3762,79 @@
         <v>45117.55208333334</v>
       </c>
       <c r="E36" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F36" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G36">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H36">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I36">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J36">
         <v>1</v>
       </c>
       <c r="K36" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L36">
-        <v>1.8</v>
+        <v>2.05</v>
       </c>
       <c r="M36">
-        <v>3.2</v>
+        <v>2.9</v>
       </c>
       <c r="N36">
-        <v>4</v>
+        <v>3.6</v>
       </c>
       <c r="O36">
-        <v>2.5</v>
+        <v>1.65</v>
       </c>
       <c r="P36">
-        <v>3</v>
+        <v>3.25</v>
       </c>
       <c r="Q36">
-        <v>2.625</v>
+        <v>5</v>
       </c>
       <c r="R36">
-        <v>0</v>
+        <v>-0.75</v>
       </c>
       <c r="S36">
-        <v>1.85</v>
+        <v>1.9</v>
       </c>
       <c r="T36">
-        <v>1.95</v>
+        <v>1.9</v>
       </c>
       <c r="U36">
-        <v>1.75</v>
+        <v>2.25</v>
       </c>
       <c r="V36">
+        <v>2.025</v>
+      </c>
+      <c r="W36">
         <v>1.775</v>
       </c>
-      <c r="W36">
-        <v>2.025</v>
-      </c>
       <c r="X36">
-        <v>-1</v>
+        <v>0.6499999999999999</v>
       </c>
       <c r="Y36">
         <v>-1</v>
       </c>
       <c r="Z36">
-        <v>1.625</v>
+        <v>-1</v>
       </c>
       <c r="AA36">
-        <v>-1</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AB36">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
       <c r="AC36">
-        <v>0.7749999999999999</v>
+        <v>1.025</v>
       </c>
       <c r="AD36">
         <v>-1</v>
@@ -3845,7 +3845,7 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>6888613</v>
+        <v>6888614</v>
       </c>
       <c r="C37" t="s">
         <v>29</v>
@@ -3854,79 +3854,79 @@
         <v>45117.55208333334</v>
       </c>
       <c r="E37" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="F37" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="G37">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H37">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I37">
         <v>1</v>
       </c>
       <c r="J37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K37" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="L37">
-        <v>1.4</v>
+        <v>1.8</v>
       </c>
       <c r="M37">
-        <v>3.75</v>
+        <v>3.2</v>
       </c>
       <c r="N37">
-        <v>7.5</v>
+        <v>4</v>
       </c>
       <c r="O37">
-        <v>1.363</v>
+        <v>2.5</v>
       </c>
       <c r="P37">
-        <v>4.333</v>
+        <v>3</v>
       </c>
       <c r="Q37">
-        <v>7</v>
+        <v>2.625</v>
       </c>
       <c r="R37">
-        <v>-1.25</v>
+        <v>0</v>
       </c>
       <c r="S37">
-        <v>1.925</v>
+        <v>1.85</v>
       </c>
       <c r="T37">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="U37">
-        <v>2.25</v>
+        <v>1.75</v>
       </c>
       <c r="V37">
-        <v>1.975</v>
+        <v>1.775</v>
       </c>
       <c r="W37">
-        <v>1.825</v>
+        <v>2.025</v>
       </c>
       <c r="X37">
-        <v>0.363</v>
+        <v>-1</v>
       </c>
       <c r="Y37">
         <v>-1</v>
       </c>
       <c r="Z37">
-        <v>-1</v>
+        <v>1.625</v>
       </c>
       <c r="AA37">
-        <v>-0.5</v>
+        <v>-1</v>
       </c>
       <c r="AB37">
-        <v>0.4375</v>
+        <v>0.95</v>
       </c>
       <c r="AC37">
-        <v>0.9750000000000001</v>
+        <v>0.7749999999999999</v>
       </c>
       <c r="AD37">
         <v>-1</v>
@@ -3937,7 +3937,7 @@
         <v>36</v>
       </c>
       <c r="B38">
-        <v>6888612</v>
+        <v>6888615</v>
       </c>
       <c r="C38" t="s">
         <v>29</v>
@@ -3946,19 +3946,19 @@
         <v>45117.55208333334</v>
       </c>
       <c r="E38" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="F38" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="G38">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H38">
         <v>0</v>
       </c>
       <c r="I38">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J38">
         <v>0</v>
@@ -3967,43 +3967,43 @@
         <v>47</v>
       </c>
       <c r="L38">
-        <v>1.727</v>
+        <v>3.5</v>
       </c>
       <c r="M38">
-        <v>3.2</v>
+        <v>2.875</v>
       </c>
       <c r="N38">
-        <v>4.5</v>
+        <v>2.1</v>
       </c>
       <c r="O38">
-        <v>1.65</v>
+        <v>1.7</v>
       </c>
       <c r="P38">
-        <v>3.3</v>
+        <v>3</v>
       </c>
       <c r="Q38">
-        <v>5.75</v>
+        <v>5.25</v>
       </c>
       <c r="R38">
-        <v>-0.75</v>
+        <v>-0.5</v>
       </c>
       <c r="S38">
+        <v>1.775</v>
+      </c>
+      <c r="T38">
+        <v>2.025</v>
+      </c>
+      <c r="U38">
+        <v>2</v>
+      </c>
+      <c r="V38">
         <v>1.875</v>
       </c>
-      <c r="T38">
+      <c r="W38">
         <v>1.925</v>
       </c>
-      <c r="U38">
-        <v>1.75</v>
-      </c>
-      <c r="V38">
-        <v>1.9</v>
-      </c>
-      <c r="W38">
-        <v>1.9</v>
-      </c>
       <c r="X38">
-        <v>0.6499999999999999</v>
+        <v>0.7</v>
       </c>
       <c r="Y38">
         <v>-1</v>
@@ -4012,16 +4012,16 @@
         <v>-1</v>
       </c>
       <c r="AA38">
-        <v>0.4375</v>
+        <v>0.7749999999999999</v>
       </c>
       <c r="AB38">
-        <v>-0.5</v>
+        <v>-1</v>
       </c>
       <c r="AC38">
-        <v>-1</v>
+        <v>0.875</v>
       </c>
       <c r="AD38">
-        <v>0.8999999999999999</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="39" spans="1:30">
@@ -4029,7 +4029,7 @@
         <v>37</v>
       </c>
       <c r="B39">
-        <v>6888609</v>
+        <v>6888613</v>
       </c>
       <c r="C39" t="s">
         <v>29</v>
@@ -4038,82 +4038,82 @@
         <v>45117.55208333334</v>
       </c>
       <c r="E39" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="F39" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="G39">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H39">
         <v>1</v>
       </c>
       <c r="I39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K39" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="L39">
-        <v>1.666</v>
+        <v>1.4</v>
       </c>
       <c r="M39">
-        <v>3</v>
+        <v>3.75</v>
       </c>
       <c r="N39">
-        <v>5.5</v>
+        <v>7.5</v>
       </c>
       <c r="O39">
-        <v>1.833</v>
+        <v>1.363</v>
       </c>
       <c r="P39">
-        <v>3</v>
+        <v>4.333</v>
       </c>
       <c r="Q39">
-        <v>4.2</v>
+        <v>7</v>
       </c>
       <c r="R39">
+        <v>-1.25</v>
+      </c>
+      <c r="S39">
+        <v>1.925</v>
+      </c>
+      <c r="T39">
+        <v>1.875</v>
+      </c>
+      <c r="U39">
+        <v>2.25</v>
+      </c>
+      <c r="V39">
+        <v>1.975</v>
+      </c>
+      <c r="W39">
+        <v>1.825</v>
+      </c>
+      <c r="X39">
+        <v>0.363</v>
+      </c>
+      <c r="Y39">
+        <v>-1</v>
+      </c>
+      <c r="Z39">
+        <v>-1</v>
+      </c>
+      <c r="AA39">
         <v>-0.5</v>
       </c>
-      <c r="S39">
-        <v>2.025</v>
-      </c>
-      <c r="T39">
-        <v>1.775</v>
-      </c>
-      <c r="U39">
-        <v>2</v>
-      </c>
-      <c r="V39">
-        <v>1.95</v>
-      </c>
-      <c r="W39">
-        <v>1.85</v>
-      </c>
-      <c r="X39">
-        <v>-1</v>
-      </c>
-      <c r="Y39">
-        <v>2</v>
-      </c>
-      <c r="Z39">
-        <v>-1</v>
-      </c>
-      <c r="AA39">
-        <v>-1</v>
-      </c>
       <c r="AB39">
-        <v>0.7749999999999999</v>
+        <v>0.4375</v>
       </c>
       <c r="AC39">
-        <v>0</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="AD39">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="40" spans="1:30">
@@ -4225,7 +4225,7 @@
         <v>42</v>
       </c>
       <c r="F41" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G41">
         <v>1</v>
@@ -4409,7 +4409,7 @@
         <v>34</v>
       </c>
       <c r="F43" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G43">
         <v>1</v>
@@ -4866,7 +4866,7 @@
         <v>45191.5</v>
       </c>
       <c r="E48" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F48" t="s">
         <v>44</v>
@@ -5053,7 +5053,7 @@
         <v>35</v>
       </c>
       <c r="F50" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G50">
         <v>0</v>
@@ -5510,7 +5510,7 @@
         <v>45196.5</v>
       </c>
       <c r="E55" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F55" t="s">
         <v>36</v>
@@ -6065,7 +6065,7 @@
         <v>32</v>
       </c>
       <c r="F61" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G61">
         <v>1</v>
@@ -6154,7 +6154,7 @@
         <v>45205.48958333334</v>
       </c>
       <c r="E62" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F62" t="s">
         <v>37</v>
@@ -6329,7 +6329,7 @@
         <v>62</v>
       </c>
       <c r="B64">
-        <v>7230941</v>
+        <v>7230940</v>
       </c>
       <c r="C64" t="s">
         <v>29</v>
@@ -6338,82 +6338,82 @@
         <v>45205.625</v>
       </c>
       <c r="E64" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F64" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="G64">
         <v>0</v>
       </c>
       <c r="H64">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I64">
         <v>0</v>
       </c>
       <c r="J64">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K64" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="L64">
-        <v>1.727</v>
+        <v>1.833</v>
       </c>
       <c r="M64">
-        <v>3.2</v>
+        <v>3.1</v>
       </c>
       <c r="N64">
-        <v>4.5</v>
+        <v>4</v>
       </c>
       <c r="O64">
-        <v>1.571</v>
+        <v>1.909</v>
       </c>
       <c r="P64">
-        <v>3.4</v>
+        <v>3.1</v>
       </c>
       <c r="Q64">
-        <v>5.5</v>
+        <v>3.75</v>
       </c>
       <c r="R64">
-        <v>-0.75</v>
+        <v>-0.5</v>
       </c>
       <c r="S64">
+        <v>1.975</v>
+      </c>
+      <c r="T64">
         <v>1.825</v>
       </c>
-      <c r="T64">
-        <v>1.975</v>
-      </c>
       <c r="U64">
         <v>2</v>
       </c>
       <c r="V64">
-        <v>1.9</v>
+        <v>2</v>
       </c>
       <c r="W64">
-        <v>1.9</v>
+        <v>1.8</v>
       </c>
       <c r="X64">
         <v>-1</v>
       </c>
       <c r="Y64">
-        <v>2.4</v>
+        <v>-1</v>
       </c>
       <c r="Z64">
-        <v>-1</v>
+        <v>2.75</v>
       </c>
       <c r="AA64">
         <v>-1</v>
       </c>
       <c r="AB64">
-        <v>0.9750000000000001</v>
+        <v>0.825</v>
       </c>
       <c r="AC64">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="AD64">
-        <v>0.8999999999999999</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="65" spans="1:30">
@@ -6421,7 +6421,7 @@
         <v>63</v>
       </c>
       <c r="B65">
-        <v>7230940</v>
+        <v>7230941</v>
       </c>
       <c r="C65" t="s">
         <v>29</v>
@@ -6430,82 +6430,82 @@
         <v>45205.625</v>
       </c>
       <c r="E65" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="F65" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="G65">
         <v>0</v>
       </c>
       <c r="H65">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="I65">
         <v>0</v>
       </c>
       <c r="J65">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K65" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="L65">
-        <v>1.833</v>
+        <v>1.727</v>
       </c>
       <c r="M65">
-        <v>3.1</v>
+        <v>3.2</v>
       </c>
       <c r="N65">
-        <v>4</v>
+        <v>4.5</v>
       </c>
       <c r="O65">
-        <v>1.909</v>
+        <v>1.571</v>
       </c>
       <c r="P65">
-        <v>3.1</v>
+        <v>3.4</v>
       </c>
       <c r="Q65">
-        <v>3.75</v>
+        <v>5.5</v>
       </c>
       <c r="R65">
-        <v>-0.5</v>
+        <v>-0.75</v>
       </c>
       <c r="S65">
+        <v>1.825</v>
+      </c>
+      <c r="T65">
         <v>1.975</v>
       </c>
-      <c r="T65">
-        <v>1.825</v>
-      </c>
       <c r="U65">
         <v>2</v>
       </c>
       <c r="V65">
-        <v>2</v>
+        <v>1.9</v>
       </c>
       <c r="W65">
-        <v>1.8</v>
+        <v>1.9</v>
       </c>
       <c r="X65">
         <v>-1</v>
       </c>
       <c r="Y65">
-        <v>-1</v>
+        <v>2.4</v>
       </c>
       <c r="Z65">
-        <v>2.75</v>
+        <v>-1</v>
       </c>
       <c r="AA65">
         <v>-1</v>
       </c>
       <c r="AB65">
-        <v>0.825</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="AC65">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AD65">
-        <v>-1</v>
+        <v>0.8999999999999999</v>
       </c>
     </row>
     <row r="66" spans="1:30">
@@ -7074,7 +7074,7 @@
         <v>45240.47916666666</v>
       </c>
       <c r="E72" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F72" t="s">
         <v>43</v>
@@ -7169,7 +7169,7 @@
         <v>46</v>
       </c>
       <c r="F73" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G73">
         <v>3</v>
@@ -7810,7 +7810,7 @@
         <v>45244.45833333334</v>
       </c>
       <c r="E80" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F80" t="s">
         <v>40</v>
@@ -7994,7 +7994,7 @@
         <v>45247.47569444445</v>
       </c>
       <c r="E82" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F82" t="s">
         <v>41</v>
@@ -8365,7 +8365,7 @@
         <v>45</v>
       </c>
       <c r="F86" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G86">
         <v>0</v>
@@ -8721,7 +8721,7 @@
         <v>88</v>
       </c>
       <c r="B90">
-        <v>7480684</v>
+        <v>7480688</v>
       </c>
       <c r="C90" t="s">
         <v>29</v>
@@ -8730,16 +8730,16 @@
         <v>45254.46875</v>
       </c>
       <c r="E90" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="F90" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G90">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H90">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I90">
         <v>0</v>
@@ -8751,61 +8751,61 @@
         <v>49</v>
       </c>
       <c r="L90">
-        <v>1.85</v>
+        <v>1.7</v>
       </c>
       <c r="M90">
+        <v>3.2</v>
+      </c>
+      <c r="N90">
+        <v>4.75</v>
+      </c>
+      <c r="O90">
+        <v>1.95</v>
+      </c>
+      <c r="P90">
         <v>3</v>
-      </c>
-      <c r="N90">
-        <v>4.25</v>
-      </c>
-      <c r="O90">
-        <v>2</v>
-      </c>
-      <c r="P90">
-        <v>2.9</v>
       </c>
       <c r="Q90">
         <v>3.8</v>
       </c>
       <c r="R90">
-        <v>-0.25</v>
+        <v>-0.5</v>
       </c>
       <c r="S90">
-        <v>1.75</v>
+        <v>1.975</v>
       </c>
       <c r="T90">
-        <v>2.05</v>
+        <v>1.825</v>
       </c>
       <c r="U90">
-        <v>1.75</v>
+        <v>2</v>
       </c>
       <c r="V90">
-        <v>1.75</v>
+        <v>1.925</v>
       </c>
       <c r="W90">
-        <v>2.05</v>
+        <v>1.875</v>
       </c>
       <c r="X90">
         <v>-1</v>
       </c>
       <c r="Y90">
-        <v>1.9</v>
+        <v>2</v>
       </c>
       <c r="Z90">
         <v>-1</v>
       </c>
       <c r="AA90">
-        <v>-0.5</v>
+        <v>-1</v>
       </c>
       <c r="AB90">
-        <v>0.5249999999999999</v>
+        <v>0.825</v>
       </c>
       <c r="AC90">
-        <v>0.375</v>
+        <v>-1</v>
       </c>
       <c r="AD90">
-        <v>-0.5</v>
+        <v>0.875</v>
       </c>
     </row>
     <row r="91" spans="1:30">
@@ -8813,7 +8813,7 @@
         <v>89</v>
       </c>
       <c r="B91">
-        <v>7480688</v>
+        <v>7480684</v>
       </c>
       <c r="C91" t="s">
         <v>29</v>
@@ -8822,16 +8822,16 @@
         <v>45254.46875</v>
       </c>
       <c r="E91" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="F91" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="G91">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H91">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I91">
         <v>0</v>
@@ -8843,61 +8843,61 @@
         <v>49</v>
       </c>
       <c r="L91">
-        <v>1.7</v>
+        <v>1.85</v>
       </c>
       <c r="M91">
-        <v>3.2</v>
+        <v>3</v>
       </c>
       <c r="N91">
-        <v>4.75</v>
+        <v>4.25</v>
       </c>
       <c r="O91">
-        <v>1.95</v>
+        <v>2</v>
       </c>
       <c r="P91">
-        <v>3</v>
+        <v>2.9</v>
       </c>
       <c r="Q91">
         <v>3.8</v>
       </c>
       <c r="R91">
+        <v>-0.25</v>
+      </c>
+      <c r="S91">
+        <v>1.75</v>
+      </c>
+      <c r="T91">
+        <v>2.05</v>
+      </c>
+      <c r="U91">
+        <v>1.75</v>
+      </c>
+      <c r="V91">
+        <v>1.75</v>
+      </c>
+      <c r="W91">
+        <v>2.05</v>
+      </c>
+      <c r="X91">
+        <v>-1</v>
+      </c>
+      <c r="Y91">
+        <v>1.9</v>
+      </c>
+      <c r="Z91">
+        <v>-1</v>
+      </c>
+      <c r="AA91">
         <v>-0.5</v>
       </c>
-      <c r="S91">
-        <v>1.975</v>
-      </c>
-      <c r="T91">
-        <v>1.825</v>
-      </c>
-      <c r="U91">
-        <v>2</v>
-      </c>
-      <c r="V91">
-        <v>1.925</v>
-      </c>
-      <c r="W91">
-        <v>1.875</v>
-      </c>
-      <c r="X91">
-        <v>-1</v>
-      </c>
-      <c r="Y91">
-        <v>2</v>
-      </c>
-      <c r="Z91">
-        <v>-1</v>
-      </c>
-      <c r="AA91">
-        <v>-1</v>
-      </c>
       <c r="AB91">
-        <v>0.825</v>
+        <v>0.5249999999999999</v>
       </c>
       <c r="AC91">
-        <v>-1</v>
+        <v>0.375</v>
       </c>
       <c r="AD91">
-        <v>0.875</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="92" spans="1:30">
@@ -9193,7 +9193,7 @@
         <v>34</v>
       </c>
       <c r="F95" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G95">
         <v>1</v>
@@ -9374,7 +9374,7 @@
         <v>45261.58333333334</v>
       </c>
       <c r="E97" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F97" t="s">
         <v>33</v>
@@ -9745,7 +9745,7 @@
         <v>44</v>
       </c>
       <c r="F101" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G101">
         <v>1</v>
@@ -10285,7 +10285,7 @@
         <v>105</v>
       </c>
       <c r="B107">
-        <v>7567197</v>
+        <v>7567876</v>
       </c>
       <c r="C107" t="s">
         <v>29</v>
@@ -10294,10 +10294,10 @@
         <v>45275.46875</v>
       </c>
       <c r="E107" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="F107" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="G107">
         <v>1</v>
@@ -10309,67 +10309,67 @@
         <v>0</v>
       </c>
       <c r="J107">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K107" t="s">
         <v>49</v>
       </c>
       <c r="L107">
-        <v>2</v>
+        <v>4.75</v>
       </c>
       <c r="M107">
-        <v>3</v>
+        <v>3.1</v>
       </c>
       <c r="N107">
-        <v>3.6</v>
+        <v>1.727</v>
       </c>
       <c r="O107">
+        <v>6</v>
+      </c>
+      <c r="P107">
+        <v>3.1</v>
+      </c>
+      <c r="Q107">
+        <v>1.65</v>
+      </c>
+      <c r="R107">
+        <v>0.75</v>
+      </c>
+      <c r="S107">
+        <v>1.975</v>
+      </c>
+      <c r="T107">
+        <v>1.825</v>
+      </c>
+      <c r="U107">
+        <v>2</v>
+      </c>
+      <c r="V107">
+        <v>2</v>
+      </c>
+      <c r="W107">
+        <v>1.8</v>
+      </c>
+      <c r="X107">
+        <v>-1</v>
+      </c>
+      <c r="Y107">
         <v>2.1</v>
       </c>
-      <c r="P107">
-        <v>2.9</v>
-      </c>
-      <c r="Q107">
-        <v>3.5</v>
-      </c>
-      <c r="R107">
-        <v>-0.25</v>
-      </c>
-      <c r="S107">
-        <v>1.825</v>
-      </c>
-      <c r="T107">
-        <v>1.975</v>
-      </c>
-      <c r="U107">
-        <v>1.75</v>
-      </c>
-      <c r="V107">
-        <v>1.85</v>
-      </c>
-      <c r="W107">
-        <v>1.95</v>
-      </c>
-      <c r="X107">
-        <v>-1</v>
-      </c>
-      <c r="Y107">
-        <v>1.9</v>
-      </c>
       <c r="Z107">
         <v>-1</v>
       </c>
       <c r="AA107">
-        <v>-0.5</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="AB107">
-        <v>0.4875</v>
+        <v>-1</v>
       </c>
       <c r="AC107">
-        <v>0.425</v>
+        <v>0</v>
       </c>
       <c r="AD107">
-        <v>-0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="108" spans="1:30">
@@ -10377,7 +10377,7 @@
         <v>106</v>
       </c>
       <c r="B108">
-        <v>7567876</v>
+        <v>7567197</v>
       </c>
       <c r="C108" t="s">
         <v>29</v>
@@ -10386,10 +10386,10 @@
         <v>45275.46875</v>
       </c>
       <c r="E108" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="F108" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="G108">
         <v>1</v>
@@ -10401,67 +10401,67 @@
         <v>0</v>
       </c>
       <c r="J108">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K108" t="s">
         <v>49</v>
       </c>
       <c r="L108">
-        <v>4.75</v>
+        <v>2</v>
       </c>
       <c r="M108">
-        <v>3.1</v>
+        <v>3</v>
       </c>
       <c r="N108">
-        <v>1.727</v>
+        <v>3.6</v>
       </c>
       <c r="O108">
-        <v>6</v>
+        <v>2.1</v>
       </c>
       <c r="P108">
-        <v>3.1</v>
+        <v>2.9</v>
       </c>
       <c r="Q108">
-        <v>1.65</v>
+        <v>3.5</v>
       </c>
       <c r="R108">
-        <v>0.75</v>
+        <v>-0.25</v>
       </c>
       <c r="S108">
+        <v>1.825</v>
+      </c>
+      <c r="T108">
         <v>1.975</v>
       </c>
-      <c r="T108">
-        <v>1.825</v>
-      </c>
       <c r="U108">
-        <v>2</v>
+        <v>1.75</v>
       </c>
       <c r="V108">
-        <v>2</v>
+        <v>1.85</v>
       </c>
       <c r="W108">
-        <v>1.8</v>
+        <v>1.95</v>
       </c>
       <c r="X108">
         <v>-1</v>
       </c>
       <c r="Y108">
-        <v>2.1</v>
+        <v>1.9</v>
       </c>
       <c r="Z108">
         <v>-1</v>
       </c>
       <c r="AA108">
-        <v>0.9750000000000001</v>
+        <v>-0.5</v>
       </c>
       <c r="AB108">
-        <v>-1</v>
+        <v>0.4875</v>
       </c>
       <c r="AC108">
-        <v>0</v>
+        <v>0.425</v>
       </c>
       <c r="AD108">
-        <v>0</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="109" spans="1:30">
@@ -10478,7 +10478,7 @@
         <v>45275.53125</v>
       </c>
       <c r="E109" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F109" t="s">
         <v>35</v>
@@ -10573,7 +10573,7 @@
         <v>32</v>
       </c>
       <c r="F110" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G110">
         <v>1</v>
@@ -11033,7 +11033,7 @@
         <v>40</v>
       </c>
       <c r="F115" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G115">
         <v>2</v>
@@ -11306,7 +11306,7 @@
         <v>45289.46875</v>
       </c>
       <c r="E118" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F118" t="s">
         <v>37</v>
@@ -11665,7 +11665,7 @@
         <v>120</v>
       </c>
       <c r="B122">
-        <v>7656900</v>
+        <v>7624657</v>
       </c>
       <c r="C122" t="s">
         <v>29</v>
@@ -11674,61 +11674,61 @@
         <v>45296.46875</v>
       </c>
       <c r="E122" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="F122" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="G122">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H122">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I122">
         <v>0</v>
       </c>
       <c r="J122">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K122" t="s">
         <v>48</v>
       </c>
       <c r="L122">
-        <v>1.833</v>
+        <v>3</v>
       </c>
       <c r="M122">
-        <v>3.1</v>
+        <v>2.8</v>
       </c>
       <c r="N122">
-        <v>4</v>
+        <v>2.375</v>
       </c>
       <c r="O122">
-        <v>2.875</v>
+        <v>4.333</v>
       </c>
       <c r="P122">
         <v>3</v>
       </c>
       <c r="Q122">
-        <v>2.625</v>
+        <v>1.85</v>
       </c>
       <c r="R122">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="S122">
-        <v>1.975</v>
+        <v>1.85</v>
       </c>
       <c r="T122">
-        <v>1.825</v>
+        <v>1.95</v>
       </c>
       <c r="U122">
         <v>2</v>
       </c>
       <c r="V122">
-        <v>1.925</v>
+        <v>2.025</v>
       </c>
       <c r="W122">
-        <v>1.875</v>
+        <v>1.775</v>
       </c>
       <c r="X122">
         <v>-1</v>
@@ -11737,19 +11737,19 @@
         <v>-1</v>
       </c>
       <c r="Z122">
-        <v>1.625</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AA122">
         <v>-1</v>
       </c>
       <c r="AB122">
-        <v>0.825</v>
+        <v>0.95</v>
       </c>
       <c r="AC122">
-        <v>-1</v>
+        <v>1.025</v>
       </c>
       <c r="AD122">
-        <v>0.875</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="123" spans="1:30">
@@ -11849,7 +11849,7 @@
         <v>122</v>
       </c>
       <c r="B124">
-        <v>7624657</v>
+        <v>7656900</v>
       </c>
       <c r="C124" t="s">
         <v>29</v>
@@ -11858,61 +11858,61 @@
         <v>45296.46875</v>
       </c>
       <c r="E124" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="F124" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="G124">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H124">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I124">
         <v>0</v>
       </c>
       <c r="J124">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K124" t="s">
         <v>48</v>
       </c>
       <c r="L124">
-        <v>3</v>
+        <v>1.833</v>
       </c>
       <c r="M124">
-        <v>2.8</v>
+        <v>3.1</v>
       </c>
       <c r="N124">
-        <v>2.375</v>
+        <v>4</v>
       </c>
       <c r="O124">
-        <v>4.333</v>
+        <v>2.875</v>
       </c>
       <c r="P124">
         <v>3</v>
       </c>
       <c r="Q124">
-        <v>1.85</v>
+        <v>2.625</v>
       </c>
       <c r="R124">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="S124">
-        <v>1.85</v>
+        <v>1.975</v>
       </c>
       <c r="T124">
-        <v>1.95</v>
+        <v>1.825</v>
       </c>
       <c r="U124">
         <v>2</v>
       </c>
       <c r="V124">
-        <v>2.025</v>
+        <v>1.925</v>
       </c>
       <c r="W124">
-        <v>1.775</v>
+        <v>1.875</v>
       </c>
       <c r="X124">
         <v>-1</v>
@@ -11921,19 +11921,19 @@
         <v>-1</v>
       </c>
       <c r="Z124">
-        <v>0.8500000000000001</v>
+        <v>1.625</v>
       </c>
       <c r="AA124">
         <v>-1</v>
       </c>
       <c r="AB124">
-        <v>0.95</v>
+        <v>0.825</v>
       </c>
       <c r="AC124">
-        <v>1.025</v>
+        <v>-1</v>
       </c>
       <c r="AD124">
-        <v>-1</v>
+        <v>0.875</v>
       </c>
     </row>
     <row r="125" spans="1:30">
@@ -12042,7 +12042,7 @@
         <v>45296.60416666666</v>
       </c>
       <c r="E126" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F126" t="s">
         <v>39</v>
@@ -12413,7 +12413,7 @@
         <v>43</v>
       </c>
       <c r="F130" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G130">
         <v>1</v>
@@ -12594,7 +12594,7 @@
         <v>45303.46875</v>
       </c>
       <c r="E132" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F132" t="s">
         <v>41</v>
@@ -13238,7 +13238,7 @@
         <v>45310.47916666666</v>
       </c>
       <c r="E139" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F139" t="s">
         <v>38</v>
@@ -13698,7 +13698,7 @@
         <v>45310.53125</v>
       </c>
       <c r="E144" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F144" t="s">
         <v>45</v>
@@ -13965,7 +13965,7 @@
         <v>145</v>
       </c>
       <c r="B147">
-        <v>7624533</v>
+        <v>7590958</v>
       </c>
       <c r="C147" t="s">
         <v>29</v>
@@ -13974,10 +13974,10 @@
         <v>45314.54166666666</v>
       </c>
       <c r="E147" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="F147" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="G147">
         <v>0</v>
@@ -13995,31 +13995,31 @@
         <v>49</v>
       </c>
       <c r="L147">
-        <v>1.4</v>
+        <v>2.6</v>
       </c>
       <c r="M147">
-        <v>3.75</v>
+        <v>2.9</v>
       </c>
       <c r="N147">
-        <v>7.5</v>
+        <v>2.6</v>
       </c>
       <c r="O147">
-        <v>1.5</v>
+        <v>3.3</v>
       </c>
       <c r="P147">
-        <v>3.4</v>
+        <v>3</v>
       </c>
       <c r="Q147">
-        <v>6.5</v>
+        <v>2.15</v>
       </c>
       <c r="R147">
-        <v>-1</v>
+        <v>0.25</v>
       </c>
       <c r="S147">
-        <v>1.975</v>
+        <v>1.9</v>
       </c>
       <c r="T147">
-        <v>1.825</v>
+        <v>1.9</v>
       </c>
       <c r="U147">
         <v>2</v>
@@ -14034,16 +14034,16 @@
         <v>-1</v>
       </c>
       <c r="Y147">
-        <v>2.4</v>
+        <v>2</v>
       </c>
       <c r="Z147">
         <v>-1</v>
       </c>
       <c r="AA147">
-        <v>-1</v>
+        <v>0.45</v>
       </c>
       <c r="AB147">
-        <v>0.825</v>
+        <v>-0.5</v>
       </c>
       <c r="AC147">
         <v>-1</v>
@@ -14057,7 +14057,7 @@
         <v>146</v>
       </c>
       <c r="B148">
-        <v>7590958</v>
+        <v>7624533</v>
       </c>
       <c r="C148" t="s">
         <v>29</v>
@@ -14066,10 +14066,10 @@
         <v>45314.54166666666</v>
       </c>
       <c r="E148" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="F148" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="G148">
         <v>0</v>
@@ -14087,31 +14087,31 @@
         <v>49</v>
       </c>
       <c r="L148">
-        <v>2.6</v>
+        <v>1.4</v>
       </c>
       <c r="M148">
-        <v>2.9</v>
+        <v>3.75</v>
       </c>
       <c r="N148">
-        <v>2.6</v>
+        <v>7.5</v>
       </c>
       <c r="O148">
-        <v>3.3</v>
+        <v>1.5</v>
       </c>
       <c r="P148">
-        <v>3</v>
+        <v>3.4</v>
       </c>
       <c r="Q148">
-        <v>2.15</v>
+        <v>6.5</v>
       </c>
       <c r="R148">
-        <v>0.25</v>
+        <v>-1</v>
       </c>
       <c r="S148">
-        <v>1.9</v>
+        <v>1.975</v>
       </c>
       <c r="T148">
-        <v>1.9</v>
+        <v>1.825</v>
       </c>
       <c r="U148">
         <v>2</v>
@@ -14126,16 +14126,16 @@
         <v>-1</v>
       </c>
       <c r="Y148">
-        <v>2</v>
+        <v>2.4</v>
       </c>
       <c r="Z148">
         <v>-1</v>
       </c>
       <c r="AA148">
-        <v>0.45</v>
+        <v>-1</v>
       </c>
       <c r="AB148">
-        <v>-0.5</v>
+        <v>0.825</v>
       </c>
       <c r="AC148">
         <v>-1</v>
@@ -14161,7 +14161,7 @@
         <v>33</v>
       </c>
       <c r="F149" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G149">
         <v>1</v>
@@ -14253,7 +14253,7 @@
         <v>38</v>
       </c>
       <c r="F150" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G150">
         <v>2</v>
@@ -14989,7 +14989,7 @@
         <v>36</v>
       </c>
       <c r="F158" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G158">
         <v>1</v>
@@ -15354,7 +15354,7 @@
         <v>45332.5</v>
       </c>
       <c r="E162" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F162" t="s">
         <v>34</v>
@@ -15725,7 +15725,7 @@
         <v>36</v>
       </c>
       <c r="F166" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G166">
         <v>1</v>
@@ -15897,7 +15897,7 @@
         <v>166</v>
       </c>
       <c r="B168">
-        <v>7768182</v>
+        <v>7768219</v>
       </c>
       <c r="C168" t="s">
         <v>29</v>
@@ -15906,82 +15906,82 @@
         <v>45338.47916666666</v>
       </c>
       <c r="E168" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F168" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G168">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H168">
         <v>0</v>
       </c>
       <c r="I168">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J168">
         <v>0</v>
       </c>
       <c r="K168" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="L168">
-        <v>2</v>
+        <v>1.833</v>
       </c>
       <c r="M168">
-        <v>2.9</v>
+        <v>3</v>
       </c>
       <c r="N168">
-        <v>3.75</v>
+        <v>4.2</v>
       </c>
       <c r="O168">
-        <v>2.375</v>
+        <v>1.833</v>
       </c>
       <c r="P168">
-        <v>2.9</v>
+        <v>2.8</v>
       </c>
       <c r="Q168">
-        <v>3</v>
+        <v>4.5</v>
       </c>
       <c r="R168">
-        <v>-0.25</v>
+        <v>-0.5</v>
       </c>
       <c r="S168">
-        <v>2.075</v>
+        <v>1.95</v>
       </c>
       <c r="T168">
-        <v>1.725</v>
+        <v>1.85</v>
       </c>
       <c r="U168">
         <v>1.75</v>
       </c>
       <c r="V168">
-        <v>1.75</v>
+        <v>1.975</v>
       </c>
       <c r="W168">
-        <v>2.05</v>
+        <v>1.825</v>
       </c>
       <c r="X168">
-        <v>1.375</v>
+        <v>-1</v>
       </c>
       <c r="Y168">
-        <v>-1</v>
+        <v>1.8</v>
       </c>
       <c r="Z168">
         <v>-1</v>
       </c>
       <c r="AA168">
-        <v>1.075</v>
+        <v>-1</v>
       </c>
       <c r="AB168">
-        <v>-1</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AC168">
         <v>-1</v>
       </c>
       <c r="AD168">
-        <v>1.05</v>
+        <v>0.825</v>
       </c>
     </row>
     <row r="169" spans="1:30">
@@ -15989,7 +15989,7 @@
         <v>167</v>
       </c>
       <c r="B169">
-        <v>7768219</v>
+        <v>7768182</v>
       </c>
       <c r="C169" t="s">
         <v>29</v>
@@ -15998,82 +15998,82 @@
         <v>45338.47916666666</v>
       </c>
       <c r="E169" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F169" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G169">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H169">
         <v>0</v>
       </c>
       <c r="I169">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J169">
         <v>0</v>
       </c>
       <c r="K169" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="L169">
-        <v>1.833</v>
+        <v>2</v>
       </c>
       <c r="M169">
+        <v>2.9</v>
+      </c>
+      <c r="N169">
+        <v>3.75</v>
+      </c>
+      <c r="O169">
+        <v>2.375</v>
+      </c>
+      <c r="P169">
+        <v>2.9</v>
+      </c>
+      <c r="Q169">
         <v>3</v>
       </c>
-      <c r="N169">
-        <v>4.2</v>
-      </c>
-      <c r="O169">
-        <v>1.833</v>
-      </c>
-      <c r="P169">
-        <v>2.8</v>
-      </c>
-      <c r="Q169">
-        <v>4.5</v>
-      </c>
       <c r="R169">
-        <v>-0.5</v>
+        <v>-0.25</v>
       </c>
       <c r="S169">
-        <v>1.95</v>
+        <v>2.075</v>
       </c>
       <c r="T169">
-        <v>1.85</v>
+        <v>1.725</v>
       </c>
       <c r="U169">
         <v>1.75</v>
       </c>
       <c r="V169">
-        <v>1.975</v>
+        <v>1.75</v>
       </c>
       <c r="W169">
-        <v>1.825</v>
+        <v>2.05</v>
       </c>
       <c r="X169">
-        <v>-1</v>
+        <v>1.375</v>
       </c>
       <c r="Y169">
-        <v>1.8</v>
+        <v>-1</v>
       </c>
       <c r="Z169">
         <v>-1</v>
       </c>
       <c r="AA169">
-        <v>-1</v>
+        <v>1.075</v>
       </c>
       <c r="AB169">
-        <v>0.8500000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AC169">
         <v>-1</v>
       </c>
       <c r="AD169">
-        <v>0.825</v>
+        <v>1.05</v>
       </c>
     </row>
     <row r="170" spans="1:30">
@@ -16369,7 +16369,7 @@
         <v>44</v>
       </c>
       <c r="F173" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G173">
         <v>2</v>
@@ -16918,7 +16918,7 @@
         <v>45346.53125</v>
       </c>
       <c r="E179" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F179" t="s">
         <v>32</v>
@@ -17286,7 +17286,7 @@
         <v>45353.54166666666</v>
       </c>
       <c r="E183" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F183" t="s">
         <v>39</v>
@@ -17381,7 +17381,7 @@
         <v>37</v>
       </c>
       <c r="F184" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G184">
         <v>2</v>
@@ -17746,7 +17746,7 @@
         <v>45366.75</v>
       </c>
       <c r="E188" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F188" t="s">
         <v>46</v>
@@ -18025,7 +18025,7 @@
         <v>43</v>
       </c>
       <c r="F191" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G191">
         <v>2</v>
@@ -18669,7 +18669,7 @@
         <v>41</v>
       </c>
       <c r="F198" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G198">
         <v>2</v>
@@ -19034,7 +19034,7 @@
         <v>45376.47916666666</v>
       </c>
       <c r="E202" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F202" t="s">
         <v>45</v>
@@ -19770,10 +19770,10 @@
         <v>45388.75</v>
       </c>
       <c r="E210" t="s">
+        <v>31</v>
+      </c>
+      <c r="F210" t="s">
         <v>30</v>
-      </c>
-      <c r="F210" t="s">
-        <v>31</v>
       </c>
       <c r="G210">
         <v>2</v>
@@ -19957,7 +19957,7 @@
         <v>40</v>
       </c>
       <c r="F212" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G212">
         <v>1</v>
@@ -20129,7 +20129,7 @@
         <v>212</v>
       </c>
       <c r="B214">
-        <v>8082744</v>
+        <v>8082743</v>
       </c>
       <c r="C214" t="s">
         <v>29</v>
@@ -20138,55 +20138,55 @@
         <v>45401.5</v>
       </c>
       <c r="E214" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F214" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="G214">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H214">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I214">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J214">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K214" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="L214">
-        <v>3.6</v>
+        <v>2</v>
       </c>
       <c r="M214">
-        <v>3</v>
+        <v>3.1</v>
       </c>
       <c r="N214">
-        <v>2</v>
+        <v>3.4</v>
       </c>
       <c r="O214">
-        <v>4.5</v>
+        <v>1.666</v>
       </c>
       <c r="P214">
-        <v>3</v>
+        <v>3.75</v>
       </c>
       <c r="Q214">
-        <v>1.833</v>
+        <v>4.333</v>
       </c>
       <c r="R214">
-        <v>0.5</v>
+        <v>-0.75</v>
       </c>
       <c r="S214">
-        <v>1.925</v>
+        <v>1.9</v>
       </c>
       <c r="T214">
-        <v>1.875</v>
+        <v>1.9</v>
       </c>
       <c r="U214">
-        <v>2</v>
+        <v>2.25</v>
       </c>
       <c r="V214">
         <v>2.025</v>
@@ -20198,22 +20198,22 @@
         <v>-1</v>
       </c>
       <c r="Y214">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="Z214">
-        <v>-1</v>
+        <v>3.333</v>
       </c>
       <c r="AA214">
-        <v>0.925</v>
+        <v>-1</v>
       </c>
       <c r="AB214">
-        <v>-1</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AC214">
-        <v>-1</v>
+        <v>1.025</v>
       </c>
       <c r="AD214">
-        <v>0.7749999999999999</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="215" spans="1:30">
@@ -20221,7 +20221,7 @@
         <v>213</v>
       </c>
       <c r="B215">
-        <v>8082743</v>
+        <v>8082744</v>
       </c>
       <c r="C215" t="s">
         <v>29</v>
@@ -20230,55 +20230,55 @@
         <v>45401.5</v>
       </c>
       <c r="E215" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="F215" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="G215">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H215">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I215">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J215">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K215" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="L215">
-        <v>2</v>
+        <v>3.6</v>
       </c>
       <c r="M215">
-        <v>3.1</v>
+        <v>3</v>
       </c>
       <c r="N215">
-        <v>3.4</v>
+        <v>2</v>
       </c>
       <c r="O215">
-        <v>1.666</v>
+        <v>4.5</v>
       </c>
       <c r="P215">
-        <v>3.75</v>
+        <v>3</v>
       </c>
       <c r="Q215">
-        <v>4.333</v>
+        <v>1.833</v>
       </c>
       <c r="R215">
-        <v>-0.75</v>
+        <v>0.5</v>
       </c>
       <c r="S215">
-        <v>1.9</v>
+        <v>1.925</v>
       </c>
       <c r="T215">
-        <v>1.9</v>
+        <v>1.875</v>
       </c>
       <c r="U215">
-        <v>2.25</v>
+        <v>2</v>
       </c>
       <c r="V215">
         <v>2.025</v>
@@ -20290,22 +20290,22 @@
         <v>-1</v>
       </c>
       <c r="Y215">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="Z215">
-        <v>3.333</v>
+        <v>-1</v>
       </c>
       <c r="AA215">
-        <v>-1</v>
+        <v>0.925</v>
       </c>
       <c r="AB215">
-        <v>0.8999999999999999</v>
+        <v>-1</v>
       </c>
       <c r="AC215">
-        <v>1.025</v>
+        <v>-1</v>
       </c>
       <c r="AD215">
-        <v>-1</v>
+        <v>0.7749999999999999</v>
       </c>
     </row>
     <row r="216" spans="1:30">
@@ -20414,7 +20414,7 @@
         <v>45402.5</v>
       </c>
       <c r="E217" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F217" t="s">
         <v>34</v>
@@ -20969,7 +20969,7 @@
         <v>44</v>
       </c>
       <c r="F223" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G223">
         <v>1</v>
@@ -21518,7 +21518,7 @@
         <v>45423.54166666666</v>
       </c>
       <c r="E229" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F229" t="s">
         <v>32</v>
@@ -21705,7 +21705,7 @@
         <v>35</v>
       </c>
       <c r="F231" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G231">
         <v>0</v>
@@ -22061,7 +22061,7 @@
         <v>233</v>
       </c>
       <c r="B235">
-        <v>8202020</v>
+        <v>8202016</v>
       </c>
       <c r="C235" t="s">
         <v>29</v>
@@ -22070,82 +22070,82 @@
         <v>45429.54166666666</v>
       </c>
       <c r="E235" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F235" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G235">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H235">
         <v>1</v>
       </c>
       <c r="I235">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J235">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K235" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="L235">
-        <v>2.25</v>
+        <v>1.666</v>
       </c>
       <c r="M235">
-        <v>3</v>
+        <v>3.25</v>
       </c>
       <c r="N235">
-        <v>3</v>
+        <v>4.75</v>
       </c>
       <c r="O235">
-        <v>1.6</v>
+        <v>1.533</v>
       </c>
       <c r="P235">
-        <v>3.1</v>
+        <v>3.6</v>
       </c>
       <c r="Q235">
-        <v>6</v>
+        <v>5.75</v>
       </c>
       <c r="R235">
-        <v>-0.75</v>
+        <v>-1</v>
       </c>
       <c r="S235">
+        <v>1.95</v>
+      </c>
+      <c r="T235">
         <v>1.85</v>
       </c>
-      <c r="T235">
-        <v>1.95</v>
-      </c>
       <c r="U235">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="V235">
-        <v>2.025</v>
+        <v>1.9</v>
       </c>
       <c r="W235">
-        <v>1.775</v>
+        <v>1.9</v>
       </c>
       <c r="X235">
-        <v>-1</v>
+        <v>0.5329999999999999</v>
       </c>
       <c r="Y235">
-        <v>2.1</v>
+        <v>-1</v>
       </c>
       <c r="Z235">
         <v>-1</v>
       </c>
       <c r="AA235">
-        <v>-1</v>
+        <v>0.95</v>
       </c>
       <c r="AB235">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
       <c r="AC235">
-        <v>0</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AD235">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="236" spans="1:30">
@@ -22153,7 +22153,7 @@
         <v>234</v>
       </c>
       <c r="B236">
-        <v>8202016</v>
+        <v>8202020</v>
       </c>
       <c r="C236" t="s">
         <v>29</v>
@@ -22162,82 +22162,82 @@
         <v>45429.54166666666</v>
       </c>
       <c r="E236" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F236" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G236">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H236">
         <v>1</v>
       </c>
       <c r="I236">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J236">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K236" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="L236">
-        <v>1.666</v>
+        <v>2.25</v>
       </c>
       <c r="M236">
-        <v>3.25</v>
+        <v>3</v>
       </c>
       <c r="N236">
-        <v>4.75</v>
+        <v>3</v>
       </c>
       <c r="O236">
-        <v>1.533</v>
+        <v>1.6</v>
       </c>
       <c r="P236">
-        <v>3.6</v>
+        <v>3.1</v>
       </c>
       <c r="Q236">
-        <v>5.75</v>
+        <v>6</v>
       </c>
       <c r="R236">
-        <v>-1</v>
+        <v>-0.75</v>
       </c>
       <c r="S236">
+        <v>1.85</v>
+      </c>
+      <c r="T236">
         <v>1.95</v>
       </c>
-      <c r="T236">
-        <v>1.85</v>
-      </c>
       <c r="U236">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="V236">
-        <v>1.9</v>
+        <v>2.025</v>
       </c>
       <c r="W236">
-        <v>1.9</v>
+        <v>1.775</v>
       </c>
       <c r="X236">
-        <v>0.5329999999999999</v>
+        <v>-1</v>
       </c>
       <c r="Y236">
-        <v>-1</v>
+        <v>2.1</v>
       </c>
       <c r="Z236">
         <v>-1</v>
       </c>
       <c r="AA236">
+        <v>-1</v>
+      </c>
+      <c r="AB236">
         <v>0.95</v>
       </c>
-      <c r="AB236">
-        <v>-1</v>
-      </c>
       <c r="AC236">
-        <v>0.8999999999999999</v>
+        <v>0</v>
       </c>
       <c r="AD236">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="237" spans="1:30">
@@ -22254,7 +22254,7 @@
         <v>45429.54166666666</v>
       </c>
       <c r="E237" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F237" t="s">
         <v>40</v>
@@ -22441,7 +22441,7 @@
         <v>37</v>
       </c>
       <c r="F239" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G239">
         <v>2</v>
@@ -23334,7 +23334,7 @@
         <v>45438.53125</v>
       </c>
       <c r="E249" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F249" t="s">
         <v>46</v>
@@ -23423,7 +23423,7 @@
         <v>39</v>
       </c>
       <c r="F250" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G250">
         <v>0</v>

</xml_diff>

<commit_message>
Atualização de bases das ligas, do dia: 19-06-2024 às 21:51
</commit_message>
<xml_diff>
--- a/Algeria Division 1/Algeria Division 1.xlsx
+++ b/Algeria Division 1/Algeria Division 1.xlsx
@@ -2189,7 +2189,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>6744018</v>
+        <v>6744005</v>
       </c>
       <c r="C19" t="s">
         <v>29</v>
@@ -2198,19 +2198,19 @@
         <v>45111.54166666666</v>
       </c>
       <c r="E19" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="F19" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="G19">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J19">
         <v>0</v>
@@ -2219,61 +2219,61 @@
         <v>47</v>
       </c>
       <c r="L19">
-        <v>2.2</v>
+        <v>1.615</v>
       </c>
       <c r="M19">
-        <v>2.875</v>
+        <v>3.4</v>
       </c>
       <c r="N19">
-        <v>3.2</v>
+        <v>5</v>
       </c>
       <c r="O19">
+        <v>1.4</v>
+      </c>
+      <c r="P19">
+        <v>3.75</v>
+      </c>
+      <c r="Q19">
+        <v>7.5</v>
+      </c>
+      <c r="R19">
+        <v>-1.25</v>
+      </c>
+      <c r="S19">
+        <v>2.05</v>
+      </c>
+      <c r="T19">
+        <v>1.75</v>
+      </c>
+      <c r="U19">
+        <v>2</v>
+      </c>
+      <c r="V19">
         <v>1.85</v>
       </c>
-      <c r="P19">
-        <v>2.9</v>
-      </c>
-      <c r="Q19">
-        <v>4.5</v>
-      </c>
-      <c r="R19">
+      <c r="W19">
+        <v>1.95</v>
+      </c>
+      <c r="X19">
+        <v>0.3999999999999999</v>
+      </c>
+      <c r="Y19">
+        <v>-1</v>
+      </c>
+      <c r="Z19">
+        <v>-1</v>
+      </c>
+      <c r="AA19">
         <v>-0.5</v>
       </c>
-      <c r="S19">
-        <v>1.9</v>
-      </c>
-      <c r="T19">
-        <v>1.9</v>
-      </c>
-      <c r="U19">
-        <v>1.75</v>
-      </c>
-      <c r="V19">
-        <v>1.825</v>
-      </c>
-      <c r="W19">
-        <v>1.975</v>
-      </c>
-      <c r="X19">
-        <v>0.8500000000000001</v>
-      </c>
-      <c r="Y19">
-        <v>-1</v>
-      </c>
-      <c r="Z19">
-        <v>-1</v>
-      </c>
-      <c r="AA19">
-        <v>0.8999999999999999</v>
-      </c>
       <c r="AB19">
-        <v>-1</v>
+        <v>0.375</v>
       </c>
       <c r="AC19">
-        <v>0.825</v>
+        <v>-1</v>
       </c>
       <c r="AD19">
-        <v>-1</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="20" spans="1:30">
@@ -2281,7 +2281,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>6744005</v>
+        <v>6743977</v>
       </c>
       <c r="C20" t="s">
         <v>29</v>
@@ -2290,82 +2290,82 @@
         <v>45111.54166666666</v>
       </c>
       <c r="E20" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="F20" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H20">
         <v>0</v>
       </c>
       <c r="I20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J20">
         <v>0</v>
       </c>
       <c r="K20" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="L20">
-        <v>1.615</v>
+        <v>1.444</v>
       </c>
       <c r="M20">
-        <v>3.4</v>
+        <v>3.6</v>
       </c>
       <c r="N20">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="O20">
-        <v>1.4</v>
+        <v>1.363</v>
       </c>
       <c r="P20">
-        <v>3.75</v>
+        <v>3.8</v>
       </c>
       <c r="Q20">
-        <v>7.5</v>
+        <v>8</v>
       </c>
       <c r="R20">
         <v>-1.25</v>
       </c>
       <c r="S20">
-        <v>2.05</v>
+        <v>2</v>
       </c>
       <c r="T20">
-        <v>1.75</v>
+        <v>1.8</v>
       </c>
       <c r="U20">
-        <v>2</v>
+        <v>2.25</v>
       </c>
       <c r="V20">
-        <v>1.85</v>
+        <v>1.875</v>
       </c>
       <c r="W20">
-        <v>1.95</v>
+        <v>1.925</v>
       </c>
       <c r="X20">
-        <v>0.3999999999999999</v>
+        <v>-1</v>
       </c>
       <c r="Y20">
-        <v>-1</v>
+        <v>2.8</v>
       </c>
       <c r="Z20">
         <v>-1</v>
       </c>
       <c r="AA20">
-        <v>-0.5</v>
+        <v>-1</v>
       </c>
       <c r="AB20">
-        <v>0.375</v>
+        <v>0.8</v>
       </c>
       <c r="AC20">
         <v>-1</v>
       </c>
       <c r="AD20">
-        <v>0.95</v>
+        <v>0.925</v>
       </c>
     </row>
     <row r="21" spans="1:30">
@@ -2373,7 +2373,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>6743977</v>
+        <v>6744018</v>
       </c>
       <c r="C21" t="s">
         <v>29</v>
@@ -2382,16 +2382,16 @@
         <v>45111.54166666666</v>
       </c>
       <c r="E21" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="F21" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G21">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I21">
         <v>0</v>
@@ -2400,64 +2400,64 @@
         <v>0</v>
       </c>
       <c r="K21" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="L21">
-        <v>1.444</v>
+        <v>2.2</v>
       </c>
       <c r="M21">
-        <v>3.6</v>
+        <v>2.875</v>
       </c>
       <c r="N21">
-        <v>7</v>
+        <v>3.2</v>
       </c>
       <c r="O21">
-        <v>1.363</v>
+        <v>1.85</v>
       </c>
       <c r="P21">
-        <v>3.8</v>
+        <v>2.9</v>
       </c>
       <c r="Q21">
-        <v>8</v>
+        <v>4.5</v>
       </c>
       <c r="R21">
-        <v>-1.25</v>
+        <v>-0.5</v>
       </c>
       <c r="S21">
-        <v>2</v>
+        <v>1.9</v>
       </c>
       <c r="T21">
-        <v>1.8</v>
+        <v>1.9</v>
       </c>
       <c r="U21">
-        <v>2.25</v>
+        <v>1.75</v>
       </c>
       <c r="V21">
-        <v>1.875</v>
+        <v>1.825</v>
       </c>
       <c r="W21">
-        <v>1.925</v>
+        <v>1.975</v>
       </c>
       <c r="X21">
-        <v>-1</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="Y21">
-        <v>2.8</v>
+        <v>-1</v>
       </c>
       <c r="Z21">
         <v>-1</v>
       </c>
       <c r="AA21">
-        <v>-1</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AB21">
-        <v>0.8</v>
+        <v>-1</v>
       </c>
       <c r="AC21">
-        <v>-1</v>
+        <v>0.825</v>
       </c>
       <c r="AD21">
-        <v>0.925</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="22" spans="1:30">
@@ -5593,7 +5593,7 @@
         <v>54</v>
       </c>
       <c r="B56">
-        <v>7230936</v>
+        <v>7230948</v>
       </c>
       <c r="C56" t="s">
         <v>29</v>
@@ -5602,10 +5602,10 @@
         <v>45198.48958333334</v>
       </c>
       <c r="E56" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F56" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="G56">
         <v>2</v>
@@ -5617,49 +5617,49 @@
         <v>0</v>
       </c>
       <c r="J56">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K56" t="s">
         <v>47</v>
       </c>
       <c r="L56">
-        <v>2</v>
+        <v>3.2</v>
       </c>
       <c r="M56">
-        <v>3</v>
+        <v>2.9</v>
       </c>
       <c r="N56">
-        <v>3.75</v>
+        <v>2.2</v>
       </c>
       <c r="O56">
-        <v>2</v>
+        <v>2.05</v>
       </c>
       <c r="P56">
         <v>3</v>
       </c>
       <c r="Q56">
-        <v>3.75</v>
+        <v>3.6</v>
       </c>
       <c r="R56">
         <v>-0.25</v>
       </c>
       <c r="S56">
-        <v>1.8</v>
+        <v>1.75</v>
       </c>
       <c r="T56">
-        <v>2</v>
+        <v>2.05</v>
       </c>
       <c r="U56">
         <v>1.75</v>
       </c>
       <c r="V56">
-        <v>1.825</v>
+        <v>1.9</v>
       </c>
       <c r="W56">
-        <v>1.975</v>
+        <v>1.9</v>
       </c>
       <c r="X56">
-        <v>1</v>
+        <v>1.05</v>
       </c>
       <c r="Y56">
         <v>-1</v>
@@ -5668,13 +5668,13 @@
         <v>-1</v>
       </c>
       <c r="AA56">
-        <v>0.8</v>
+        <v>0.75</v>
       </c>
       <c r="AB56">
         <v>-1</v>
       </c>
       <c r="AC56">
-        <v>0.825</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AD56">
         <v>-1</v>
@@ -5685,7 +5685,7 @@
         <v>55</v>
       </c>
       <c r="B57">
-        <v>7230948</v>
+        <v>7230934</v>
       </c>
       <c r="C57" t="s">
         <v>29</v>
@@ -5694,16 +5694,16 @@
         <v>45198.48958333334</v>
       </c>
       <c r="E57" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="F57" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="G57">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H57">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I57">
         <v>0</v>
@@ -5712,64 +5712,64 @@
         <v>0</v>
       </c>
       <c r="K57" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="L57">
         <v>3.2</v>
       </c>
       <c r="M57">
+        <v>2.8</v>
+      </c>
+      <c r="N57">
+        <v>2.25</v>
+      </c>
+      <c r="O57">
+        <v>1.95</v>
+      </c>
+      <c r="P57">
         <v>2.9</v>
       </c>
-      <c r="N57">
-        <v>2.2</v>
-      </c>
-      <c r="O57">
-        <v>2.05</v>
-      </c>
-      <c r="P57">
-        <v>3</v>
-      </c>
       <c r="Q57">
-        <v>3.6</v>
+        <v>3.75</v>
       </c>
       <c r="R57">
         <v>-0.25</v>
       </c>
       <c r="S57">
-        <v>1.75</v>
+        <v>1.775</v>
       </c>
       <c r="T57">
-        <v>2.05</v>
+        <v>2.025</v>
       </c>
       <c r="U57">
         <v>1.75</v>
       </c>
       <c r="V57">
+        <v>1.8</v>
+      </c>
+      <c r="W57">
+        <v>2</v>
+      </c>
+      <c r="X57">
+        <v>-1</v>
+      </c>
+      <c r="Y57">
         <v>1.9</v>
       </c>
-      <c r="W57">
-        <v>1.9</v>
-      </c>
-      <c r="X57">
-        <v>1.05</v>
-      </c>
-      <c r="Y57">
-        <v>-1</v>
-      </c>
       <c r="Z57">
         <v>-1</v>
       </c>
       <c r="AA57">
-        <v>0.75</v>
+        <v>-0.5</v>
       </c>
       <c r="AB57">
-        <v>-1</v>
+        <v>0.5125</v>
       </c>
       <c r="AC57">
-        <v>0.8999999999999999</v>
+        <v>-1</v>
       </c>
       <c r="AD57">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:30">
@@ -5777,7 +5777,7 @@
         <v>56</v>
       </c>
       <c r="B58">
-        <v>7230934</v>
+        <v>7230936</v>
       </c>
       <c r="C58" t="s">
         <v>29</v>
@@ -5786,40 +5786,40 @@
         <v>45198.48958333334</v>
       </c>
       <c r="E58" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="F58" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="G58">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H58">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I58">
         <v>0</v>
       </c>
       <c r="J58">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K58" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="L58">
-        <v>3.2</v>
+        <v>2</v>
       </c>
       <c r="M58">
-        <v>2.8</v>
+        <v>3</v>
       </c>
       <c r="N58">
-        <v>2.25</v>
+        <v>3.75</v>
       </c>
       <c r="O58">
-        <v>1.95</v>
+        <v>2</v>
       </c>
       <c r="P58">
-        <v>2.9</v>
+        <v>3</v>
       </c>
       <c r="Q58">
         <v>3.75</v>
@@ -5828,40 +5828,40 @@
         <v>-0.25</v>
       </c>
       <c r="S58">
-        <v>1.775</v>
+        <v>1.8</v>
       </c>
       <c r="T58">
-        <v>2.025</v>
+        <v>2</v>
       </c>
       <c r="U58">
         <v>1.75</v>
       </c>
       <c r="V58">
-        <v>1.8</v>
+        <v>1.825</v>
       </c>
       <c r="W58">
-        <v>2</v>
+        <v>1.975</v>
       </c>
       <c r="X58">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="Y58">
-        <v>1.9</v>
+        <v>-1</v>
       </c>
       <c r="Z58">
         <v>-1</v>
       </c>
       <c r="AA58">
-        <v>-0.5</v>
+        <v>0.8</v>
       </c>
       <c r="AB58">
-        <v>0.5125</v>
+        <v>-1</v>
       </c>
       <c r="AC58">
-        <v>-1</v>
+        <v>0.825</v>
       </c>
       <c r="AD58">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="59" spans="1:30">
@@ -10009,7 +10009,7 @@
         <v>102</v>
       </c>
       <c r="B104">
-        <v>7537791</v>
+        <v>7537790</v>
       </c>
       <c r="C104" t="s">
         <v>29</v>
@@ -10018,82 +10018,82 @@
         <v>45269.45833333334</v>
       </c>
       <c r="E104" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="F104" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="G104">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H104">
         <v>1</v>
       </c>
       <c r="I104">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J104">
         <v>0</v>
       </c>
       <c r="K104" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="L104">
-        <v>2.4</v>
+        <v>1.8</v>
       </c>
       <c r="M104">
-        <v>2.875</v>
+        <v>3</v>
       </c>
       <c r="N104">
-        <v>2.875</v>
+        <v>4.333</v>
       </c>
       <c r="O104">
-        <v>2.8</v>
+        <v>2.2</v>
       </c>
       <c r="P104">
         <v>2.875</v>
       </c>
       <c r="Q104">
-        <v>2.45</v>
+        <v>3.1</v>
       </c>
       <c r="R104">
-        <v>0</v>
+        <v>-0.25</v>
       </c>
       <c r="S104">
-        <v>2.05</v>
+        <v>2</v>
       </c>
       <c r="T104">
-        <v>1.75</v>
+        <v>1.8</v>
       </c>
       <c r="U104">
         <v>2</v>
       </c>
       <c r="V104">
-        <v>1.925</v>
+        <v>1.975</v>
       </c>
       <c r="W104">
+        <v>1.825</v>
+      </c>
+      <c r="X104">
+        <v>-1</v>
+      </c>
+      <c r="Y104">
         <v>1.875</v>
       </c>
-      <c r="X104">
-        <v>-1</v>
-      </c>
-      <c r="Y104">
-        <v>-1</v>
-      </c>
       <c r="Z104">
-        <v>1.45</v>
+        <v>-1</v>
       </c>
       <c r="AA104">
-        <v>-1</v>
+        <v>-0.5</v>
       </c>
       <c r="AB104">
-        <v>0.75</v>
+        <v>0.4</v>
       </c>
       <c r="AC104">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AD104">
-        <v>0.875</v>
+        <v>0</v>
       </c>
     </row>
     <row r="105" spans="1:30">
@@ -10101,7 +10101,7 @@
         <v>103</v>
       </c>
       <c r="B105">
-        <v>7537790</v>
+        <v>7537791</v>
       </c>
       <c r="C105" t="s">
         <v>29</v>
@@ -10110,82 +10110,82 @@
         <v>45269.45833333334</v>
       </c>
       <c r="E105" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="F105" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="G105">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H105">
         <v>1</v>
       </c>
       <c r="I105">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J105">
         <v>0</v>
       </c>
       <c r="K105" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="L105">
-        <v>1.8</v>
+        <v>2.4</v>
       </c>
       <c r="M105">
-        <v>3</v>
+        <v>2.875</v>
       </c>
       <c r="N105">
-        <v>4.333</v>
+        <v>2.875</v>
       </c>
       <c r="O105">
-        <v>2.2</v>
+        <v>2.8</v>
       </c>
       <c r="P105">
         <v>2.875</v>
       </c>
       <c r="Q105">
-        <v>3.1</v>
+        <v>2.45</v>
       </c>
       <c r="R105">
-        <v>-0.25</v>
+        <v>0</v>
       </c>
       <c r="S105">
-        <v>2</v>
+        <v>2.05</v>
       </c>
       <c r="T105">
-        <v>1.8</v>
+        <v>1.75</v>
       </c>
       <c r="U105">
         <v>2</v>
       </c>
       <c r="V105">
-        <v>1.975</v>
+        <v>1.925</v>
       </c>
       <c r="W105">
-        <v>1.825</v>
+        <v>1.875</v>
       </c>
       <c r="X105">
         <v>-1</v>
       </c>
       <c r="Y105">
-        <v>1.875</v>
+        <v>-1</v>
       </c>
       <c r="Z105">
-        <v>-1</v>
+        <v>1.45</v>
       </c>
       <c r="AA105">
-        <v>-0.5</v>
+        <v>-1</v>
       </c>
       <c r="AB105">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AC105">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AD105">
-        <v>0</v>
+        <v>0.875</v>
       </c>
     </row>
     <row r="106" spans="1:30">
@@ -11481,7 +11481,7 @@
         <v>118</v>
       </c>
       <c r="B120">
-        <v>7624498</v>
+        <v>7624597</v>
       </c>
       <c r="C120" t="s">
         <v>29</v>
@@ -11490,82 +11490,82 @@
         <v>45289.58333333334</v>
       </c>
       <c r="E120" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F120" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G120">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H120">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I120">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J120">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K120" t="s">
         <v>49</v>
       </c>
       <c r="L120">
-        <v>1.45</v>
+        <v>3.4</v>
       </c>
       <c r="M120">
-        <v>3.9</v>
+        <v>3.2</v>
       </c>
       <c r="N120">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="O120">
-        <v>1.45</v>
+        <v>3.4</v>
       </c>
       <c r="P120">
-        <v>3.8</v>
+        <v>2.9</v>
       </c>
       <c r="Q120">
-        <v>6.5</v>
+        <v>2.15</v>
       </c>
       <c r="R120">
-        <v>-1</v>
+        <v>0.25</v>
       </c>
       <c r="S120">
-        <v>1.775</v>
+        <v>1.925</v>
       </c>
       <c r="T120">
-        <v>2.025</v>
+        <v>1.875</v>
       </c>
       <c r="U120">
         <v>2</v>
       </c>
       <c r="V120">
-        <v>1.75</v>
+        <v>1.95</v>
       </c>
       <c r="W120">
-        <v>2.05</v>
+        <v>1.85</v>
       </c>
       <c r="X120">
         <v>-1</v>
       </c>
       <c r="Y120">
-        <v>2.8</v>
+        <v>1.9</v>
       </c>
       <c r="Z120">
         <v>-1</v>
       </c>
       <c r="AA120">
-        <v>-1</v>
+        <v>0.4625</v>
       </c>
       <c r="AB120">
-        <v>1.025</v>
+        <v>-0.5</v>
       </c>
       <c r="AC120">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AD120">
-        <v>0</v>
+        <v>0.8500000000000001</v>
       </c>
     </row>
     <row r="121" spans="1:30">
@@ -11573,7 +11573,7 @@
         <v>119</v>
       </c>
       <c r="B121">
-        <v>7624597</v>
+        <v>7624498</v>
       </c>
       <c r="C121" t="s">
         <v>29</v>
@@ -11582,82 +11582,82 @@
         <v>45289.58333333334</v>
       </c>
       <c r="E121" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="F121" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G121">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H121">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I121">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J121">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K121" t="s">
         <v>49</v>
       </c>
       <c r="L121">
-        <v>3.4</v>
+        <v>1.45</v>
       </c>
       <c r="M121">
-        <v>3.2</v>
+        <v>3.9</v>
       </c>
       <c r="N121">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="O121">
-        <v>3.4</v>
+        <v>1.45</v>
       </c>
       <c r="P121">
-        <v>2.9</v>
+        <v>3.8</v>
       </c>
       <c r="Q121">
-        <v>2.15</v>
+        <v>6.5</v>
       </c>
       <c r="R121">
-        <v>0.25</v>
+        <v>-1</v>
       </c>
       <c r="S121">
-        <v>1.925</v>
+        <v>1.775</v>
       </c>
       <c r="T121">
-        <v>1.875</v>
+        <v>2.025</v>
       </c>
       <c r="U121">
         <v>2</v>
       </c>
       <c r="V121">
-        <v>1.95</v>
+        <v>1.75</v>
       </c>
       <c r="W121">
-        <v>1.85</v>
+        <v>2.05</v>
       </c>
       <c r="X121">
         <v>-1</v>
       </c>
       <c r="Y121">
-        <v>1.9</v>
+        <v>2.8</v>
       </c>
       <c r="Z121">
         <v>-1</v>
       </c>
       <c r="AA121">
-        <v>0.4625</v>
+        <v>-1</v>
       </c>
       <c r="AB121">
-        <v>-0.5</v>
+        <v>1.025</v>
       </c>
       <c r="AC121">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AD121">
-        <v>0.8500000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="122" spans="1:30">
@@ -15437,7 +15437,7 @@
         <v>161</v>
       </c>
       <c r="B163">
-        <v>7768216</v>
+        <v>7768215</v>
       </c>
       <c r="C163" t="s">
         <v>29</v>
@@ -15446,64 +15446,64 @@
         <v>45332.5</v>
       </c>
       <c r="E163" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="F163" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="G163">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H163">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I163">
         <v>0</v>
       </c>
       <c r="J163">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K163" t="s">
         <v>47</v>
       </c>
       <c r="L163">
-        <v>2.375</v>
+        <v>1.5</v>
       </c>
       <c r="M163">
-        <v>2.75</v>
+        <v>3.4</v>
       </c>
       <c r="N163">
-        <v>3.1</v>
+        <v>6.5</v>
       </c>
       <c r="O163">
-        <v>2.5</v>
+        <v>1.4</v>
       </c>
       <c r="P163">
-        <v>2.625</v>
+        <v>3.6</v>
       </c>
       <c r="Q163">
-        <v>3.1</v>
+        <v>10</v>
       </c>
       <c r="R163">
-        <v>0</v>
+        <v>-1.25</v>
       </c>
       <c r="S163">
-        <v>1.7</v>
+        <v>2</v>
       </c>
       <c r="T163">
-        <v>2.1</v>
+        <v>1.8</v>
       </c>
       <c r="U163">
-        <v>1.75</v>
+        <v>2</v>
       </c>
       <c r="V163">
+        <v>1.85</v>
+      </c>
+      <c r="W163">
         <v>1.95</v>
       </c>
-      <c r="W163">
-        <v>1.85</v>
-      </c>
       <c r="X163">
-        <v>1.5</v>
+        <v>0.3999999999999999</v>
       </c>
       <c r="Y163">
         <v>-1</v>
@@ -15512,16 +15512,16 @@
         <v>-1</v>
       </c>
       <c r="AA163">
-        <v>0.7</v>
+        <v>-0.5</v>
       </c>
       <c r="AB163">
-        <v>-1</v>
+        <v>0.4</v>
       </c>
       <c r="AC163">
+        <v>-1</v>
+      </c>
+      <c r="AD163">
         <v>0.95</v>
-      </c>
-      <c r="AD163">
-        <v>-1</v>
       </c>
     </row>
     <row r="164" spans="1:30">
@@ -15529,7 +15529,7 @@
         <v>162</v>
       </c>
       <c r="B164">
-        <v>7768215</v>
+        <v>7768216</v>
       </c>
       <c r="C164" t="s">
         <v>29</v>
@@ -15538,65 +15538,65 @@
         <v>45332.5</v>
       </c>
       <c r="E164" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="F164" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="G164">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H164">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I164">
         <v>0</v>
       </c>
       <c r="J164">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K164" t="s">
         <v>47</v>
       </c>
       <c r="L164">
+        <v>2.375</v>
+      </c>
+      <c r="M164">
+        <v>2.75</v>
+      </c>
+      <c r="N164">
+        <v>3.1</v>
+      </c>
+      <c r="O164">
+        <v>2.5</v>
+      </c>
+      <c r="P164">
+        <v>2.625</v>
+      </c>
+      <c r="Q164">
+        <v>3.1</v>
+      </c>
+      <c r="R164">
+        <v>0</v>
+      </c>
+      <c r="S164">
+        <v>1.7</v>
+      </c>
+      <c r="T164">
+        <v>2.1</v>
+      </c>
+      <c r="U164">
+        <v>1.75</v>
+      </c>
+      <c r="V164">
+        <v>1.95</v>
+      </c>
+      <c r="W164">
+        <v>1.85</v>
+      </c>
+      <c r="X164">
         <v>1.5</v>
       </c>
-      <c r="M164">
-        <v>3.4</v>
-      </c>
-      <c r="N164">
-        <v>6.5</v>
-      </c>
-      <c r="O164">
-        <v>1.4</v>
-      </c>
-      <c r="P164">
-        <v>3.6</v>
-      </c>
-      <c r="Q164">
-        <v>10</v>
-      </c>
-      <c r="R164">
-        <v>-1.25</v>
-      </c>
-      <c r="S164">
-        <v>2</v>
-      </c>
-      <c r="T164">
-        <v>1.8</v>
-      </c>
-      <c r="U164">
-        <v>2</v>
-      </c>
-      <c r="V164">
-        <v>1.85</v>
-      </c>
-      <c r="W164">
-        <v>1.95</v>
-      </c>
-      <c r="X164">
-        <v>0.3999999999999999</v>
-      </c>
       <c r="Y164">
         <v>-1</v>
       </c>
@@ -15604,16 +15604,16 @@
         <v>-1</v>
       </c>
       <c r="AA164">
-        <v>-0.5</v>
+        <v>0.7</v>
       </c>
       <c r="AB164">
-        <v>0.4</v>
+        <v>-1</v>
       </c>
       <c r="AC164">
-        <v>-1</v>
+        <v>0.95</v>
       </c>
       <c r="AD164">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="165" spans="1:30">
@@ -19393,7 +19393,7 @@
         <v>204</v>
       </c>
       <c r="B206">
-        <v>8007205</v>
+        <v>8007204</v>
       </c>
       <c r="C206" t="s">
         <v>29</v>
@@ -19402,55 +19402,55 @@
         <v>45387.75</v>
       </c>
       <c r="E206" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="F206" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G206">
         <v>1</v>
       </c>
       <c r="H206">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I206">
         <v>0</v>
       </c>
       <c r="J206">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K206" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L206">
-        <v>1.571</v>
+        <v>2</v>
       </c>
       <c r="M206">
+        <v>3</v>
+      </c>
+      <c r="N206">
         <v>3.6</v>
       </c>
-      <c r="N206">
-        <v>5</v>
-      </c>
       <c r="O206">
-        <v>1.85</v>
+        <v>2.375</v>
       </c>
       <c r="P206">
-        <v>3.3</v>
+        <v>2.625</v>
       </c>
       <c r="Q206">
-        <v>3.6</v>
+        <v>3.4</v>
       </c>
       <c r="R206">
-        <v>-0.5</v>
+        <v>-0.25</v>
       </c>
       <c r="S206">
-        <v>2</v>
+        <v>2.025</v>
       </c>
       <c r="T206">
-        <v>1.8</v>
+        <v>1.775</v>
       </c>
       <c r="U206">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="V206">
         <v>1.775</v>
@@ -19459,25 +19459,25 @@
         <v>2.025</v>
       </c>
       <c r="X206">
-        <v>-1</v>
+        <v>1.375</v>
       </c>
       <c r="Y206">
         <v>-1</v>
       </c>
       <c r="Z206">
-        <v>2.6</v>
+        <v>-1</v>
       </c>
       <c r="AA206">
-        <v>-1</v>
+        <v>1.025</v>
       </c>
       <c r="AB206">
-        <v>0.8</v>
+        <v>-1</v>
       </c>
       <c r="AC206">
-        <v>0.7749999999999999</v>
+        <v>-1</v>
       </c>
       <c r="AD206">
-        <v>-1</v>
+        <v>1.025</v>
       </c>
     </row>
     <row r="207" spans="1:30">
@@ -19577,7 +19577,7 @@
         <v>206</v>
       </c>
       <c r="B208">
-        <v>8007204</v>
+        <v>8007205</v>
       </c>
       <c r="C208" t="s">
         <v>29</v>
@@ -19586,55 +19586,55 @@
         <v>45387.75</v>
       </c>
       <c r="E208" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="F208" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G208">
         <v>1</v>
       </c>
       <c r="H208">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I208">
         <v>0</v>
       </c>
       <c r="J208">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K208" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="L208">
-        <v>2</v>
+        <v>1.571</v>
       </c>
       <c r="M208">
-        <v>3</v>
+        <v>3.6</v>
       </c>
       <c r="N208">
+        <v>5</v>
+      </c>
+      <c r="O208">
+        <v>1.85</v>
+      </c>
+      <c r="P208">
+        <v>3.3</v>
+      </c>
+      <c r="Q208">
         <v>3.6</v>
       </c>
-      <c r="O208">
-        <v>2.375</v>
-      </c>
-      <c r="P208">
-        <v>2.625</v>
-      </c>
-      <c r="Q208">
-        <v>3.4</v>
-      </c>
       <c r="R208">
-        <v>-0.25</v>
+        <v>-0.5</v>
       </c>
       <c r="S208">
-        <v>2.025</v>
+        <v>2</v>
       </c>
       <c r="T208">
-        <v>1.775</v>
+        <v>1.8</v>
       </c>
       <c r="U208">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="V208">
         <v>1.775</v>
@@ -19643,25 +19643,25 @@
         <v>2.025</v>
       </c>
       <c r="X208">
-        <v>1.375</v>
+        <v>-1</v>
       </c>
       <c r="Y208">
         <v>-1</v>
       </c>
       <c r="Z208">
-        <v>-1</v>
+        <v>2.6</v>
       </c>
       <c r="AA208">
-        <v>1.025</v>
+        <v>-1</v>
       </c>
       <c r="AB208">
-        <v>-1</v>
+        <v>0.8</v>
       </c>
       <c r="AC208">
-        <v>-1</v>
+        <v>0.7749999999999999</v>
       </c>
       <c r="AD208">
-        <v>1.025</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="209" spans="1:30">
@@ -21601,7 +21601,7 @@
         <v>228</v>
       </c>
       <c r="B230">
-        <v>8184370</v>
+        <v>8184371</v>
       </c>
       <c r="C230" t="s">
         <v>29</v>
@@ -21610,13 +21610,13 @@
         <v>45423.54166666666</v>
       </c>
       <c r="E230" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="F230" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="G230">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H230">
         <v>0</v>
@@ -21628,64 +21628,64 @@
         <v>0</v>
       </c>
       <c r="K230" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="L230">
-        <v>2</v>
+        <v>2.3</v>
       </c>
       <c r="M230">
-        <v>3.1</v>
+        <v>3.2</v>
       </c>
       <c r="N230">
-        <v>3.4</v>
+        <v>2.75</v>
       </c>
       <c r="O230">
-        <v>2.25</v>
+        <v>2.45</v>
       </c>
       <c r="P230">
+        <v>2.9</v>
+      </c>
+      <c r="Q230">
         <v>2.8</v>
       </c>
-      <c r="Q230">
-        <v>3.1</v>
-      </c>
       <c r="R230">
-        <v>-0.25</v>
+        <v>0</v>
       </c>
       <c r="S230">
-        <v>1.975</v>
+        <v>1.75</v>
       </c>
       <c r="T230">
-        <v>1.825</v>
+        <v>2.05</v>
       </c>
       <c r="U230">
         <v>2</v>
       </c>
       <c r="V230">
-        <v>2</v>
+        <v>1.8</v>
       </c>
       <c r="W230">
-        <v>1.8</v>
+        <v>2</v>
       </c>
       <c r="X230">
-        <v>1.25</v>
+        <v>-1</v>
       </c>
       <c r="Y230">
-        <v>-1</v>
+        <v>1.9</v>
       </c>
       <c r="Z230">
         <v>-1</v>
       </c>
       <c r="AA230">
-        <v>0.9750000000000001</v>
+        <v>0</v>
       </c>
       <c r="AB230">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AC230">
         <v>-1</v>
       </c>
       <c r="AD230">
-        <v>0.8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="231" spans="1:30">
@@ -21785,7 +21785,7 @@
         <v>230</v>
       </c>
       <c r="B232">
-        <v>8184371</v>
+        <v>8184370</v>
       </c>
       <c r="C232" t="s">
         <v>29</v>
@@ -21794,13 +21794,13 @@
         <v>45423.54166666666</v>
       </c>
       <c r="E232" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="F232" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="G232">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H232">
         <v>0</v>
@@ -21812,64 +21812,64 @@
         <v>0</v>
       </c>
       <c r="K232" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="L232">
-        <v>2.3</v>
+        <v>2</v>
       </c>
       <c r="M232">
-        <v>3.2</v>
+        <v>3.1</v>
       </c>
       <c r="N232">
-        <v>2.75</v>
+        <v>3.4</v>
       </c>
       <c r="O232">
-        <v>2.45</v>
+        <v>2.25</v>
       </c>
       <c r="P232">
-        <v>2.9</v>
+        <v>2.8</v>
       </c>
       <c r="Q232">
-        <v>2.8</v>
+        <v>3.1</v>
       </c>
       <c r="R232">
-        <v>0</v>
+        <v>-0.25</v>
       </c>
       <c r="S232">
-        <v>1.75</v>
+        <v>1.975</v>
       </c>
       <c r="T232">
-        <v>2.05</v>
+        <v>1.825</v>
       </c>
       <c r="U232">
         <v>2</v>
       </c>
       <c r="V232">
+        <v>2</v>
+      </c>
+      <c r="W232">
         <v>1.8</v>
       </c>
-      <c r="W232">
-        <v>2</v>
-      </c>
       <c r="X232">
-        <v>-1</v>
+        <v>1.25</v>
       </c>
       <c r="Y232">
-        <v>1.9</v>
+        <v>-1</v>
       </c>
       <c r="Z232">
         <v>-1</v>
       </c>
       <c r="AA232">
-        <v>0</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="AB232">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AC232">
         <v>-1</v>
       </c>
       <c r="AD232">
-        <v>1</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="233" spans="1:30">
@@ -21877,7 +21877,7 @@
         <v>231</v>
       </c>
       <c r="B233">
-        <v>8184368</v>
+        <v>8184338</v>
       </c>
       <c r="C233" t="s">
         <v>29</v>
@@ -21886,67 +21886,67 @@
         <v>45423.54166666666</v>
       </c>
       <c r="E233" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="F233" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G233">
         <v>1</v>
       </c>
       <c r="H233">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I233">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J233">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K233" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="L233">
-        <v>3.5</v>
+        <v>1.615</v>
       </c>
       <c r="M233">
-        <v>3.3</v>
+        <v>3.4</v>
       </c>
       <c r="N233">
-        <v>1.909</v>
+        <v>5</v>
       </c>
       <c r="O233">
-        <v>2.7</v>
+        <v>1.5</v>
       </c>
       <c r="P233">
-        <v>3</v>
+        <v>3.8</v>
       </c>
       <c r="Q233">
-        <v>2.4</v>
+        <v>5.5</v>
       </c>
       <c r="R233">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="S233">
-        <v>2.025</v>
+        <v>1.9</v>
       </c>
       <c r="T233">
-        <v>1.775</v>
+        <v>1.9</v>
       </c>
       <c r="U233">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="V233">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="W233">
-        <v>1.925</v>
+        <v>1.85</v>
       </c>
       <c r="X233">
-        <v>-1</v>
+        <v>0.5</v>
       </c>
       <c r="Y233">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="Z233">
         <v>-1</v>
@@ -21958,10 +21958,10 @@
         <v>0</v>
       </c>
       <c r="AC233">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AD233">
-        <v>0</v>
+        <v>0.8500000000000001</v>
       </c>
     </row>
     <row r="234" spans="1:30">
@@ -21969,7 +21969,7 @@
         <v>232</v>
       </c>
       <c r="B234">
-        <v>8184338</v>
+        <v>8184368</v>
       </c>
       <c r="C234" t="s">
         <v>29</v>
@@ -21978,67 +21978,67 @@
         <v>45423.54166666666</v>
       </c>
       <c r="E234" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="F234" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G234">
         <v>1</v>
       </c>
       <c r="H234">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I234">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J234">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K234" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="L234">
-        <v>1.615</v>
+        <v>3.5</v>
       </c>
       <c r="M234">
-        <v>3.4</v>
+        <v>3.3</v>
       </c>
       <c r="N234">
-        <v>5</v>
+        <v>1.909</v>
       </c>
       <c r="O234">
-        <v>1.5</v>
+        <v>2.7</v>
       </c>
       <c r="P234">
-        <v>3.8</v>
+        <v>3</v>
       </c>
       <c r="Q234">
-        <v>5.5</v>
+        <v>2.4</v>
       </c>
       <c r="R234">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="S234">
-        <v>1.9</v>
+        <v>2.025</v>
       </c>
       <c r="T234">
-        <v>1.9</v>
+        <v>1.775</v>
       </c>
       <c r="U234">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="V234">
-        <v>1.95</v>
+        <v>1.875</v>
       </c>
       <c r="W234">
-        <v>1.85</v>
+        <v>1.925</v>
       </c>
       <c r="X234">
-        <v>0.5</v>
+        <v>-1</v>
       </c>
       <c r="Y234">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="Z234">
         <v>-1</v>
@@ -22050,10 +22050,10 @@
         <v>0</v>
       </c>
       <c r="AC234">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AD234">
-        <v>0.8500000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="235" spans="1:30">

</xml_diff>

<commit_message>
Atualização de bases das ligas, do dia: 28-06-2024 às 19:47
</commit_message>
<xml_diff>
--- a/Algeria Division 1/Algeria Division 1.xlsx
+++ b/Algeria Division 1/Algeria Division 1.xlsx
@@ -112,16 +112,16 @@
     <t>CS Constantine</t>
   </si>
   <si>
-    <t>JS Kabylie</t>
+    <t>ASO Chlef</t>
+  </si>
+  <si>
+    <t>USM Khenchela</t>
   </si>
   <si>
     <t>MC El Bayadh</t>
   </si>
   <si>
-    <t>USM Khenchela</t>
-  </si>
-  <si>
-    <t>ASO Chlef</t>
+    <t>JS Kabylie</t>
   </si>
   <si>
     <t>USM Alger</t>
@@ -139,13 +139,13 @@
     <t>CR Belouizdad</t>
   </si>
   <si>
-    <t>MC Oran</t>
+    <t>NC Magra</t>
   </si>
   <si>
     <t>RC Arba</t>
   </si>
   <si>
-    <t>NC Magra</t>
+    <t>MC Oran</t>
   </si>
   <si>
     <t>MC Alger</t>
@@ -637,7 +637,7 @@
         <v>30</v>
       </c>
       <c r="F2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="G2">
         <v>4</v>
@@ -809,7 +809,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>6687020</v>
+        <v>6687387</v>
       </c>
       <c r="C4" t="s">
         <v>29</v>
@@ -821,79 +821,79 @@
         <v>32</v>
       </c>
       <c r="F4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="L4">
-        <v>1.666</v>
+        <v>1.5</v>
       </c>
       <c r="M4">
-        <v>3</v>
+        <v>3.6</v>
       </c>
       <c r="N4">
-        <v>6</v>
+        <v>6.5</v>
       </c>
       <c r="O4">
-        <v>1.666</v>
+        <v>1.5</v>
       </c>
       <c r="P4">
-        <v>3</v>
+        <v>3.6</v>
       </c>
       <c r="Q4">
-        <v>6</v>
+        <v>6.5</v>
       </c>
       <c r="R4">
-        <v>-0.5</v>
+        <v>-1</v>
       </c>
       <c r="S4">
-        <v>1.8</v>
+        <v>1.95</v>
       </c>
       <c r="T4">
-        <v>2</v>
+        <v>1.85</v>
       </c>
       <c r="U4">
-        <v>1.75</v>
+        <v>2.25</v>
       </c>
       <c r="V4">
-        <v>1.95</v>
+        <v>2.025</v>
       </c>
       <c r="W4">
-        <v>1.85</v>
+        <v>1.775</v>
       </c>
       <c r="X4">
-        <v>0.6659999999999999</v>
+        <v>-1</v>
       </c>
       <c r="Y4">
         <v>-1</v>
       </c>
       <c r="Z4">
-        <v>-1</v>
+        <v>5.5</v>
       </c>
       <c r="AA4">
-        <v>0.8</v>
+        <v>-1</v>
       </c>
       <c r="AB4">
-        <v>-1</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AC4">
-        <v>0.475</v>
+        <v>-1</v>
       </c>
       <c r="AD4">
-        <v>-0.5</v>
+        <v>0.7749999999999999</v>
       </c>
     </row>
     <row r="5" spans="1:30">
@@ -901,7 +901,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>6687019</v>
+        <v>6687390</v>
       </c>
       <c r="C5" t="s">
         <v>29</v>
@@ -913,49 +913,49 @@
         <v>33</v>
       </c>
       <c r="F5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H5">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="L5">
-        <v>3.1</v>
+        <v>1.95</v>
       </c>
       <c r="M5">
-        <v>2.8</v>
+        <v>2.875</v>
       </c>
       <c r="N5">
-        <v>2.4</v>
+        <v>4</v>
       </c>
       <c r="O5">
-        <v>3</v>
+        <v>2.05</v>
       </c>
       <c r="P5">
         <v>2.9</v>
       </c>
       <c r="Q5">
-        <v>2.45</v>
+        <v>3.8</v>
       </c>
       <c r="R5">
-        <v>0</v>
+        <v>-0.5</v>
       </c>
       <c r="S5">
-        <v>2.05</v>
+        <v>2</v>
       </c>
       <c r="T5">
-        <v>1.75</v>
+        <v>1.8</v>
       </c>
       <c r="U5">
         <v>1.75</v>
@@ -970,22 +970,22 @@
         <v>-1</v>
       </c>
       <c r="Y5">
-        <v>-1</v>
+        <v>1.9</v>
       </c>
       <c r="Z5">
-        <v>1.45</v>
+        <v>-1</v>
       </c>
       <c r="AA5">
         <v>-1</v>
       </c>
       <c r="AB5">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="AC5">
-        <v>0.8</v>
+        <v>-1</v>
       </c>
       <c r="AD5">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:30">
@@ -993,7 +993,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>6687390</v>
+        <v>6687019</v>
       </c>
       <c r="C6" t="s">
         <v>29</v>
@@ -1005,49 +1005,49 @@
         <v>34</v>
       </c>
       <c r="F6" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="L6">
-        <v>1.95</v>
+        <v>3.1</v>
       </c>
       <c r="M6">
-        <v>2.875</v>
+        <v>2.8</v>
       </c>
       <c r="N6">
-        <v>4</v>
+        <v>2.4</v>
       </c>
       <c r="O6">
-        <v>2.05</v>
+        <v>3</v>
       </c>
       <c r="P6">
         <v>2.9</v>
       </c>
       <c r="Q6">
-        <v>3.8</v>
+        <v>2.45</v>
       </c>
       <c r="R6">
-        <v>-0.5</v>
+        <v>0</v>
       </c>
       <c r="S6">
-        <v>2</v>
+        <v>2.05</v>
       </c>
       <c r="T6">
-        <v>1.8</v>
+        <v>1.75</v>
       </c>
       <c r="U6">
         <v>1.75</v>
@@ -1062,22 +1062,22 @@
         <v>-1</v>
       </c>
       <c r="Y6">
-        <v>1.9</v>
+        <v>-1</v>
       </c>
       <c r="Z6">
-        <v>-1</v>
+        <v>1.45</v>
       </c>
       <c r="AA6">
         <v>-1</v>
       </c>
       <c r="AB6">
+        <v>0.75</v>
+      </c>
+      <c r="AC6">
         <v>0.8</v>
       </c>
-      <c r="AC6">
-        <v>-1</v>
-      </c>
       <c r="AD6">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="7" spans="1:30">
@@ -1085,7 +1085,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>6687387</v>
+        <v>6687020</v>
       </c>
       <c r="C7" t="s">
         <v>29</v>
@@ -1097,79 +1097,79 @@
         <v>35</v>
       </c>
       <c r="F7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L7">
-        <v>1.5</v>
+        <v>1.666</v>
       </c>
       <c r="M7">
-        <v>3.6</v>
+        <v>3</v>
       </c>
       <c r="N7">
-        <v>6.5</v>
+        <v>6</v>
       </c>
       <c r="O7">
-        <v>1.5</v>
+        <v>1.666</v>
       </c>
       <c r="P7">
-        <v>3.6</v>
+        <v>3</v>
       </c>
       <c r="Q7">
-        <v>6.5</v>
+        <v>6</v>
       </c>
       <c r="R7">
-        <v>-1</v>
+        <v>-0.5</v>
       </c>
       <c r="S7">
+        <v>1.8</v>
+      </c>
+      <c r="T7">
+        <v>2</v>
+      </c>
+      <c r="U7">
+        <v>1.75</v>
+      </c>
+      <c r="V7">
         <v>1.95</v>
       </c>
-      <c r="T7">
+      <c r="W7">
         <v>1.85</v>
       </c>
-      <c r="U7">
-        <v>2.25</v>
-      </c>
-      <c r="V7">
-        <v>2.025</v>
-      </c>
-      <c r="W7">
-        <v>1.775</v>
-      </c>
       <c r="X7">
-        <v>-1</v>
+        <v>0.6659999999999999</v>
       </c>
       <c r="Y7">
         <v>-1</v>
       </c>
       <c r="Z7">
-        <v>5.5</v>
+        <v>-1</v>
       </c>
       <c r="AA7">
-        <v>-1</v>
+        <v>0.8</v>
       </c>
       <c r="AB7">
-        <v>0.8500000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AC7">
-        <v>-1</v>
+        <v>0.475</v>
       </c>
       <c r="AD7">
-        <v>0.7749999999999999</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="8" spans="1:30">
@@ -1281,7 +1281,7 @@
         <v>36</v>
       </c>
       <c r="F9" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="G9">
         <v>0</v>
@@ -1649,7 +1649,7 @@
         <v>39</v>
       </c>
       <c r="F13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G13">
         <v>1</v>
@@ -1741,7 +1741,7 @@
         <v>40</v>
       </c>
       <c r="F14" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G14">
         <v>1</v>
@@ -1821,7 +1821,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>6765585</v>
+        <v>6765583</v>
       </c>
       <c r="C15" t="s">
         <v>29</v>
@@ -1833,79 +1833,79 @@
         <v>41</v>
       </c>
       <c r="F15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H15">
         <v>1</v>
       </c>
       <c r="I15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="L15">
-        <v>2</v>
+        <v>2.8</v>
       </c>
       <c r="M15">
         <v>2.8</v>
       </c>
       <c r="N15">
-        <v>4</v>
+        <v>2.55</v>
       </c>
       <c r="O15">
-        <v>2.05</v>
+        <v>2</v>
       </c>
       <c r="P15">
-        <v>2.7</v>
+        <v>3</v>
       </c>
       <c r="Q15">
-        <v>4</v>
+        <v>3.75</v>
       </c>
       <c r="R15">
         <v>-0.25</v>
       </c>
       <c r="S15">
+        <v>1.725</v>
+      </c>
+      <c r="T15">
+        <v>2.075</v>
+      </c>
+      <c r="U15">
+        <v>2</v>
+      </c>
+      <c r="V15">
+        <v>2.05</v>
+      </c>
+      <c r="W15">
         <v>1.75</v>
       </c>
-      <c r="T15">
-        <v>2.05</v>
-      </c>
-      <c r="U15">
-        <v>1.75</v>
-      </c>
-      <c r="V15">
-        <v>1.875</v>
-      </c>
-      <c r="W15">
-        <v>1.925</v>
-      </c>
       <c r="X15">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="Y15">
-        <v>1.7</v>
+        <v>-1</v>
       </c>
       <c r="Z15">
         <v>-1</v>
       </c>
       <c r="AA15">
-        <v>-0.5</v>
+        <v>0.7250000000000001</v>
       </c>
       <c r="AB15">
-        <v>0.5249999999999999</v>
+        <v>-1</v>
       </c>
       <c r="AC15">
-        <v>0.4375</v>
+        <v>1.05</v>
       </c>
       <c r="AD15">
-        <v>-0.5</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="16" spans="1:30">
@@ -2005,7 +2005,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>6765583</v>
+        <v>6765585</v>
       </c>
       <c r="C17" t="s">
         <v>29</v>
@@ -2017,79 +2017,79 @@
         <v>43</v>
       </c>
       <c r="F17" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="G17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H17">
         <v>1</v>
       </c>
       <c r="I17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K17" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="L17">
-        <v>2.8</v>
+        <v>2</v>
       </c>
       <c r="M17">
         <v>2.8</v>
       </c>
       <c r="N17">
-        <v>2.55</v>
+        <v>4</v>
       </c>
       <c r="O17">
-        <v>2</v>
+        <v>2.05</v>
       </c>
       <c r="P17">
-        <v>3</v>
+        <v>2.7</v>
       </c>
       <c r="Q17">
-        <v>3.75</v>
+        <v>4</v>
       </c>
       <c r="R17">
         <v>-0.25</v>
       </c>
       <c r="S17">
-        <v>1.725</v>
+        <v>1.75</v>
       </c>
       <c r="T17">
-        <v>2.075</v>
+        <v>2.05</v>
       </c>
       <c r="U17">
-        <v>2</v>
+        <v>1.75</v>
       </c>
       <c r="V17">
-        <v>2.05</v>
+        <v>1.875</v>
       </c>
       <c r="W17">
-        <v>1.75</v>
+        <v>1.925</v>
       </c>
       <c r="X17">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="Y17">
-        <v>-1</v>
+        <v>1.7</v>
       </c>
       <c r="Z17">
         <v>-1</v>
       </c>
       <c r="AA17">
-        <v>0.7250000000000001</v>
+        <v>-0.5</v>
       </c>
       <c r="AB17">
-        <v>-1</v>
+        <v>0.5249999999999999</v>
       </c>
       <c r="AC17">
-        <v>1.05</v>
+        <v>0.4375</v>
       </c>
       <c r="AD17">
-        <v>-1</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="18" spans="1:30">
@@ -2109,7 +2109,7 @@
         <v>37</v>
       </c>
       <c r="F18" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="G18">
         <v>2</v>
@@ -2290,7 +2290,7 @@
         <v>45111.54166666666</v>
       </c>
       <c r="E20" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F20" t="s">
         <v>38</v>
@@ -2385,7 +2385,7 @@
         <v>36</v>
       </c>
       <c r="F21" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G21">
         <v>0</v>
@@ -2465,7 +2465,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>6858630</v>
+        <v>6743989</v>
       </c>
       <c r="C22" t="s">
         <v>29</v>
@@ -2474,82 +2474,82 @@
         <v>45111.54166666666</v>
       </c>
       <c r="E22" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F22" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="G22">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K22" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="L22">
-        <v>2.375</v>
+        <v>1.666</v>
       </c>
       <c r="M22">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="N22">
-        <v>2.8</v>
+        <v>4.5</v>
       </c>
       <c r="O22">
-        <v>2.45</v>
+        <v>1.5</v>
       </c>
       <c r="P22">
-        <v>2.8</v>
+        <v>3.75</v>
       </c>
       <c r="Q22">
-        <v>3</v>
+        <v>5.5</v>
       </c>
       <c r="R22">
-        <v>-0.25</v>
+        <v>-1</v>
       </c>
       <c r="S22">
-        <v>2.075</v>
+        <v>1.975</v>
       </c>
       <c r="T22">
-        <v>1.725</v>
+        <v>1.825</v>
       </c>
       <c r="U22">
-        <v>1.75</v>
+        <v>2.25</v>
       </c>
       <c r="V22">
-        <v>1.775</v>
+        <v>1.975</v>
       </c>
       <c r="W22">
-        <v>2.025</v>
+        <v>1.825</v>
       </c>
       <c r="X22">
-        <v>-1</v>
+        <v>0.5</v>
       </c>
       <c r="Y22">
-        <v>1.8</v>
+        <v>-1</v>
       </c>
       <c r="Z22">
         <v>-1</v>
       </c>
       <c r="AA22">
-        <v>-0.5</v>
+        <v>0</v>
       </c>
       <c r="AB22">
-        <v>0.3625</v>
+        <v>0</v>
       </c>
       <c r="AC22">
-        <v>-1</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="AD22">
-        <v>1.025</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="23" spans="1:30">
@@ -2557,7 +2557,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>6743989</v>
+        <v>6743297</v>
       </c>
       <c r="C23" t="s">
         <v>29</v>
@@ -2566,64 +2566,64 @@
         <v>45111.54166666666</v>
       </c>
       <c r="E23" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F23" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G23">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K23" t="s">
         <v>47</v>
       </c>
       <c r="L23">
-        <v>1.666</v>
+        <v>1.285</v>
       </c>
       <c r="M23">
-        <v>3.5</v>
+        <v>4.5</v>
       </c>
       <c r="N23">
-        <v>4.5</v>
+        <v>9</v>
       </c>
       <c r="O23">
-        <v>1.5</v>
+        <v>1.166</v>
       </c>
       <c r="P23">
-        <v>3.75</v>
+        <v>6</v>
       </c>
       <c r="Q23">
-        <v>5.5</v>
+        <v>17</v>
       </c>
       <c r="R23">
-        <v>-1</v>
+        <v>-1.75</v>
       </c>
       <c r="S23">
+        <v>1.825</v>
+      </c>
+      <c r="T23">
         <v>1.975</v>
       </c>
-      <c r="T23">
+      <c r="U23">
+        <v>2.5</v>
+      </c>
+      <c r="V23">
         <v>1.825</v>
       </c>
-      <c r="U23">
-        <v>2.25</v>
-      </c>
-      <c r="V23">
+      <c r="W23">
         <v>1.975</v>
       </c>
-      <c r="W23">
-        <v>1.825</v>
-      </c>
       <c r="X23">
-        <v>0.5</v>
+        <v>0.1659999999999999</v>
       </c>
       <c r="Y23">
         <v>-1</v>
@@ -2632,16 +2632,16 @@
         <v>-1</v>
       </c>
       <c r="AA23">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AB23">
-        <v>0</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="AC23">
+        <v>-1</v>
+      </c>
+      <c r="AD23">
         <v>0.9750000000000001</v>
-      </c>
-      <c r="AD23">
-        <v>-1</v>
       </c>
     </row>
     <row r="24" spans="1:30">
@@ -2649,7 +2649,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>6743297</v>
+        <v>6743978</v>
       </c>
       <c r="C24" t="s">
         <v>29</v>
@@ -2658,13 +2658,13 @@
         <v>45111.54166666666</v>
       </c>
       <c r="E24" t="s">
+        <v>34</v>
+      </c>
+      <c r="F24" t="s">
         <v>32</v>
       </c>
-      <c r="F24" t="s">
-        <v>39</v>
-      </c>
       <c r="G24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H24">
         <v>0</v>
@@ -2679,25 +2679,25 @@
         <v>47</v>
       </c>
       <c r="L24">
-        <v>1.285</v>
+        <v>2</v>
       </c>
       <c r="M24">
-        <v>4.5</v>
+        <v>2.9</v>
       </c>
       <c r="N24">
-        <v>9</v>
+        <v>3.6</v>
       </c>
       <c r="O24">
-        <v>1.166</v>
+        <v>2.1</v>
       </c>
       <c r="P24">
-        <v>6</v>
+        <v>2.9</v>
       </c>
       <c r="Q24">
-        <v>17</v>
+        <v>3.6</v>
       </c>
       <c r="R24">
-        <v>-1.75</v>
+        <v>-0.25</v>
       </c>
       <c r="S24">
         <v>1.825</v>
@@ -2706,16 +2706,16 @@
         <v>1.975</v>
       </c>
       <c r="U24">
-        <v>2.5</v>
+        <v>1.75</v>
       </c>
       <c r="V24">
-        <v>1.825</v>
+        <v>1.75</v>
       </c>
       <c r="W24">
-        <v>1.975</v>
+        <v>2.05</v>
       </c>
       <c r="X24">
-        <v>0.1659999999999999</v>
+        <v>1.1</v>
       </c>
       <c r="Y24">
         <v>-1</v>
@@ -2724,16 +2724,16 @@
         <v>-1</v>
       </c>
       <c r="AA24">
-        <v>-1</v>
+        <v>0.825</v>
       </c>
       <c r="AB24">
-        <v>0.9750000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AC24">
-        <v>-1</v>
+        <v>0.375</v>
       </c>
       <c r="AD24">
-        <v>0.9750000000000001</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="25" spans="1:30">
@@ -2741,7 +2741,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>6743978</v>
+        <v>6858630</v>
       </c>
       <c r="C25" t="s">
         <v>29</v>
@@ -2750,13 +2750,13 @@
         <v>45111.54166666666</v>
       </c>
       <c r="E25" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F25" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="G25">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H25">
         <v>0</v>
@@ -2768,64 +2768,64 @@
         <v>0</v>
       </c>
       <c r="K25" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="L25">
-        <v>2</v>
+        <v>2.375</v>
       </c>
       <c r="M25">
-        <v>2.9</v>
+        <v>3</v>
       </c>
       <c r="N25">
-        <v>3.6</v>
+        <v>2.8</v>
       </c>
       <c r="O25">
-        <v>2.1</v>
+        <v>2.45</v>
       </c>
       <c r="P25">
-        <v>2.9</v>
+        <v>2.8</v>
       </c>
       <c r="Q25">
-        <v>3.6</v>
+        <v>3</v>
       </c>
       <c r="R25">
         <v>-0.25</v>
       </c>
       <c r="S25">
-        <v>1.825</v>
+        <v>2.075</v>
       </c>
       <c r="T25">
-        <v>1.975</v>
+        <v>1.725</v>
       </c>
       <c r="U25">
         <v>1.75</v>
       </c>
       <c r="V25">
-        <v>1.75</v>
+        <v>1.775</v>
       </c>
       <c r="W25">
-        <v>2.05</v>
+        <v>2.025</v>
       </c>
       <c r="X25">
-        <v>1.1</v>
+        <v>-1</v>
       </c>
       <c r="Y25">
-        <v>-1</v>
+        <v>1.8</v>
       </c>
       <c r="Z25">
         <v>-1</v>
       </c>
       <c r="AA25">
-        <v>0.825</v>
+        <v>-0.5</v>
       </c>
       <c r="AB25">
-        <v>-1</v>
+        <v>0.3625</v>
       </c>
       <c r="AC25">
-        <v>0.375</v>
+        <v>-1</v>
       </c>
       <c r="AD25">
-        <v>-0.5</v>
+        <v>1.025</v>
       </c>
     </row>
     <row r="26" spans="1:30">
@@ -2845,7 +2845,7 @@
         <v>44</v>
       </c>
       <c r="F26" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="G26">
         <v>1</v>
@@ -3121,7 +3121,7 @@
         <v>38</v>
       </c>
       <c r="F29" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G29">
         <v>1</v>
@@ -3210,7 +3210,7 @@
         <v>45114.55208333334</v>
       </c>
       <c r="E30" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F30" t="s">
         <v>31</v>
@@ -3305,7 +3305,7 @@
         <v>42</v>
       </c>
       <c r="F31" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="G31">
         <v>1</v>
@@ -3394,10 +3394,10 @@
         <v>45114.55208333334</v>
       </c>
       <c r="E32" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F32" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G32">
         <v>2</v>
@@ -3486,7 +3486,7 @@
         <v>45117.55208333334</v>
       </c>
       <c r="E33" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F33" t="s">
         <v>31</v>
@@ -3578,10 +3578,10 @@
         <v>45117.55208333334</v>
       </c>
       <c r="E34" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="F34" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G34">
         <v>2</v>
@@ -3670,7 +3670,7 @@
         <v>45117.55208333334</v>
       </c>
       <c r="E35" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F35" t="s">
         <v>40</v>
@@ -3765,7 +3765,7 @@
         <v>36</v>
       </c>
       <c r="F36" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G36">
         <v>1</v>
@@ -3946,7 +3946,7 @@
         <v>45117.55208333334</v>
       </c>
       <c r="E38" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F38" t="s">
         <v>37</v>
@@ -4121,7 +4121,7 @@
         <v>38</v>
       </c>
       <c r="B40">
-        <v>6913588</v>
+        <v>6913587</v>
       </c>
       <c r="C40" t="s">
         <v>29</v>
@@ -4130,82 +4130,82 @@
         <v>45122.55208333334</v>
       </c>
       <c r="E40" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F40" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="G40">
         <v>1</v>
       </c>
       <c r="H40">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I40">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J40">
         <v>0</v>
       </c>
       <c r="K40" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L40">
-        <v>2.3</v>
+        <v>1.727</v>
       </c>
       <c r="M40">
-        <v>3</v>
+        <v>3.2</v>
       </c>
       <c r="N40">
-        <v>2.875</v>
+        <v>4.5</v>
       </c>
       <c r="O40">
-        <v>1.85</v>
+        <v>1.65</v>
       </c>
       <c r="P40">
-        <v>3.25</v>
+        <v>3.4</v>
       </c>
       <c r="Q40">
-        <v>3.6</v>
+        <v>4.75</v>
       </c>
       <c r="R40">
+        <v>-0.75</v>
+      </c>
+      <c r="S40">
+        <v>1.925</v>
+      </c>
+      <c r="T40">
+        <v>1.875</v>
+      </c>
+      <c r="U40">
+        <v>2</v>
+      </c>
+      <c r="V40">
+        <v>1.9</v>
+      </c>
+      <c r="W40">
+        <v>1.9</v>
+      </c>
+      <c r="X40">
+        <v>0.6499999999999999</v>
+      </c>
+      <c r="Y40">
+        <v>-1</v>
+      </c>
+      <c r="Z40">
+        <v>-1</v>
+      </c>
+      <c r="AA40">
+        <v>0.4625</v>
+      </c>
+      <c r="AB40">
         <v>-0.5</v>
       </c>
-      <c r="S40">
-        <v>1.95</v>
-      </c>
-      <c r="T40">
-        <v>1.85</v>
-      </c>
-      <c r="U40">
-        <v>2.5</v>
-      </c>
-      <c r="V40">
-        <v>2</v>
-      </c>
-      <c r="W40">
-        <v>1.8</v>
-      </c>
-      <c r="X40">
-        <v>-1</v>
-      </c>
-      <c r="Y40">
-        <v>-1</v>
-      </c>
-      <c r="Z40">
-        <v>2.6</v>
-      </c>
-      <c r="AA40">
-        <v>-1</v>
-      </c>
-      <c r="AB40">
-        <v>0.8500000000000001</v>
-      </c>
       <c r="AC40">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AD40">
-        <v>-1</v>
+        <v>0.8999999999999999</v>
       </c>
     </row>
     <row r="41" spans="1:30">
@@ -4213,7 +4213,7 @@
         <v>39</v>
       </c>
       <c r="B41">
-        <v>6913587</v>
+        <v>6913588</v>
       </c>
       <c r="C41" t="s">
         <v>29</v>
@@ -4222,82 +4222,82 @@
         <v>45122.55208333334</v>
       </c>
       <c r="E41" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F41" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G41">
         <v>1</v>
       </c>
       <c r="H41">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I41">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J41">
         <v>0</v>
       </c>
       <c r="K41" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="L41">
-        <v>1.727</v>
+        <v>2.3</v>
       </c>
       <c r="M41">
-        <v>3.2</v>
+        <v>3</v>
       </c>
       <c r="N41">
-        <v>4.5</v>
+        <v>2.875</v>
       </c>
       <c r="O41">
-        <v>1.65</v>
+        <v>1.85</v>
       </c>
       <c r="P41">
-        <v>3.4</v>
+        <v>3.25</v>
       </c>
       <c r="Q41">
-        <v>4.75</v>
+        <v>3.6</v>
       </c>
       <c r="R41">
-        <v>-0.75</v>
+        <v>-0.5</v>
       </c>
       <c r="S41">
-        <v>1.925</v>
+        <v>1.95</v>
       </c>
       <c r="T41">
-        <v>1.875</v>
+        <v>1.85</v>
       </c>
       <c r="U41">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="V41">
-        <v>1.9</v>
+        <v>2</v>
       </c>
       <c r="W41">
-        <v>1.9</v>
+        <v>1.8</v>
       </c>
       <c r="X41">
-        <v>0.6499999999999999</v>
+        <v>-1</v>
       </c>
       <c r="Y41">
         <v>-1</v>
       </c>
       <c r="Z41">
-        <v>-1</v>
+        <v>2.6</v>
       </c>
       <c r="AA41">
-        <v>0.4625</v>
+        <v>-1</v>
       </c>
       <c r="AB41">
-        <v>-0.5</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AC41">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="AD41">
-        <v>0.8999999999999999</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="42" spans="1:30">
@@ -4314,7 +4314,7 @@
         <v>45184.5</v>
       </c>
       <c r="E42" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F42" t="s">
         <v>31</v>
@@ -4406,7 +4406,7 @@
         <v>45184.5</v>
       </c>
       <c r="E43" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F43" t="s">
         <v>38</v>
@@ -4498,10 +4498,10 @@
         <v>45184.625</v>
       </c>
       <c r="E44" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F44" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="G44">
         <v>2</v>
@@ -4590,10 +4590,10 @@
         <v>45185.5</v>
       </c>
       <c r="E45" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F45" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="G45">
         <v>0</v>
@@ -4961,7 +4961,7 @@
         <v>45</v>
       </c>
       <c r="F49" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G49">
         <v>2</v>
@@ -5050,7 +5050,7 @@
         <v>45191.625</v>
       </c>
       <c r="E50" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="F50" t="s">
         <v>30</v>
@@ -5145,7 +5145,7 @@
         <v>40</v>
       </c>
       <c r="F51" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G51">
         <v>1</v>
@@ -5329,7 +5329,7 @@
         <v>38</v>
       </c>
       <c r="F53" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G53">
         <v>2</v>
@@ -5418,7 +5418,7 @@
         <v>45192.625</v>
       </c>
       <c r="E54" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F54" t="s">
         <v>37</v>
@@ -5602,7 +5602,7 @@
         <v>45198.48958333334</v>
       </c>
       <c r="E56" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F56" t="s">
         <v>39</v>
@@ -5694,10 +5694,10 @@
         <v>45198.48958333334</v>
       </c>
       <c r="E57" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F57" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="G57">
         <v>2</v>
@@ -5789,7 +5789,7 @@
         <v>46</v>
       </c>
       <c r="F58" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="G58">
         <v>0</v>
@@ -5881,7 +5881,7 @@
         <v>44</v>
       </c>
       <c r="F59" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G59">
         <v>2</v>
@@ -6062,7 +6062,7 @@
         <v>45199.625</v>
       </c>
       <c r="E61" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F61" t="s">
         <v>31</v>
@@ -6430,10 +6430,10 @@
         <v>45205.625</v>
       </c>
       <c r="E65" t="s">
+        <v>43</v>
+      </c>
+      <c r="F65" t="s">
         <v>41</v>
-      </c>
-      <c r="F65" t="s">
-        <v>43</v>
       </c>
       <c r="G65">
         <v>0</v>
@@ -6617,7 +6617,7 @@
         <v>40</v>
       </c>
       <c r="F67" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G67">
         <v>2</v>
@@ -6706,10 +6706,10 @@
         <v>45206.48958333334</v>
       </c>
       <c r="E68" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F68" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G68">
         <v>1</v>
@@ -6798,7 +6798,7 @@
         <v>45206.625</v>
       </c>
       <c r="E69" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="F69" t="s">
         <v>36</v>
@@ -6985,7 +6985,7 @@
         <v>36</v>
       </c>
       <c r="F71" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G71">
         <v>3</v>
@@ -7077,7 +7077,7 @@
         <v>30</v>
       </c>
       <c r="F72" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="G72">
         <v>1</v>
@@ -7261,7 +7261,7 @@
         <v>38</v>
       </c>
       <c r="F74" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="G74">
         <v>1</v>
@@ -7442,7 +7442,7 @@
         <v>45241.45833333334</v>
       </c>
       <c r="E76" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F76" t="s">
         <v>39</v>
@@ -7534,7 +7534,7 @@
         <v>45241.45833333334</v>
       </c>
       <c r="E77" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F77" t="s">
         <v>45</v>
@@ -7626,7 +7626,7 @@
         <v>45241.54166666666</v>
       </c>
       <c r="E78" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F78" t="s">
         <v>44</v>
@@ -7721,7 +7721,7 @@
         <v>37</v>
       </c>
       <c r="F79" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G79">
         <v>0</v>
@@ -7997,7 +7997,7 @@
         <v>31</v>
       </c>
       <c r="F82" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G82">
         <v>0</v>
@@ -8086,7 +8086,7 @@
         <v>45247.47916666666</v>
       </c>
       <c r="E83" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F83" t="s">
         <v>46</v>
@@ -8178,10 +8178,10 @@
         <v>45247.53125</v>
       </c>
       <c r="E84" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F84" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G84">
         <v>1</v>
@@ -8454,7 +8454,7 @@
         <v>45248.54166666666</v>
       </c>
       <c r="E87" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F87" t="s">
         <v>38</v>
@@ -8641,7 +8641,7 @@
         <v>40</v>
       </c>
       <c r="F89" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="G89">
         <v>1</v>
@@ -8730,10 +8730,10 @@
         <v>45254.46875</v>
       </c>
       <c r="E90" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F90" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G90">
         <v>1</v>
@@ -8914,7 +8914,7 @@
         <v>45255.45833333334</v>
       </c>
       <c r="E92" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F92" t="s">
         <v>45</v>
@@ -9006,7 +9006,7 @@
         <v>45255.53125</v>
       </c>
       <c r="E93" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="F93" t="s">
         <v>39</v>
@@ -9101,7 +9101,7 @@
         <v>37</v>
       </c>
       <c r="F94" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G94">
         <v>3</v>
@@ -9190,7 +9190,7 @@
         <v>45261.46875</v>
       </c>
       <c r="E95" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F95" t="s">
         <v>30</v>
@@ -9285,7 +9285,7 @@
         <v>44</v>
       </c>
       <c r="F96" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G96">
         <v>4</v>
@@ -9377,7 +9377,7 @@
         <v>31</v>
       </c>
       <c r="F97" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G97">
         <v>2</v>
@@ -9466,7 +9466,7 @@
         <v>45262.53125</v>
       </c>
       <c r="E98" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F98" t="s">
         <v>46</v>
@@ -9650,10 +9650,10 @@
         <v>45262.58333333334</v>
       </c>
       <c r="E100" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F100" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="G100">
         <v>1</v>
@@ -9834,10 +9834,10 @@
         <v>45268.46875</v>
       </c>
       <c r="E102" t="s">
+        <v>33</v>
+      </c>
+      <c r="F102" t="s">
         <v>34</v>
-      </c>
-      <c r="F102" t="s">
-        <v>33</v>
       </c>
       <c r="G102">
         <v>2</v>
@@ -9926,7 +9926,7 @@
         <v>45268.58333333334</v>
       </c>
       <c r="E103" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="F103" t="s">
         <v>45</v>
@@ -10018,10 +10018,10 @@
         <v>45269.45833333334</v>
       </c>
       <c r="E104" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F104" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G104">
         <v>1</v>
@@ -10294,7 +10294,7 @@
         <v>45275.46875</v>
       </c>
       <c r="E107" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F107" t="s">
         <v>36</v>
@@ -10481,7 +10481,7 @@
         <v>31</v>
       </c>
       <c r="F109" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="G109">
         <v>2</v>
@@ -10570,7 +10570,7 @@
         <v>45275.58333333334</v>
       </c>
       <c r="E110" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F110" t="s">
         <v>30</v>
@@ -10757,7 +10757,7 @@
         <v>37</v>
       </c>
       <c r="F112" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G112">
         <v>2</v>
@@ -10849,7 +10849,7 @@
         <v>44</v>
       </c>
       <c r="F113" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G113">
         <v>3</v>
@@ -10938,7 +10938,7 @@
         <v>45276.625</v>
       </c>
       <c r="E114" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F114" t="s">
         <v>39</v>
@@ -11122,7 +11122,7 @@
         <v>45289.46875</v>
       </c>
       <c r="E116" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F116" t="s">
         <v>46</v>
@@ -11214,10 +11214,10 @@
         <v>45289.46875</v>
       </c>
       <c r="E117" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F117" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G117">
         <v>2</v>
@@ -11401,7 +11401,7 @@
         <v>38</v>
       </c>
       <c r="F119" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="G119">
         <v>1</v>
@@ -11769,7 +11769,7 @@
         <v>45</v>
       </c>
       <c r="F123" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="G123">
         <v>2</v>
@@ -11858,7 +11858,7 @@
         <v>45296.46875</v>
       </c>
       <c r="E124" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F124" t="s">
         <v>38</v>
@@ -11950,7 +11950,7 @@
         <v>45296.48958333334</v>
       </c>
       <c r="E125" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F125" t="s">
         <v>36</v>
@@ -12137,7 +12137,7 @@
         <v>37</v>
       </c>
       <c r="F127" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G127">
         <v>0</v>
@@ -12229,7 +12229,7 @@
         <v>44</v>
       </c>
       <c r="F128" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="G128">
         <v>1</v>
@@ -12410,7 +12410,7 @@
         <v>45302.53125</v>
       </c>
       <c r="E130" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F130" t="s">
         <v>31</v>
@@ -12597,7 +12597,7 @@
         <v>30</v>
       </c>
       <c r="F132" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G132">
         <v>0</v>
@@ -12686,7 +12686,7 @@
         <v>45304.45833333334</v>
       </c>
       <c r="E133" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F133" t="s">
         <v>46</v>
@@ -12781,7 +12781,7 @@
         <v>39</v>
       </c>
       <c r="F134" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G134">
         <v>0</v>
@@ -12870,10 +12870,10 @@
         <v>45304.53125</v>
       </c>
       <c r="E135" t="s">
+        <v>35</v>
+      </c>
+      <c r="F135" t="s">
         <v>32</v>
-      </c>
-      <c r="F135" t="s">
-        <v>35</v>
       </c>
       <c r="G135">
         <v>2</v>
@@ -13149,7 +13149,7 @@
         <v>36</v>
       </c>
       <c r="F138" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="G138">
         <v>2</v>
@@ -13330,10 +13330,10 @@
         <v>45310.47916666666</v>
       </c>
       <c r="E140" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F140" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G140">
         <v>1</v>
@@ -13422,10 +13422,10 @@
         <v>45310.47916666666</v>
       </c>
       <c r="E141" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F141" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="G141">
         <v>0</v>
@@ -13514,7 +13514,7 @@
         <v>45310.48958333334</v>
       </c>
       <c r="E142" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F142" t="s">
         <v>40</v>
@@ -13609,7 +13609,7 @@
         <v>37</v>
       </c>
       <c r="F143" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="G143">
         <v>3</v>
@@ -13974,10 +13974,10 @@
         <v>45314.54166666666</v>
       </c>
       <c r="E147" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="F147" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G147">
         <v>0</v>
@@ -14158,7 +14158,7 @@
         <v>45317.47916666666</v>
       </c>
       <c r="E149" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F149" t="s">
         <v>30</v>
@@ -14342,7 +14342,7 @@
         <v>45317.54166666666</v>
       </c>
       <c r="E151" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F151" t="s">
         <v>44</v>
@@ -14437,7 +14437,7 @@
         <v>45</v>
       </c>
       <c r="F152" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G152">
         <v>1</v>
@@ -14526,7 +14526,7 @@
         <v>45318.5</v>
       </c>
       <c r="E153" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="F153" t="s">
         <v>46</v>
@@ -14621,7 +14621,7 @@
         <v>39</v>
       </c>
       <c r="F154" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G154">
         <v>2</v>
@@ -14805,7 +14805,7 @@
         <v>36</v>
       </c>
       <c r="F156" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G156">
         <v>3</v>
@@ -14897,7 +14897,7 @@
         <v>40</v>
       </c>
       <c r="F157" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="G157">
         <v>2</v>
@@ -15078,7 +15078,7 @@
         <v>45326.47916666666</v>
       </c>
       <c r="E159" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F159" t="s">
         <v>40</v>
@@ -15170,10 +15170,10 @@
         <v>45331.48958333334</v>
       </c>
       <c r="E160" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F160" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G160">
         <v>1</v>
@@ -15265,7 +15265,7 @@
         <v>38</v>
       </c>
       <c r="F161" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G161">
         <v>2</v>
@@ -15357,7 +15357,7 @@
         <v>31</v>
       </c>
       <c r="F162" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G162">
         <v>2</v>
@@ -15446,10 +15446,10 @@
         <v>45332.5</v>
       </c>
       <c r="E163" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="F163" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G163">
         <v>1</v>
@@ -15814,7 +15814,7 @@
         <v>45337.47916666666</v>
       </c>
       <c r="E167" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F167" t="s">
         <v>38</v>
@@ -15909,7 +15909,7 @@
         <v>30</v>
       </c>
       <c r="F168" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="G168">
         <v>0</v>
@@ -15998,7 +15998,7 @@
         <v>45338.47916666666</v>
       </c>
       <c r="E169" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F169" t="s">
         <v>36</v>
@@ -16090,7 +16090,7 @@
         <v>45338.53125</v>
       </c>
       <c r="E170" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F170" t="s">
         <v>45</v>
@@ -16277,7 +16277,7 @@
         <v>37</v>
       </c>
       <c r="F172" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="G172">
         <v>1</v>
@@ -16461,7 +16461,7 @@
         <v>39</v>
       </c>
       <c r="F174" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G174">
         <v>0</v>
@@ -16642,7 +16642,7 @@
         <v>45346.5</v>
       </c>
       <c r="E176" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F176" t="s">
         <v>44</v>
@@ -16734,10 +16734,10 @@
         <v>45346.5</v>
       </c>
       <c r="E177" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="F177" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G177">
         <v>0</v>
@@ -16826,7 +16826,7 @@
         <v>45346.53125</v>
       </c>
       <c r="E178" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F178" t="s">
         <v>46</v>
@@ -16921,7 +16921,7 @@
         <v>31</v>
       </c>
       <c r="F179" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G179">
         <v>3</v>
@@ -17010,10 +17010,10 @@
         <v>45352.5</v>
       </c>
       <c r="E180" t="s">
+        <v>41</v>
+      </c>
+      <c r="F180" t="s">
         <v>43</v>
-      </c>
-      <c r="F180" t="s">
-        <v>41</v>
       </c>
       <c r="G180">
         <v>1</v>
@@ -17194,10 +17194,10 @@
         <v>45353.53125</v>
       </c>
       <c r="E182" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F182" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G182">
         <v>2</v>
@@ -17565,7 +17565,7 @@
         <v>44</v>
       </c>
       <c r="F186" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G186">
         <v>6</v>
@@ -17657,7 +17657,7 @@
         <v>45</v>
       </c>
       <c r="F187" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G187">
         <v>3</v>
@@ -17930,7 +17930,7 @@
         <v>45366.75</v>
       </c>
       <c r="E190" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="F190" t="s">
         <v>38</v>
@@ -18022,7 +18022,7 @@
         <v>45366.75</v>
       </c>
       <c r="E191" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F191" t="s">
         <v>30</v>
@@ -18114,7 +18114,7 @@
         <v>45367.47916666666</v>
       </c>
       <c r="E192" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F192" t="s">
         <v>37</v>
@@ -18209,7 +18209,7 @@
         <v>39</v>
       </c>
       <c r="F193" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G193">
         <v>2</v>
@@ -18298,7 +18298,7 @@
         <v>45370.47916666666</v>
       </c>
       <c r="E194" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F194" t="s">
         <v>40</v>
@@ -18574,10 +18574,10 @@
         <v>45374.47916666666</v>
       </c>
       <c r="E197" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F197" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="G197">
         <v>0</v>
@@ -18666,7 +18666,7 @@
         <v>45375.47916666666</v>
       </c>
       <c r="E198" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F198" t="s">
         <v>31</v>
@@ -18850,7 +18850,7 @@
         <v>45375.75</v>
       </c>
       <c r="E200" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="F200" t="s">
         <v>40</v>
@@ -18945,7 +18945,7 @@
         <v>38</v>
       </c>
       <c r="F201" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G201">
         <v>0</v>
@@ -19310,10 +19310,10 @@
         <v>45387.48958333334</v>
       </c>
       <c r="E205" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F205" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G205">
         <v>0</v>
@@ -19393,7 +19393,7 @@
         <v>204</v>
       </c>
       <c r="B206">
-        <v>8007205</v>
+        <v>8007204</v>
       </c>
       <c r="C206" t="s">
         <v>29</v>
@@ -19402,55 +19402,55 @@
         <v>45387.75</v>
       </c>
       <c r="E206" t="s">
+        <v>39</v>
+      </c>
+      <c r="F206" t="s">
         <v>35</v>
       </c>
-      <c r="F206" t="s">
-        <v>37</v>
-      </c>
       <c r="G206">
         <v>1</v>
       </c>
       <c r="H206">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I206">
         <v>0</v>
       </c>
       <c r="J206">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K206" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L206">
-        <v>1.571</v>
+        <v>2</v>
       </c>
       <c r="M206">
+        <v>3</v>
+      </c>
+      <c r="N206">
         <v>3.6</v>
       </c>
-      <c r="N206">
-        <v>5</v>
-      </c>
       <c r="O206">
-        <v>1.85</v>
+        <v>2.375</v>
       </c>
       <c r="P206">
-        <v>3.3</v>
+        <v>2.625</v>
       </c>
       <c r="Q206">
-        <v>3.6</v>
+        <v>3.4</v>
       </c>
       <c r="R206">
-        <v>-0.5</v>
+        <v>-0.25</v>
       </c>
       <c r="S206">
-        <v>2</v>
+        <v>2.025</v>
       </c>
       <c r="T206">
-        <v>1.8</v>
+        <v>1.775</v>
       </c>
       <c r="U206">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="V206">
         <v>1.775</v>
@@ -19459,25 +19459,25 @@
         <v>2.025</v>
       </c>
       <c r="X206">
-        <v>-1</v>
+        <v>1.375</v>
       </c>
       <c r="Y206">
         <v>-1</v>
       </c>
       <c r="Z206">
-        <v>2.6</v>
+        <v>-1</v>
       </c>
       <c r="AA206">
-        <v>-1</v>
+        <v>1.025</v>
       </c>
       <c r="AB206">
-        <v>0.8</v>
+        <v>-1</v>
       </c>
       <c r="AC206">
-        <v>0.7749999999999999</v>
+        <v>-1</v>
       </c>
       <c r="AD206">
-        <v>-1</v>
+        <v>1.025</v>
       </c>
     </row>
     <row r="207" spans="1:30">
@@ -19577,7 +19577,7 @@
         <v>206</v>
       </c>
       <c r="B208">
-        <v>8007204</v>
+        <v>8007205</v>
       </c>
       <c r="C208" t="s">
         <v>29</v>
@@ -19586,55 +19586,55 @@
         <v>45387.75</v>
       </c>
       <c r="E208" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="F208" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="G208">
         <v>1</v>
       </c>
       <c r="H208">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I208">
         <v>0</v>
       </c>
       <c r="J208">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K208" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="L208">
-        <v>2</v>
+        <v>1.571</v>
       </c>
       <c r="M208">
-        <v>3</v>
+        <v>3.6</v>
       </c>
       <c r="N208">
+        <v>5</v>
+      </c>
+      <c r="O208">
+        <v>1.85</v>
+      </c>
+      <c r="P208">
+        <v>3.3</v>
+      </c>
+      <c r="Q208">
         <v>3.6</v>
       </c>
-      <c r="O208">
-        <v>2.375</v>
-      </c>
-      <c r="P208">
-        <v>2.625</v>
-      </c>
-      <c r="Q208">
-        <v>3.4</v>
-      </c>
       <c r="R208">
-        <v>-0.25</v>
+        <v>-0.5</v>
       </c>
       <c r="S208">
-        <v>2.025</v>
+        <v>2</v>
       </c>
       <c r="T208">
-        <v>1.775</v>
+        <v>1.8</v>
       </c>
       <c r="U208">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="V208">
         <v>1.775</v>
@@ -19643,25 +19643,25 @@
         <v>2.025</v>
       </c>
       <c r="X208">
-        <v>1.375</v>
+        <v>-1</v>
       </c>
       <c r="Y208">
         <v>-1</v>
       </c>
       <c r="Z208">
-        <v>-1</v>
+        <v>2.6</v>
       </c>
       <c r="AA208">
-        <v>1.025</v>
+        <v>-1</v>
       </c>
       <c r="AB208">
-        <v>-1</v>
+        <v>0.8</v>
       </c>
       <c r="AC208">
-        <v>-1</v>
+        <v>0.7749999999999999</v>
       </c>
       <c r="AD208">
-        <v>1.025</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="209" spans="1:30">
@@ -19681,7 +19681,7 @@
         <v>45</v>
       </c>
       <c r="F209" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G209">
         <v>3</v>
@@ -19862,10 +19862,10 @@
         <v>45398.58333333334</v>
       </c>
       <c r="E211" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="F211" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="G211">
         <v>3</v>
@@ -20046,7 +20046,7 @@
         <v>45401.5</v>
       </c>
       <c r="E213" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F213" t="s">
         <v>31</v>
@@ -20138,7 +20138,7 @@
         <v>45401.5</v>
       </c>
       <c r="E214" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F214" t="s">
         <v>44</v>
@@ -20417,7 +20417,7 @@
         <v>30</v>
       </c>
       <c r="F217" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G217">
         <v>1</v>
@@ -20506,10 +20506,10 @@
         <v>45408.5</v>
       </c>
       <c r="E218" t="s">
+        <v>34</v>
+      </c>
+      <c r="F218" t="s">
         <v>33</v>
-      </c>
-      <c r="F218" t="s">
-        <v>34</v>
       </c>
       <c r="G218">
         <v>1</v>
@@ -20785,7 +20785,7 @@
         <v>45</v>
       </c>
       <c r="F221" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="G221">
         <v>2</v>
@@ -20874,10 +20874,10 @@
         <v>45409.5</v>
       </c>
       <c r="E222" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F222" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G222">
         <v>2</v>
@@ -21058,7 +21058,7 @@
         <v>45410.625</v>
       </c>
       <c r="E224" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F224" t="s">
         <v>40</v>
@@ -21150,7 +21150,7 @@
         <v>45416.5</v>
       </c>
       <c r="E225" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F225" t="s">
         <v>40</v>
@@ -21245,7 +21245,7 @@
         <v>36</v>
       </c>
       <c r="F226" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="G226">
         <v>2</v>
@@ -21337,7 +21337,7 @@
         <v>36</v>
       </c>
       <c r="F227" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G227">
         <v>2</v>
@@ -21521,7 +21521,7 @@
         <v>30</v>
       </c>
       <c r="F229" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G229">
         <v>2</v>
@@ -21610,7 +21610,7 @@
         <v>45423.54166666666</v>
       </c>
       <c r="E230" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F230" t="s">
         <v>37</v>
@@ -21693,7 +21693,7 @@
         <v>229</v>
       </c>
       <c r="B231">
-        <v>8184371</v>
+        <v>8184372</v>
       </c>
       <c r="C231" t="s">
         <v>29</v>
@@ -21702,10 +21702,10 @@
         <v>45423.54166666666</v>
       </c>
       <c r="E231" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="F231" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="G231">
         <v>0</v>
@@ -21723,46 +21723,46 @@
         <v>49</v>
       </c>
       <c r="L231">
-        <v>2.3</v>
+        <v>2.1</v>
       </c>
       <c r="M231">
+        <v>3.1</v>
+      </c>
+      <c r="N231">
         <v>3.2</v>
       </c>
-      <c r="N231">
-        <v>2.75</v>
-      </c>
       <c r="O231">
-        <v>2.45</v>
+        <v>2.5</v>
       </c>
       <c r="P231">
-        <v>2.9</v>
+        <v>2.7</v>
       </c>
       <c r="Q231">
-        <v>2.8</v>
+        <v>3</v>
       </c>
       <c r="R231">
         <v>0</v>
       </c>
       <c r="S231">
+        <v>1.725</v>
+      </c>
+      <c r="T231">
+        <v>2.075</v>
+      </c>
+      <c r="U231">
         <v>1.75</v>
       </c>
-      <c r="T231">
-        <v>2.05</v>
-      </c>
-      <c r="U231">
-        <v>2</v>
-      </c>
       <c r="V231">
+        <v>2</v>
+      </c>
+      <c r="W231">
         <v>1.8</v>
       </c>
-      <c r="W231">
-        <v>2</v>
-      </c>
       <c r="X231">
         <v>-1</v>
       </c>
       <c r="Y231">
-        <v>1.9</v>
+        <v>1.7</v>
       </c>
       <c r="Z231">
         <v>-1</v>
@@ -21777,7 +21777,7 @@
         <v>-1</v>
       </c>
       <c r="AD231">
-        <v>1</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="232" spans="1:30">
@@ -21785,7 +21785,7 @@
         <v>230</v>
       </c>
       <c r="B232">
-        <v>8184372</v>
+        <v>8184338</v>
       </c>
       <c r="C232" t="s">
         <v>29</v>
@@ -21794,13 +21794,13 @@
         <v>45423.54166666666</v>
       </c>
       <c r="E232" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F232" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="G232">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H232">
         <v>0</v>
@@ -21812,49 +21812,49 @@
         <v>0</v>
       </c>
       <c r="K232" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="L232">
-        <v>2.1</v>
+        <v>1.615</v>
       </c>
       <c r="M232">
-        <v>3.1</v>
+        <v>3.4</v>
       </c>
       <c r="N232">
-        <v>3.2</v>
+        <v>5</v>
       </c>
       <c r="O232">
+        <v>1.5</v>
+      </c>
+      <c r="P232">
+        <v>3.8</v>
+      </c>
+      <c r="Q232">
+        <v>5.5</v>
+      </c>
+      <c r="R232">
+        <v>-1</v>
+      </c>
+      <c r="S232">
+        <v>1.9</v>
+      </c>
+      <c r="T232">
+        <v>1.9</v>
+      </c>
+      <c r="U232">
         <v>2.5</v>
       </c>
-      <c r="P232">
-        <v>2.7</v>
-      </c>
-      <c r="Q232">
-        <v>3</v>
-      </c>
-      <c r="R232">
-        <v>0</v>
-      </c>
-      <c r="S232">
-        <v>1.725</v>
-      </c>
-      <c r="T232">
-        <v>2.075</v>
-      </c>
-      <c r="U232">
-        <v>1.75</v>
-      </c>
       <c r="V232">
-        <v>2</v>
+        <v>1.95</v>
       </c>
       <c r="W232">
-        <v>1.8</v>
+        <v>1.85</v>
       </c>
       <c r="X232">
-        <v>-1</v>
+        <v>0.5</v>
       </c>
       <c r="Y232">
-        <v>1.7</v>
+        <v>-1</v>
       </c>
       <c r="Z232">
         <v>-1</v>
@@ -21869,7 +21869,7 @@
         <v>-1</v>
       </c>
       <c r="AD232">
-        <v>0.8</v>
+        <v>0.8500000000000001</v>
       </c>
     </row>
     <row r="233" spans="1:30">
@@ -21877,7 +21877,7 @@
         <v>231</v>
       </c>
       <c r="B233">
-        <v>8184338</v>
+        <v>8184368</v>
       </c>
       <c r="C233" t="s">
         <v>29</v>
@@ -21886,67 +21886,67 @@
         <v>45423.54166666666</v>
       </c>
       <c r="E233" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="F233" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G233">
         <v>1</v>
       </c>
       <c r="H233">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I233">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J233">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K233" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="L233">
-        <v>1.615</v>
+        <v>3.5</v>
       </c>
       <c r="M233">
-        <v>3.4</v>
+        <v>3.3</v>
       </c>
       <c r="N233">
-        <v>5</v>
+        <v>1.909</v>
       </c>
       <c r="O233">
-        <v>1.5</v>
+        <v>2.7</v>
       </c>
       <c r="P233">
-        <v>3.8</v>
+        <v>3</v>
       </c>
       <c r="Q233">
-        <v>5.5</v>
+        <v>2.4</v>
       </c>
       <c r="R233">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="S233">
-        <v>1.9</v>
+        <v>2.025</v>
       </c>
       <c r="T233">
-        <v>1.9</v>
+        <v>1.775</v>
       </c>
       <c r="U233">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="V233">
-        <v>1.95</v>
+        <v>1.875</v>
       </c>
       <c r="W233">
-        <v>1.85</v>
+        <v>1.925</v>
       </c>
       <c r="X233">
-        <v>0.5</v>
+        <v>-1</v>
       </c>
       <c r="Y233">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="Z233">
         <v>-1</v>
@@ -21958,10 +21958,10 @@
         <v>0</v>
       </c>
       <c r="AC233">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AD233">
-        <v>0.8500000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="234" spans="1:30">
@@ -21969,7 +21969,7 @@
         <v>232</v>
       </c>
       <c r="B234">
-        <v>8184368</v>
+        <v>8184371</v>
       </c>
       <c r="C234" t="s">
         <v>29</v>
@@ -21978,67 +21978,67 @@
         <v>45423.54166666666</v>
       </c>
       <c r="E234" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F234" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="G234">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H234">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I234">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J234">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K234" t="s">
         <v>49</v>
       </c>
       <c r="L234">
-        <v>3.5</v>
+        <v>2.3</v>
       </c>
       <c r="M234">
-        <v>3.3</v>
+        <v>3.2</v>
       </c>
       <c r="N234">
-        <v>1.909</v>
+        <v>2.75</v>
       </c>
       <c r="O234">
-        <v>2.7</v>
+        <v>2.45</v>
       </c>
       <c r="P234">
-        <v>3</v>
+        <v>2.9</v>
       </c>
       <c r="Q234">
-        <v>2.4</v>
+        <v>2.8</v>
       </c>
       <c r="R234">
         <v>0</v>
       </c>
       <c r="S234">
-        <v>2.025</v>
+        <v>1.75</v>
       </c>
       <c r="T234">
-        <v>1.775</v>
+        <v>2.05</v>
       </c>
       <c r="U234">
         <v>2</v>
       </c>
       <c r="V234">
-        <v>1.875</v>
+        <v>1.8</v>
       </c>
       <c r="W234">
-        <v>1.925</v>
+        <v>2</v>
       </c>
       <c r="X234">
         <v>-1</v>
       </c>
       <c r="Y234">
-        <v>2</v>
+        <v>1.9</v>
       </c>
       <c r="Z234">
         <v>-1</v>
@@ -22050,10 +22050,10 @@
         <v>0</v>
       </c>
       <c r="AC234">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AD234">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="235" spans="1:30">
@@ -22070,10 +22070,10 @@
         <v>45429.54166666666</v>
       </c>
       <c r="E235" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F235" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G235">
         <v>4</v>
@@ -22162,10 +22162,10 @@
         <v>45429.54166666666</v>
       </c>
       <c r="E236" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F236" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="G236">
         <v>1</v>
@@ -22254,7 +22254,7 @@
         <v>45429.54166666666</v>
       </c>
       <c r="E237" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F237" t="s">
         <v>38</v>
@@ -22441,7 +22441,7 @@
         <v>46</v>
       </c>
       <c r="F239" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G239">
         <v>0</v>
@@ -22521,7 +22521,7 @@
         <v>238</v>
       </c>
       <c r="B240">
-        <v>8202022</v>
+        <v>8202017</v>
       </c>
       <c r="C240" t="s">
         <v>29</v>
@@ -22530,10 +22530,10 @@
         <v>45429.54166666666</v>
       </c>
       <c r="E240" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="F240" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="G240">
         <v>2</v>
@@ -22542,7 +22542,7 @@
         <v>1</v>
       </c>
       <c r="I240">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J240">
         <v>0</v>
@@ -22551,43 +22551,43 @@
         <v>47</v>
       </c>
       <c r="L240">
-        <v>1.8</v>
+        <v>2.375</v>
       </c>
       <c r="M240">
-        <v>3.2</v>
+        <v>2.8</v>
       </c>
       <c r="N240">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O240">
-        <v>1.55</v>
+        <v>1.615</v>
       </c>
       <c r="P240">
-        <v>3.1</v>
+        <v>3.4</v>
       </c>
       <c r="Q240">
-        <v>7</v>
+        <v>4.75</v>
       </c>
       <c r="R240">
         <v>-0.75</v>
       </c>
       <c r="S240">
-        <v>1.75</v>
+        <v>1.875</v>
       </c>
       <c r="T240">
-        <v>2.05</v>
+        <v>1.925</v>
       </c>
       <c r="U240">
-        <v>1.75</v>
+        <v>2</v>
       </c>
       <c r="V240">
-        <v>1.825</v>
+        <v>1.775</v>
       </c>
       <c r="W240">
-        <v>1.975</v>
+        <v>2.025</v>
       </c>
       <c r="X240">
-        <v>0.55</v>
+        <v>0.615</v>
       </c>
       <c r="Y240">
         <v>-1</v>
@@ -22596,13 +22596,13 @@
         <v>-1</v>
       </c>
       <c r="AA240">
-        <v>0.375</v>
+        <v>0.4375</v>
       </c>
       <c r="AB240">
         <v>-0.5</v>
       </c>
       <c r="AC240">
-        <v>0.825</v>
+        <v>0.7749999999999999</v>
       </c>
       <c r="AD240">
         <v>-1</v>
@@ -22613,7 +22613,7 @@
         <v>239</v>
       </c>
       <c r="B241">
-        <v>8202017</v>
+        <v>8202022</v>
       </c>
       <c r="C241" t="s">
         <v>29</v>
@@ -22622,10 +22622,10 @@
         <v>45429.54166666666</v>
       </c>
       <c r="E241" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="F241" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="G241">
         <v>2</v>
@@ -22634,7 +22634,7 @@
         <v>1</v>
       </c>
       <c r="I241">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J241">
         <v>0</v>
@@ -22643,43 +22643,43 @@
         <v>47</v>
       </c>
       <c r="L241">
-        <v>2.375</v>
+        <v>1.8</v>
       </c>
       <c r="M241">
-        <v>2.8</v>
+        <v>3.2</v>
       </c>
       <c r="N241">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O241">
-        <v>1.615</v>
+        <v>1.55</v>
       </c>
       <c r="P241">
-        <v>3.4</v>
+        <v>3.1</v>
       </c>
       <c r="Q241">
-        <v>4.75</v>
+        <v>7</v>
       </c>
       <c r="R241">
         <v>-0.75</v>
       </c>
       <c r="S241">
-        <v>1.875</v>
+        <v>1.75</v>
       </c>
       <c r="T241">
-        <v>1.925</v>
+        <v>2.05</v>
       </c>
       <c r="U241">
-        <v>2</v>
+        <v>1.75</v>
       </c>
       <c r="V241">
-        <v>1.775</v>
+        <v>1.825</v>
       </c>
       <c r="W241">
-        <v>2.025</v>
+        <v>1.975</v>
       </c>
       <c r="X241">
-        <v>0.615</v>
+        <v>0.55</v>
       </c>
       <c r="Y241">
         <v>-1</v>
@@ -22688,13 +22688,13 @@
         <v>-1</v>
       </c>
       <c r="AA241">
-        <v>0.4375</v>
+        <v>0.375</v>
       </c>
       <c r="AB241">
         <v>-0.5</v>
       </c>
       <c r="AC241">
-        <v>0.7749999999999999</v>
+        <v>0.825</v>
       </c>
       <c r="AD241">
         <v>-1</v>
@@ -22806,7 +22806,7 @@
         <v>45433.625</v>
       </c>
       <c r="E243" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F243" t="s">
         <v>36</v>
@@ -22901,7 +22901,7 @@
         <v>36</v>
       </c>
       <c r="F244" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G244">
         <v>2</v>
@@ -22981,7 +22981,7 @@
         <v>243</v>
       </c>
       <c r="B245">
-        <v>8245121</v>
+        <v>8245122</v>
       </c>
       <c r="C245" t="s">
         <v>29</v>
@@ -22990,49 +22990,49 @@
         <v>45438.53125</v>
       </c>
       <c r="E245" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="F245" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="G245">
         <v>1</v>
       </c>
       <c r="H245">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K245" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="L245">
-        <v>2.5</v>
+        <v>1.222</v>
       </c>
       <c r="M245">
-        <v>2.75</v>
+        <v>5</v>
       </c>
       <c r="N245">
-        <v>2.875</v>
+        <v>10</v>
       </c>
       <c r="O245">
-        <v>2.6</v>
+        <v>1.222</v>
       </c>
       <c r="P245">
-        <v>2.75</v>
+        <v>6</v>
       </c>
       <c r="Q245">
-        <v>2.7</v>
+        <v>11</v>
       </c>
       <c r="R245">
-        <v>0</v>
+        <v>-1.75</v>
       </c>
       <c r="S245">
-        <v>1.875</v>
+        <v>1.975</v>
       </c>
       <c r="T245">
-        <v>1.925</v>
+        <v>1.825</v>
       </c>
       <c r="U245">
-        <v>1.75</v>
+        <v>2.25</v>
       </c>
       <c r="V245">
         <v>1.8</v>
@@ -23041,25 +23041,25 @@
         <v>2</v>
       </c>
       <c r="X245">
-        <v>-1</v>
+        <v>0.222</v>
       </c>
       <c r="Y245">
-        <v>1.75</v>
+        <v>-1</v>
       </c>
       <c r="Z245">
         <v>-1</v>
       </c>
       <c r="AA245">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AB245">
-        <v>0</v>
+        <v>0.825</v>
       </c>
       <c r="AC245">
-        <v>0.4</v>
+        <v>-1</v>
       </c>
       <c r="AD245">
-        <v>-0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="246" spans="1:30">
@@ -23067,7 +23067,7 @@
         <v>244</v>
       </c>
       <c r="B246">
-        <v>8245123</v>
+        <v>8245124</v>
       </c>
       <c r="C246" t="s">
         <v>29</v>
@@ -23076,76 +23076,76 @@
         <v>45438.53125</v>
       </c>
       <c r="E246" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="F246" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="G246">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H246">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K246" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L246">
-        <v>2.1</v>
+        <v>1.727</v>
       </c>
       <c r="M246">
-        <v>3.25</v>
+        <v>3.2</v>
       </c>
       <c r="N246">
-        <v>3</v>
+        <v>4.5</v>
       </c>
       <c r="O246">
-        <v>2.3</v>
+        <v>1.5</v>
       </c>
       <c r="P246">
-        <v>3</v>
+        <v>3.8</v>
       </c>
       <c r="Q246">
-        <v>2.875</v>
+        <v>5.25</v>
       </c>
       <c r="R246">
-        <v>-0.25</v>
+        <v>-1</v>
       </c>
       <c r="S246">
-        <v>2.05</v>
+        <v>1.975</v>
       </c>
       <c r="T246">
-        <v>1.75</v>
+        <v>1.825</v>
       </c>
       <c r="U246">
-        <v>2</v>
+        <v>2.25</v>
       </c>
       <c r="V246">
-        <v>1.975</v>
+        <v>1.95</v>
       </c>
       <c r="W246">
-        <v>1.825</v>
+        <v>1.85</v>
       </c>
       <c r="X246">
-        <v>-1</v>
+        <v>0.5</v>
       </c>
       <c r="Y246">
         <v>-1</v>
       </c>
       <c r="Z246">
-        <v>1.875</v>
+        <v>-1</v>
       </c>
       <c r="AA246">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AB246">
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="AC246">
         <v>-1</v>
       </c>
       <c r="AD246">
-        <v>0.825</v>
+        <v>0.8500000000000001</v>
       </c>
     </row>
     <row r="247" spans="1:30">
@@ -23153,7 +23153,7 @@
         <v>245</v>
       </c>
       <c r="B247">
-        <v>8245118</v>
+        <v>8245121</v>
       </c>
       <c r="C247" t="s">
         <v>29</v>
@@ -23162,76 +23162,76 @@
         <v>45438.53125</v>
       </c>
       <c r="E247" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F247" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="G247">
         <v>1</v>
       </c>
       <c r="H247">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K247" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="L247">
-        <v>1.666</v>
+        <v>2.5</v>
       </c>
       <c r="M247">
-        <v>3.4</v>
+        <v>2.75</v>
       </c>
       <c r="N247">
-        <v>4.5</v>
+        <v>2.875</v>
       </c>
       <c r="O247">
-        <v>1.533</v>
+        <v>2.6</v>
       </c>
       <c r="P247">
-        <v>3.5</v>
+        <v>2.75</v>
       </c>
       <c r="Q247">
-        <v>5.75</v>
+        <v>2.7</v>
       </c>
       <c r="R247">
-        <v>-0.75</v>
+        <v>0</v>
       </c>
       <c r="S247">
-        <v>1.775</v>
+        <v>1.875</v>
       </c>
       <c r="T247">
-        <v>2.025</v>
+        <v>1.925</v>
       </c>
       <c r="U247">
-        <v>2.25</v>
+        <v>1.75</v>
       </c>
       <c r="V247">
-        <v>1.975</v>
+        <v>1.8</v>
       </c>
       <c r="W247">
-        <v>1.825</v>
+        <v>2</v>
       </c>
       <c r="X247">
-        <v>0.5329999999999999</v>
+        <v>-1</v>
       </c>
       <c r="Y247">
-        <v>-1</v>
+        <v>1.75</v>
       </c>
       <c r="Z247">
         <v>-1</v>
       </c>
       <c r="AA247">
-        <v>0.3875</v>
+        <v>0</v>
       </c>
       <c r="AB247">
+        <v>0</v>
+      </c>
+      <c r="AC247">
+        <v>0.4</v>
+      </c>
+      <c r="AD247">
         <v>-0.5</v>
-      </c>
-      <c r="AC247">
-        <v>-1</v>
-      </c>
-      <c r="AD247">
-        <v>0.825</v>
       </c>
     </row>
     <row r="248" spans="1:30">
@@ -23325,7 +23325,7 @@
         <v>247</v>
       </c>
       <c r="B249">
-        <v>8245120</v>
+        <v>8245118</v>
       </c>
       <c r="C249" t="s">
         <v>29</v>
@@ -23334,76 +23334,76 @@
         <v>45438.53125</v>
       </c>
       <c r="E249" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="F249" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="G249">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H249">
         <v>0</v>
       </c>
       <c r="K249" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="L249">
-        <v>1.5</v>
+        <v>1.666</v>
       </c>
       <c r="M249">
         <v>3.4</v>
       </c>
       <c r="N249">
-        <v>6.5</v>
+        <v>4.5</v>
       </c>
       <c r="O249">
-        <v>1.45</v>
+        <v>1.533</v>
       </c>
       <c r="P249">
         <v>3.5</v>
       </c>
       <c r="Q249">
-        <v>7</v>
+        <v>5.75</v>
       </c>
       <c r="R249">
-        <v>-1</v>
+        <v>-0.75</v>
       </c>
       <c r="S249">
-        <v>1.825</v>
+        <v>1.775</v>
       </c>
       <c r="T249">
-        <v>1.975</v>
+        <v>2.025</v>
       </c>
       <c r="U249">
         <v>2.25</v>
       </c>
       <c r="V249">
-        <v>1.875</v>
+        <v>1.975</v>
       </c>
       <c r="W249">
-        <v>1.925</v>
+        <v>1.825</v>
       </c>
       <c r="X249">
-        <v>-1</v>
+        <v>0.5329999999999999</v>
       </c>
       <c r="Y249">
-        <v>2.5</v>
+        <v>-1</v>
       </c>
       <c r="Z249">
         <v>-1</v>
       </c>
       <c r="AA249">
-        <v>-1</v>
+        <v>0.3875</v>
       </c>
       <c r="AB249">
-        <v>0.9750000000000001</v>
+        <v>-0.5</v>
       </c>
       <c r="AC249">
         <v>-1</v>
       </c>
       <c r="AD249">
-        <v>0.925</v>
+        <v>0.825</v>
       </c>
     </row>
     <row r="250" spans="1:30">
@@ -23411,7 +23411,7 @@
         <v>248</v>
       </c>
       <c r="B250">
-        <v>8245122</v>
+        <v>8245123</v>
       </c>
       <c r="C250" t="s">
         <v>29</v>
@@ -23420,76 +23420,76 @@
         <v>45438.53125</v>
       </c>
       <c r="E250" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F250" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G250">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H250">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K250" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="L250">
-        <v>1.222</v>
+        <v>2.1</v>
       </c>
       <c r="M250">
-        <v>5</v>
+        <v>3.25</v>
       </c>
       <c r="N250">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="O250">
-        <v>1.222</v>
+        <v>2.3</v>
       </c>
       <c r="P250">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="Q250">
-        <v>11</v>
+        <v>2.875</v>
       </c>
       <c r="R250">
-        <v>-1.75</v>
+        <v>-0.25</v>
       </c>
       <c r="S250">
+        <v>2.05</v>
+      </c>
+      <c r="T250">
+        <v>1.75</v>
+      </c>
+      <c r="U250">
+        <v>2</v>
+      </c>
+      <c r="V250">
         <v>1.975</v>
       </c>
-      <c r="T250">
+      <c r="W250">
         <v>1.825</v>
       </c>
-      <c r="U250">
-        <v>2.25</v>
-      </c>
-      <c r="V250">
-        <v>1.8</v>
-      </c>
-      <c r="W250">
-        <v>2</v>
-      </c>
       <c r="X250">
-        <v>0.222</v>
+        <v>-1</v>
       </c>
       <c r="Y250">
         <v>-1</v>
       </c>
       <c r="Z250">
-        <v>-1</v>
+        <v>1.875</v>
       </c>
       <c r="AA250">
         <v>-1</v>
       </c>
       <c r="AB250">
+        <v>0.75</v>
+      </c>
+      <c r="AC250">
+        <v>-1</v>
+      </c>
+      <c r="AD250">
         <v>0.825</v>
-      </c>
-      <c r="AC250">
-        <v>-1</v>
-      </c>
-      <c r="AD250">
-        <v>1</v>
       </c>
     </row>
     <row r="251" spans="1:30">
@@ -23497,7 +23497,7 @@
         <v>249</v>
       </c>
       <c r="B251">
-        <v>8245124</v>
+        <v>8245120</v>
       </c>
       <c r="C251" t="s">
         <v>29</v>
@@ -23506,76 +23506,76 @@
         <v>45438.53125</v>
       </c>
       <c r="E251" t="s">
+        <v>38</v>
+      </c>
+      <c r="F251" t="s">
         <v>41</v>
       </c>
-      <c r="F251" t="s">
-        <v>45</v>
-      </c>
       <c r="G251">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H251">
         <v>0</v>
       </c>
       <c r="K251" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="L251">
-        <v>1.727</v>
+        <v>1.5</v>
       </c>
       <c r="M251">
-        <v>3.2</v>
+        <v>3.4</v>
       </c>
       <c r="N251">
-        <v>4.5</v>
+        <v>6.5</v>
       </c>
       <c r="O251">
-        <v>1.5</v>
+        <v>1.45</v>
       </c>
       <c r="P251">
-        <v>3.8</v>
+        <v>3.5</v>
       </c>
       <c r="Q251">
-        <v>5.25</v>
+        <v>7</v>
       </c>
       <c r="R251">
         <v>-1</v>
       </c>
       <c r="S251">
+        <v>1.825</v>
+      </c>
+      <c r="T251">
         <v>1.975</v>
-      </c>
-      <c r="T251">
-        <v>1.825</v>
       </c>
       <c r="U251">
         <v>2.25</v>
       </c>
       <c r="V251">
-        <v>1.95</v>
+        <v>1.875</v>
       </c>
       <c r="W251">
-        <v>1.85</v>
+        <v>1.925</v>
       </c>
       <c r="X251">
-        <v>0.5</v>
+        <v>-1</v>
       </c>
       <c r="Y251">
-        <v>-1</v>
+        <v>2.5</v>
       </c>
       <c r="Z251">
         <v>-1</v>
       </c>
       <c r="AA251">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AB251">
-        <v>0</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="AC251">
         <v>-1</v>
       </c>
       <c r="AD251">
-        <v>0.8500000000000001</v>
+        <v>0.925</v>
       </c>
     </row>
     <row r="252" spans="1:30">

</xml_diff>